<commit_message>
Actu excel y draft assistant
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -535,7 +535,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N72"/>
+  <dimension ref="A3:N75"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5589,6 +5589,222 @@
       <c r="N72" s="16" t="inlineStr">
         <is>
           <t>20250710T122719.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="13" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="B73" s="13" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C73" s="13" t="inlineStr">
+        <is>
+          <t>SHELLY</t>
+        </is>
+      </c>
+      <c r="D73" s="14" t="inlineStr">
+        <is>
+          <t>EL PRIMO</t>
+        </is>
+      </c>
+      <c r="E73" s="14" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="F73" s="14" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="G73" s="15" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H73" s="16" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="I73" s="16" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825🇱🇻</t>
+        </is>
+      </c>
+      <c r="J73" s="16" t="inlineStr">
+        <is>
+          <t>SK|OPE🏒</t>
+        </is>
+      </c>
+      <c r="K73" s="16" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="L73" s="16" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="M73" s="16" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="N73" s="16" t="inlineStr">
+        <is>
+          <t>20250710T133708.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="13" t="inlineStr">
+        <is>
+          <t>SHELLY</t>
+        </is>
+      </c>
+      <c r="B74" s="13" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C74" s="13" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D74" s="14" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="E74" s="14" t="inlineStr">
+        <is>
+          <t>EL PRIMO</t>
+        </is>
+      </c>
+      <c r="F74" s="14" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G74" s="15" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H74" s="16" t="inlineStr">
+        <is>
+          <t>SK|OPE🏒</t>
+        </is>
+      </c>
+      <c r="I74" s="16" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="J74" s="16" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825🇱🇻</t>
+        </is>
+      </c>
+      <c r="K74" s="16" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L74" s="16" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="M74" s="16" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N74" s="16" t="inlineStr">
+        <is>
+          <t>20250710T133325.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="13" t="inlineStr">
+        <is>
+          <t>SHELLY</t>
+        </is>
+      </c>
+      <c r="B75" s="13" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C75" s="13" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D75" s="14" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="E75" s="14" t="inlineStr">
+        <is>
+          <t>EL PRIMO</t>
+        </is>
+      </c>
+      <c r="F75" s="14" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G75" s="15" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H75" s="16" t="inlineStr">
+        <is>
+          <t>SK|OPE🏒</t>
+        </is>
+      </c>
+      <c r="I75" s="16" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="J75" s="16" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825🇱🇻</t>
+        </is>
+      </c>
+      <c r="K75" s="16" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L75" s="16" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="M75" s="16" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N75" s="16" t="inlineStr">
+        <is>
+          <t>20250710T133141.000Z</t>
         </is>
       </c>
     </row>
@@ -13417,7 +13633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N74"/>
+  <dimension ref="A3:N77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18606,6 +18822,222 @@
       <c r="N74" s="16" t="inlineStr">
         <is>
           <t>20250710T130614.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="13" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="B75" s="13" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C75" s="13" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="D75" s="14" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E75" s="14" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F75" s="14" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G75" s="17" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H75" s="16" t="inlineStr">
+        <is>
+          <t>NOVO|26is</t>
+        </is>
+      </c>
+      <c r="I75" s="16" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J75" s="16" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K75" s="16" t="inlineStr">
+        <is>
+          <t>TH|IKAUSSA</t>
+        </is>
+      </c>
+      <c r="L75" s="16" t="inlineStr">
+        <is>
+          <t>TH|Code: LeNain</t>
+        </is>
+      </c>
+      <c r="M75" s="16" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N75" s="16" t="inlineStr">
+        <is>
+          <t>20250710T132132.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="13" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="B76" s="13" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C76" s="13" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="D76" s="14" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E76" s="14" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F76" s="14" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G76" s="15" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H76" s="16" t="inlineStr">
+        <is>
+          <t>NOVO|26is</t>
+        </is>
+      </c>
+      <c r="I76" s="16" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J76" s="16" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K76" s="16" t="inlineStr">
+        <is>
+          <t>TH|IKAUSSA</t>
+        </is>
+      </c>
+      <c r="L76" s="16" t="inlineStr">
+        <is>
+          <t>TH|Code: LeNain</t>
+        </is>
+      </c>
+      <c r="M76" s="16" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N76" s="16" t="inlineStr">
+        <is>
+          <t>20250710T131852.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="13" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="B77" s="13" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C77" s="13" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="D77" s="14" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E77" s="14" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F77" s="14" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G77" s="17" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H77" s="16" t="inlineStr">
+        <is>
+          <t>NOVO|26is</t>
+        </is>
+      </c>
+      <c r="I77" s="16" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J77" s="16" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K77" s="16" t="inlineStr">
+        <is>
+          <t>TH|IKAUSSA</t>
+        </is>
+      </c>
+      <c r="L77" s="16" t="inlineStr">
+        <is>
+          <t>TH|Code: LeNain</t>
+        </is>
+      </c>
+      <c r="M77" s="16" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N77" s="16" t="inlineStr">
+        <is>
+          <t>20250710T131554.000Z</t>
         </is>
       </c>
     </row>
@@ -22671,7 +23103,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N52"/>
+  <dimension ref="A3:N55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26276,6 +26708,222 @@
       <c r="N52" s="16" t="inlineStr">
         <is>
           <t>20250710T102009.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="13" t="inlineStr">
+        <is>
+          <t>SURGE</t>
+        </is>
+      </c>
+      <c r="B53" s="13" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="C53" s="13" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="D53" s="14" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="E53" s="14" t="inlineStr">
+        <is>
+          <t>FANG</t>
+        </is>
+      </c>
+      <c r="F53" s="14" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="G53" s="15" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H53" s="16" t="inlineStr">
+        <is>
+          <t>nyamura</t>
+        </is>
+      </c>
+      <c r="I53" s="16" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J53" s="16" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K53" s="16" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="L53" s="16" t="inlineStr">
+        <is>
+          <t>ZETA|Sitetampo</t>
+        </is>
+      </c>
+      <c r="M53" s="16" t="inlineStr">
+        <is>
+          <t>ZETA|Sizuku</t>
+        </is>
+      </c>
+      <c r="N53" s="16" t="inlineStr">
+        <is>
+          <t>20250710T133706.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="13" t="inlineStr">
+        <is>
+          <t>SURGE</t>
+        </is>
+      </c>
+      <c r="B54" s="13" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="C54" s="13" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="D54" s="14" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="E54" s="14" t="inlineStr">
+        <is>
+          <t>FANG</t>
+        </is>
+      </c>
+      <c r="F54" s="14" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="G54" s="17" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H54" s="16" t="inlineStr">
+        <is>
+          <t>nyamura</t>
+        </is>
+      </c>
+      <c r="I54" s="16" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J54" s="16" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K54" s="16" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="L54" s="16" t="inlineStr">
+        <is>
+          <t>ZETA|Sitetampo</t>
+        </is>
+      </c>
+      <c r="M54" s="16" t="inlineStr">
+        <is>
+          <t>ZETA|Sizuku</t>
+        </is>
+      </c>
+      <c r="N54" s="16" t="inlineStr">
+        <is>
+          <t>20250710T133513.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="13" t="inlineStr">
+        <is>
+          <t>SURGE</t>
+        </is>
+      </c>
+      <c r="B55" s="13" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="C55" s="13" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="D55" s="14" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="E55" s="14" t="inlineStr">
+        <is>
+          <t>FANG</t>
+        </is>
+      </c>
+      <c r="F55" s="14" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="G55" s="15" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H55" s="16" t="inlineStr">
+        <is>
+          <t>nyamura</t>
+        </is>
+      </c>
+      <c r="I55" s="16" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J55" s="16" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K55" s="16" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="L55" s="16" t="inlineStr">
+        <is>
+          <t>ZETA|Sitetampo</t>
+        </is>
+      </c>
+      <c r="M55" s="16" t="inlineStr">
+        <is>
+          <t>ZETA|Sizuku</t>
+        </is>
+      </c>
+      <c r="N55" s="16" t="inlineStr">
+        <is>
+          <t>20250710T133240.000Z</t>
         </is>
       </c>
     </row>
@@ -33005,7 +33653,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N57"/>
+  <dimension ref="A3:N61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -36970,6 +37618,294 @@
       <c r="N57" s="16" t="inlineStr">
         <is>
           <t>20250710T125159.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="13" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="B58" s="13" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C58" s="13" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="D58" s="14" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="E58" s="14" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="F58" s="14" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="G58" s="17" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H58" s="16" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="I58" s="16" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="J58" s="16" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="K58" s="16" t="inlineStr">
+        <is>
+          <t>KDS|Decaii</t>
+        </is>
+      </c>
+      <c r="L58" s="16" t="inlineStr">
+        <is>
+          <t>KDS|Ćiro</t>
+        </is>
+      </c>
+      <c r="M58" s="16" t="inlineStr">
+        <is>
+          <t>KDS|Remica</t>
+        </is>
+      </c>
+      <c r="N58" s="16" t="inlineStr">
+        <is>
+          <t>20250710T132920.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="13" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="B59" s="13" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C59" s="13" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="D59" s="14" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="E59" s="14" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="F59" s="14" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="G59" s="17" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H59" s="16" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="I59" s="16" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="J59" s="16" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="K59" s="16" t="inlineStr">
+        <is>
+          <t>KDS|Decaii</t>
+        </is>
+      </c>
+      <c r="L59" s="16" t="inlineStr">
+        <is>
+          <t>KDS|Ćiro</t>
+        </is>
+      </c>
+      <c r="M59" s="16" t="inlineStr">
+        <is>
+          <t>KDS|Remica</t>
+        </is>
+      </c>
+      <c r="N59" s="16" t="inlineStr">
+        <is>
+          <t>20250710T132702.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="13" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="B60" s="13" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C60" s="13" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="D60" s="14" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="E60" s="14" t="inlineStr">
+        <is>
+          <t>MANDY</t>
+        </is>
+      </c>
+      <c r="F60" s="14" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="G60" s="17" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H60" s="16" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="I60" s="16" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="J60" s="16" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="K60" s="16" t="inlineStr">
+        <is>
+          <t>KDS|Decaii</t>
+        </is>
+      </c>
+      <c r="L60" s="16" t="inlineStr">
+        <is>
+          <t>KDS|Remica</t>
+        </is>
+      </c>
+      <c r="M60" s="16" t="inlineStr">
+        <is>
+          <t>KDS|Ćiro</t>
+        </is>
+      </c>
+      <c r="N60" s="16" t="inlineStr">
+        <is>
+          <t>20250710T133825.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="13" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B61" s="13" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="C61" s="13" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="D61" s="14" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="E61" s="14" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="F61" s="14" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="G61" s="15" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H61" s="16" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="I61" s="16" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="J61" s="16" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="K61" s="16" t="inlineStr">
+        <is>
+          <t>KDS|Decaii</t>
+        </is>
+      </c>
+      <c r="L61" s="16" t="inlineStr">
+        <is>
+          <t>KDS|Remica</t>
+        </is>
+      </c>
+      <c r="M61" s="16" t="inlineStr">
+        <is>
+          <t>KDS|Ćiro</t>
+        </is>
+      </c>
+      <c r="N61" s="16" t="inlineStr">
+        <is>
+          <t>20250710T133207.000Z</t>
         </is>
       </c>
     </row>
@@ -36984,7 +37920,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N76"/>
+  <dimension ref="A3:N88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -42317,6 +43253,870 @@
       <c r="N76" s="16" t="inlineStr">
         <is>
           <t>20250710T131044.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="13" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B77" s="13" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C77" s="13" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="D77" s="14" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="E77" s="14" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F77" s="14" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="G77" s="15" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H77" s="16" t="inlineStr">
+        <is>
+          <t>nyamura</t>
+        </is>
+      </c>
+      <c r="I77" s="16" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J77" s="16" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K77" s="16" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="L77" s="16" t="inlineStr">
+        <is>
+          <t>ZETA|Sizuku</t>
+        </is>
+      </c>
+      <c r="M77" s="16" t="inlineStr">
+        <is>
+          <t>ZETA|Sitetampo</t>
+        </is>
+      </c>
+      <c r="N77" s="16" t="inlineStr">
+        <is>
+          <t>20250710T132428.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="13" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B78" s="13" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C78" s="13" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="D78" s="14" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="E78" s="14" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F78" s="14" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="G78" s="17" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H78" s="16" t="inlineStr">
+        <is>
+          <t>nyamura</t>
+        </is>
+      </c>
+      <c r="I78" s="16" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J78" s="16" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K78" s="16" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="L78" s="16" t="inlineStr">
+        <is>
+          <t>ZETA|Sizuku</t>
+        </is>
+      </c>
+      <c r="M78" s="16" t="inlineStr">
+        <is>
+          <t>ZETA|Sitetampo</t>
+        </is>
+      </c>
+      <c r="N78" s="16" t="inlineStr">
+        <is>
+          <t>20250710T132313.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="13" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B79" s="13" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C79" s="13" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="D79" s="14" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="E79" s="14" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F79" s="14" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="G79" s="15" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H79" s="16" t="inlineStr">
+        <is>
+          <t>nyamura</t>
+        </is>
+      </c>
+      <c r="I79" s="16" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J79" s="16" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K79" s="16" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="L79" s="16" t="inlineStr">
+        <is>
+          <t>ZETA|Sizuku</t>
+        </is>
+      </c>
+      <c r="M79" s="16" t="inlineStr">
+        <is>
+          <t>ZETA|Sitetampo</t>
+        </is>
+      </c>
+      <c r="N79" s="16" t="inlineStr">
+        <is>
+          <t>20250710T132112.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="13" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="B80" s="13" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="C80" s="13" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D80" s="14" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E80" s="14" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F80" s="14" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="G80" s="15" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H80" s="16" t="inlineStr">
+        <is>
+          <t>nyamura</t>
+        </is>
+      </c>
+      <c r="I80" s="16" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J80" s="16" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K80" s="16" t="inlineStr">
+        <is>
+          <t>ZETA|Sizuku</t>
+        </is>
+      </c>
+      <c r="L80" s="16" t="inlineStr">
+        <is>
+          <t>ZETA|Sitetampo</t>
+        </is>
+      </c>
+      <c r="M80" s="16" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N80" s="16" t="inlineStr">
+        <is>
+          <t>20250710T131315.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="13" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="B81" s="13" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="C81" s="13" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D81" s="14" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E81" s="14" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="F81" s="14" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G81" s="17" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H81" s="16" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="I81" s="16" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="J81" s="16" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="K81" s="16" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="L81" s="16" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="M81" s="16" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="N81" s="16" t="inlineStr">
+        <is>
+          <t>20250710T133012.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="13" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="B82" s="13" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="C82" s="13" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D82" s="14" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E82" s="14" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="F82" s="14" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G82" s="17" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H82" s="16" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="I82" s="16" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="J82" s="16" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="K82" s="16" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="L82" s="16" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="M82" s="16" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="N82" s="16" t="inlineStr">
+        <is>
+          <t>20250710T132722.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="13" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="B83" s="13" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C83" s="13" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D83" s="14" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E83" s="14" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="F83" s="14" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="G83" s="17" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H83" s="16" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825🇱🇻</t>
+        </is>
+      </c>
+      <c r="I83" s="16" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="J83" s="16" t="inlineStr">
+        <is>
+          <t>SK|OPE🏒</t>
+        </is>
+      </c>
+      <c r="K83" s="16" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="L83" s="16" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="M83" s="16" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="N83" s="16" t="inlineStr">
+        <is>
+          <t>20250710T132616.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="13" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="B84" s="13" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C84" s="13" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D84" s="14" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E84" s="14" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="F84" s="14" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="G84" s="15" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H84" s="16" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825🇱🇻</t>
+        </is>
+      </c>
+      <c r="I84" s="16" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="J84" s="16" t="inlineStr">
+        <is>
+          <t>SK|OPE🏒</t>
+        </is>
+      </c>
+      <c r="K84" s="16" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="L84" s="16" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="M84" s="16" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="N84" s="16" t="inlineStr">
+        <is>
+          <t>20250710T132435.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="13" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="B85" s="13" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C85" s="13" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D85" s="14" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E85" s="14" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="F85" s="14" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="G85" s="17" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H85" s="16" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825🇱🇻</t>
+        </is>
+      </c>
+      <c r="I85" s="16" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="J85" s="16" t="inlineStr">
+        <is>
+          <t>SK|OPE🏒</t>
+        </is>
+      </c>
+      <c r="K85" s="16" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="L85" s="16" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="M85" s="16" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="N85" s="16" t="inlineStr">
+        <is>
+          <t>20250710T132323.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="13" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B86" s="13" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="C86" s="13" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="D86" s="14" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E86" s="14" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F86" s="14" t="inlineStr">
+        <is>
+          <t>EDGAR</t>
+        </is>
+      </c>
+      <c r="G86" s="15" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H86" s="16" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825🇱🇻</t>
+        </is>
+      </c>
+      <c r="I86" s="16" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="J86" s="16" t="inlineStr">
+        <is>
+          <t>SK|OPE🏒</t>
+        </is>
+      </c>
+      <c r="K86" s="16" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L86" s="16" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="M86" s="16" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N86" s="16" t="inlineStr">
+        <is>
+          <t>20250710T131502.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="13" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="B87" s="13" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C87" s="13" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D87" s="14" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="E87" s="14" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="F87" s="14" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="G87" s="17" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H87" s="16" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="I87" s="16" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="J87" s="16" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="K87" s="16" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="L87" s="16" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="M87" s="16" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="N87" s="16" t="inlineStr">
+        <is>
+          <t>20250710T133743.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="13" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="B88" s="13" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C88" s="13" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D88" s="14" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="E88" s="14" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="F88" s="14" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="G88" s="17" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H88" s="16" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="I88" s="16" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="J88" s="16" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="K88" s="16" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="L88" s="16" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="M88" s="16" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="N88" s="16" t="inlineStr">
+        <is>
+          <t>20250710T133557.000Z</t>
         </is>
       </c>
     </row>
@@ -50001,7 +51801,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N105"/>
+  <dimension ref="A3:N108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="S28" sqref="S28"/>
@@ -57422,6 +59222,222 @@
       <c r="N105" s="16" t="inlineStr">
         <is>
           <t>20250710T130350.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="13" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B106" s="13" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C106" s="13" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D106" s="14" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="E106" s="14" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="F106" s="14" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G106" s="15" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H106" s="16" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="I106" s="16" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="J106" s="16" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="K106" s="16" t="inlineStr">
+        <is>
+          <t>KDS|Decaii</t>
+        </is>
+      </c>
+      <c r="L106" s="16" t="inlineStr">
+        <is>
+          <t>KDS|Remica</t>
+        </is>
+      </c>
+      <c r="M106" s="16" t="inlineStr">
+        <is>
+          <t>KDS|Ćiro</t>
+        </is>
+      </c>
+      <c r="N106" s="16" t="inlineStr">
+        <is>
+          <t>20250710T131956.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="13" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B107" s="13" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C107" s="13" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D107" s="14" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="E107" s="14" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="F107" s="14" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G107" s="15" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H107" s="16" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="I107" s="16" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="J107" s="16" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="K107" s="16" t="inlineStr">
+        <is>
+          <t>KDS|Decaii</t>
+        </is>
+      </c>
+      <c r="L107" s="16" t="inlineStr">
+        <is>
+          <t>KDS|Remica</t>
+        </is>
+      </c>
+      <c r="M107" s="16" t="inlineStr">
+        <is>
+          <t>KDS|Ćiro</t>
+        </is>
+      </c>
+      <c r="N107" s="16" t="inlineStr">
+        <is>
+          <t>20250710T131807.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="13" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B108" s="13" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C108" s="13" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D108" s="14" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="E108" s="14" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="F108" s="14" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G108" s="17" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H108" s="16" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="I108" s="16" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="J108" s="16" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="K108" s="16" t="inlineStr">
+        <is>
+          <t>KDS|Decaii</t>
+        </is>
+      </c>
+      <c r="L108" s="16" t="inlineStr">
+        <is>
+          <t>KDS|Remica</t>
+        </is>
+      </c>
+      <c r="M108" s="16" t="inlineStr">
+        <is>
+          <t>KDS|Ćiro</t>
+        </is>
+      </c>
+      <c r="N108" s="16" t="inlineStr">
+        <is>
+          <t>20250710T131641.000Z</t>
         </is>
       </c>
     </row>
@@ -57436,7 +59452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N45"/>
+  <dimension ref="A3:N52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -60537,6 +62553,510 @@
       <c r="N45" s="16" t="inlineStr">
         <is>
           <t>20250710T124655.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="13" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B46" s="13" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="C46" s="13" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="D46" s="14" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="E46" s="14" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F46" s="14" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G46" s="15" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H46" s="16" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="I46" s="16" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="J46" s="16" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="K46" s="16" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="L46" s="16" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="M46" s="16" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="N46" s="16" t="inlineStr">
+        <is>
+          <t>20250710T132037.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="13" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B47" s="13" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="C47" s="13" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="D47" s="14" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="E47" s="14" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F47" s="14" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G47" s="17" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H47" s="16" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="I47" s="16" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="J47" s="16" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="K47" s="16" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="L47" s="16" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="M47" s="16" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="N47" s="16" t="inlineStr">
+        <is>
+          <t>20250710T131935.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="13" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B48" s="13" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="C48" s="13" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="D48" s="14" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="E48" s="14" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F48" s="14" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G48" s="15" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H48" s="16" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="I48" s="16" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="J48" s="16" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="K48" s="16" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="L48" s="16" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="M48" s="16" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="N48" s="16" t="inlineStr">
+        <is>
+          <t>20250710T131841.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="13" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B49" s="13" t="inlineStr">
+        <is>
+          <t>JACKY</t>
+        </is>
+      </c>
+      <c r="C49" s="13" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="D49" s="14" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="E49" s="14" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="F49" s="14" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G49" s="17" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H49" s="16" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="I49" s="16" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="J49" s="16" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="K49" s="16" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="L49" s="16" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="M49" s="16" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="N49" s="16" t="inlineStr">
+        <is>
+          <t>20250710T131335.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="13" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="B50" s="13" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C50" s="13" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D50" s="14" t="inlineStr">
+        <is>
+          <t>EL PRIMO</t>
+        </is>
+      </c>
+      <c r="E50" s="14" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="F50" s="14" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="G50" s="15" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H50" s="16" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="I50" s="16" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="J50" s="16" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="K50" s="16" t="inlineStr">
+        <is>
+          <t>Isee in Bush</t>
+        </is>
+      </c>
+      <c r="L50" s="16" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="M50" s="16" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="N50" s="16" t="inlineStr">
+        <is>
+          <t>20250710T132312.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="13" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="B51" s="13" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C51" s="13" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D51" s="14" t="inlineStr">
+        <is>
+          <t>EL PRIMO</t>
+        </is>
+      </c>
+      <c r="E51" s="14" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="F51" s="14" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="G51" s="15" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H51" s="16" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="I51" s="16" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="J51" s="16" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="K51" s="16" t="inlineStr">
+        <is>
+          <t>Isee in Bush</t>
+        </is>
+      </c>
+      <c r="L51" s="16" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="M51" s="16" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="N51" s="16" t="inlineStr">
+        <is>
+          <t>20250710T131953.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="13" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="B52" s="13" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C52" s="13" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D52" s="14" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E52" s="14" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F52" s="14" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="G52" s="15" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H52" s="16" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="I52" s="16" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="J52" s="16" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="K52" s="16" t="inlineStr">
+        <is>
+          <t>Isee in Bush</t>
+        </is>
+      </c>
+      <c r="L52" s="16" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="M52" s="16" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="N52" s="16" t="inlineStr">
+        <is>
+          <t>20250710T131431.000Z</t>
         </is>
       </c>
     </row>
@@ -70672,7 +73192,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N76"/>
+  <dimension ref="A3:N80"/>
   <sheetViews>
     <sheetView topLeftCell="A41" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -76011,6 +78531,294 @@
         </is>
       </c>
     </row>
+    <row r="77">
+      <c r="A77" s="13" t="inlineStr">
+        <is>
+          <t>JACKY</t>
+        </is>
+      </c>
+      <c r="B77" s="13" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C77" s="13" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="D77" s="14" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="E77" s="14" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="F77" s="14" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="G77" s="15" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H77" s="16" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="I77" s="16" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="J77" s="16" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="K77" s="16" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L77" s="16" t="inlineStr">
+        <is>
+          <t>Isee in Bush</t>
+        </is>
+      </c>
+      <c r="M77" s="16" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="N77" s="16" t="inlineStr">
+        <is>
+          <t>20250710T132858.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="13" t="inlineStr">
+        <is>
+          <t>CHESTER</t>
+        </is>
+      </c>
+      <c r="B78" s="13" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C78" s="13" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="D78" s="14" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="E78" s="14" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F78" s="14" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="G78" s="15" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H78" s="16" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="I78" s="16" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="J78" s="16" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="K78" s="16" t="inlineStr">
+        <is>
+          <t>Isee in Bush</t>
+        </is>
+      </c>
+      <c r="L78" s="16" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="M78" s="16" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="N78" s="16" t="inlineStr">
+        <is>
+          <t>20250710T133651.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="13" t="inlineStr">
+        <is>
+          <t>CHESTER</t>
+        </is>
+      </c>
+      <c r="B79" s="13" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C79" s="13" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="D79" s="14" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="E79" s="14" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F79" s="14" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="G79" s="15" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H79" s="16" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="I79" s="16" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="J79" s="16" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="K79" s="16" t="inlineStr">
+        <is>
+          <t>Isee in Bush</t>
+        </is>
+      </c>
+      <c r="L79" s="16" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="M79" s="16" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="N79" s="16" t="inlineStr">
+        <is>
+          <t>20250710T133551.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="13" t="inlineStr">
+        <is>
+          <t>JACKY</t>
+        </is>
+      </c>
+      <c r="B80" s="13" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C80" s="13" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="D80" s="14" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="E80" s="14" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="F80" s="14" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="G80" s="15" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H80" s="16" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="I80" s="16" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="J80" s="16" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="K80" s="16" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L80" s="16" t="inlineStr">
+        <is>
+          <t>Isee in Bush</t>
+        </is>
+      </c>
+      <c r="M80" s="16" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="N80" s="16" t="inlineStr">
+        <is>
+          <t>20250710T133209.000Z</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -76022,7 +78830,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N76"/>
+  <dimension ref="A3:N80"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -81358,6 +84166,294 @@
       <c r="N76" s="16" t="inlineStr">
         <is>
           <t>20250710T122827.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="13" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="B77" s="13" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="C77" s="13" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="D77" s="14" t="inlineStr">
+        <is>
+          <t>SPROUT</t>
+        </is>
+      </c>
+      <c r="E77" s="14" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F77" s="14" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="G77" s="15" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H77" s="16" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="I77" s="16" t="inlineStr">
+        <is>
+          <t>NOVO|26is</t>
+        </is>
+      </c>
+      <c r="J77" s="16" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K77" s="16" t="inlineStr">
+        <is>
+          <t>TH|IKAUSSA</t>
+        </is>
+      </c>
+      <c r="L77" s="16" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="M77" s="16" t="inlineStr">
+        <is>
+          <t>TH|Code: LeNain</t>
+        </is>
+      </c>
+      <c r="N77" s="16" t="inlineStr">
+        <is>
+          <t>20250710T132941.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="13" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="B78" s="13" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="C78" s="13" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="D78" s="14" t="inlineStr">
+        <is>
+          <t>SPROUT</t>
+        </is>
+      </c>
+      <c r="E78" s="14" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F78" s="14" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="G78" s="15" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H78" s="16" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="I78" s="16" t="inlineStr">
+        <is>
+          <t>NOVO|26is</t>
+        </is>
+      </c>
+      <c r="J78" s="16" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K78" s="16" t="inlineStr">
+        <is>
+          <t>TH|IKAUSSA</t>
+        </is>
+      </c>
+      <c r="L78" s="16" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="M78" s="16" t="inlineStr">
+        <is>
+          <t>TH|Code: LeNain</t>
+        </is>
+      </c>
+      <c r="N78" s="16" t="inlineStr">
+        <is>
+          <t>20250710T132818.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="13" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="B79" s="13" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="C79" s="13" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D79" s="14" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="E79" s="14" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="F79" s="14" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="G79" s="17" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H79" s="16" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="I79" s="16" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J79" s="16" t="inlineStr">
+        <is>
+          <t>NOVO|26is</t>
+        </is>
+      </c>
+      <c r="K79" s="16" t="inlineStr">
+        <is>
+          <t>TH|Code: LeNain</t>
+        </is>
+      </c>
+      <c r="L79" s="16" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="M79" s="16" t="inlineStr">
+        <is>
+          <t>TH|IKAUSSA</t>
+        </is>
+      </c>
+      <c r="N79" s="16" t="inlineStr">
+        <is>
+          <t>20250710T133931.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="13" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="B80" s="13" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="C80" s="13" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D80" s="14" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="E80" s="14" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="F80" s="14" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="G80" s="15" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H80" s="16" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="I80" s="16" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J80" s="16" t="inlineStr">
+        <is>
+          <t>NOVO|26is</t>
+        </is>
+      </c>
+      <c r="K80" s="16" t="inlineStr">
+        <is>
+          <t>TH|Code: LeNain</t>
+        </is>
+      </c>
+      <c r="L80" s="16" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="M80" s="16" t="inlineStr">
+        <is>
+          <t>TH|IKAUSSA</t>
+        </is>
+      </c>
+      <c r="N80" s="16" t="inlineStr">
+        <is>
+          <t>20250710T133638.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-23 16:24:20)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -451,7 +451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N28"/>
+  <dimension ref="A3:N29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2328,6 +2328,78 @@
       <c r="N28" s="3" t="inlineStr">
         <is>
           <t>20250719T005705.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B29" s="1" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="C29" s="1" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="inlineStr">
+        <is>
+          <t>SAM</t>
+        </is>
+      </c>
+      <c r="E29" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="F29" s="2" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="G29" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H29" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="I29" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="J29" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="K29" s="3" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="L29" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="M29" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="N29" s="3" t="inlineStr">
+        <is>
+          <t>20250723T141950.000Z</t>
         </is>
       </c>
     </row>
@@ -3858,7 +3930,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N4"/>
+  <dimension ref="A3:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4007,6 +4079,150 @@
       <c r="N4" s="3" t="inlineStr">
         <is>
           <t>20250720T182517.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="G5" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H5" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I5" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J5" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K5" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L5" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M5" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N5" s="3" t="inlineStr">
+        <is>
+          <t>20250723T142130.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="G6" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H6" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I6" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J6" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K6" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L6" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M6" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N6" s="3" t="inlineStr">
+        <is>
+          <t>20250723T141810.000Z</t>
         </is>
       </c>
     </row>
@@ -4256,7 +4472,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N13"/>
+  <dimension ref="A3:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5053,6 +5269,150 @@
       <c r="N13" s="3" t="inlineStr">
         <is>
           <t>20250722T142014.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>CHESTER</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>8-BIT</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G14" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H14" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="J14" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="K14" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L14" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M14" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="N14" s="3" t="inlineStr">
+        <is>
+          <t>20250723T142254.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>CHESTER</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>8-BIT</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G15" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H15" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="J15" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="K15" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L15" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M15" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="N15" s="3" t="inlineStr">
+        <is>
+          <t>20250723T142048.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-23 16:55:41)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -451,7 +451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N29"/>
+  <dimension ref="A3:N34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2400,6 +2400,366 @@
       <c r="N29" s="3" t="inlineStr">
         <is>
           <t>20250723T141950.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="B30" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="C30" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F30" s="2" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="G30" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H30" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="I30" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="J30" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K30" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L30" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="M30" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="N30" s="3" t="inlineStr">
+        <is>
+          <t>20250723T144828.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="B31" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="C31" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D31" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F31" s="2" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="G31" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H31" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="I31" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="J31" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K31" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L31" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="M31" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="N31" s="3" t="inlineStr">
+        <is>
+          <t>20250723T144544.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="F32" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="G32" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H32" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I32" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J32" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K32" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L32" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M32" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N32" s="3" t="inlineStr">
+        <is>
+          <t>20250723T144000.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B33" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="C33" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D33" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="E33" s="2" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="F33" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="G33" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H33" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I33" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J33" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K33" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L33" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M33" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N33" s="3" t="inlineStr">
+        <is>
+          <t>20250723T143711.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B34" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="C34" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="E34" s="2" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="F34" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="G34" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H34" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I34" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J34" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K34" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L34" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M34" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N34" s="3" t="inlineStr">
+        <is>
+          <t>20250723T143353.000Z</t>
         </is>
       </c>
     </row>
@@ -2865,7 +3225,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N6"/>
+  <dimension ref="A3:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3158,6 +3518,366 @@
       <c r="N6" s="3" t="inlineStr">
         <is>
           <t>20250723T140918.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="G7" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H7" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I7" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J7" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="K7" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="L7" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="M7" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="N7" s="3" t="inlineStr">
+        <is>
+          <t>20250723T145253.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>JESSIE</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="G8" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H8" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="I8" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J8" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="K8" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="L8" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="M8" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="N8" s="3" t="inlineStr">
+        <is>
+          <t>20250723T144637.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>JESSIE</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="G9" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H9" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="I9" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J9" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="K9" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="L9" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="M9" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="N9" s="3" t="inlineStr">
+        <is>
+          <t>20250723T144507.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>JESSIE</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="G10" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H10" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I10" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J10" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K10" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L10" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M10" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N10" s="3" t="inlineStr">
+        <is>
+          <t>20250723T142608.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>JESSIE</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="G11" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H11" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I11" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J11" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K11" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L11" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M11" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N11" s="3" t="inlineStr">
+        <is>
+          <t>20250723T142352.000Z</t>
         </is>
       </c>
     </row>
@@ -3930,7 +4650,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N6"/>
+  <dimension ref="A3:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4223,6 +4943,222 @@
       <c r="N6" s="3" t="inlineStr">
         <is>
           <t>20250723T141810.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G7" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H7" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I7" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J7" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K7" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L7" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M7" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N7" s="3" t="inlineStr">
+        <is>
+          <t>20250723T143253.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G8" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H8" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I8" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J8" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K8" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L8" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M8" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N8" s="3" t="inlineStr">
+        <is>
+          <t>20250723T143033.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="G9" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H9" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I9" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J9" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K9" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L9" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M9" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N9" s="3" t="inlineStr">
+        <is>
+          <t>20250723T142404.000Z</t>
         </is>
       </c>
     </row>
@@ -4472,7 +5408,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N15"/>
+  <dimension ref="A3:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5413,6 +6349,150 @@
       <c r="N15" s="3" t="inlineStr">
         <is>
           <t>20250723T142048.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="G16" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H16" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I16" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="J16" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K16" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L16" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M16" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="N16" s="3" t="inlineStr">
+        <is>
+          <t>20250723T142953.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="G17" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H17" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I17" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="J17" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K17" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L17" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M17" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="N17" s="3" t="inlineStr">
+        <is>
+          <t>20250723T142814.000Z</t>
         </is>
       </c>
     </row>
@@ -5427,7 +6507,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N8"/>
+  <dimension ref="A3:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5864,6 +6944,294 @@
       <c r="N8" s="3" t="inlineStr">
         <is>
           <t>20250723T132309.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="G9" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H9" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I9" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="J9" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="K9" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L9" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M9" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N9" s="3" t="inlineStr">
+        <is>
+          <t>20250723T144841.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H10" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I10" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="J10" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="K10" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L10" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M10" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N10" s="3" t="inlineStr">
+        <is>
+          <t>20250723T144527.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G11" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H11" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I11" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="J11" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K11" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L11" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M11" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N11" s="3" t="inlineStr">
+        <is>
+          <t>20250723T143934.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G12" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H12" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I12" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="J12" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K12" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L12" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M12" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N12" s="3" t="inlineStr">
+        <is>
+          <t>20250723T143654.000Z</t>
         </is>
       </c>
     </row>
@@ -5878,7 +7246,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N14"/>
+  <dimension ref="A3:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6747,6 +8115,510 @@
       <c r="N14" s="3" t="inlineStr">
         <is>
           <t>20250720T183042.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>COLETTE</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="G15" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H15" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="J15" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K15" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L15" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M15" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N15" s="3" t="inlineStr">
+        <is>
+          <t>20250723T145419.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="G16" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H16" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I16" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J16" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K16" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L16" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M16" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N16" s="3" t="inlineStr">
+        <is>
+          <t>20250723T145213.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="G17" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H17" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I17" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J17" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K17" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L17" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M17" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N17" s="3" t="inlineStr">
+        <is>
+          <t>20250723T145036.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="F18" s="2" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="G18" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H18" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I18" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J18" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K18" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L18" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M18" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N18" s="3" t="inlineStr">
+        <is>
+          <t>20250723T144915.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F19" s="2" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="G19" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H19" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="I19" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J19" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="K19" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L19" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M19" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N19" s="3" t="inlineStr">
+        <is>
+          <t>20250723T144355.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F20" s="2" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="G20" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H20" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="I20" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J20" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="K20" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L20" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M20" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N20" s="3" t="inlineStr">
+        <is>
+          <t>20250723T144122.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="C21" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F21" s="2" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="G21" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H21" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="I21" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J21" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="K21" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L21" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M21" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N21" s="3" t="inlineStr">
+        <is>
+          <t>20250723T143951.000Z</t>
         </is>
       </c>
     </row>
@@ -6761,7 +8633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N9"/>
+  <dimension ref="A3:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7270,6 +9142,78 @@
       <c r="N9" s="3" t="inlineStr">
         <is>
           <t>20250720T184648.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H10" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I10" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J10" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K10" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L10" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="M10" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N10" s="3" t="inlineStr">
+        <is>
+          <t>20250723T145447.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-23 17:27:02)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -22,6 +22,7 @@
     <sheet name="Goldarm Gulch" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="Belle's Rock" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="Ring of Fire" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="Pit Stop" sheetId="16" state="visible" r:id="rId16"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -3225,7 +3226,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N11"/>
+  <dimension ref="A3:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3878,6 +3879,438 @@
       <c r="N11" s="3" t="inlineStr">
         <is>
           <t>20250723T142352.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="G12" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H12" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I12" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J12" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="K12" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="L12" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="M12" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="N12" s="3" t="inlineStr">
+        <is>
+          <t>20250723T145539.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>POCO</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="G13" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H13" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I13" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J13" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K13" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L13" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M13" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N13" s="3" t="inlineStr">
+        <is>
+          <t>20250723T150902.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>POCO</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="G14" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H14" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J14" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K14" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L14" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M14" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N14" s="3" t="inlineStr">
+        <is>
+          <t>20250723T150726.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="G15" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H15" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J15" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K15" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L15" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M15" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N15" s="3" t="inlineStr">
+        <is>
+          <t>20250723T150149.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="G16" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H16" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I16" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J16" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K16" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L16" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M16" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N16" s="3" t="inlineStr">
+        <is>
+          <t>20250723T145909.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="G17" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H17" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I17" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J17" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K17" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L17" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M17" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N17" s="3" t="inlineStr">
+        <is>
+          <t>20250723T145701.000Z</t>
         </is>
       </c>
     </row>
@@ -5402,6 +5835,457 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A3:N8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>B1</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>B1</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>Ganador</t>
+        </is>
+      </c>
+      <c r="H3" s="3" t="inlineStr">
+        <is>
+          <t>Jugador 1</t>
+        </is>
+      </c>
+      <c r="I3" s="3" t="inlineStr">
+        <is>
+          <t>Jugador 2</t>
+        </is>
+      </c>
+      <c r="J3" s="3" t="inlineStr">
+        <is>
+          <t>Jugador 3</t>
+        </is>
+      </c>
+      <c r="K3" s="3" t="inlineStr">
+        <is>
+          <t>Jugador 4</t>
+        </is>
+      </c>
+      <c r="L3" s="3" t="inlineStr">
+        <is>
+          <t>Jugador 5</t>
+        </is>
+      </c>
+      <c r="M3" s="3" t="inlineStr">
+        <is>
+          <t>Jugador 6</t>
+        </is>
+      </c>
+      <c r="N3" s="3" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="G4" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H4" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I4" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J4" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K4" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L4" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="M4" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N4" s="3" t="inlineStr">
+        <is>
+          <t>20250723T152247.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="G5" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H5" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I5" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J5" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K5" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L5" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="M5" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N5" s="3" t="inlineStr">
+        <is>
+          <t>20250723T152118.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="G6" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H6" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I6" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J6" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K6" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L6" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="M6" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N6" s="3" t="inlineStr">
+        <is>
+          <t>20250723T151951.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>DYNAMIKE</t>
+        </is>
+      </c>
+      <c r="G7" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H7" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I7" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J7" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K7" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L7" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M7" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N7" s="3" t="inlineStr">
+        <is>
+          <t>20250723T151409.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="inlineStr">
+        <is>
+          <t>DYNAMIKE</t>
+        </is>
+      </c>
+      <c r="G8" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H8" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I8" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J8" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K8" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L8" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M8" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N8" s="3" t="inlineStr">
+        <is>
+          <t>20250723T151223.000Z</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -7246,7 +8130,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N21"/>
+  <dimension ref="A3:N27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8619,6 +9503,438 @@
       <c r="N21" s="3" t="inlineStr">
         <is>
           <t>20250723T143951.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F22" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="G22" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H22" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="I22" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J22" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="K22" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="L22" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="M22" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="N22" s="3" t="inlineStr">
+        <is>
+          <t>20250723T152442.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F23" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="G23" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H23" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="I23" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J23" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="K23" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="L23" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="M23" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="N23" s="3" t="inlineStr">
+        <is>
+          <t>20250723T152300.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="D24" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F24" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="G24" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H24" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="I24" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J24" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="K24" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="L24" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="M24" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="N24" s="3" t="inlineStr">
+        <is>
+          <t>20250723T152140.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="C25" s="1" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="D25" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="F25" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G25" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H25" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I25" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="J25" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K25" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L25" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M25" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N25" s="3" t="inlineStr">
+        <is>
+          <t>20250723T150425.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="B26" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="C26" s="1" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="F26" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G26" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H26" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I26" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="J26" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K26" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L26" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M26" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N26" s="3" t="inlineStr">
+        <is>
+          <t>20250723T150201.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B27" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C27" s="1" t="inlineStr">
+        <is>
+          <t>COLETTE</t>
+        </is>
+      </c>
+      <c r="D27" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="G27" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H27" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="I27" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="J27" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K27" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L27" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M27" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N27" s="3" t="inlineStr">
+        <is>
+          <t>20250723T145611.000Z</t>
         </is>
       </c>
     </row>
@@ -8633,7 +9949,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N10"/>
+  <dimension ref="A3:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9214,6 +10530,1302 @@
       <c r="N10" s="3" t="inlineStr">
         <is>
           <t>20250723T145447.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="G11" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H11" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I11" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J11" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K11" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="L11" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="M11" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="N11" s="3" t="inlineStr">
+        <is>
+          <t>20250723T151411.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="G12" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H12" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I12" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J12" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K12" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="L12" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="M12" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="N12" s="3" t="inlineStr">
+        <is>
+          <t>20250723T151205.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>PENNY</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="G13" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H13" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I13" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J13" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="K13" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="L13" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="M13" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="N13" s="3" t="inlineStr">
+        <is>
+          <t>20250723T150607.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>PENNY</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="G14" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H14" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J14" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="K14" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="L14" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="M14" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="N14" s="3" t="inlineStr">
+        <is>
+          <t>20250723T150353.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>PENNY</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="G15" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H15" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J15" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="K15" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="L15" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="M15" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="N15" s="3" t="inlineStr">
+        <is>
+          <t>20250723T150138.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="G16" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H16" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="I16" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="J16" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="K16" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L16" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M16" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N16" s="3" t="inlineStr">
+        <is>
+          <t>20250723T152513.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="G17" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H17" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="I17" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="J17" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="K17" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L17" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M17" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N17" s="3" t="inlineStr">
+        <is>
+          <t>20250723T152301.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="F18" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="G18" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H18" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="I18" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="J18" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="K18" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L18" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M18" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N18" s="3" t="inlineStr">
+        <is>
+          <t>20250723T152042.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F19" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="G19" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H19" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I19" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="J19" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K19" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L19" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M19" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N19" s="3" t="inlineStr">
+        <is>
+          <t>20250723T151542.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F20" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="G20" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H20" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I20" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="J20" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K20" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L20" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M20" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N20" s="3" t="inlineStr">
+        <is>
+          <t>20250723T151326.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="C21" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F21" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="G21" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H21" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I21" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="J21" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K21" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L21" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M21" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N21" s="3" t="inlineStr">
+        <is>
+          <t>20250723T151106.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="F22" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="G22" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H22" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I22" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="J22" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="K22" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L22" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="M22" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="N22" s="3" t="inlineStr">
+        <is>
+          <t>20250723T150735.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="F23" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="G23" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H23" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I23" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="J23" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="K23" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L23" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="M23" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="N23" s="3" t="inlineStr">
+        <is>
+          <t>20250723T150515.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D24" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F24" s="2" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="G24" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H24" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I24" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J24" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K24" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L24" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="M24" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N24" s="3" t="inlineStr">
+        <is>
+          <t>20250723T145914.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="C25" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D25" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F25" s="2" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="G25" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H25" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I25" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J25" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K25" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L25" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="M25" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N25" s="3" t="inlineStr">
+        <is>
+          <t>20250723T145653.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B26" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="C26" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="F26" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="G26" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H26" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I26" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J26" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K26" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="L26" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="M26" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="N26" s="3" t="inlineStr">
+        <is>
+          <t>20250723T152515.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B27" s="1" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="C27" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="D27" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="G27" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H27" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="I27" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="J27" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K27" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L27" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M27" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N27" s="3" t="inlineStr">
+        <is>
+          <t>20250723T151932.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B28" s="1" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="C28" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="D28" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="F28" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="G28" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H28" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="I28" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="J28" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K28" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L28" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M28" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N28" s="3" t="inlineStr">
+        <is>
+          <t>20250723T151712.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-23 17:58:22)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N34"/>
+  <dimension ref="A3:N38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2761,6 +2761,294 @@
       <c r="N34" s="3" t="inlineStr">
         <is>
           <t>20250723T143353.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B35" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="C35" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D35" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="E35" s="2" t="inlineStr">
+        <is>
+          <t>GALE</t>
+        </is>
+      </c>
+      <c r="F35" s="2" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="G35" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H35" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I35" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J35" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K35" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L35" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M35" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N35" s="3" t="inlineStr">
+        <is>
+          <t>20250723T154433.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B36" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="C36" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D36" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="inlineStr">
+        <is>
+          <t>GALE</t>
+        </is>
+      </c>
+      <c r="F36" s="2" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="G36" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H36" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I36" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J36" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K36" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L36" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M36" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N36" s="3" t="inlineStr">
+        <is>
+          <t>20250723T154143.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="B37" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="C37" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="D37" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="inlineStr">
+        <is>
+          <t>GALE</t>
+        </is>
+      </c>
+      <c r="F37" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="G37" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H37" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="I37" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J37" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="K37" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L37" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M37" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N37" s="3" t="inlineStr">
+        <is>
+          <t>20250723T153730.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="B38" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="C38" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="D38" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="inlineStr">
+        <is>
+          <t>GALE</t>
+        </is>
+      </c>
+      <c r="F38" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="G38" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H38" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="I38" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J38" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="K38" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L38" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M38" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N38" s="3" t="inlineStr">
+        <is>
+          <t>20250723T153603.000Z</t>
         </is>
       </c>
     </row>
@@ -3226,7 +3514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N17"/>
+  <dimension ref="A3:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4311,6 +4599,294 @@
       <c r="N17" s="3" t="inlineStr">
         <is>
           <t>20250723T145701.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="F18" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G18" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H18" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I18" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="J18" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K18" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L18" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M18" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="N18" s="3" t="inlineStr">
+        <is>
+          <t>20250723T154317.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="F19" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G19" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H19" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I19" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="J19" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K19" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L19" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M19" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="N19" s="3" t="inlineStr">
+        <is>
+          <t>20250723T154059.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F20" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G20" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H20" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I20" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="J20" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K20" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L20" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M20" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="N20" s="3" t="inlineStr">
+        <is>
+          <t>20250723T153445.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C21" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F21" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G21" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H21" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I21" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="J21" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K21" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L21" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M21" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="N21" s="3" t="inlineStr">
+        <is>
+          <t>20250723T153253.000Z</t>
         </is>
       </c>
     </row>
@@ -7391,7 +7967,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N12"/>
+  <dimension ref="A3:N23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8116,6 +8692,798 @@
       <c r="N12" s="3" t="inlineStr">
         <is>
           <t>20250723T143654.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="G13" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H13" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I13" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J13" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K13" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="L13" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="M13" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="N13" s="3" t="inlineStr">
+        <is>
+          <t>20250723T155203.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="G14" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H14" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J14" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K14" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="L14" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="M14" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="N14" s="3" t="inlineStr">
+        <is>
+          <t>20250723T155004.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="G15" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H15" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J15" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K15" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="L15" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="M15" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="N15" s="3" t="inlineStr">
+        <is>
+          <t>20250723T154747.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>SPROUT</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="G16" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H16" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I16" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J16" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K16" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="L16" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="M16" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="N16" s="3" t="inlineStr">
+        <is>
+          <t>20250723T154247.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>SPROUT</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="G17" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H17" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I17" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J17" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K17" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="L17" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="M17" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="N17" s="3" t="inlineStr">
+        <is>
+          <t>20250723T154015.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>SPROUT</t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="F18" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="G18" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H18" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I18" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J18" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K18" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="L18" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="M18" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="N18" s="3" t="inlineStr">
+        <is>
+          <t>20250723T153735.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="F19" s="2" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="G19" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H19" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I19" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J19" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K19" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L19" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M19" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N19" s="3" t="inlineStr">
+        <is>
+          <t>20250723T154618.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="F20" s="2" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="G20" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H20" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I20" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J20" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K20" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L20" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M20" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N20" s="3" t="inlineStr">
+        <is>
+          <t>20250723T154417.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="C21" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="F21" s="2" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="G21" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H21" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I21" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J21" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K21" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L21" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M21" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N21" s="3" t="inlineStr">
+        <is>
+          <t>20250723T154022.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="F22" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="G22" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H22" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I22" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J22" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K22" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="L22" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M22" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="N22" s="3" t="inlineStr">
+        <is>
+          <t>20250723T153339.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="F23" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="G23" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H23" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I23" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J23" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K23" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="L23" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M23" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="N23" s="3" t="inlineStr">
+        <is>
+          <t>20250723T153120.000Z</t>
         </is>
       </c>
     </row>
@@ -8130,7 +9498,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N27"/>
+  <dimension ref="A3:N29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9935,6 +11303,150 @@
       <c r="N27" s="3" t="inlineStr">
         <is>
           <t>20250723T145611.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="B28" s="1" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="C28" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D28" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F28" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="G28" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H28" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I28" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J28" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="K28" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="L28" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="M28" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="N28" s="3" t="inlineStr">
+        <is>
+          <t>20250723T153102.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="B29" s="1" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="C29" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E29" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F29" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="G29" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H29" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I29" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J29" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="K29" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="L29" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="M29" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="N29" s="3" t="inlineStr">
+        <is>
+          <t>20250723T152924.000Z</t>
         </is>
       </c>
     </row>
@@ -9949,7 +11461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N28"/>
+  <dimension ref="A3:N30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11826,6 +13338,150 @@
       <c r="N28" s="3" t="inlineStr">
         <is>
           <t>20250723T151712.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B29" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="C29" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="E29" s="2" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="F29" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="G29" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H29" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I29" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J29" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K29" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="L29" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="M29" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="N29" s="3" t="inlineStr">
+        <is>
+          <t>20250723T152944.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B30" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="C30" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="F30" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="G30" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H30" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I30" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J30" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K30" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="L30" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="M30" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="N30" s="3" t="inlineStr">
+        <is>
+          <t>20250723T152724.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-23 18:29:43)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N38"/>
+  <dimension ref="A3:N40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3049,6 +3049,150 @@
       <c r="N38" s="3" t="inlineStr">
         <is>
           <t>20250723T153603.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="B39" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="C39" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="D39" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F39" s="2" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="G39" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H39" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="I39" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="J39" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K39" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L39" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M39" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N39" s="3" t="inlineStr">
+        <is>
+          <t>20250723T162138.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="B40" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="C40" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="D40" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F40" s="2" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="G40" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H40" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="I40" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="J40" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K40" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L40" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M40" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N40" s="3" t="inlineStr">
+        <is>
+          <t>20250723T162047.000Z</t>
         </is>
       </c>
     </row>
@@ -6182,7 +6326,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N5"/>
+  <dimension ref="A3:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6403,6 +6547,294 @@
       <c r="N5" s="3" t="inlineStr">
         <is>
           <t>20250719T004820.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="G6" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H6" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="I6" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J6" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="K6" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="L6" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M6" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="N6" s="3" t="inlineStr">
+        <is>
+          <t>20250723T162258.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="G7" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H7" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="I7" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J7" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="K7" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="L7" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M7" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="N7" s="3" t="inlineStr">
+        <is>
+          <t>20250723T162056.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>COLETTE</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G8" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H8" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="I8" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J8" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="K8" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L8" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M8" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N8" s="3" t="inlineStr">
+        <is>
+          <t>20250723T161357.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>COLETTE</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G9" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H9" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="I9" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J9" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="K9" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L9" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M9" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N9" s="3" t="inlineStr">
+        <is>
+          <t>20250723T161218.000Z</t>
         </is>
       </c>
     </row>
@@ -6868,7 +7300,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N17"/>
+  <dimension ref="A3:N26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7953,6 +8385,654 @@
       <c r="N17" s="3" t="inlineStr">
         <is>
           <t>20250723T142814.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>MAX</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>GALE</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="F18" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="G18" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H18" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I18" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J18" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K18" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="L18" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="M18" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="N18" s="3" t="inlineStr">
+        <is>
+          <t>20250723T161006.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>MAX</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>GALE</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="F19" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="G19" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H19" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I19" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J19" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K19" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="L19" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="M19" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="N19" s="3" t="inlineStr">
+        <is>
+          <t>20250723T160730.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>MAX</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>GALE</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="F20" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="G20" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H20" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I20" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J20" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K20" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="L20" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="M20" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="N20" s="3" t="inlineStr">
+        <is>
+          <t>20250723T160543.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="C21" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F21" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="G21" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H21" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I21" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J21" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K21" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="L21" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="M21" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="N21" s="3" t="inlineStr">
+        <is>
+          <t>20250723T160005.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F22" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="G22" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H22" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I22" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J22" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K22" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="L22" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="M22" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="N22" s="3" t="inlineStr">
+        <is>
+          <t>20250723T155807.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="F23" s="2" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="G23" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H23" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I23" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J23" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K23" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L23" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M23" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N23" s="3" t="inlineStr">
+        <is>
+          <t>20250723T162040.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D24" s="2" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="F24" s="2" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="G24" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H24" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I24" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J24" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K24" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L24" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M24" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N24" s="3" t="inlineStr">
+        <is>
+          <t>20250723T161806.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="C25" s="1" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="D25" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="F25" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="G25" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H25" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="I25" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="J25" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K25" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="L25" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="M25" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="N25" s="3" t="inlineStr">
+        <is>
+          <t>20250723T161133.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="B26" s="1" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="C26" s="1" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="F26" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="G26" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H26" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="I26" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="J26" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K26" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="L26" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="M26" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="N26" s="3" t="inlineStr">
+        <is>
+          <t>20250723T160930.000Z</t>
         </is>
       </c>
     </row>
@@ -16073,7 +17153,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N16"/>
+  <dimension ref="A3:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17089,6 +18169,78 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G17" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H17" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I17" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="J17" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="K17" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L17" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M17" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N17" s="3" t="inlineStr">
+        <is>
+          <t>20250723T162626.000Z</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-23 19:01:02)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N40"/>
+  <dimension ref="A3:N43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3193,6 +3193,222 @@
       <c r="N40" s="3" t="inlineStr">
         <is>
           <t>20250723T162047.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="B41" s="1" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="C41" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="D41" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E41" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F41" s="2" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="G41" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H41" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="I41" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J41" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="K41" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L41" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M41" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="N41" s="3" t="inlineStr">
+        <is>
+          <t>20250723T165858.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="B42" s="1" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="C42" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="D42" s="2" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="E42" s="2" t="inlineStr">
+        <is>
+          <t>GALE</t>
+        </is>
+      </c>
+      <c r="F42" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G42" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H42" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I42" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J42" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="K42" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L42" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M42" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N42" s="3" t="inlineStr">
+        <is>
+          <t>20250723T163256.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="B43" s="1" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="C43" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="D43" s="2" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="E43" s="2" t="inlineStr">
+        <is>
+          <t>GALE</t>
+        </is>
+      </c>
+      <c r="F43" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G43" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H43" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I43" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J43" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="K43" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L43" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M43" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N43" s="3" t="inlineStr">
+        <is>
+          <t>20250723T162925.000Z</t>
         </is>
       </c>
     </row>
@@ -5045,7 +5261,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N5"/>
+  <dimension ref="A3:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5266,6 +5482,294 @@
       <c r="N5" s="3" t="inlineStr">
         <is>
           <t>20250723T005200.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="G6" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H6" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="I6" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="J6" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="K6" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L6" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M6" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N6" s="3" t="inlineStr">
+        <is>
+          <t>20250723T165150.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="G7" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H7" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="I7" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="J7" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="K7" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L7" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M7" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N7" s="3" t="inlineStr">
+        <is>
+          <t>20250723T165010.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G8" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H8" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="I8" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="J8" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="K8" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L8" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M8" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N8" s="3" t="inlineStr">
+        <is>
+          <t>20250723T164308.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G9" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H9" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="I9" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="J9" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="K9" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L9" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M9" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N9" s="3" t="inlineStr">
+        <is>
+          <t>20250723T164047.000Z</t>
         </is>
       </c>
     </row>
@@ -6326,7 +6830,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N9"/>
+  <dimension ref="A3:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6835,6 +7339,150 @@
       <c r="N9" s="3" t="inlineStr">
         <is>
           <t>20250723T161218.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="G10" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H10" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="I10" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="J10" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="K10" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L10" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M10" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N10" s="3" t="inlineStr">
+        <is>
+          <t>20250723T163221.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="G11" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H11" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="I11" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="J11" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="K11" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L11" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M11" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N11" s="3" t="inlineStr">
+        <is>
+          <t>20250723T163003.000Z</t>
         </is>
       </c>
     </row>
@@ -6849,7 +7497,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N8"/>
+  <dimension ref="A3:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7286,6 +7934,366 @@
       <c r="N8" s="3" t="inlineStr">
         <is>
           <t>20250723T151223.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="inlineStr">
+        <is>
+          <t>EDGAR</t>
+        </is>
+      </c>
+      <c r="G9" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H9" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I9" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J9" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K9" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L9" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M9" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N9" s="3" t="inlineStr">
+        <is>
+          <t>20250723T165429.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>EDGAR</t>
+        </is>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H10" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I10" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J10" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K10" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L10" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M10" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N10" s="3" t="inlineStr">
+        <is>
+          <t>20250723T165246.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="G11" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H11" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I11" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J11" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K11" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L11" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M11" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N11" s="3" t="inlineStr">
+        <is>
+          <t>20250723T164558.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="G12" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H12" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I12" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J12" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K12" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L12" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M12" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N12" s="3" t="inlineStr">
+        <is>
+          <t>20250723T164404.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="G13" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H13" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I13" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J13" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K13" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L13" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M13" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N13" s="3" t="inlineStr">
+        <is>
+          <t>20250723T164146.000Z</t>
         </is>
       </c>
     </row>
@@ -15459,7 +16467,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N15"/>
+  <dimension ref="A3:N19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16400,6 +17408,294 @@
       <c r="N15" s="3" t="inlineStr">
         <is>
           <t>20250720T192055.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="G16" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H16" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I16" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J16" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K16" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L16" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M16" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N16" s="3" t="inlineStr">
+        <is>
+          <t>20250723T165749.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>8-BIT</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G17" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H17" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I17" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J17" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K17" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="L17" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="M17" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="N17" s="3" t="inlineStr">
+        <is>
+          <t>20250723T165128.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="inlineStr">
+        <is>
+          <t>8-BIT</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="F18" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G18" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H18" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I18" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J18" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K18" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="L18" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="M18" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="N18" s="3" t="inlineStr">
+        <is>
+          <t>20250723T164934.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="inlineStr">
+        <is>
+          <t>8-BIT</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="F19" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G19" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H19" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I19" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J19" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K19" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="L19" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="M19" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="N19" s="3" t="inlineStr">
+        <is>
+          <t>20250723T164646.000Z</t>
         </is>
       </c>
     </row>
@@ -17153,7 +18449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N17"/>
+  <dimension ref="A3:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18241,6 +19537,366 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F18" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="G18" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H18" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I18" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J18" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K18" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L18" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M18" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N18" s="3" t="inlineStr">
+        <is>
+          <t>20250723T164106.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F19" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="G19" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H19" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I19" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J19" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K19" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L19" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M19" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N19" s="3" t="inlineStr">
+        <is>
+          <t>20250723T163924.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F20" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="G20" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H20" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I20" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J20" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K20" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L20" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M20" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N20" s="3" t="inlineStr">
+        <is>
+          <t>20250723T163709.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C21" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F21" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G21" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H21" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I21" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="J21" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="K21" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L21" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M21" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N21" s="3" t="inlineStr">
+        <is>
+          <t>20250723T163038.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F22" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G22" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H22" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I22" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="J22" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="K22" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L22" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M22" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N22" s="3" t="inlineStr">
+        <is>
+          <t>20250723T162903.000Z</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-23 19:32:22)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N43"/>
+  <dimension ref="A3:N49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3409,6 +3409,438 @@
       <c r="N43" s="3" t="inlineStr">
         <is>
           <t>20250723T162925.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="B44" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="C44" s="1" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="D44" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E44" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="F44" s="2" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="G44" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H44" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I44" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="J44" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="K44" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L44" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M44" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="N44" s="3" t="inlineStr">
+        <is>
+          <t>20250723T172408.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="B45" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="C45" s="1" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="D45" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E45" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="F45" s="2" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="G45" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H45" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I45" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="J45" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="K45" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L45" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M45" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="N45" s="3" t="inlineStr">
+        <is>
+          <t>20250723T172117.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B46" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C46" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="D46" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E46" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="F46" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G46" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H46" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="I46" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="J46" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="K46" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L46" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M46" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="N46" s="3" t="inlineStr">
+        <is>
+          <t>20250723T171445.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B47" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C47" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="D47" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E47" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="F47" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G47" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H47" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="I47" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="J47" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="K47" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L47" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M47" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="N47" s="3" t="inlineStr">
+        <is>
+          <t>20250723T171153.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B48" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C48" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="D48" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E48" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="F48" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G48" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H48" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="I48" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="J48" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="K48" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L48" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M48" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="N48" s="3" t="inlineStr">
+        <is>
+          <t>20250723T170902.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="B49" s="1" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="C49" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="D49" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E49" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F49" s="2" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="G49" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H49" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="I49" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J49" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="K49" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L49" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M49" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="N49" s="3" t="inlineStr">
+        <is>
+          <t>20250723T170026.000Z</t>
         </is>
       </c>
     </row>
@@ -6307,7 +6739,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N9"/>
+  <dimension ref="A3:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6816,6 +7248,438 @@
       <c r="N9" s="3" t="inlineStr">
         <is>
           <t>20250723T142404.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H10" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I10" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J10" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K10" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L10" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M10" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N10" s="3" t="inlineStr">
+        <is>
+          <t>20250723T172420.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="G11" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H11" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I11" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J11" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K11" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L11" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M11" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N11" s="3" t="inlineStr">
+        <is>
+          <t>20250723T172257.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="G12" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H12" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I12" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J12" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K12" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L12" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M12" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N12" s="3" t="inlineStr">
+        <is>
+          <t>20250723T172043.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="G13" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H13" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I13" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J13" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K13" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="L13" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="M13" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="N13" s="3" t="inlineStr">
+        <is>
+          <t>20250723T171352.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="G14" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H14" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J14" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K14" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="L14" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="M14" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="N14" s="3" t="inlineStr">
+        <is>
+          <t>20250723T171149.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="G15" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H15" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J15" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K15" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="L15" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="M15" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="N15" s="3" t="inlineStr">
+        <is>
+          <t>20250723T171010.000Z</t>
         </is>
       </c>
     </row>
@@ -6830,7 +7694,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N11"/>
+  <dimension ref="A3:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7483,6 +8347,366 @@
       <c r="N11" s="3" t="inlineStr">
         <is>
           <t>20250723T163003.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>ROSA</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="G12" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H12" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I12" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J12" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K12" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L12" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M12" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N12" s="3" t="inlineStr">
+        <is>
+          <t>20250723T171506.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>ROSA</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="G13" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H13" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I13" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J13" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K13" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L13" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M13" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N13" s="3" t="inlineStr">
+        <is>
+          <t>20250723T171313.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>ROSA</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="G14" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H14" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J14" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K14" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L14" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M14" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N14" s="3" t="inlineStr">
+        <is>
+          <t>20250723T171101.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>CHESTER</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>8-BIT</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>PENNY</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G15" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H15" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J15" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="K15" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="L15" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="M15" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="N15" s="3" t="inlineStr">
+        <is>
+          <t>20250723T170518.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>CHESTER</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>8-BIT</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>PENNY</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G16" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H16" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I16" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J16" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="K16" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="L16" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="M16" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="N16" s="3" t="inlineStr">
+        <is>
+          <t>20250723T170252.000Z</t>
         </is>
       </c>
     </row>
@@ -15584,7 +16808,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N14"/>
+  <dimension ref="A3:N18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16453,6 +17677,294 @@
       <c r="N14" s="3" t="inlineStr">
         <is>
           <t>20250718T233314.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="G15" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H15" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J15" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="K15" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L15" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="M15" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="N15" s="3" t="inlineStr">
+        <is>
+          <t>20250723T173053.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>MAX</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="G16" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H16" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I16" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J16" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K16" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="L16" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="M16" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="N16" s="3" t="inlineStr">
+        <is>
+          <t>20250723T172304.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>MAX</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="G17" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H17" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I17" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J17" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K17" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="L17" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="M17" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="N17" s="3" t="inlineStr">
+        <is>
+          <t>20250723T172120.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="F18" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="G18" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H18" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I18" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="J18" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="K18" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L18" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M18" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N18" s="3" t="inlineStr">
+        <is>
+          <t>20250723T173022.000Z</t>
         </is>
       </c>
     </row>
@@ -16467,7 +17979,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N19"/>
+  <dimension ref="A3:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17696,6 +19208,150 @@
       <c r="N19" s="3" t="inlineStr">
         <is>
           <t>20250723T164646.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="F20" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="G20" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H20" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I20" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J20" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K20" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L20" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M20" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N20" s="3" t="inlineStr">
+        <is>
+          <t>20250723T170326.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="C21" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="F21" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="G21" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H21" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I21" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J21" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K21" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L21" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M21" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N21" s="3" t="inlineStr">
+        <is>
+          <t>20250723T170038.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-23 20:03:41)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -23,6 +23,7 @@
     <sheet name="Belle's Rock" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="Ring of Fire" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="Pit Stop" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="Sneaky Fields" sheetId="17" state="visible" r:id="rId17"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -8721,7 +8722,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N13"/>
+  <dimension ref="A3:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9518,6 +9519,457 @@
       <c r="N13" s="3" t="inlineStr">
         <is>
           <t>20250723T164146.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>EDGAR</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="G14" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H14" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="J14" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="K14" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L14" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="M14" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="N14" s="3" t="inlineStr">
+        <is>
+          <t>20250723T174004.000Z</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A3:N7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>B1</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>B1</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>Ganador</t>
+        </is>
+      </c>
+      <c r="H3" s="3" t="inlineStr">
+        <is>
+          <t>Jugador 1</t>
+        </is>
+      </c>
+      <c r="I3" s="3" t="inlineStr">
+        <is>
+          <t>Jugador 2</t>
+        </is>
+      </c>
+      <c r="J3" s="3" t="inlineStr">
+        <is>
+          <t>Jugador 3</t>
+        </is>
+      </c>
+      <c r="K3" s="3" t="inlineStr">
+        <is>
+          <t>Jugador 4</t>
+        </is>
+      </c>
+      <c r="L3" s="3" t="inlineStr">
+        <is>
+          <t>Jugador 5</t>
+        </is>
+      </c>
+      <c r="M3" s="3" t="inlineStr">
+        <is>
+          <t>Jugador 6</t>
+        </is>
+      </c>
+      <c r="N3" s="3" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="G4" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H4" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I4" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J4" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="K4" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L4" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M4" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N4" s="3" t="inlineStr">
+        <is>
+          <t>20250723T175519.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="G5" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H5" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I5" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J5" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="K5" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L5" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M5" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N5" s="3" t="inlineStr">
+        <is>
+          <t>20250723T175411.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>EL PRIMO</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="G6" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H6" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I6" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J6" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K6" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L6" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M6" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N6" s="3" t="inlineStr">
+        <is>
+          <t>20250723T174811.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>EL PRIMO</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="G7" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H7" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I7" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J7" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K7" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L7" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M7" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N7" s="3" t="inlineStr">
+        <is>
+          <t>20250723T174615.000Z</t>
         </is>
       </c>
     </row>
@@ -16808,7 +17260,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N18"/>
+  <dimension ref="A3:N29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17965,6 +18417,798 @@
       <c r="N18" s="3" t="inlineStr">
         <is>
           <t>20250723T173022.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F19" s="2" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="G19" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H19" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I19" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J19" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="K19" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="L19" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M19" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="N19" s="3" t="inlineStr">
+        <is>
+          <t>20250723T174629.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F20" s="2" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="G20" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H20" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I20" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J20" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="K20" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="L20" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M20" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="N20" s="3" t="inlineStr">
+        <is>
+          <t>20250723T174422.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="C21" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F21" s="2" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="G21" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H21" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I21" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J21" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="K21" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="L21" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M21" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="N21" s="3" t="inlineStr">
+        <is>
+          <t>20250723T174223.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="F22" s="2" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="G22" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H22" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="I22" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="J22" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="K22" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L22" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M22" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="N22" s="3" t="inlineStr">
+        <is>
+          <t>20250723T173623.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="F23" s="2" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="G23" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H23" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="I23" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="J23" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="K23" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L23" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M23" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="N23" s="3" t="inlineStr">
+        <is>
+          <t>20250723T173403.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="D24" s="2" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="F24" s="2" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="G24" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H24" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="I24" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="J24" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="K24" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L24" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M24" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="N24" s="3" t="inlineStr">
+        <is>
+          <t>20250723T173143.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="C25" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D25" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="F25" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="G25" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H25" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I25" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J25" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="K25" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L25" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="M25" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="N25" s="3" t="inlineStr">
+        <is>
+          <t>20250723T173533.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B26" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="C26" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="F26" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="G26" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H26" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I26" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J26" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="K26" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L26" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="M26" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="N26" s="3" t="inlineStr">
+        <is>
+          <t>20250723T173313.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B27" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="C27" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="D27" s="2" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G27" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H27" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I27" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J27" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K27" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="L27" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="M27" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="N27" s="3" t="inlineStr">
+        <is>
+          <t>20250723T173941.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B28" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="C28" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="D28" s="2" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="F28" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G28" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H28" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I28" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J28" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K28" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="L28" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="M28" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="N28" s="3" t="inlineStr">
+        <is>
+          <t>20250723T173809.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B29" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C29" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E29" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="F29" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="G29" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H29" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I29" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="J29" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="K29" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L29" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M29" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N29" s="3" t="inlineStr">
+        <is>
+          <t>20250723T173242.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-23 20:35:01)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N49"/>
+  <dimension ref="A3:N54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3842,6 +3842,366 @@
       <c r="N49" s="3" t="inlineStr">
         <is>
           <t>20250723T170026.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="B50" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="C50" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D50" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E50" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="F50" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="G50" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H50" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I50" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J50" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="K50" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L50" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="M50" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N50" s="3" t="inlineStr">
+        <is>
+          <t>20250723T182648.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="B51" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="C51" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D51" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E51" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="F51" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="G51" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H51" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I51" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J51" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="K51" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L51" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="M51" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N51" s="3" t="inlineStr">
+        <is>
+          <t>20250723T182421.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="B52" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="C52" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D52" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E52" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="F52" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="G52" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H52" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I52" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J52" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="K52" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L52" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="M52" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N52" s="3" t="inlineStr">
+        <is>
+          <t>20250723T182245.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="B53" s="1" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="C53" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D53" s="2" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="E53" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="F53" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="G53" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H53" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="I53" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="J53" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="K53" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L53" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="M53" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="N53" s="3" t="inlineStr">
+        <is>
+          <t>20250723T181802.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="B54" s="1" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="C54" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D54" s="2" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="E54" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="F54" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="G54" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H54" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="I54" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="J54" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="K54" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L54" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="M54" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="N54" s="3" t="inlineStr">
+        <is>
+          <t>20250723T181618.000Z</t>
         </is>
       </c>
     </row>
@@ -4307,7 +4667,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N21"/>
+  <dimension ref="A3:N30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5680,6 +6040,654 @@
       <c r="N21" s="3" t="inlineStr">
         <is>
           <t>20250723T153253.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F22" s="2" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="G22" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H22" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I22" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J22" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K22" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L22" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M22" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N22" s="3" t="inlineStr">
+        <is>
+          <t>20250723T182553.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F23" s="2" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="G23" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H23" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I23" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J23" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K23" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L23" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M23" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N23" s="3" t="inlineStr">
+        <is>
+          <t>20250723T182244.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D24" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="F24" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="G24" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H24" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="I24" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="J24" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="K24" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L24" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M24" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N24" s="3" t="inlineStr">
+        <is>
+          <t>20250723T181528.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="C25" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D25" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="F25" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="G25" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H25" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="I25" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="J25" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="K25" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L25" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M25" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N25" s="3" t="inlineStr">
+        <is>
+          <t>20250723T181314.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="B26" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C26" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F26" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="G26" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H26" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="I26" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J26" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="K26" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L26" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M26" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N26" s="3" t="inlineStr">
+        <is>
+          <t>20250723T182241.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="B27" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C27" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D27" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="G27" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H27" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="I27" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J27" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="K27" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L27" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M27" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N27" s="3" t="inlineStr">
+        <is>
+          <t>20250723T182023.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B28" s="1" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="C28" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D28" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F28" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G28" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H28" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I28" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J28" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K28" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L28" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M28" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N28" s="3" t="inlineStr">
+        <is>
+          <t>20250723T181450.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B29" s="1" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="C29" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E29" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F29" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G29" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H29" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I29" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J29" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K29" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L29" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M29" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N29" s="3" t="inlineStr">
+        <is>
+          <t>20250723T181243.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B30" s="1" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="C30" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F30" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G30" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H30" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I30" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J30" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K30" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L30" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M30" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N30" s="3" t="inlineStr">
+        <is>
+          <t>20250723T181050.000Z</t>
         </is>
       </c>
     </row>
@@ -8722,7 +9730,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N14"/>
+  <dimension ref="A3:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9591,6 +10599,150 @@
       <c r="N14" s="3" t="inlineStr">
         <is>
           <t>20250723T174004.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="G15" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H15" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="J15" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="K15" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="L15" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="M15" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="N15" s="3" t="inlineStr">
+        <is>
+          <t>20250723T183335.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="G16" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H16" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I16" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="J16" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="K16" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="L16" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="M16" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="N16" s="3" t="inlineStr">
+        <is>
+          <t>20250723T183200.000Z</t>
         </is>
       </c>
     </row>
@@ -15225,7 +16377,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N30"/>
+  <dimension ref="A3:N35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17246,6 +18398,366 @@
       <c r="N30" s="3" t="inlineStr">
         <is>
           <t>20250723T152724.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B31" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="C31" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="D31" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="F31" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="G31" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H31" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="I31" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="J31" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="K31" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L31" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M31" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N31" s="3" t="inlineStr">
+        <is>
+          <t>20250723T183354.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="F32" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="G32" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H32" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="I32" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="J32" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="K32" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L32" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M32" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N32" s="3" t="inlineStr">
+        <is>
+          <t>20250723T183133.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="B33" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C33" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="D33" s="2" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="E33" s="2" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="F33" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="G33" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H33" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I33" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J33" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K33" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L33" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M33" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N33" s="3" t="inlineStr">
+        <is>
+          <t>20250723T183332.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="B34" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C34" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="E34" s="2" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="F34" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="G34" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H34" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I34" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J34" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K34" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L34" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M34" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N34" s="3" t="inlineStr">
+        <is>
+          <t>20250723T183112.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="B35" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C35" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="D35" s="2" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="E35" s="2" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="F35" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="G35" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H35" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I35" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J35" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K35" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L35" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M35" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N35" s="3" t="inlineStr">
+        <is>
+          <t>20250723T182852.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-23 21:06:20)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -8703,7 +8703,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N16"/>
+  <dimension ref="A3:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9716,6 +9716,294 @@
       <c r="N16" s="3" t="inlineStr">
         <is>
           <t>20250723T170252.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>8-BIT</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="G17" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H17" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="I17" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="J17" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="K17" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L17" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="M17" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="N17" s="3" t="inlineStr">
+        <is>
+          <t>20250723T190340.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="F18" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="G18" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H18" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="I18" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="J18" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="K18" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L18" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="M18" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N18" s="3" t="inlineStr">
+        <is>
+          <t>20250723T185753.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="F19" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="G19" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H19" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="I19" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="J19" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="K19" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L19" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="M19" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N19" s="3" t="inlineStr">
+        <is>
+          <t>20250723T185516.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="F20" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="G20" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H20" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="I20" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="J20" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="K20" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L20" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="M20" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N20" s="3" t="inlineStr">
+        <is>
+          <t>20250723T185319.000Z</t>
         </is>
       </c>
     </row>
@@ -9730,7 +10018,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N16"/>
+  <dimension ref="A3:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10743,6 +11031,294 @@
       <c r="N16" s="3" t="inlineStr">
         <is>
           <t>20250723T183200.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="G17" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H17" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I17" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="J17" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="K17" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L17" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="M17" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N17" s="3" t="inlineStr">
+        <is>
+          <t>20250723T184551.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="F18" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="G18" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H18" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I18" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="J18" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="K18" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L18" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="M18" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N18" s="3" t="inlineStr">
+        <is>
+          <t>20250723T184357.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="F19" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="G19" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H19" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I19" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="J19" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="K19" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L19" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="M19" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N19" s="3" t="inlineStr">
+        <is>
+          <t>20250723T184230.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>EDGAR</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="F20" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G20" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H20" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I20" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J20" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K20" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L20" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M20" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N20" s="3" t="inlineStr">
+        <is>
+          <t>20250723T183644.000Z</t>
         </is>
       </c>
     </row>
@@ -12883,7 +13459,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N23"/>
+  <dimension ref="A3:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14400,6 +14976,78 @@
       <c r="N23" s="3" t="inlineStr">
         <is>
           <t>20250723T153120.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="D24" s="2" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="inlineStr">
+        <is>
+          <t>POCO</t>
+        </is>
+      </c>
+      <c r="F24" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="G24" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H24" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="I24" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="J24" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="K24" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L24" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="M24" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="N24" s="3" t="inlineStr">
+        <is>
+          <t>20250723T190423.000Z</t>
         </is>
       </c>
     </row>
@@ -14414,7 +15062,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N29"/>
+  <dimension ref="A3:N39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16363,6 +17011,726 @@
       <c r="N29" s="3" t="inlineStr">
         <is>
           <t>20250723T152924.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B30" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="C30" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="F30" s="2" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="G30" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H30" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I30" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J30" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K30" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L30" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M30" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N30" s="3" t="inlineStr">
+        <is>
+          <t>20250723T185953.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B31" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="C31" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D31" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="F31" s="2" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="G31" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H31" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I31" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J31" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K31" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L31" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M31" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N31" s="3" t="inlineStr">
+        <is>
+          <t>20250723T185702.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="F32" s="2" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="G32" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H32" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I32" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J32" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K32" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L32" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M32" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N32" s="3" t="inlineStr">
+        <is>
+          <t>20250723T185600.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B33" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C33" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D33" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E33" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="F33" s="2" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="G33" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H33" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I33" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J33" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K33" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L33" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M33" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N33" s="3" t="inlineStr">
+        <is>
+          <t>20250723T185055.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B34" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C34" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E34" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="F34" s="2" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="G34" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H34" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I34" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J34" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K34" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L34" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M34" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N34" s="3" t="inlineStr">
+        <is>
+          <t>20250723T184915.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B35" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C35" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="D35" s="2" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="E35" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F35" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G35" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H35" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I35" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J35" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K35" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L35" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M35" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N35" s="3" t="inlineStr">
+        <is>
+          <t>20250723T190429.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B36" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C36" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="D36" s="2" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F36" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G36" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H36" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I36" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J36" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K36" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L36" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M36" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N36" s="3" t="inlineStr">
+        <is>
+          <t>20250723T190210.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B37" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="C37" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="D37" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="F37" s="2" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="G37" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H37" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I37" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J37" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K37" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L37" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M37" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N37" s="3" t="inlineStr">
+        <is>
+          <t>20250723T185545.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B38" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="C38" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="D38" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="F38" s="2" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="G38" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H38" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I38" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J38" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K38" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L38" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M38" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N38" s="3" t="inlineStr">
+        <is>
+          <t>20250723T185344.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B39" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="C39" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="D39" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="F39" s="2" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="G39" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H39" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I39" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J39" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K39" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L39" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M39" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N39" s="3" t="inlineStr">
+        <is>
+          <t>20250723T185107.000Z</t>
         </is>
       </c>
     </row>
@@ -16377,7 +17745,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N35"/>
+  <dimension ref="A3:N42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18758,6 +20126,510 @@
       <c r="N35" s="3" t="inlineStr">
         <is>
           <t>20250723T182852.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B36" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="C36" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="D36" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="F36" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="G36" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H36" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I36" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J36" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K36" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="L36" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="M36" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="N36" s="3" t="inlineStr">
+        <is>
+          <t>20250723T184355.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B37" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="C37" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="D37" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="F37" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="G37" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H37" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I37" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J37" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K37" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="L37" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="M37" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="N37" s="3" t="inlineStr">
+        <is>
+          <t>20250723T184217.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B38" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="C38" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="D38" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="F38" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="G38" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H38" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I38" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J38" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K38" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="L38" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="M38" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="N38" s="3" t="inlineStr">
+        <is>
+          <t>20250723T184046.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B39" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="C39" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="D39" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="F39" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="G39" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H39" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="I39" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="J39" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="K39" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L39" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M39" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N39" s="3" t="inlineStr">
+        <is>
+          <t>20250723T183543.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="B40" s="1" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="C40" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D40" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F40" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="G40" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H40" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I40" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J40" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K40" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L40" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M40" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N40" s="3" t="inlineStr">
+        <is>
+          <t>20250723T184352.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="B41" s="1" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="C41" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D41" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E41" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F41" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="G41" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H41" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I41" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J41" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K41" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L41" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M41" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N41" s="3" t="inlineStr">
+        <is>
+          <t>20250723T184133.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="B42" s="1" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="C42" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D42" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E42" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F42" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="G42" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H42" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I42" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J42" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K42" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L42" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M42" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N42" s="3" t="inlineStr">
+        <is>
+          <t>20250723T183913.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-23 21:37:40)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -8703,7 +8703,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N20"/>
+  <dimension ref="A3:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10004,6 +10004,150 @@
       <c r="N20" s="3" t="inlineStr">
         <is>
           <t>20250723T185319.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="C21" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>8-BIT</t>
+        </is>
+      </c>
+      <c r="F21" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="G21" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H21" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="I21" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="J21" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="K21" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L21" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="M21" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="N21" s="3" t="inlineStr">
+        <is>
+          <t>20250723T190839.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="inlineStr">
+        <is>
+          <t>8-BIT</t>
+        </is>
+      </c>
+      <c r="F22" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="G22" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H22" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="I22" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="J22" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="K22" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L22" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="M22" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="N22" s="3" t="inlineStr">
+        <is>
+          <t>20250723T190617.000Z</t>
         </is>
       </c>
     </row>
@@ -13459,7 +13603,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N24"/>
+  <dimension ref="A3:N33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15048,6 +15192,654 @@
       <c r="N24" s="3" t="inlineStr">
         <is>
           <t>20250723T190423.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C25" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D25" s="2" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="inlineStr">
+        <is>
+          <t>MAX</t>
+        </is>
+      </c>
+      <c r="F25" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="G25" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H25" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I25" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J25" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K25" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L25" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M25" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N25" s="3" t="inlineStr">
+        <is>
+          <t>20250723T192017.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B26" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C26" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="inlineStr">
+        <is>
+          <t>MAX</t>
+        </is>
+      </c>
+      <c r="F26" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="G26" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H26" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I26" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J26" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K26" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L26" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M26" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N26" s="3" t="inlineStr">
+        <is>
+          <t>20250723T191721.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B27" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C27" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D27" s="2" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="inlineStr">
+        <is>
+          <t>MAX</t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="G27" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H27" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I27" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J27" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K27" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L27" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M27" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N27" s="3" t="inlineStr">
+        <is>
+          <t>20250723T191316.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="B28" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="C28" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="D28" s="2" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="inlineStr">
+        <is>
+          <t>POCO</t>
+        </is>
+      </c>
+      <c r="F28" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="G28" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H28" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="I28" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="J28" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="K28" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L28" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="M28" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="N28" s="3" t="inlineStr">
+        <is>
+          <t>20250723T190632.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B29" s="1" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="C29" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E29" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="F29" s="2" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="G29" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H29" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="I29" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="J29" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K29" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L29" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="M29" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="N29" s="3" t="inlineStr">
+        <is>
+          <t>20250723T193329.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B30" s="1" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="C30" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="F30" s="2" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="G30" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H30" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="I30" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="J30" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K30" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L30" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="M30" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="N30" s="3" t="inlineStr">
+        <is>
+          <t>20250723T193122.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B31" s="1" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="C31" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="D31" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="F31" s="2" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="G31" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H31" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="I31" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="J31" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K31" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L31" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="M31" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="N31" s="3" t="inlineStr">
+        <is>
+          <t>20250723T192757.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="F32" s="2" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="G32" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H32" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="I32" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="J32" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K32" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L32" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M32" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N32" s="3" t="inlineStr">
+        <is>
+          <t>20250723T192116.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B33" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="C33" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="D33" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="E33" s="2" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="F33" s="2" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="G33" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H33" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="I33" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="J33" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K33" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L33" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M33" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N33" s="3" t="inlineStr">
+        <is>
+          <t>20250723T191844.000Z</t>
         </is>
       </c>
     </row>
@@ -15062,7 +15854,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N39"/>
+  <dimension ref="A3:N41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17731,6 +18523,150 @@
       <c r="N39" s="3" t="inlineStr">
         <is>
           <t>20250723T185107.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B40" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C40" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="D40" s="2" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F40" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G40" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H40" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I40" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J40" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K40" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L40" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M40" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N40" s="3" t="inlineStr">
+        <is>
+          <t>20250723T191034.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B41" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C41" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="D41" s="2" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="E41" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F41" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G41" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H41" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I41" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J41" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K41" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L41" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M41" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N41" s="3" t="inlineStr">
+        <is>
+          <t>20250723T190644.000Z</t>
         </is>
       </c>
     </row>
@@ -20644,7 +21580,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N29"/>
+  <dimension ref="A3:N34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22593,6 +23529,366 @@
       <c r="N29" s="3" t="inlineStr">
         <is>
           <t>20250723T173242.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="B30" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="C30" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="F30" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="G30" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H30" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I30" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J30" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K30" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="L30" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M30" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="N30" s="3" t="inlineStr">
+        <is>
+          <t>20250723T193558.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="B31" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="C31" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D31" s="2" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="F31" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G31" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H31" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I31" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J31" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="K31" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L31" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="M31" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N31" s="3" t="inlineStr">
+        <is>
+          <t>20250723T193327.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="inlineStr">
+        <is>
+          <t>PENNY</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="F32" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G32" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H32" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I32" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J32" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="K32" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L32" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="M32" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N32" s="3" t="inlineStr">
+        <is>
+          <t>20250723T192116.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="B33" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="C33" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="D33" s="2" t="inlineStr">
+        <is>
+          <t>PENNY</t>
+        </is>
+      </c>
+      <c r="E33" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="F33" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G33" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H33" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I33" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J33" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="K33" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L33" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="M33" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N33" s="3" t="inlineStr">
+        <is>
+          <t>20250723T191857.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="B34" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="C34" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
+          <t>PENNY</t>
+        </is>
+      </c>
+      <c r="E34" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="F34" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G34" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H34" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I34" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J34" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="K34" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L34" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="M34" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N34" s="3" t="inlineStr">
+        <is>
+          <t>20250723T191637.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-23 22:09:01)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -11856,7 +11856,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N26"/>
+  <dimension ref="A3:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13589,6 +13589,150 @@
       <c r="N26" s="3" t="inlineStr">
         <is>
           <t>20250723T160930.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B27" s="1" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="C27" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="D27" s="2" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G27" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H27" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I27" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J27" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K27" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L27" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M27" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N27" s="3" t="inlineStr">
+        <is>
+          <t>20250723T194214.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B28" s="1" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="C28" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="D28" s="2" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F28" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G28" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H28" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I28" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J28" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K28" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L28" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M28" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N28" s="3" t="inlineStr">
+        <is>
+          <t>20250723T194003.000Z</t>
         </is>
       </c>
     </row>
@@ -21580,7 +21724,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N34"/>
+  <dimension ref="A3:N35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23889,6 +24033,78 @@
       <c r="N34" s="3" t="inlineStr">
         <is>
           <t>20250723T191637.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="B35" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="C35" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="D35" s="2" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="E35" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F35" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="G35" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H35" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I35" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="J35" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K35" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L35" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="M35" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="N35" s="3" t="inlineStr">
+        <is>
+          <t>20250723T193737.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-23 22:40:26)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -4667,7 +4667,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N30"/>
+  <dimension ref="A3:N35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6688,6 +6688,366 @@
       <c r="N30" s="3" t="inlineStr">
         <is>
           <t>20250723T181050.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="B31" s="1" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="C31" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D31" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="F31" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="G31" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H31" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="I31" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="J31" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="K31" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="L31" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Zoulan</t>
+        </is>
+      </c>
+      <c r="M31" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="N31" s="3" t="inlineStr">
+        <is>
+          <t>20250723T203134.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="F32" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="G32" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H32" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="I32" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="J32" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="K32" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="L32" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Zoulan</t>
+        </is>
+      </c>
+      <c r="M32" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="N32" s="3" t="inlineStr">
+        <is>
+          <t>20250723T202922.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="B33" s="1" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="C33" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D33" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E33" s="2" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="F33" s="2" t="inlineStr">
+        <is>
+          <t>JESSIE</t>
+        </is>
+      </c>
+      <c r="G33" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H33" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="I33" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="J33" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="K33" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="L33" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="M33" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Zoulan</t>
+        </is>
+      </c>
+      <c r="N33" s="3" t="inlineStr">
+        <is>
+          <t>20250723T202204.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="B34" s="1" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="C34" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E34" s="2" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="F34" s="2" t="inlineStr">
+        <is>
+          <t>JESSIE</t>
+        </is>
+      </c>
+      <c r="G34" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H34" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="I34" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="J34" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="K34" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="L34" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="M34" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Zoulan</t>
+        </is>
+      </c>
+      <c r="N34" s="3" t="inlineStr">
+        <is>
+          <t>20250723T202032.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="B35" s="1" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="C35" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D35" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E35" s="2" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="F35" s="2" t="inlineStr">
+        <is>
+          <t>JESSIE</t>
+        </is>
+      </c>
+      <c r="G35" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H35" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="I35" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="J35" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="K35" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="L35" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="M35" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Zoulan</t>
+        </is>
+      </c>
+      <c r="N35" s="3" t="inlineStr">
+        <is>
+          <t>20250723T201744.000Z</t>
         </is>
       </c>
     </row>
@@ -18825,7 +19185,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N42"/>
+  <dimension ref="A3:N43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21710,6 +22070,78 @@
       <c r="N42" s="3" t="inlineStr">
         <is>
           <t>20250723T183913.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="B43" s="1" t="inlineStr">
+        <is>
+          <t>MANDY</t>
+        </is>
+      </c>
+      <c r="C43" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D43" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="E43" s="2" t="inlineStr">
+        <is>
+          <t>CHESTER</t>
+        </is>
+      </c>
+      <c r="F43" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="G43" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H43" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="I43" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="J43" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="K43" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="L43" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Zoulan</t>
+        </is>
+      </c>
+      <c r="M43" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="N43" s="3" t="inlineStr">
+        <is>
+          <t>20250723T203907.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-23 23:11:48)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -16358,7 +16358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N41"/>
+  <dimension ref="A3:N44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19171,6 +19171,222 @@
       <c r="N41" s="3" t="inlineStr">
         <is>
           <t>20250723T190644.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>OTIS</t>
+        </is>
+      </c>
+      <c r="B42" s="1" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="C42" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D42" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E42" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="F42" s="2" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="G42" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H42" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="I42" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="J42" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="K42" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L42" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="M42" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="N42" s="3" t="inlineStr">
+        <is>
+          <t>20250723T210916.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="B43" s="1" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="C43" s="1" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="D43" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E43" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F43" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="G43" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H43" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="I43" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="J43" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="K43" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="L43" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Zoulan</t>
+        </is>
+      </c>
+      <c r="M43" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="N43" s="3" t="inlineStr">
+        <is>
+          <t>20250723T205905.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="B44" s="1" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="C44" s="1" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="D44" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E44" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F44" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="G44" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H44" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="I44" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="J44" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="K44" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="L44" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Zoulan</t>
+        </is>
+      </c>
+      <c r="M44" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="N44" s="3" t="inlineStr">
+        <is>
+          <t>20250723T205709.000Z</t>
         </is>
       </c>
     </row>
@@ -19185,7 +19401,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N43"/>
+  <dimension ref="A3:N47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22142,6 +22358,294 @@
       <c r="N43" s="3" t="inlineStr">
         <is>
           <t>20250723T203907.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="B44" s="1" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="C44" s="1" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="D44" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="E44" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F44" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G44" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H44" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="I44" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="J44" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="K44" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Zoulan</t>
+        </is>
+      </c>
+      <c r="L44" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="M44" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="N44" s="3" t="inlineStr">
+        <is>
+          <t>20250723T205134.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="B45" s="1" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="C45" s="1" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="D45" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="E45" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F45" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G45" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H45" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="I45" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="J45" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="K45" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Zoulan</t>
+        </is>
+      </c>
+      <c r="L45" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="M45" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="N45" s="3" t="inlineStr">
+        <is>
+          <t>20250723T204933.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="B46" s="1" t="inlineStr">
+        <is>
+          <t>MANDY</t>
+        </is>
+      </c>
+      <c r="C46" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D46" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="E46" s="2" t="inlineStr">
+        <is>
+          <t>CHESTER</t>
+        </is>
+      </c>
+      <c r="F46" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="G46" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H46" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="I46" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="J46" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="K46" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="L46" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Zoulan</t>
+        </is>
+      </c>
+      <c r="M46" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="N46" s="3" t="inlineStr">
+        <is>
+          <t>20250723T204346.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="B47" s="1" t="inlineStr">
+        <is>
+          <t>MANDY</t>
+        </is>
+      </c>
+      <c r="C47" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D47" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="E47" s="2" t="inlineStr">
+        <is>
+          <t>CHESTER</t>
+        </is>
+      </c>
+      <c r="F47" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="G47" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H47" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="I47" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="J47" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="K47" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="L47" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Zoulan</t>
+        </is>
+      </c>
+      <c r="M47" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="N47" s="3" t="inlineStr">
+        <is>
+          <t>20250723T204126.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-23 23:43:20)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -12216,7 +12216,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N28"/>
+  <dimension ref="A3:N29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14093,6 +14093,78 @@
       <c r="N28" s="3" t="inlineStr">
         <is>
           <t>20250723T194003.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="B29" s="1" t="inlineStr">
+        <is>
+          <t>FANG</t>
+        </is>
+      </c>
+      <c r="C29" s="1" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="E29" s="2" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="F29" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G29" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H29" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="I29" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="J29" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="K29" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L29" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="M29" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="N29" s="3" t="inlineStr">
+        <is>
+          <t>20250723T214219.000Z</t>
         </is>
       </c>
     </row>
@@ -14107,7 +14179,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N33"/>
+  <dimension ref="A3:N39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16344,6 +16416,438 @@
       <c r="N33" s="3" t="inlineStr">
         <is>
           <t>20250723T191844.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="B34" s="1" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="C34" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="E34" s="2" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="F34" s="2" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="G34" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H34" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="I34" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="J34" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="K34" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L34" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="M34" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="N34" s="3" t="inlineStr">
+        <is>
+          <t>20250723T213441.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="B35" s="1" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="C35" s="1" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="D35" s="2" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="E35" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F35" s="2" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="G35" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H35" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="I35" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="J35" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="K35" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="L35" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="M35" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="N35" s="3" t="inlineStr">
+        <is>
+          <t>20250723T213259.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="B36" s="1" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="C36" s="1" t="inlineStr">
+        <is>
+          <t>COLT</t>
+        </is>
+      </c>
+      <c r="D36" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="F36" s="2" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="G36" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H36" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="I36" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="J36" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="K36" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L36" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="M36" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="N36" s="3" t="inlineStr">
+        <is>
+          <t>20250723T213012.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="B37" s="1" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="C37" s="1" t="inlineStr">
+        <is>
+          <t>COLT</t>
+        </is>
+      </c>
+      <c r="D37" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="F37" s="2" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="G37" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H37" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="I37" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="J37" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="K37" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L37" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="M37" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="N37" s="3" t="inlineStr">
+        <is>
+          <t>20250723T212737.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>GROM</t>
+        </is>
+      </c>
+      <c r="B38" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C38" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="D38" s="2" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="F38" s="2" t="inlineStr">
+        <is>
+          <t>MANDY</t>
+        </is>
+      </c>
+      <c r="G38" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H38" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="I38" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="J38" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="K38" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L38" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="M38" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="N38" s="3" t="inlineStr">
+        <is>
+          <t>20250723T212215.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>GROM</t>
+        </is>
+      </c>
+      <c r="B39" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C39" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="D39" s="2" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="F39" s="2" t="inlineStr">
+        <is>
+          <t>MANDY</t>
+        </is>
+      </c>
+      <c r="G39" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H39" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="I39" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="J39" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="K39" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L39" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="M39" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="N39" s="3" t="inlineStr">
+        <is>
+          <t>20250723T212017.000Z</t>
         </is>
       </c>
     </row>
@@ -16358,7 +16862,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N44"/>
+  <dimension ref="A3:N45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19387,6 +19891,78 @@
       <c r="N44" s="3" t="inlineStr">
         <is>
           <t>20250723T205709.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>OTIS</t>
+        </is>
+      </c>
+      <c r="B45" s="1" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="C45" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D45" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E45" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="F45" s="2" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="G45" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H45" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="I45" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="J45" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="K45" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L45" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="M45" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="N45" s="3" t="inlineStr">
+        <is>
+          <t>20250723T211205.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-24 00:14:41)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -12216,7 +12216,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N29"/>
+  <dimension ref="A3:N33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14165,6 +14165,294 @@
       <c r="N29" s="3" t="inlineStr">
         <is>
           <t>20250723T214219.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="B30" s="1" t="inlineStr">
+        <is>
+          <t>FANG</t>
+        </is>
+      </c>
+      <c r="C30" s="1" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F30" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G30" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H30" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="I30" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="J30" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="K30" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L30" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="M30" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="N30" s="3" t="inlineStr">
+        <is>
+          <t>20250723T215318.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="B31" s="1" t="inlineStr">
+        <is>
+          <t>FANG</t>
+        </is>
+      </c>
+      <c r="C31" s="1" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="D31" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F31" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G31" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H31" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="I31" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="J31" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="K31" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L31" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="M31" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="N31" s="3" t="inlineStr">
+        <is>
+          <t>20250723T215136.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>FANG</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F32" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G32" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H32" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="I32" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="J32" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="K32" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L32" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="M32" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="N32" s="3" t="inlineStr">
+        <is>
+          <t>20250723T214926.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="B33" s="1" t="inlineStr">
+        <is>
+          <t>FANG</t>
+        </is>
+      </c>
+      <c r="C33" s="1" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="D33" s="2" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="E33" s="2" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="F33" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G33" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H33" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="I33" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="J33" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="K33" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L33" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="M33" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="N33" s="3" t="inlineStr">
+        <is>
+          <t>20250723T214405.000Z</t>
         </is>
       </c>
     </row>
@@ -16862,7 +17150,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N45"/>
+  <dimension ref="A3:N47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19963,6 +20251,150 @@
       <c r="N45" s="3" t="inlineStr">
         <is>
           <t>20250723T211205.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B46" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="C46" s="1" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="D46" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E46" s="2" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="F46" s="2" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="G46" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H46" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="I46" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="J46" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="K46" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L46" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="M46" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="N46" s="3" t="inlineStr">
+        <is>
+          <t>20250723T220010.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B47" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="C47" s="1" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="D47" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E47" s="2" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="F47" s="2" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="G47" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H47" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="I47" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="J47" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="K47" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L47" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="M47" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="N47" s="3" t="inlineStr">
+        <is>
+          <t>20250723T215842.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-24 01:48:39)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -24,6 +24,7 @@
     <sheet name="Ring of Fire" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="Pit Stop" sheetId="16" state="visible" r:id="rId16"/>
     <sheet name="Sneaky Fields" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="Hideout" sheetId="18" state="visible" r:id="rId18"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -453,7 +454,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N54"/>
+  <dimension ref="A3:N56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4202,6 +4203,150 @@
       <c r="N54" s="3" t="inlineStr">
         <is>
           <t>20250723T181618.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="B55" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="C55" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="D55" s="2" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="E55" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F55" s="2" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="G55" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H55" s="3" t="inlineStr">
+        <is>
+          <t>Always cool🧃</t>
+        </is>
+      </c>
+      <c r="I55" s="3" t="inlineStr">
+        <is>
+          <t>DMO|Marco</t>
+        </is>
+      </c>
+      <c r="J55" s="3" t="inlineStr">
+        <is>
+          <t>Dan-YT</t>
+        </is>
+      </c>
+      <c r="K55" s="3" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="L55" s="3" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="M55" s="3" t="inlineStr">
+        <is>
+          <t>Jxcccr🐻‍❄️</t>
+        </is>
+      </c>
+      <c r="N55" s="3" t="inlineStr">
+        <is>
+          <t>20250723T233911.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="B56" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="C56" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="D56" s="2" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="E56" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F56" s="2" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="G56" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H56" s="3" t="inlineStr">
+        <is>
+          <t>Always cool🧃</t>
+        </is>
+      </c>
+      <c r="I56" s="3" t="inlineStr">
+        <is>
+          <t>DMO|Marco</t>
+        </is>
+      </c>
+      <c r="J56" s="3" t="inlineStr">
+        <is>
+          <t>Dan-YT</t>
+        </is>
+      </c>
+      <c r="K56" s="3" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="L56" s="3" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="M56" s="3" t="inlineStr">
+        <is>
+          <t>Jxcccr🐻‍❄️</t>
+        </is>
+      </c>
+      <c r="N56" s="3" t="inlineStr">
+        <is>
+          <t>20250723T233746.000Z</t>
         </is>
       </c>
     </row>
@@ -12210,6 +12355,169 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A3:N4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>B1</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>B1</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>Ganador</t>
+        </is>
+      </c>
+      <c r="H3" s="3" t="inlineStr">
+        <is>
+          <t>Jugador 1</t>
+        </is>
+      </c>
+      <c r="I3" s="3" t="inlineStr">
+        <is>
+          <t>Jugador 2</t>
+        </is>
+      </c>
+      <c r="J3" s="3" t="inlineStr">
+        <is>
+          <t>Jugador 3</t>
+        </is>
+      </c>
+      <c r="K3" s="3" t="inlineStr">
+        <is>
+          <t>Jugador 4</t>
+        </is>
+      </c>
+      <c r="L3" s="3" t="inlineStr">
+        <is>
+          <t>Jugador 5</t>
+        </is>
+      </c>
+      <c r="M3" s="3" t="inlineStr">
+        <is>
+          <t>Jugador 6</t>
+        </is>
+      </c>
+      <c r="N3" s="3" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="G4" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H4" s="3" t="inlineStr">
+        <is>
+          <t>Always cool🧃</t>
+        </is>
+      </c>
+      <c r="I4" s="3" t="inlineStr">
+        <is>
+          <t>DMO|Marco</t>
+        </is>
+      </c>
+      <c r="J4" s="3" t="inlineStr">
+        <is>
+          <t>Dan-YT</t>
+        </is>
+      </c>
+      <c r="K4" s="3" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="L4" s="3" t="inlineStr">
+        <is>
+          <t>Jxcccr🐻‍❄️</t>
+        </is>
+      </c>
+      <c r="M4" s="3" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="N4" s="3" t="inlineStr">
+        <is>
+          <t>20250723T234640.000Z</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -26063,7 +26371,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N21"/>
+  <dimension ref="A3:N23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -27436,6 +27744,150 @@
       <c r="N21" s="3" t="inlineStr">
         <is>
           <t>20250723T170038.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="F22" s="2" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="G22" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H22" s="3" t="inlineStr">
+        <is>
+          <t>DMO|Marco</t>
+        </is>
+      </c>
+      <c r="I22" s="3" t="inlineStr">
+        <is>
+          <t>Dan-YT</t>
+        </is>
+      </c>
+      <c r="J22" s="3" t="inlineStr">
+        <is>
+          <t>Always cool🧃</t>
+        </is>
+      </c>
+      <c r="K22" s="3" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="L22" s="3" t="inlineStr">
+        <is>
+          <t>Jxcccr🐻‍❄️</t>
+        </is>
+      </c>
+      <c r="M22" s="3" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="N22" s="3" t="inlineStr">
+        <is>
+          <t>20250723T232930.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="F23" s="2" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="G23" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H23" s="3" t="inlineStr">
+        <is>
+          <t>DMO|Marco</t>
+        </is>
+      </c>
+      <c r="I23" s="3" t="inlineStr">
+        <is>
+          <t>Dan-YT</t>
+        </is>
+      </c>
+      <c r="J23" s="3" t="inlineStr">
+        <is>
+          <t>Always cool🧃</t>
+        </is>
+      </c>
+      <c r="K23" s="3" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="L23" s="3" t="inlineStr">
+        <is>
+          <t>Jxcccr🐻‍❄️</t>
+        </is>
+      </c>
+      <c r="M23" s="3" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="N23" s="3" t="inlineStr">
+        <is>
+          <t>20250723T232641.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-24 02:20:00)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -12361,7 +12361,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N4"/>
+  <dimension ref="A3:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12510,6 +12510,78 @@
       <c r="N4" s="3" t="inlineStr">
         <is>
           <t>20250723T234640.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="G5" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H5" s="3" t="inlineStr">
+        <is>
+          <t>Always cool🧃</t>
+        </is>
+      </c>
+      <c r="I5" s="3" t="inlineStr">
+        <is>
+          <t>DMO|Marco</t>
+        </is>
+      </c>
+      <c r="J5" s="3" t="inlineStr">
+        <is>
+          <t>Dan-YT</t>
+        </is>
+      </c>
+      <c r="K5" s="3" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="L5" s="3" t="inlineStr">
+        <is>
+          <t>Jxcccr🐻‍❄️</t>
+        </is>
+      </c>
+      <c r="M5" s="3" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="N5" s="3" t="inlineStr">
+        <is>
+          <t>20250723T234900.000Z</t>
         </is>
       </c>
     </row>
@@ -12524,7 +12596,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N33"/>
+  <dimension ref="A3:N35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14761,6 +14833,150 @@
       <c r="N33" s="3" t="inlineStr">
         <is>
           <t>20250723T214405.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="B34" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C34" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="E34" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F34" s="2" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="G34" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H34" s="3" t="inlineStr">
+        <is>
+          <t>Always cool🧃</t>
+        </is>
+      </c>
+      <c r="I34" s="3" t="inlineStr">
+        <is>
+          <t>Dan-YT</t>
+        </is>
+      </c>
+      <c r="J34" s="3" t="inlineStr">
+        <is>
+          <t>DMO|Marco</t>
+        </is>
+      </c>
+      <c r="K34" s="3" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="L34" s="3" t="inlineStr">
+        <is>
+          <t>Jxcccr🐻‍❄️</t>
+        </is>
+      </c>
+      <c r="M34" s="3" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="N34" s="3" t="inlineStr">
+        <is>
+          <t>20250723T235810.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="B35" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C35" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="D35" s="2" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="E35" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F35" s="2" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="G35" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H35" s="3" t="inlineStr">
+        <is>
+          <t>Always cool🧃</t>
+        </is>
+      </c>
+      <c r="I35" s="3" t="inlineStr">
+        <is>
+          <t>Dan-YT</t>
+        </is>
+      </c>
+      <c r="J35" s="3" t="inlineStr">
+        <is>
+          <t>DMO|Marco</t>
+        </is>
+      </c>
+      <c r="K35" s="3" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="L35" s="3" t="inlineStr">
+        <is>
+          <t>Jxcccr🐻‍❄️</t>
+        </is>
+      </c>
+      <c r="M35" s="3" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="N35" s="3" t="inlineStr">
+        <is>
+          <t>20250723T235543.000Z</t>
         </is>
       </c>
     </row>
@@ -27902,7 +28118,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N12"/>
+  <dimension ref="A3:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -28627,6 +28843,150 @@
       <c r="N12" s="3" t="inlineStr">
         <is>
           <t>20250719T011742.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="G13" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H13" s="3" t="inlineStr">
+        <is>
+          <t>Solar Ray ☀️</t>
+        </is>
+      </c>
+      <c r="I13" s="3" t="inlineStr">
+        <is>
+          <t>Finki is back.</t>
+        </is>
+      </c>
+      <c r="J13" s="3" t="inlineStr">
+        <is>
+          <t>Xyz</t>
+        </is>
+      </c>
+      <c r="K13" s="3" t="inlineStr">
+        <is>
+          <t>BC*|Jubileubr</t>
+        </is>
+      </c>
+      <c r="L13" s="3" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="M13" s="3" t="inlineStr">
+        <is>
+          <t>CASA|Doritos</t>
+        </is>
+      </c>
+      <c r="N13" s="3" t="inlineStr">
+        <is>
+          <t>20250724T001158.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="G14" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H14" s="3" t="inlineStr">
+        <is>
+          <t>Solar Ray ☀️</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
+          <t>Finki is back.</t>
+        </is>
+      </c>
+      <c r="J14" s="3" t="inlineStr">
+        <is>
+          <t>Xyz</t>
+        </is>
+      </c>
+      <c r="K14" s="3" t="inlineStr">
+        <is>
+          <t>BC*|Jubileubr</t>
+        </is>
+      </c>
+      <c r="L14" s="3" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="M14" s="3" t="inlineStr">
+        <is>
+          <t>CASA|Doritos</t>
+        </is>
+      </c>
+      <c r="N14" s="3" t="inlineStr">
+        <is>
+          <t>20250724T001013.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-24 02:51:20)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -454,7 +454,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N56"/>
+  <dimension ref="A3:N61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4347,6 +4347,366 @@
       <c r="N56" s="3" t="inlineStr">
         <is>
           <t>20250723T233746.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B57" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="C57" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D57" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E57" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F57" s="2" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="G57" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H57" s="3" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="I57" s="3" t="inlineStr">
+        <is>
+          <t>MTM|snoiy</t>
+        </is>
+      </c>
+      <c r="J57" s="3" t="inlineStr">
+        <is>
+          <t>PLP|Mine</t>
+        </is>
+      </c>
+      <c r="K57" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L57" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="M57" s="3" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="N57" s="3" t="inlineStr">
+        <is>
+          <t>20250724T004228.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B58" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="C58" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D58" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E58" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F58" s="2" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="G58" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H58" s="3" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="I58" s="3" t="inlineStr">
+        <is>
+          <t>MTM|snoiy</t>
+        </is>
+      </c>
+      <c r="J58" s="3" t="inlineStr">
+        <is>
+          <t>PLP|Mine</t>
+        </is>
+      </c>
+      <c r="K58" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L58" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="M58" s="3" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="N58" s="3" t="inlineStr">
+        <is>
+          <t>20250724T004029.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B59" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="C59" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D59" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E59" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F59" s="2" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="G59" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H59" s="3" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="I59" s="3" t="inlineStr">
+        <is>
+          <t>MTM|snoiy</t>
+        </is>
+      </c>
+      <c r="J59" s="3" t="inlineStr">
+        <is>
+          <t>PLP|Mine</t>
+        </is>
+      </c>
+      <c r="K59" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L59" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="M59" s="3" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="N59" s="3" t="inlineStr">
+        <is>
+          <t>20250724T003739.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B60" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="C60" s="1" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="D60" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E60" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="F60" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="G60" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H60" s="3" t="inlineStr">
+        <is>
+          <t>MTM|snoiy</t>
+        </is>
+      </c>
+      <c r="I60" s="3" t="inlineStr">
+        <is>
+          <t>PLP|Mine</t>
+        </is>
+      </c>
+      <c r="J60" s="3" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="K60" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L60" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="M60" s="3" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="N60" s="3" t="inlineStr">
+        <is>
+          <t>20250724T003149.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B61" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="C61" s="1" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="D61" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E61" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="F61" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="G61" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H61" s="3" t="inlineStr">
+        <is>
+          <t>MTM|snoiy</t>
+        </is>
+      </c>
+      <c r="I61" s="3" t="inlineStr">
+        <is>
+          <t>PLP|Mine</t>
+        </is>
+      </c>
+      <c r="J61" s="3" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="K61" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L61" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="M61" s="3" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="N61" s="3" t="inlineStr">
+        <is>
+          <t>20250724T002859.000Z</t>
         </is>
       </c>
     </row>
@@ -4361,7 +4721,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N8"/>
+  <dimension ref="A3:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4798,6 +5158,150 @@
       <c r="N8" s="3" t="inlineStr">
         <is>
           <t>20250720T193837.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>BIBI</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>MANDY</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G9" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H9" s="3" t="inlineStr">
+        <is>
+          <t>Finki is back.</t>
+        </is>
+      </c>
+      <c r="I9" s="3" t="inlineStr">
+        <is>
+          <t>Solar Ray ☀️</t>
+        </is>
+      </c>
+      <c r="J9" s="3" t="inlineStr">
+        <is>
+          <t>Xyz</t>
+        </is>
+      </c>
+      <c r="K9" s="3" t="inlineStr">
+        <is>
+          <t>BC*|Jubileubr</t>
+        </is>
+      </c>
+      <c r="L9" s="3" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="M9" s="3" t="inlineStr">
+        <is>
+          <t>CASA|Doritos</t>
+        </is>
+      </c>
+      <c r="N9" s="3" t="inlineStr">
+        <is>
+          <t>20250724T002248.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>BIBI</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>MANDY</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G10" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H10" s="3" t="inlineStr">
+        <is>
+          <t>Finki is back.</t>
+        </is>
+      </c>
+      <c r="I10" s="3" t="inlineStr">
+        <is>
+          <t>Solar Ray ☀️</t>
+        </is>
+      </c>
+      <c r="J10" s="3" t="inlineStr">
+        <is>
+          <t>Xyz</t>
+        </is>
+      </c>
+      <c r="K10" s="3" t="inlineStr">
+        <is>
+          <t>BC*|Jubileubr</t>
+        </is>
+      </c>
+      <c r="L10" s="3" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="M10" s="3" t="inlineStr">
+        <is>
+          <t>CASA|Doritos</t>
+        </is>
+      </c>
+      <c r="N10" s="3" t="inlineStr">
+        <is>
+          <t>20250724T001957.000Z</t>
         </is>
       </c>
     </row>
@@ -4812,7 +5316,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N35"/>
+  <dimension ref="A3:N43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7193,6 +7697,582 @@
       <c r="N35" s="3" t="inlineStr">
         <is>
           <t>20250723T201744.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B36" s="1" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="C36" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D36" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="F36" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G36" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H36" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I36" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="J36" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K36" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L36" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="M36" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="N36" s="3" t="inlineStr">
+        <is>
+          <t>20250724T004041.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B37" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="C37" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D37" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F37" s="2" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="G37" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H37" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I37" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="J37" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K37" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L37" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="M37" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="N37" s="3" t="inlineStr">
+        <is>
+          <t>20250724T003715.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B38" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="C38" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D38" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F38" s="2" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="G38" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H38" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I38" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="J38" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K38" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L38" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="M38" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="N38" s="3" t="inlineStr">
+        <is>
+          <t>20250724T003540.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B39" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="C39" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D39" s="2" t="inlineStr">
+        <is>
+          <t>JESSIE</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="F39" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="G39" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H39" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I39" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="J39" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K39" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L39" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="M39" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="N39" s="3" t="inlineStr">
+        <is>
+          <t>20250724T002751.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B40" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="C40" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D40" s="2" t="inlineStr">
+        <is>
+          <t>JESSIE</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="F40" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="G40" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H40" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I40" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="J40" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K40" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L40" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="M40" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="N40" s="3" t="inlineStr">
+        <is>
+          <t>20250724T002523.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B41" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="C41" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D41" s="2" t="inlineStr">
+        <is>
+          <t>JESSIE</t>
+        </is>
+      </c>
+      <c r="E41" s="2" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="F41" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="G41" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H41" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I41" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="J41" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K41" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L41" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="M41" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="N41" s="3" t="inlineStr">
+        <is>
+          <t>20250724T002308.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B42" s="1" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="C42" s="1" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="D42" s="2" t="inlineStr">
+        <is>
+          <t>SAM</t>
+        </is>
+      </c>
+      <c r="E42" s="2" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="F42" s="2" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="G42" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H42" s="3" t="inlineStr">
+        <is>
+          <t>Finki is back.</t>
+        </is>
+      </c>
+      <c r="I42" s="3" t="inlineStr">
+        <is>
+          <t>Solar Ray ☀️</t>
+        </is>
+      </c>
+      <c r="J42" s="3" t="inlineStr">
+        <is>
+          <t>Xyz</t>
+        </is>
+      </c>
+      <c r="K42" s="3" t="inlineStr">
+        <is>
+          <t>BC*|Jubileubr</t>
+        </is>
+      </c>
+      <c r="L42" s="3" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="M42" s="3" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="N42" s="3" t="inlineStr">
+        <is>
+          <t>20250724T003147.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B43" s="1" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="C43" s="1" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="D43" s="2" t="inlineStr">
+        <is>
+          <t>SAM</t>
+        </is>
+      </c>
+      <c r="E43" s="2" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="F43" s="2" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="G43" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H43" s="3" t="inlineStr">
+        <is>
+          <t>Finki is back.</t>
+        </is>
+      </c>
+      <c r="I43" s="3" t="inlineStr">
+        <is>
+          <t>Solar Ray ☀️</t>
+        </is>
+      </c>
+      <c r="J43" s="3" t="inlineStr">
+        <is>
+          <t>Xyz</t>
+        </is>
+      </c>
+      <c r="K43" s="3" t="inlineStr">
+        <is>
+          <t>BC*|Jubileubr</t>
+        </is>
+      </c>
+      <c r="L43" s="3" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="M43" s="3" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="N43" s="3" t="inlineStr">
+        <is>
+          <t>20250724T002947.000Z</t>
         </is>
       </c>
     </row>
@@ -20933,7 +22013,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N47"/>
+  <dimension ref="A3:N49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24178,6 +25258,150 @@
       <c r="N47" s="3" t="inlineStr">
         <is>
           <t>20250723T204126.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="B48" s="1" t="inlineStr">
+        <is>
+          <t>PENNY</t>
+        </is>
+      </c>
+      <c r="C48" s="1" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="D48" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E48" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="F48" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G48" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H48" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I48" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="J48" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K48" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L48" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="M48" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="N48" s="3" t="inlineStr">
+        <is>
+          <t>20250724T004857.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="B49" s="1" t="inlineStr">
+        <is>
+          <t>PENNY</t>
+        </is>
+      </c>
+      <c r="C49" s="1" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="D49" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E49" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="F49" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G49" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H49" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I49" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="J49" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K49" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L49" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="M49" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="N49" s="3" t="inlineStr">
+        <is>
+          <t>20250724T004637.000Z</t>
         </is>
       </c>
     </row>
@@ -24192,7 +25416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N35"/>
+  <dimension ref="A3:N37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26573,6 +27797,150 @@
       <c r="N35" s="3" t="inlineStr">
         <is>
           <t>20250723T193737.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="B36" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C36" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D36" s="2" t="inlineStr">
+        <is>
+          <t>MANDY</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F36" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="G36" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H36" s="3" t="inlineStr">
+        <is>
+          <t>Finki is back.</t>
+        </is>
+      </c>
+      <c r="I36" s="3" t="inlineStr">
+        <is>
+          <t>Solar Ray ☀️</t>
+        </is>
+      </c>
+      <c r="J36" s="3" t="inlineStr">
+        <is>
+          <t>Xyz</t>
+        </is>
+      </c>
+      <c r="K36" s="3" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="L36" s="3" t="inlineStr">
+        <is>
+          <t>CASA|Doritos</t>
+        </is>
+      </c>
+      <c r="M36" s="3" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="N36" s="3" t="inlineStr">
+        <is>
+          <t>20250724T004000.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="B37" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C37" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D37" s="2" t="inlineStr">
+        <is>
+          <t>MANDY</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F37" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="G37" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H37" s="3" t="inlineStr">
+        <is>
+          <t>Finki is back.</t>
+        </is>
+      </c>
+      <c r="I37" s="3" t="inlineStr">
+        <is>
+          <t>Solar Ray ☀️</t>
+        </is>
+      </c>
+      <c r="J37" s="3" t="inlineStr">
+        <is>
+          <t>Xyz</t>
+        </is>
+      </c>
+      <c r="K37" s="3" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="L37" s="3" t="inlineStr">
+        <is>
+          <t>CASA|Doritos</t>
+        </is>
+      </c>
+      <c r="M37" s="3" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="N37" s="3" t="inlineStr">
+        <is>
+          <t>20250724T003739.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-24 03:22:41)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -11747,7 +11747,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N20"/>
+  <dimension ref="A3:N27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13048,6 +13048,510 @@
       <c r="N20" s="3" t="inlineStr">
         <is>
           <t>20250723T183644.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>EL PRIMO</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="C21" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="F21" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="G21" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H21" s="3" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="I21" s="3" t="inlineStr">
+        <is>
+          <t>MTM|snoiy</t>
+        </is>
+      </c>
+      <c r="J21" s="3" t="inlineStr">
+        <is>
+          <t>PLP|Mine</t>
+        </is>
+      </c>
+      <c r="K21" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L21" s="3" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="M21" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="N21" s="3" t="inlineStr">
+        <is>
+          <t>20250724T012024.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>EL PRIMO</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="F22" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="G22" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H22" s="3" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="I22" s="3" t="inlineStr">
+        <is>
+          <t>MTM|snoiy</t>
+        </is>
+      </c>
+      <c r="J22" s="3" t="inlineStr">
+        <is>
+          <t>PLP|Mine</t>
+        </is>
+      </c>
+      <c r="K22" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L22" s="3" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="M22" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="N22" s="3" t="inlineStr">
+        <is>
+          <t>20250724T011836.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F23" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G23" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H23" s="3" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="I23" s="3" t="inlineStr">
+        <is>
+          <t>MTM|snoiy</t>
+        </is>
+      </c>
+      <c r="J23" s="3" t="inlineStr">
+        <is>
+          <t>PLP|Mine</t>
+        </is>
+      </c>
+      <c r="K23" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="L23" s="3" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="M23" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="N23" s="3" t="inlineStr">
+        <is>
+          <t>20250724T011227.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D24" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F24" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G24" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H24" s="3" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="I24" s="3" t="inlineStr">
+        <is>
+          <t>MTM|snoiy</t>
+        </is>
+      </c>
+      <c r="J24" s="3" t="inlineStr">
+        <is>
+          <t>PLP|Mine</t>
+        </is>
+      </c>
+      <c r="K24" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="L24" s="3" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="M24" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="N24" s="3" t="inlineStr">
+        <is>
+          <t>20250724T011025.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C25" s="1" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="D25" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="inlineStr">
+        <is>
+          <t>OTIS</t>
+        </is>
+      </c>
+      <c r="F25" s="2" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="G25" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H25" s="3" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="I25" s="3" t="inlineStr">
+        <is>
+          <t>MTM|snoiy</t>
+        </is>
+      </c>
+      <c r="J25" s="3" t="inlineStr">
+        <is>
+          <t>PLP|Mine</t>
+        </is>
+      </c>
+      <c r="K25" s="3" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="L25" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="M25" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="N25" s="3" t="inlineStr">
+        <is>
+          <t>20250724T010505.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B26" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C26" s="1" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="inlineStr">
+        <is>
+          <t>OTIS</t>
+        </is>
+      </c>
+      <c r="F26" s="2" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="G26" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H26" s="3" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="I26" s="3" t="inlineStr">
+        <is>
+          <t>MTM|snoiy</t>
+        </is>
+      </c>
+      <c r="J26" s="3" t="inlineStr">
+        <is>
+          <t>PLP|Mine</t>
+        </is>
+      </c>
+      <c r="K26" s="3" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="L26" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="M26" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="N26" s="3" t="inlineStr">
+        <is>
+          <t>20250724T010329.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B27" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C27" s="1" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="D27" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="inlineStr">
+        <is>
+          <t>OTIS</t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="G27" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H27" s="3" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="I27" s="3" t="inlineStr">
+        <is>
+          <t>MTM|snoiy</t>
+        </is>
+      </c>
+      <c r="J27" s="3" t="inlineStr">
+        <is>
+          <t>PLP|Mine</t>
+        </is>
+      </c>
+      <c r="K27" s="3" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="L27" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="M27" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="N27" s="3" t="inlineStr">
+        <is>
+          <t>20250724T010039.000Z</t>
         </is>
       </c>
     </row>
@@ -18754,7 +19258,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N47"/>
+  <dimension ref="A3:N52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21999,6 +22503,366 @@
       <c r="N47" s="3" t="inlineStr">
         <is>
           <t>20250723T215842.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B48" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C48" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="D48" s="2" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="E48" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F48" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G48" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H48" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I48" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="J48" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K48" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L48" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="M48" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="N48" s="3" t="inlineStr">
+        <is>
+          <t>20250724T011858.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B49" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C49" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="D49" s="2" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="E49" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F49" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G49" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H49" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I49" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="J49" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K49" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L49" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="M49" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="N49" s="3" t="inlineStr">
+        <is>
+          <t>20250724T011722.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B50" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="C50" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D50" s="2" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="E50" s="2" t="inlineStr">
+        <is>
+          <t>SAM</t>
+        </is>
+      </c>
+      <c r="F50" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G50" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H50" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I50" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="J50" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K50" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L50" s="3" t="inlineStr">
+        <is>
+          <t>T1|Keria</t>
+        </is>
+      </c>
+      <c r="M50" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="N50" s="3" t="inlineStr">
+        <is>
+          <t>20250724T011146.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B51" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="C51" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D51" s="2" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="E51" s="2" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="F51" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G51" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H51" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I51" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="J51" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K51" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L51" s="3" t="inlineStr">
+        <is>
+          <t>T1|Keria</t>
+        </is>
+      </c>
+      <c r="M51" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="N51" s="3" t="inlineStr">
+        <is>
+          <t>20250724T010850.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B52" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="C52" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D52" s="2" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="E52" s="2" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="F52" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G52" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H52" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I52" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="J52" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K52" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L52" s="3" t="inlineStr">
+        <is>
+          <t>T1|Keria</t>
+        </is>
+      </c>
+      <c r="M52" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="N52" s="3" t="inlineStr">
+        <is>
+          <t>20250724T010717.000Z</t>
         </is>
       </c>
     </row>
@@ -22013,7 +22877,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N49"/>
+  <dimension ref="A3:N53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25402,6 +26266,294 @@
       <c r="N49" s="3" t="inlineStr">
         <is>
           <t>20250724T004637.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="B50" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="C50" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D50" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="E50" s="2" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="F50" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G50" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H50" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I50" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="J50" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K50" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L50" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="M50" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="N50" s="3" t="inlineStr">
+        <is>
+          <t>20250724T010145.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="B51" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="C51" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D51" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="E51" s="2" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="F51" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G51" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H51" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I51" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="J51" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K51" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L51" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="M51" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="N51" s="3" t="inlineStr">
+        <is>
+          <t>20250724T005945.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="B52" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="C52" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D52" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="E52" s="2" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="F52" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G52" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H52" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I52" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="J52" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K52" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L52" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="M52" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="N52" s="3" t="inlineStr">
+        <is>
+          <t>20250724T005725.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="B53" s="1" t="inlineStr">
+        <is>
+          <t>PENNY</t>
+        </is>
+      </c>
+      <c r="C53" s="1" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="D53" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E53" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="F53" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G53" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H53" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I53" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="J53" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K53" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L53" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="M53" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="N53" s="3" t="inlineStr">
+        <is>
+          <t>20250724T005117.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-24 03:54:01)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -10288,7 +10288,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N22"/>
+  <dimension ref="A3:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11733,6 +11733,438 @@
       <c r="N22" s="3" t="inlineStr">
         <is>
           <t>20250723T190617.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F23" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="G23" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H23" s="3" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="I23" s="3" t="inlineStr">
+        <is>
+          <t>MTM|snoiy</t>
+        </is>
+      </c>
+      <c r="J23" s="3" t="inlineStr">
+        <is>
+          <t>PLP|Mine</t>
+        </is>
+      </c>
+      <c r="K23" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L23" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="M23" s="3" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="N23" s="3" t="inlineStr">
+        <is>
+          <t>20250724T014508.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="D24" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F24" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="G24" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H24" s="3" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="I24" s="3" t="inlineStr">
+        <is>
+          <t>MTM|snoiy</t>
+        </is>
+      </c>
+      <c r="J24" s="3" t="inlineStr">
+        <is>
+          <t>PLP|Mine</t>
+        </is>
+      </c>
+      <c r="K24" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L24" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="M24" s="3" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="N24" s="3" t="inlineStr">
+        <is>
+          <t>20250724T014333.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="C25" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="D25" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="F25" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="G25" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H25" s="3" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="I25" s="3" t="inlineStr">
+        <is>
+          <t>PLP|Mine</t>
+        </is>
+      </c>
+      <c r="J25" s="3" t="inlineStr">
+        <is>
+          <t>MTM|snoiy</t>
+        </is>
+      </c>
+      <c r="K25" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L25" s="3" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="M25" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="N25" s="3" t="inlineStr">
+        <is>
+          <t>20250724T013841.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="B26" s="1" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="C26" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="F26" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="G26" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H26" s="3" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="I26" s="3" t="inlineStr">
+        <is>
+          <t>PLP|Mine</t>
+        </is>
+      </c>
+      <c r="J26" s="3" t="inlineStr">
+        <is>
+          <t>MTM|snoiy</t>
+        </is>
+      </c>
+      <c r="K26" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L26" s="3" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="M26" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="N26" s="3" t="inlineStr">
+        <is>
+          <t>20250724T013629.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="B27" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="C27" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D27" s="2" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="G27" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H27" s="3" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="I27" s="3" t="inlineStr">
+        <is>
+          <t>MTM|snoiy</t>
+        </is>
+      </c>
+      <c r="J27" s="3" t="inlineStr">
+        <is>
+          <t>PLP|Mine</t>
+        </is>
+      </c>
+      <c r="K27" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L27" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="M27" s="3" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="N27" s="3" t="inlineStr">
+        <is>
+          <t>20250724T013157.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="B28" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="C28" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D28" s="2" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F28" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="G28" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H28" s="3" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="I28" s="3" t="inlineStr">
+        <is>
+          <t>MTM|snoiy</t>
+        </is>
+      </c>
+      <c r="J28" s="3" t="inlineStr">
+        <is>
+          <t>PLP|Mine</t>
+        </is>
+      </c>
+      <c r="K28" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L28" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="M28" s="3" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="N28" s="3" t="inlineStr">
+        <is>
+          <t>20250724T012940.000Z</t>
         </is>
       </c>
     </row>
@@ -11747,7 +12179,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N27"/>
+  <dimension ref="A3:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13552,6 +13984,78 @@
       <c r="N27" s="3" t="inlineStr">
         <is>
           <t>20250724T010039.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>EL PRIMO</t>
+        </is>
+      </c>
+      <c r="B28" s="1" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="C28" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="D28" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="F28" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="G28" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H28" s="3" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="I28" s="3" t="inlineStr">
+        <is>
+          <t>MTM|snoiy</t>
+        </is>
+      </c>
+      <c r="J28" s="3" t="inlineStr">
+        <is>
+          <t>PLP|Mine</t>
+        </is>
+      </c>
+      <c r="K28" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L28" s="3" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="M28" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="N28" s="3" t="inlineStr">
+        <is>
+          <t>20250724T012247.000Z</t>
         </is>
       </c>
     </row>
@@ -14180,7 +14684,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N35"/>
+  <dimension ref="A3:N40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16561,6 +17065,366 @@
       <c r="N35" s="3" t="inlineStr">
         <is>
           <t>20250723T235543.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B36" s="1" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="C36" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="D36" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="F36" s="2" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="G36" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H36" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I36" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="J36" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K36" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L36" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="M36" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="N36" s="3" t="inlineStr">
+        <is>
+          <t>20250724T015301.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B37" s="1" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="C37" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="D37" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="F37" s="2" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="G37" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H37" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I37" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="J37" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K37" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L37" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="M37" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="N37" s="3" t="inlineStr">
+        <is>
+          <t>20250724T015106.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B38" s="1" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="C38" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="D38" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="F38" s="2" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="G38" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H38" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I38" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="J38" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K38" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L38" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="M38" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="N38" s="3" t="inlineStr">
+        <is>
+          <t>20250724T014927.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B39" s="1" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="C39" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D39" s="2" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="F39" s="2" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="G39" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H39" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I39" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="J39" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K39" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L39" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="M39" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="N39" s="3" t="inlineStr">
+        <is>
+          <t>20250724T014330.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B40" s="1" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="C40" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D40" s="2" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="F40" s="2" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="G40" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H40" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I40" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="J40" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K40" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L40" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="M40" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="N40" s="3" t="inlineStr">
+        <is>
+          <t>20250724T014150.000Z</t>
         </is>
       </c>
     </row>
@@ -16575,7 +17439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N39"/>
+  <dimension ref="A3:N43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19244,6 +20108,294 @@
       <c r="N39" s="3" t="inlineStr">
         <is>
           <t>20250723T212017.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B40" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C40" s="1" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="D40" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="F40" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G40" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H40" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I40" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="J40" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="K40" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L40" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="M40" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="N40" s="3" t="inlineStr">
+        <is>
+          <t>20250724T013435.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B41" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C41" s="1" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="D41" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="E41" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="F41" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G41" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H41" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I41" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="J41" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="K41" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L41" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="M41" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="N41" s="3" t="inlineStr">
+        <is>
+          <t>20250724T013314.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="B42" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C42" s="1" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="D42" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E42" s="2" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="F42" s="2" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="G42" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H42" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I42" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="J42" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K42" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="L42" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="M42" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="N42" s="3" t="inlineStr">
+        <is>
+          <t>20250724T012752.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="B43" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C43" s="1" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="D43" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E43" s="2" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="F43" s="2" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="G43" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H43" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I43" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="J43" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K43" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="L43" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="M43" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="N43" s="3" t="inlineStr">
+        <is>
+          <t>20250724T012537.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-24 04:25:21)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -27720,7 +27720,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N37"/>
+  <dimension ref="A3:N41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -30245,6 +30245,294 @@
       <c r="N37" s="3" t="inlineStr">
         <is>
           <t>20250724T003739.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="B38" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="C38" s="1" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="D38" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="F38" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="G38" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H38" s="3" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="I38" s="3" t="inlineStr">
+        <is>
+          <t>PLP|Mine</t>
+        </is>
+      </c>
+      <c r="J38" s="3" t="inlineStr">
+        <is>
+          <t>PLP|ultbob19</t>
+        </is>
+      </c>
+      <c r="K38" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L38" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="M38" s="3" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="N38" s="3" t="inlineStr">
+        <is>
+          <t>20250724T020731.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="B39" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="C39" s="1" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="D39" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="F39" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="G39" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H39" s="3" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="I39" s="3" t="inlineStr">
+        <is>
+          <t>PLP|Mine</t>
+        </is>
+      </c>
+      <c r="J39" s="3" t="inlineStr">
+        <is>
+          <t>PLP|ultbob19</t>
+        </is>
+      </c>
+      <c r="K39" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L39" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="M39" s="3" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="N39" s="3" t="inlineStr">
+        <is>
+          <t>20250724T020512.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="B40" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C40" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D40" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="F40" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="G40" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H40" s="3" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="I40" s="3" t="inlineStr">
+        <is>
+          <t>PLP|ultbob19</t>
+        </is>
+      </c>
+      <c r="J40" s="3" t="inlineStr">
+        <is>
+          <t>PLP|Mine</t>
+        </is>
+      </c>
+      <c r="K40" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L40" s="3" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="M40" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="N40" s="3" t="inlineStr">
+        <is>
+          <t>20250724T015945.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="B41" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C41" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D41" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E41" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="F41" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="G41" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H41" s="3" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="I41" s="3" t="inlineStr">
+        <is>
+          <t>PLP|ultbob19</t>
+        </is>
+      </c>
+      <c r="J41" s="3" t="inlineStr">
+        <is>
+          <t>PLP|Mine</t>
+        </is>
+      </c>
+      <c r="K41" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="L41" s="3" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="M41" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="N41" s="3" t="inlineStr">
+        <is>
+          <t>20250724T015733.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-24 14:41:29)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -3121,7 +3121,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N13"/>
+  <dimension ref="A3:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3918,6 +3918,150 @@
       <c r="N13" s="3" t="inlineStr">
         <is>
           <t>20250718T231646.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G14" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H14" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J14" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="K14" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L14" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="M14" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="N14" s="3" t="inlineStr">
+        <is>
+          <t>20250724T123527.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G15" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H15" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J15" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="K15" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L15" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="M15" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="N15" s="3" t="inlineStr">
+        <is>
+          <t>20250724T123344.000Z</t>
         </is>
       </c>
     </row>
@@ -4978,7 +5122,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N8"/>
+  <dimension ref="A3:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5415,6 +5559,510 @@
       <c r="N8" s="3" t="inlineStr">
         <is>
           <t>20250719T012141.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="G9" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H9" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I9" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J9" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="K9" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="L9" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="M9" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="N9" s="3" t="inlineStr">
+        <is>
+          <t>20250724T122621.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="G10" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H10" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I10" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J10" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="K10" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="L10" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="M10" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="N10" s="3" t="inlineStr">
+        <is>
+          <t>20250724T122422.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="G11" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H11" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I11" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J11" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="K11" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="L11" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="M11" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="N11" s="3" t="inlineStr">
+        <is>
+          <t>20250724T122137.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="G12" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H12" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I12" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J12" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="K12" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L12" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M12" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N12" s="3" t="inlineStr">
+        <is>
+          <t>20250724T121601.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="G13" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H13" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I13" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J13" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="K13" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L13" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M13" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N13" s="3" t="inlineStr">
+        <is>
+          <t>20250724T121336.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="G14" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H14" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J14" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="K14" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L14" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M14" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N14" s="3" t="inlineStr">
+        <is>
+          <t>20250724T121108.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>MAX</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G15" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H15" s="3" t="inlineStr">
+        <is>
+          <t>Clarx</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="inlineStr">
+        <is>
+          <t>Ratis</t>
+        </is>
+      </c>
+      <c r="J15" s="3" t="inlineStr">
+        <is>
+          <t>Tinasha</t>
+        </is>
+      </c>
+      <c r="K15" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="L15" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="M15" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="N15" s="3" t="inlineStr">
+        <is>
+          <t>20250724T123957.000Z</t>
         </is>
       </c>
     </row>
@@ -11769,7 +12417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N31"/>
+  <dimension ref="A3:N34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13862,6 +14510,222 @@
       <c r="N31" s="3" t="inlineStr">
         <is>
           <t>20250720T184648.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="F32" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G32" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H32" s="3" t="inlineStr">
+        <is>
+          <t>Responseyy</t>
+        </is>
+      </c>
+      <c r="I32" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|X9Jay</t>
+        </is>
+      </c>
+      <c r="J32" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|Sergeant</t>
+        </is>
+      </c>
+      <c r="K32" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L32" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M32" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N32" s="3" t="inlineStr">
+        <is>
+          <t>20250724T123652.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="B33" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="C33" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="D33" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="E33" s="2" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="F33" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G33" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H33" s="3" t="inlineStr">
+        <is>
+          <t>Responseyy</t>
+        </is>
+      </c>
+      <c r="I33" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|X9Jay</t>
+        </is>
+      </c>
+      <c r="J33" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|Sergeant</t>
+        </is>
+      </c>
+      <c r="K33" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L33" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M33" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N33" s="3" t="inlineStr">
+        <is>
+          <t>20250724T123431.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="B34" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="C34" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="E34" s="2" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="F34" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G34" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H34" s="3" t="inlineStr">
+        <is>
+          <t>Responseyy</t>
+        </is>
+      </c>
+      <c r="I34" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|X9Jay</t>
+        </is>
+      </c>
+      <c r="J34" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|Sergeant</t>
+        </is>
+      </c>
+      <c r="K34" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L34" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M34" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N34" s="3" t="inlineStr">
+        <is>
+          <t>20250724T123211.000Z</t>
         </is>
       </c>
     </row>
@@ -13876,7 +14740,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N25"/>
+  <dimension ref="A3:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15537,6 +16401,510 @@
       <c r="N25" s="3" t="inlineStr">
         <is>
           <t>20250724T002947.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="B26" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C26" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="F26" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="G26" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H26" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I26" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J26" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K26" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L26" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M26" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N26" s="3" t="inlineStr">
+        <is>
+          <t>20250724T123435.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="B27" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C27" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="D27" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="G27" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H27" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I27" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J27" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K27" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L27" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M27" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N27" s="3" t="inlineStr">
+        <is>
+          <t>20250724T123222.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="B28" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="C28" s="1" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="D28" s="2" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F28" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="G28" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H28" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|Sergeant</t>
+        </is>
+      </c>
+      <c r="I28" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|X9Jay</t>
+        </is>
+      </c>
+      <c r="J28" s="3" t="inlineStr">
+        <is>
+          <t>Responseyy</t>
+        </is>
+      </c>
+      <c r="K28" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="L28" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M28" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="N28" s="3" t="inlineStr">
+        <is>
+          <t>20250724T122402.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="B29" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="C29" s="1" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="E29" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F29" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="G29" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H29" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|Sergeant</t>
+        </is>
+      </c>
+      <c r="I29" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|X9Jay</t>
+        </is>
+      </c>
+      <c r="J29" s="3" t="inlineStr">
+        <is>
+          <t>Responseyy</t>
+        </is>
+      </c>
+      <c r="K29" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="L29" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M29" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="N29" s="3" t="inlineStr">
+        <is>
+          <t>20250724T122206.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="B30" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="C30" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F30" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G30" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H30" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|Sergeant</t>
+        </is>
+      </c>
+      <c r="I30" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|X9Jay</t>
+        </is>
+      </c>
+      <c r="J30" s="3" t="inlineStr">
+        <is>
+          <t>Responseyy</t>
+        </is>
+      </c>
+      <c r="K30" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L30" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M30" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N30" s="3" t="inlineStr">
+        <is>
+          <t>20250724T121633.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="B31" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="C31" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="D31" s="2" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F31" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G31" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H31" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|Sergeant</t>
+        </is>
+      </c>
+      <c r="I31" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|X9Jay</t>
+        </is>
+      </c>
+      <c r="J31" s="3" t="inlineStr">
+        <is>
+          <t>Responseyy</t>
+        </is>
+      </c>
+      <c r="K31" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L31" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M31" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N31" s="3" t="inlineStr">
+        <is>
+          <t>20250724T121456.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F32" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G32" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H32" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|Sergeant</t>
+        </is>
+      </c>
+      <c r="I32" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|X9Jay</t>
+        </is>
+      </c>
+      <c r="J32" s="3" t="inlineStr">
+        <is>
+          <t>Responseyy</t>
+        </is>
+      </c>
+      <c r="K32" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L32" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M32" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N32" s="3" t="inlineStr">
+        <is>
+          <t>20250724T121231.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-24 15:12:48)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N16"/>
+  <dimension ref="A3:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1466,6 +1466,366 @@
       <c r="N16" s="3" t="inlineStr">
         <is>
           <t>20250723T233746.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="G17" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H17" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I17" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="J17" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="K17" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L17" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="M17" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="N17" s="3" t="inlineStr">
+        <is>
+          <t>20250724T130626.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F18" s="2" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="G18" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H18" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I18" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="J18" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="K18" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L18" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="M18" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="N18" s="3" t="inlineStr">
+        <is>
+          <t>20250724T130403.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="F19" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="G19" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H19" s="3" t="inlineStr">
+        <is>
+          <t>Ratis</t>
+        </is>
+      </c>
+      <c r="I19" s="3" t="inlineStr">
+        <is>
+          <t>Clarx</t>
+        </is>
+      </c>
+      <c r="J19" s="3" t="inlineStr">
+        <is>
+          <t>Tinasha</t>
+        </is>
+      </c>
+      <c r="K19" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="L19" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="M19" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="N19" s="3" t="inlineStr">
+        <is>
+          <t>20250724T131017.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="F20" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="G20" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H20" s="3" t="inlineStr">
+        <is>
+          <t>Tinasha</t>
+        </is>
+      </c>
+      <c r="I20" s="3" t="inlineStr">
+        <is>
+          <t>Clarx</t>
+        </is>
+      </c>
+      <c r="J20" s="3" t="inlineStr">
+        <is>
+          <t>Ratis</t>
+        </is>
+      </c>
+      <c r="K20" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="L20" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="M20" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="N20" s="3" t="inlineStr">
+        <is>
+          <t>20250724T130316.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="C21" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="F21" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="G21" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H21" s="3" t="inlineStr">
+        <is>
+          <t>Tinasha</t>
+        </is>
+      </c>
+      <c r="I21" s="3" t="inlineStr">
+        <is>
+          <t>Clarx</t>
+        </is>
+      </c>
+      <c r="J21" s="3" t="inlineStr">
+        <is>
+          <t>Ratis</t>
+        </is>
+      </c>
+      <c r="K21" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="L21" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="M21" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="N21" s="3" t="inlineStr">
+        <is>
+          <t>20250724T130026.000Z</t>
         </is>
       </c>
     </row>
@@ -2454,7 +2814,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N11"/>
+  <dimension ref="A3:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3107,6 +3467,294 @@
       <c r="N11" s="3" t="inlineStr">
         <is>
           <t>20250723T232641.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>JESSIE</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="G12" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H12" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I12" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="J12" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="K12" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="L12" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="M12" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="N12" s="3" t="inlineStr">
+        <is>
+          <t>20250724T125734.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>JESSIE</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="G13" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H13" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I13" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="J13" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="K13" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="L13" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="M13" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="N13" s="3" t="inlineStr">
+        <is>
+          <t>20250724T125508.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>EVE</t>
+        </is>
+      </c>
+      <c r="G14" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H14" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J14" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="K14" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L14" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M14" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N14" s="3" t="inlineStr">
+        <is>
+          <t>20250724T125022.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="inlineStr">
+        <is>
+          <t>EVE</t>
+        </is>
+      </c>
+      <c r="G15" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H15" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J15" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="K15" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L15" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M15" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N15" s="3" t="inlineStr">
+        <is>
+          <t>20250724T124909.000Z</t>
         </is>
       </c>
     </row>
@@ -3121,7 +3769,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N15"/>
+  <dimension ref="A3:N18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4062,6 +4710,222 @@
       <c r="N15" s="3" t="inlineStr">
         <is>
           <t>20250724T123344.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G16" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H16" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I16" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="J16" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="K16" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L16" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M16" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N16" s="3" t="inlineStr">
+        <is>
+          <t>20250724T124401.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G17" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H17" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I17" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="J17" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="K17" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L17" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M17" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N17" s="3" t="inlineStr">
+        <is>
+          <t>20250724T124220.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="F18" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G18" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H18" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I18" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="J18" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="K18" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L18" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M18" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N18" s="3" t="inlineStr">
+        <is>
+          <t>20250724T124044.000Z</t>
         </is>
       </c>
     </row>
@@ -5122,7 +5986,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N15"/>
+  <dimension ref="A3:N19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6063,6 +6927,294 @@
       <c r="N15" s="3" t="inlineStr">
         <is>
           <t>20250724T123957.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>POCO</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G16" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H16" s="3" t="inlineStr">
+        <is>
+          <t>Tinasha</t>
+        </is>
+      </c>
+      <c r="I16" s="3" t="inlineStr">
+        <is>
+          <t>Ratis</t>
+        </is>
+      </c>
+      <c r="J16" s="3" t="inlineStr">
+        <is>
+          <t>Clarx</t>
+        </is>
+      </c>
+      <c r="K16" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="L16" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="M16" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="N16" s="3" t="inlineStr">
+        <is>
+          <t>20250724T125242.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>POCO</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G17" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H17" s="3" t="inlineStr">
+        <is>
+          <t>Tinasha</t>
+        </is>
+      </c>
+      <c r="I17" s="3" t="inlineStr">
+        <is>
+          <t>Ratis</t>
+        </is>
+      </c>
+      <c r="J17" s="3" t="inlineStr">
+        <is>
+          <t>Clarx</t>
+        </is>
+      </c>
+      <c r="K17" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="L17" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="M17" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="N17" s="3" t="inlineStr">
+        <is>
+          <t>20250724T124946.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="inlineStr">
+        <is>
+          <t>POCO</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="F18" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G18" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H18" s="3" t="inlineStr">
+        <is>
+          <t>Tinasha</t>
+        </is>
+      </c>
+      <c r="I18" s="3" t="inlineStr">
+        <is>
+          <t>Ratis</t>
+        </is>
+      </c>
+      <c r="J18" s="3" t="inlineStr">
+        <is>
+          <t>Clarx</t>
+        </is>
+      </c>
+      <c r="K18" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="L18" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="M18" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="N18" s="3" t="inlineStr">
+        <is>
+          <t>20250724T124800.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>MAX</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="F19" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G19" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H19" s="3" t="inlineStr">
+        <is>
+          <t>Clarx</t>
+        </is>
+      </c>
+      <c r="I19" s="3" t="inlineStr">
+        <is>
+          <t>Ratis</t>
+        </is>
+      </c>
+      <c r="J19" s="3" t="inlineStr">
+        <is>
+          <t>Tinasha</t>
+        </is>
+      </c>
+      <c r="K19" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="L19" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="M19" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="N19" s="3" t="inlineStr">
+        <is>
+          <t>20250724T124228.000Z</t>
         </is>
       </c>
     </row>
@@ -8059,7 +9211,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N28"/>
+  <dimension ref="A3:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9936,6 +11088,294 @@
       <c r="N28" s="3" t="inlineStr">
         <is>
           <t>20250723T212017.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="B29" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="C29" s="1" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="E29" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F29" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="G29" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H29" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="I29" s="3" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="J29" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="K29" s="3" t="inlineStr">
+        <is>
+          <t>FG|Sun#25</t>
+        </is>
+      </c>
+      <c r="L29" s="3" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="M29" s="3" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="N29" s="3" t="inlineStr">
+        <is>
+          <t>20250724T130958.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="B30" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="C30" s="1" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="F30" s="2" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="G30" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H30" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="I30" s="3" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="J30" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="K30" s="3" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="L30" s="3" t="inlineStr">
+        <is>
+          <t>FG|Sun#25</t>
+        </is>
+      </c>
+      <c r="M30" s="3" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="N30" s="3" t="inlineStr">
+        <is>
+          <t>20250724T130448.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="B31" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="C31" s="1" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="D31" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="F31" s="2" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="G31" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H31" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="I31" s="3" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="J31" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="K31" s="3" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="L31" s="3" t="inlineStr">
+        <is>
+          <t>FG|Sun#25</t>
+        </is>
+      </c>
+      <c r="M31" s="3" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="N31" s="3" t="inlineStr">
+        <is>
+          <t>20250724T130256.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="inlineStr">
+        <is>
+          <t>MAX</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F32" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="G32" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H32" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|Sergeant</t>
+        </is>
+      </c>
+      <c r="I32" s="3" t="inlineStr">
+        <is>
+          <t>Responseyy</t>
+        </is>
+      </c>
+      <c r="J32" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|X9Jay</t>
+        </is>
+      </c>
+      <c r="K32" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L32" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M32" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N32" s="3" t="inlineStr">
+        <is>
+          <t>20250724T131120.000Z</t>
         </is>
       </c>
     </row>
@@ -9950,7 +11390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N36"/>
+  <dimension ref="A3:N45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12403,6 +13843,654 @@
       <c r="N36" s="3" t="inlineStr">
         <is>
           <t>20250720T183042.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B37" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C37" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="D37" s="2" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F37" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="G37" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H37" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I37" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J37" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K37" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L37" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M37" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N37" s="3" t="inlineStr">
+        <is>
+          <t>20250724T131127.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="B38" s="1" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="C38" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D38" s="2" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F38" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G38" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H38" s="3" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="I38" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="J38" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="K38" s="3" t="inlineStr">
+        <is>
+          <t>FG|Sun#25</t>
+        </is>
+      </c>
+      <c r="L38" s="3" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="M38" s="3" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="N38" s="3" t="inlineStr">
+        <is>
+          <t>20250724T125745.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="B39" s="1" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="C39" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D39" s="2" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F39" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G39" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H39" s="3" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="I39" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="J39" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="K39" s="3" t="inlineStr">
+        <is>
+          <t>FG|Sun#25</t>
+        </is>
+      </c>
+      <c r="L39" s="3" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="M39" s="3" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="N39" s="3" t="inlineStr">
+        <is>
+          <t>20250724T125623.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="B40" s="1" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="C40" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D40" s="2" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F40" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G40" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H40" s="3" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="I40" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="J40" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="K40" s="3" t="inlineStr">
+        <is>
+          <t>FG|Sun#25</t>
+        </is>
+      </c>
+      <c r="L40" s="3" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="M40" s="3" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="N40" s="3" t="inlineStr">
+        <is>
+          <t>20250724T125334.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B41" s="1" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="C41" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="D41" s="2" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="E41" s="2" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="F41" s="2" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="G41" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H41" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|X9Jay</t>
+        </is>
+      </c>
+      <c r="I41" s="3" t="inlineStr">
+        <is>
+          <t>Responseyy</t>
+        </is>
+      </c>
+      <c r="J41" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|Sergeant</t>
+        </is>
+      </c>
+      <c r="K41" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L41" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M41" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N41" s="3" t="inlineStr">
+        <is>
+          <t>20250724T130508.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B42" s="1" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="C42" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="D42" s="2" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="E42" s="2" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="F42" s="2" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="G42" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H42" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|X9Jay</t>
+        </is>
+      </c>
+      <c r="I42" s="3" t="inlineStr">
+        <is>
+          <t>Responseyy</t>
+        </is>
+      </c>
+      <c r="J42" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|Sergeant</t>
+        </is>
+      </c>
+      <c r="K42" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L42" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M42" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N42" s="3" t="inlineStr">
+        <is>
+          <t>20250724T130251.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="B43" s="1" t="inlineStr">
+        <is>
+          <t>COLETTE</t>
+        </is>
+      </c>
+      <c r="C43" s="1" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="D43" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E43" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F43" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G43" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H43" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|Sergeant</t>
+        </is>
+      </c>
+      <c r="I43" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|X9Jay</t>
+        </is>
+      </c>
+      <c r="J43" s="3" t="inlineStr">
+        <is>
+          <t>Responseyy</t>
+        </is>
+      </c>
+      <c r="K43" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="L43" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M43" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="N43" s="3" t="inlineStr">
+        <is>
+          <t>20250724T125606.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="B44" s="1" t="inlineStr">
+        <is>
+          <t>COLETTE</t>
+        </is>
+      </c>
+      <c r="C44" s="1" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="D44" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E44" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F44" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G44" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H44" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|Sergeant</t>
+        </is>
+      </c>
+      <c r="I44" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|X9Jay</t>
+        </is>
+      </c>
+      <c r="J44" s="3" t="inlineStr">
+        <is>
+          <t>Responseyy</t>
+        </is>
+      </c>
+      <c r="K44" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="L44" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M44" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="N44" s="3" t="inlineStr">
+        <is>
+          <t>20250724T125415.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="B45" s="1" t="inlineStr">
+        <is>
+          <t>COLETTE</t>
+        </is>
+      </c>
+      <c r="C45" s="1" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="D45" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E45" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F45" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G45" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H45" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|Sergeant</t>
+        </is>
+      </c>
+      <c r="I45" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|X9Jay</t>
+        </is>
+      </c>
+      <c r="J45" s="3" t="inlineStr">
+        <is>
+          <t>Responseyy</t>
+        </is>
+      </c>
+      <c r="K45" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="L45" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M45" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="N45" s="3" t="inlineStr">
+        <is>
+          <t>20250724T125158.000Z</t>
         </is>
       </c>
     </row>
@@ -12417,7 +14505,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N34"/>
+  <dimension ref="A3:N41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14726,6 +16814,510 @@
       <c r="N34" s="3" t="inlineStr">
         <is>
           <t>20250724T123211.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="B35" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C35" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="D35" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="E35" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F35" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="G35" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H35" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="I35" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J35" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="K35" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L35" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M35" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N35" s="3" t="inlineStr">
+        <is>
+          <t>20250724T130522.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="B36" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C36" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="D36" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F36" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="G36" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H36" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="I36" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J36" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="K36" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L36" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M36" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N36" s="3" t="inlineStr">
+        <is>
+          <t>20250724T130326.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B37" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="C37" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="D37" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="F37" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="G37" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H37" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I37" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="J37" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="K37" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L37" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M37" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N37" s="3" t="inlineStr">
+        <is>
+          <t>20250724T125546.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B38" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="C38" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="D38" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="F38" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="G38" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H38" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I38" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="J38" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="K38" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L38" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M38" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N38" s="3" t="inlineStr">
+        <is>
+          <t>20250724T125330.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B39" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="C39" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="D39" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="F39" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="G39" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H39" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I39" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="J39" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="K39" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L39" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M39" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N39" s="3" t="inlineStr">
+        <is>
+          <t>20250724T125111.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B40" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="C40" s="1" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="D40" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="F40" s="2" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="G40" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H40" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|X9Jay</t>
+        </is>
+      </c>
+      <c r="I40" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|Sergeant</t>
+        </is>
+      </c>
+      <c r="J40" s="3" t="inlineStr">
+        <is>
+          <t>Responseyy</t>
+        </is>
+      </c>
+      <c r="K40" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L40" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M40" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N40" s="3" t="inlineStr">
+        <is>
+          <t>20250724T124524.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B41" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="C41" s="1" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="D41" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="E41" s="2" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="F41" s="2" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="G41" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H41" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|X9Jay</t>
+        </is>
+      </c>
+      <c r="I41" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|Sergeant</t>
+        </is>
+      </c>
+      <c r="J41" s="3" t="inlineStr">
+        <is>
+          <t>Responseyy</t>
+        </is>
+      </c>
+      <c r="K41" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L41" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M41" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N41" s="3" t="inlineStr">
+        <is>
+          <t>20250724T124303.000Z</t>
         </is>
       </c>
     </row>
@@ -14740,7 +17332,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N32"/>
+  <dimension ref="A3:N35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16905,6 +19497,222 @@
       <c r="N32" s="3" t="inlineStr">
         <is>
           <t>20250724T121231.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B33" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="C33" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="D33" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E33" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F33" s="2" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="G33" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H33" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I33" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J33" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K33" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L33" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M33" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N33" s="3" t="inlineStr">
+        <is>
+          <t>20250724T124440.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B34" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="C34" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E34" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F34" s="2" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="G34" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H34" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I34" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J34" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K34" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L34" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M34" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N34" s="3" t="inlineStr">
+        <is>
+          <t>20250724T124245.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B35" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="C35" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="D35" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E35" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F35" s="2" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="G35" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H35" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I35" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J35" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K35" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L35" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M35" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N35" s="3" t="inlineStr">
+        <is>
+          <t>20250724T124036.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-24 15:44:09)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -45,7 +45,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -60,6 +60,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00F4CCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D9D9D9"/>
       </patternFill>
     </fill>
   </fills>
@@ -81,13 +86,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -453,7 +459,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N21"/>
+  <dimension ref="A3:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1826,6 +1832,510 @@
       <c r="N21" s="3" t="inlineStr">
         <is>
           <t>20250724T130026.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="F22" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G22" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H22" s="3" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="I22" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="J22" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="K22" s="3" t="inlineStr">
+        <is>
+          <t>FG|Sun#25</t>
+        </is>
+      </c>
+      <c r="L22" s="3" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="M22" s="3" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="N22" s="3" t="inlineStr">
+        <is>
+          <t>20250724T133810.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="F23" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G23" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H23" s="3" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="I23" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="J23" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="K23" s="3" t="inlineStr">
+        <is>
+          <t>FG|Sun#25</t>
+        </is>
+      </c>
+      <c r="L23" s="3" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="M23" s="3" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="N23" s="3" t="inlineStr">
+        <is>
+          <t>20250724T133655.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="D24" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F24" s="2" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="G24" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H24" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="I24" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J24" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="K24" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L24" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M24" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N24" s="3" t="inlineStr">
+        <is>
+          <t>20250724T131642.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="C25" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="D25" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F25" s="2" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="G25" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H25" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="I25" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J25" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="K25" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L25" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M25" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N25" s="3" t="inlineStr">
+        <is>
+          <t>20250724T131353.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="B26" s="1" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="C26" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="F26" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="G26" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H26" s="3" t="inlineStr">
+        <is>
+          <t>Ratis</t>
+        </is>
+      </c>
+      <c r="I26" s="3" t="inlineStr">
+        <is>
+          <t>Clarx</t>
+        </is>
+      </c>
+      <c r="J26" s="3" t="inlineStr">
+        <is>
+          <t>Tinasha</t>
+        </is>
+      </c>
+      <c r="K26" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="L26" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="M26" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="N26" s="3" t="inlineStr">
+        <is>
+          <t>20250724T131931.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="B27" s="1" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="C27" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D27" s="2" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="G27" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H27" s="3" t="inlineStr">
+        <is>
+          <t>Ratis</t>
+        </is>
+      </c>
+      <c r="I27" s="3" t="inlineStr">
+        <is>
+          <t>Clarx</t>
+        </is>
+      </c>
+      <c r="J27" s="3" t="inlineStr">
+        <is>
+          <t>Tinasha</t>
+        </is>
+      </c>
+      <c r="K27" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="L27" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="M27" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="N27" s="3" t="inlineStr">
+        <is>
+          <t>20250724T131656.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="B28" s="1" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="C28" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D28" s="2" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="F28" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="G28" s="6" t="inlineStr">
+        <is>
+          <t>Empate</t>
+        </is>
+      </c>
+      <c r="H28" s="3" t="inlineStr">
+        <is>
+          <t>Ratis</t>
+        </is>
+      </c>
+      <c r="I28" s="3" t="inlineStr">
+        <is>
+          <t>Clarx</t>
+        </is>
+      </c>
+      <c r="J28" s="3" t="inlineStr">
+        <is>
+          <t>Tinasha</t>
+        </is>
+      </c>
+      <c r="K28" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="L28" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="M28" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="N28" s="3" t="inlineStr">
+        <is>
+          <t>20250724T131407.000Z</t>
         </is>
       </c>
     </row>
@@ -2219,7 +2729,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N10"/>
+  <dimension ref="A3:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2800,6 +3310,366 @@
       <c r="N10" s="3" t="inlineStr">
         <is>
           <t>20250720T182517.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="G11" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H11" s="3" t="inlineStr">
+        <is>
+          <t>Tinasha</t>
+        </is>
+      </c>
+      <c r="I11" s="3" t="inlineStr">
+        <is>
+          <t>Ratis</t>
+        </is>
+      </c>
+      <c r="J11" s="3" t="inlineStr">
+        <is>
+          <t>Clarx</t>
+        </is>
+      </c>
+      <c r="K11" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="L11" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="M11" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="N11" s="3" t="inlineStr">
+        <is>
+          <t>20250724T134200.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="G12" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H12" s="3" t="inlineStr">
+        <is>
+          <t>Tinasha</t>
+        </is>
+      </c>
+      <c r="I12" s="3" t="inlineStr">
+        <is>
+          <t>Ratis</t>
+        </is>
+      </c>
+      <c r="J12" s="3" t="inlineStr">
+        <is>
+          <t>Clarx</t>
+        </is>
+      </c>
+      <c r="K12" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="L12" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="M12" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="N12" s="3" t="inlineStr">
+        <is>
+          <t>20250724T133858.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="G13" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H13" s="3" t="inlineStr">
+        <is>
+          <t>Tinasha</t>
+        </is>
+      </c>
+      <c r="I13" s="3" t="inlineStr">
+        <is>
+          <t>Ratis</t>
+        </is>
+      </c>
+      <c r="J13" s="3" t="inlineStr">
+        <is>
+          <t>Clarx</t>
+        </is>
+      </c>
+      <c r="K13" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="L13" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="M13" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="N13" s="3" t="inlineStr">
+        <is>
+          <t>20250724T133653.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>PIPER</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="G14" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H14" s="3" t="inlineStr">
+        <is>
+          <t>Tinasha</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
+          <t>Clarx</t>
+        </is>
+      </c>
+      <c r="J14" s="3" t="inlineStr">
+        <is>
+          <t>Ratis</t>
+        </is>
+      </c>
+      <c r="K14" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="L14" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="M14" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="N14" s="3" t="inlineStr">
+        <is>
+          <t>20250724T132904.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>PIPER</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="G15" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H15" s="3" t="inlineStr">
+        <is>
+          <t>Tinasha</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="inlineStr">
+        <is>
+          <t>Clarx</t>
+        </is>
+      </c>
+      <c r="J15" s="3" t="inlineStr">
+        <is>
+          <t>Ratis</t>
+        </is>
+      </c>
+      <c r="K15" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="L15" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="M15" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="N15" s="3" t="inlineStr">
+        <is>
+          <t>20250724T132544.000Z</t>
         </is>
       </c>
     </row>
@@ -7464,7 +8334,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N26"/>
+  <dimension ref="A3:N36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9197,6 +10067,726 @@
       <c r="N26" s="3" t="inlineStr">
         <is>
           <t>20250723T235543.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B27" s="1" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="C27" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D27" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="G27" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H27" s="3" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="I27" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="J27" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="K27" s="3" t="inlineStr">
+        <is>
+          <t>FG|Sun#25</t>
+        </is>
+      </c>
+      <c r="L27" s="3" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="M27" s="3" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="N27" s="3" t="inlineStr">
+        <is>
+          <t>20250724T133135.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B28" s="1" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="C28" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D28" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F28" s="2" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="G28" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H28" s="3" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="I28" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="J28" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="K28" s="3" t="inlineStr">
+        <is>
+          <t>FG|Sun#25</t>
+        </is>
+      </c>
+      <c r="L28" s="3" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="M28" s="3" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="N28" s="3" t="inlineStr">
+        <is>
+          <t>20250724T132917.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="B29" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C29" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="E29" s="2" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="F29" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G29" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H29" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="I29" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="J29" s="3" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="K29" s="3" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="L29" s="3" t="inlineStr">
+        <is>
+          <t>FG|Sun#25</t>
+        </is>
+      </c>
+      <c r="M29" s="3" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="N29" s="3" t="inlineStr">
+        <is>
+          <t>20250724T132258.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="B30" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C30" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="F30" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G30" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H30" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="I30" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="J30" s="3" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="K30" s="3" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="L30" s="3" t="inlineStr">
+        <is>
+          <t>FG|Sun#25</t>
+        </is>
+      </c>
+      <c r="M30" s="3" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="N30" s="3" t="inlineStr">
+        <is>
+          <t>20250724T132042.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="B31" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C31" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="D31" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="F31" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G31" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H31" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="I31" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="J31" s="3" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="K31" s="3" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="L31" s="3" t="inlineStr">
+        <is>
+          <t>FG|Sun#25</t>
+        </is>
+      </c>
+      <c r="M31" s="3" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="N31" s="3" t="inlineStr">
+        <is>
+          <t>20250724T131821.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>CHESTER</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="F32" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="G32" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H32" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|Sergeant</t>
+        </is>
+      </c>
+      <c r="I32" s="3" t="inlineStr">
+        <is>
+          <t>Responseyy</t>
+        </is>
+      </c>
+      <c r="J32" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|X9Jay</t>
+        </is>
+      </c>
+      <c r="K32" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L32" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M32" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N32" s="3" t="inlineStr">
+        <is>
+          <t>20250724T134225.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="B33" s="1" t="inlineStr">
+        <is>
+          <t>CHESTER</t>
+        </is>
+      </c>
+      <c r="C33" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="D33" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="E33" s="2" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="F33" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="G33" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H33" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|Sergeant</t>
+        </is>
+      </c>
+      <c r="I33" s="3" t="inlineStr">
+        <is>
+          <t>Responseyy</t>
+        </is>
+      </c>
+      <c r="J33" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|X9Jay</t>
+        </is>
+      </c>
+      <c r="K33" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L33" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M33" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N33" s="3" t="inlineStr">
+        <is>
+          <t>20250724T134022.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="B34" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C34" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E34" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="F34" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="G34" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H34" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|Sergeant</t>
+        </is>
+      </c>
+      <c r="I34" s="3" t="inlineStr">
+        <is>
+          <t>Responseyy</t>
+        </is>
+      </c>
+      <c r="J34" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|X9Jay</t>
+        </is>
+      </c>
+      <c r="K34" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="L34" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M34" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="N34" s="3" t="inlineStr">
+        <is>
+          <t>20250724T133343.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="B35" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C35" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="D35" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E35" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="F35" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="G35" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H35" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|Sergeant</t>
+        </is>
+      </c>
+      <c r="I35" s="3" t="inlineStr">
+        <is>
+          <t>Responseyy</t>
+        </is>
+      </c>
+      <c r="J35" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|X9Jay</t>
+        </is>
+      </c>
+      <c r="K35" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="L35" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M35" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="N35" s="3" t="inlineStr">
+        <is>
+          <t>20250724T133153.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="B36" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C36" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="D36" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="F36" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="G36" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H36" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|Sergeant</t>
+        </is>
+      </c>
+      <c r="I36" s="3" t="inlineStr">
+        <is>
+          <t>Responseyy</t>
+        </is>
+      </c>
+      <c r="J36" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|X9Jay</t>
+        </is>
+      </c>
+      <c r="K36" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="L36" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M36" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="N36" s="3" t="inlineStr">
+        <is>
+          <t>20250724T132949.000Z</t>
         </is>
       </c>
     </row>
@@ -9211,7 +10801,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N32"/>
+  <dimension ref="A3:N40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11376,6 +12966,582 @@
       <c r="N32" s="3" t="inlineStr">
         <is>
           <t>20250724T131120.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="B33" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C33" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="D33" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="E33" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F33" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G33" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H33" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="I33" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="J33" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="K33" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L33" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M33" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N33" s="3" t="inlineStr">
+        <is>
+          <t>20250724T134042.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="B34" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C34" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="E34" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F34" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G34" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H34" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="I34" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="J34" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="K34" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L34" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M34" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N34" s="3" t="inlineStr">
+        <is>
+          <t>20250724T133831.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="B35" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C35" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="D35" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="E35" s="2" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="F35" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="G35" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H35" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I35" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J35" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K35" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L35" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M35" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N35" s="3" t="inlineStr">
+        <is>
+          <t>20250724T133141.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="B36" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C36" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="D36" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="F36" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="G36" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H36" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I36" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J36" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K36" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L36" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M36" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N36" s="3" t="inlineStr">
+        <is>
+          <t>20250724T132851.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="B37" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="C37" s="1" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="D37" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F37" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="G37" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H37" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="I37" s="3" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="J37" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="K37" s="3" t="inlineStr">
+        <is>
+          <t>FG|Sun#25</t>
+        </is>
+      </c>
+      <c r="L37" s="3" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="M37" s="3" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="N37" s="3" t="inlineStr">
+        <is>
+          <t>20250724T131217.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="B38" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="C38" s="1" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="D38" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="F38" s="2" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="G38" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H38" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|Sergeant</t>
+        </is>
+      </c>
+      <c r="I38" s="3" t="inlineStr">
+        <is>
+          <t>Responseyy</t>
+        </is>
+      </c>
+      <c r="J38" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|X9Jay</t>
+        </is>
+      </c>
+      <c r="K38" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L38" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M38" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N38" s="3" t="inlineStr">
+        <is>
+          <t>20250724T132330.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="B39" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="C39" s="1" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="D39" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="F39" s="2" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="G39" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H39" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|Sergeant</t>
+        </is>
+      </c>
+      <c r="I39" s="3" t="inlineStr">
+        <is>
+          <t>Responseyy</t>
+        </is>
+      </c>
+      <c r="J39" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|X9Jay</t>
+        </is>
+      </c>
+      <c r="K39" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L39" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M39" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N39" s="3" t="inlineStr">
+        <is>
+          <t>20250724T132054.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="B40" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="C40" s="1" t="inlineStr">
+        <is>
+          <t>MAX</t>
+        </is>
+      </c>
+      <c r="D40" s="2" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F40" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="G40" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H40" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|Sergeant</t>
+        </is>
+      </c>
+      <c r="I40" s="3" t="inlineStr">
+        <is>
+          <t>Responseyy</t>
+        </is>
+      </c>
+      <c r="J40" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|X9Jay</t>
+        </is>
+      </c>
+      <c r="K40" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L40" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M40" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N40" s="3" t="inlineStr">
+        <is>
+          <t>20250724T131503.000Z</t>
         </is>
       </c>
     </row>
@@ -11390,7 +13556,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N45"/>
+  <dimension ref="A3:N49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14491,6 +16657,294 @@
       <c r="N45" s="3" t="inlineStr">
         <is>
           <t>20250724T125158.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B46" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="C46" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="D46" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E46" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="F46" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G46" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H46" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="I46" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="J46" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K46" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L46" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M46" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N46" s="3" t="inlineStr">
+        <is>
+          <t>20250724T132101.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B47" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="C47" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="D47" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E47" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="F47" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G47" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H47" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="I47" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="J47" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K47" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L47" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M47" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N47" s="3" t="inlineStr">
+        <is>
+          <t>20250724T131910.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B48" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="C48" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="D48" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E48" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="F48" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G48" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H48" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="I48" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="J48" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K48" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L48" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M48" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N48" s="3" t="inlineStr">
+        <is>
+          <t>20250724T131731.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B49" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C49" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="D49" s="2" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="E49" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F49" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="G49" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H49" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I49" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J49" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K49" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L49" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M49" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N49" s="3" t="inlineStr">
+        <is>
+          <t>20250724T131250.000Z</t>
         </is>
       </c>
     </row>
@@ -21762,7 +24216,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N15"/>
+  <dimension ref="A3:N18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22703,6 +25157,222 @@
       <c r="N15" s="3" t="inlineStr">
         <is>
           <t>20250724T012940.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G16" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H16" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I16" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="J16" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="K16" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="L16" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="M16" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="N16" s="3" t="inlineStr">
+        <is>
+          <t>20250724T134306.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G17" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H17" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I17" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="J17" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="K17" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="L17" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="M17" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="N17" s="3" t="inlineStr">
+        <is>
+          <t>20250724T134104.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F18" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G18" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H18" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I18" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="J18" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="K18" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="L18" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="M18" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="N18" s="3" t="inlineStr">
+        <is>
+          <t>20250724T133832.000Z</t>
         </is>
       </c>
     </row>
@@ -22717,7 +25387,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N16"/>
+  <dimension ref="A3:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23733,6 +26403,366 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>EDGAR</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G17" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H17" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="I17" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J17" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="K17" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L17" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M17" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N17" s="3" t="inlineStr">
+        <is>
+          <t>20250724T133238.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>EDGAR</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F18" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G18" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H18" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="I18" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J18" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="K18" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L18" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M18" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N18" s="3" t="inlineStr">
+        <is>
+          <t>20250724T133103.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>EDGAR</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F19" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G19" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H19" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="I19" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J19" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="K19" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L19" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M19" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N19" s="3" t="inlineStr">
+        <is>
+          <t>20250724T132910.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>EDGAR</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F20" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G20" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H20" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I20" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="J20" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="K20" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L20" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M20" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N20" s="3" t="inlineStr">
+        <is>
+          <t>20250724T132424.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C21" s="1" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>EDGAR</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F21" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G21" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H21" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="I21" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="J21" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="K21" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L21" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M21" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N21" s="3" t="inlineStr">
+        <is>
+          <t>20250724T132254.000Z</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-24 16:15:30)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -459,7 +459,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N28"/>
+  <dimension ref="A3:N33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2336,6 +2336,366 @@
       <c r="N28" s="3" t="inlineStr">
         <is>
           <t>20250724T131407.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B29" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C29" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E29" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F29" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="G29" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H29" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I29" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J29" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K29" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="L29" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="M29" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="N29" s="3" t="inlineStr">
+        <is>
+          <t>20250724T141328.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B30" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C30" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F30" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="G30" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H30" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I30" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J30" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K30" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="L30" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="M30" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="N30" s="3" t="inlineStr">
+        <is>
+          <t>20250724T141043.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B31" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C31" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D31" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F31" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="G31" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H31" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I31" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J31" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K31" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="L31" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="M31" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="N31" s="3" t="inlineStr">
+        <is>
+          <t>20250724T140728.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="F32" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G32" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H32" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="I32" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="J32" s="3" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="K32" s="3" t="inlineStr">
+        <is>
+          <t>FG|Sun#25</t>
+        </is>
+      </c>
+      <c r="L32" s="3" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="M32" s="3" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="N32" s="3" t="inlineStr">
+        <is>
+          <t>20250724T134853.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="B33" s="1" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="C33" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="D33" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E33" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="F33" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G33" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H33" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="I33" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="J33" s="3" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="K33" s="3" t="inlineStr">
+        <is>
+          <t>FG|Sun#25</t>
+        </is>
+      </c>
+      <c r="L33" s="3" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="M33" s="3" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="N33" s="3" t="inlineStr">
+        <is>
+          <t>20250724T134603.000Z</t>
         </is>
       </c>
     </row>
@@ -8334,7 +8694,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N36"/>
+  <dimension ref="A3:N43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10787,6 +11147,510 @@
       <c r="N36" s="3" t="inlineStr">
         <is>
           <t>20250724T132949.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="B37" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="C37" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D37" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="F37" s="2" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="G37" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H37" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I37" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="J37" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="K37" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L37" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M37" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N37" s="3" t="inlineStr">
+        <is>
+          <t>20250724T135911.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="B38" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="C38" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D38" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="F38" s="2" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="G38" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H38" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I38" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="J38" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="K38" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L38" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M38" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N38" s="3" t="inlineStr">
+        <is>
+          <t>20250724T135717.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="B39" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C39" s="1" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="D39" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="F39" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G39" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H39" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I39" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J39" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K39" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L39" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="M39" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="N39" s="3" t="inlineStr">
+        <is>
+          <t>20250724T135119.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="B40" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C40" s="1" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="D40" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="F40" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G40" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H40" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I40" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J40" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K40" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L40" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="M40" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="N40" s="3" t="inlineStr">
+        <is>
+          <t>20250724T134858.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="B41" s="1" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="C41" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D41" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E41" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F41" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G41" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H41" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|Sergeant</t>
+        </is>
+      </c>
+      <c r="I41" s="3" t="inlineStr">
+        <is>
+          <t>Responseyy</t>
+        </is>
+      </c>
+      <c r="J41" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|X9Jay</t>
+        </is>
+      </c>
+      <c r="K41" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L41" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M41" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N41" s="3" t="inlineStr">
+        <is>
+          <t>20250724T135230.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="B42" s="1" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="C42" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D42" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E42" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F42" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G42" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H42" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|Sergeant</t>
+        </is>
+      </c>
+      <c r="I42" s="3" t="inlineStr">
+        <is>
+          <t>Responseyy</t>
+        </is>
+      </c>
+      <c r="J42" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|X9Jay</t>
+        </is>
+      </c>
+      <c r="K42" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L42" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M42" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N42" s="3" t="inlineStr">
+        <is>
+          <t>20250724T134949.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="B43" s="1" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="C43" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D43" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E43" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F43" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G43" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H43" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|Sergeant</t>
+        </is>
+      </c>
+      <c r="I43" s="3" t="inlineStr">
+        <is>
+          <t>Responseyy</t>
+        </is>
+      </c>
+      <c r="J43" s="3" t="inlineStr">
+        <is>
+          <t>RNTX|X9Jay</t>
+        </is>
+      </c>
+      <c r="K43" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L43" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M43" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N43" s="3" t="inlineStr">
+        <is>
+          <t>20250724T134746.000Z</t>
         </is>
       </c>
     </row>
@@ -19786,7 +20650,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N35"/>
+  <dimension ref="A3:N37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22167,6 +23031,150 @@
       <c r="N35" s="3" t="inlineStr">
         <is>
           <t>20250724T124036.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B36" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C36" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="D36" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="F36" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="G36" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H36" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I36" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J36" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K36" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L36" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M36" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N36" s="3" t="inlineStr">
+        <is>
+          <t>20250724T141156.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B37" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C37" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="D37" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="F37" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="G37" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H37" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I37" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J37" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K37" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L37" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M37" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N37" s="3" t="inlineStr">
+        <is>
+          <t>20250724T141003.000Z</t>
         </is>
       </c>
     </row>
@@ -22181,7 +23189,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N30"/>
+  <dimension ref="A3:N33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24202,6 +25210,222 @@
       <c r="N30" s="3" t="inlineStr">
         <is>
           <t>20250718T233314.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B31" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C31" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="D31" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="F31" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G31" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H31" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="I31" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J31" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="K31" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L31" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M31" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N31" s="3" t="inlineStr">
+        <is>
+          <t>20250724T135651.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="F32" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G32" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H32" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="I32" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J32" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="K32" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L32" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M32" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N32" s="3" t="inlineStr">
+        <is>
+          <t>20250724T135440.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B33" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C33" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="D33" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="E33" s="2" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="F33" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G33" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H33" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="I33" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J33" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="K33" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L33" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M33" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N33" s="3" t="inlineStr">
+        <is>
+          <t>20250724T135219.000Z</t>
         </is>
       </c>
     </row>
@@ -24216,7 +25440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N18"/>
+  <dimension ref="A3:N25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25373,6 +26597,510 @@
       <c r="N18" s="3" t="inlineStr">
         <is>
           <t>20250724T133832.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>CLANCY</t>
+        </is>
+      </c>
+      <c r="F19" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="G19" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H19" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="I19" s="3" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="J19" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="K19" s="3" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="L19" s="3" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="M19" s="3" t="inlineStr">
+        <is>
+          <t>FG|Sun#25</t>
+        </is>
+      </c>
+      <c r="N19" s="3" t="inlineStr">
+        <is>
+          <t>20250724T140554.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="inlineStr">
+        <is>
+          <t>CLANCY</t>
+        </is>
+      </c>
+      <c r="F20" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="G20" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H20" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="I20" s="3" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="J20" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="K20" s="3" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="L20" s="3" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="M20" s="3" t="inlineStr">
+        <is>
+          <t>FG|Sun#25</t>
+        </is>
+      </c>
+      <c r="N20" s="3" t="inlineStr">
+        <is>
+          <t>20250724T140359.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>POCO</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="C21" s="1" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F21" s="2" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="G21" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H21" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="I21" s="3" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="J21" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="K21" s="3" t="inlineStr">
+        <is>
+          <t>FG|Sun#25</t>
+        </is>
+      </c>
+      <c r="L21" s="3" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="M21" s="3" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="N21" s="3" t="inlineStr">
+        <is>
+          <t>20250724T135829.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>POCO</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F22" s="2" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="G22" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H22" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="I22" s="3" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="J22" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="K22" s="3" t="inlineStr">
+        <is>
+          <t>FG|Sun#25</t>
+        </is>
+      </c>
+      <c r="L22" s="3" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="M22" s="3" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="N22" s="3" t="inlineStr">
+        <is>
+          <t>20250724T135653.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>POCO</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F23" s="2" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="G23" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H23" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="I23" s="3" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="J23" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="K23" s="3" t="inlineStr">
+        <is>
+          <t>FG|Sun#25</t>
+        </is>
+      </c>
+      <c r="L23" s="3" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="M23" s="3" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="N23" s="3" t="inlineStr">
+        <is>
+          <t>20250724T135444.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="D24" s="2" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F24" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G24" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H24" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I24" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J24" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K24" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L24" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M24" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N24" s="3" t="inlineStr">
+        <is>
+          <t>20250724T134635.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="C25" s="1" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="D25" s="2" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F25" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="G25" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H25" s="3" t="inlineStr">
+        <is>
+          <t>Tinasha</t>
+        </is>
+      </c>
+      <c r="I25" s="3" t="inlineStr">
+        <is>
+          <t>Ratis</t>
+        </is>
+      </c>
+      <c r="J25" s="3" t="inlineStr">
+        <is>
+          <t>Clarx</t>
+        </is>
+      </c>
+      <c r="K25" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="L25" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="M25" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="N25" s="3" t="inlineStr">
+        <is>
+          <t>20250724T141253.000Z</t>
         </is>
       </c>
     </row>
@@ -25387,7 +27115,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N21"/>
+  <dimension ref="A3:N29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26763,6 +28491,582 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>JACKY</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F22" s="2" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="G22" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H22" s="3" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="I22" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="J22" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="K22" s="3" t="inlineStr">
+        <is>
+          <t>FG|Sun#25</t>
+        </is>
+      </c>
+      <c r="L22" s="3" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="M22" s="3" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="N22" s="3" t="inlineStr">
+        <is>
+          <t>20250724T141231.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="inlineStr">
+        <is>
+          <t>JACKY</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F23" s="2" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="G23" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H23" s="3" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="I23" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="J23" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="K23" s="3" t="inlineStr">
+        <is>
+          <t>FG|Sun#25</t>
+        </is>
+      </c>
+      <c r="L23" s="3" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="M23" s="3" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="N23" s="3" t="inlineStr">
+        <is>
+          <t>20250724T141051.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="D24" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="F24" s="2" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="G24" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H24" s="3" t="inlineStr">
+        <is>
+          <t>Tinasha</t>
+        </is>
+      </c>
+      <c r="I24" s="3" t="inlineStr">
+        <is>
+          <t>Ratis</t>
+        </is>
+      </c>
+      <c r="J24" s="3" t="inlineStr">
+        <is>
+          <t>Clarx</t>
+        </is>
+      </c>
+      <c r="K24" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="L24" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="M24" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="N24" s="3" t="inlineStr">
+        <is>
+          <t>20250724T140448.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C25" s="1" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="D25" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="F25" s="2" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="G25" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H25" s="3" t="inlineStr">
+        <is>
+          <t>Tinasha</t>
+        </is>
+      </c>
+      <c r="I25" s="3" t="inlineStr">
+        <is>
+          <t>Ratis</t>
+        </is>
+      </c>
+      <c r="J25" s="3" t="inlineStr">
+        <is>
+          <t>Clarx</t>
+        </is>
+      </c>
+      <c r="K25" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="L25" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="M25" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="N25" s="3" t="inlineStr">
+        <is>
+          <t>20250724T140230.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B26" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C26" s="1" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="F26" s="2" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="G26" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H26" s="3" t="inlineStr">
+        <is>
+          <t>Tinasha</t>
+        </is>
+      </c>
+      <c r="I26" s="3" t="inlineStr">
+        <is>
+          <t>Ratis</t>
+        </is>
+      </c>
+      <c r="J26" s="3" t="inlineStr">
+        <is>
+          <t>Clarx</t>
+        </is>
+      </c>
+      <c r="K26" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="L26" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="M26" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="N26" s="3" t="inlineStr">
+        <is>
+          <t>20250724T140109.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="B27" s="1" t="inlineStr">
+        <is>
+          <t>JACKY</t>
+        </is>
+      </c>
+      <c r="C27" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D27" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="G27" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H27" s="3" t="inlineStr">
+        <is>
+          <t>Ratis</t>
+        </is>
+      </c>
+      <c r="I27" s="3" t="inlineStr">
+        <is>
+          <t>Clarx</t>
+        </is>
+      </c>
+      <c r="J27" s="3" t="inlineStr">
+        <is>
+          <t>Tinasha</t>
+        </is>
+      </c>
+      <c r="K27" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="L27" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="M27" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="N27" s="3" t="inlineStr">
+        <is>
+          <t>20250724T135334.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="B28" s="1" t="inlineStr">
+        <is>
+          <t>JACKY</t>
+        </is>
+      </c>
+      <c r="C28" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D28" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="F28" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="G28" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H28" s="3" t="inlineStr">
+        <is>
+          <t>Ratis</t>
+        </is>
+      </c>
+      <c r="I28" s="3" t="inlineStr">
+        <is>
+          <t>Clarx</t>
+        </is>
+      </c>
+      <c r="J28" s="3" t="inlineStr">
+        <is>
+          <t>Tinasha</t>
+        </is>
+      </c>
+      <c r="K28" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="L28" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="M28" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="N28" s="3" t="inlineStr">
+        <is>
+          <t>20250724T135058.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="B29" s="1" t="inlineStr">
+        <is>
+          <t>JACKY</t>
+        </is>
+      </c>
+      <c r="C29" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E29" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="F29" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="G29" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H29" s="3" t="inlineStr">
+        <is>
+          <t>Ratis</t>
+        </is>
+      </c>
+      <c r="I29" s="3" t="inlineStr">
+        <is>
+          <t>Clarx</t>
+        </is>
+      </c>
+      <c r="J29" s="3" t="inlineStr">
+        <is>
+          <t>Tinasha</t>
+        </is>
+      </c>
+      <c r="K29" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="L29" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="M29" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="N29" s="3" t="inlineStr">
+        <is>
+          <t>20250724T134843.000Z</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-24 17:18:10)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -10135,7 +10135,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N4"/>
+  <dimension ref="A3:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10284,6 +10284,222 @@
       <c r="N4" s="3" t="inlineStr">
         <is>
           <t>20250724T144355.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="G5" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H5" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="I5" s="3" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="J5" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="K5" s="3" t="inlineStr">
+        <is>
+          <t>FG|Sun#25</t>
+        </is>
+      </c>
+      <c r="L5" s="3" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="M5" s="3" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="N5" s="3" t="inlineStr">
+        <is>
+          <t>20250724T145451.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="G6" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H6" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="I6" s="3" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="J6" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="K6" s="3" t="inlineStr">
+        <is>
+          <t>FG|Sun#25</t>
+        </is>
+      </c>
+      <c r="L6" s="3" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="M6" s="3" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="N6" s="3" t="inlineStr">
+        <is>
+          <t>20250724T145256.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="G7" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H7" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="I7" s="3" t="inlineStr">
+        <is>
+          <t>RVL|Mameshi</t>
+        </is>
+      </c>
+      <c r="J7" s="3" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="K7" s="3" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="L7" s="3" t="inlineStr">
+        <is>
+          <t>FG|Sun#25</t>
+        </is>
+      </c>
+      <c r="M7" s="3" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="N7" s="3" t="inlineStr">
+        <is>
+          <t>20250724T144617.000Z</t>
         </is>
       </c>
     </row>
@@ -13269,7 +13485,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N40"/>
+  <dimension ref="A3:N43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16010,6 +16226,222 @@
       <c r="N40" s="3" t="inlineStr">
         <is>
           <t>20250724T131503.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>MAX</t>
+        </is>
+      </c>
+      <c r="B41" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C41" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="D41" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="E41" s="2" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="F41" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="G41" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H41" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="I41" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="J41" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="K41" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L41" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="M41" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="N41" s="3" t="inlineStr">
+        <is>
+          <t>20250724T151518.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="B42" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="C42" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D42" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="E42" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="F42" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="G42" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H42" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I42" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J42" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K42" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L42" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M42" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N42" s="3" t="inlineStr">
+        <is>
+          <t>20250724T151435.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="B43" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="C43" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D43" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="E43" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="F43" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="G43" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H43" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I43" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J43" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K43" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L43" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M43" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N43" s="3" t="inlineStr">
+        <is>
+          <t>20250724T151247.000Z</t>
         </is>
       </c>
     </row>
@@ -16024,7 +16456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N49"/>
+  <dimension ref="A3:N60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19413,6 +19845,798 @@
       <c r="N49" s="3" t="inlineStr">
         <is>
           <t>20250724T131250.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="B50" s="1" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="C50" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D50" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E50" s="2" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="F50" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G50" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H50" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="I50" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="J50" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="K50" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L50" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="M50" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N50" s="3" t="inlineStr">
+        <is>
+          <t>20250724T150737.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="B51" s="1" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="C51" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D51" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E51" s="2" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="F51" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G51" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H51" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="I51" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="J51" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="K51" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L51" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="M51" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N51" s="3" t="inlineStr">
+        <is>
+          <t>20250724T150609.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B52" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C52" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D52" s="2" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="E52" s="2" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="F52" s="2" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="G52" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H52" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="I52" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="J52" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="K52" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="L52" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="M52" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="N52" s="3" t="inlineStr">
+        <is>
+          <t>20250724T150054.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B53" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C53" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D53" s="2" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="E53" s="2" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="F53" s="2" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="G53" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H53" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="I53" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="J53" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="K53" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="L53" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="M53" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="N53" s="3" t="inlineStr">
+        <is>
+          <t>20250724T145917.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B54" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C54" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D54" s="2" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="E54" s="2" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="F54" s="2" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="G54" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H54" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="I54" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="J54" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="K54" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="L54" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="M54" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="N54" s="3" t="inlineStr">
+        <is>
+          <t>20250724T145751.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B55" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C55" s="1" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="D55" s="2" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="E55" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F55" s="2" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="G55" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H55" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I55" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J55" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K55" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L55" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M55" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N55" s="3" t="inlineStr">
+        <is>
+          <t>20250724T150552.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B56" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C56" s="1" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="D56" s="2" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="E56" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F56" s="2" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="G56" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H56" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I56" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J56" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K56" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L56" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M56" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N56" s="3" t="inlineStr">
+        <is>
+          <t>20250724T150429.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B57" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C57" s="1" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="D57" s="2" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="E57" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F57" s="2" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="G57" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H57" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I57" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J57" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K57" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L57" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M57" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N57" s="3" t="inlineStr">
+        <is>
+          <t>20250724T150235.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="B58" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="C58" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D58" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E58" s="2" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="F58" s="2" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="G58" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H58" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I58" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J58" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K58" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L58" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M58" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N58" s="3" t="inlineStr">
+        <is>
+          <t>20250724T145715.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="B59" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="C59" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D59" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E59" s="2" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="F59" s="2" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="G59" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H59" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I59" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J59" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K59" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L59" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M59" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N59" s="3" t="inlineStr">
+        <is>
+          <t>20250724T145508.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="B60" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="C60" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D60" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E60" s="2" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="F60" s="2" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="G60" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H60" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I60" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J60" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K60" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L60" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M60" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N60" s="3" t="inlineStr">
+        <is>
+          <t>20250724T145308.000Z</t>
         </is>
       </c>
     </row>
@@ -19427,7 +20651,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N50"/>
+  <dimension ref="A3:N59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22888,6 +24112,654 @@
       <c r="N50" s="3" t="inlineStr">
         <is>
           <t>20250724T144549.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="B51" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="C51" s="1" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="D51" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E51" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F51" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G51" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H51" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="I51" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="J51" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="K51" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L51" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="M51" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N51" s="3" t="inlineStr">
+        <is>
+          <t>20250724T145058.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="B52" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="C52" s="1" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="D52" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E52" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F52" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G52" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H52" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="I52" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="J52" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="K52" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L52" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="M52" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N52" s="3" t="inlineStr">
+        <is>
+          <t>20250724T144837.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="B53" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="C53" s="1" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="D53" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E53" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F53" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G53" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H53" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="I53" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="J53" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="K53" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L53" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="M53" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N53" s="3" t="inlineStr">
+        <is>
+          <t>20250724T144617.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="B54" s="1" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="C54" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D54" s="2" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="E54" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="F54" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="G54" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H54" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="I54" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="J54" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="K54" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L54" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M54" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N54" s="3" t="inlineStr">
+        <is>
+          <t>20250724T151326.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="B55" s="1" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="C55" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D55" s="2" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="E55" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="F55" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="G55" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H55" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="I55" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="J55" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="K55" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L55" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M55" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N55" s="3" t="inlineStr">
+        <is>
+          <t>20250724T151133.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="B56" s="1" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="C56" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D56" s="2" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="E56" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="F56" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="G56" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H56" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="I56" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="J56" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="K56" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L56" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M56" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N56" s="3" t="inlineStr">
+        <is>
+          <t>20250724T150913.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="B57" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="C57" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D57" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E57" s="2" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="F57" s="2" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="G57" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H57" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="I57" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="J57" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="K57" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L57" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="M57" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="N57" s="3" t="inlineStr">
+        <is>
+          <t>20250724T150136.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="B58" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="C58" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D58" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E58" s="2" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="F58" s="2" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="G58" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H58" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="I58" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="J58" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="K58" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L58" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="M58" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="N58" s="3" t="inlineStr">
+        <is>
+          <t>20250724T145916.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="B59" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="C59" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D59" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E59" s="2" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="F59" s="2" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="G59" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H59" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="I59" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="J59" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="K59" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L59" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="M59" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="N59" s="3" t="inlineStr">
+        <is>
+          <t>20250724T145703.000Z</t>
         </is>
       </c>
     </row>
@@ -22902,7 +24774,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N49"/>
+  <dimension ref="A3:N52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26291,6 +28163,222 @@
       <c r="N49" s="3" t="inlineStr">
         <is>
           <t>20250724T143703.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B50" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="C50" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="D50" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E50" s="2" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="F50" s="2" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="G50" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H50" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="I50" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="J50" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="K50" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L50" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M50" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N50" s="3" t="inlineStr">
+        <is>
+          <t>20250724T145107.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B51" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="C51" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="D51" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E51" s="2" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="F51" s="2" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="G51" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H51" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="I51" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="J51" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="K51" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L51" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M51" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N51" s="3" t="inlineStr">
+        <is>
+          <t>20250724T144834.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B52" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="C52" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="D52" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E52" s="2" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="F52" s="2" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="G52" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H52" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="I52" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="J52" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="K52" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L52" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M52" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N52" s="3" t="inlineStr">
+        <is>
+          <t>20250724T144604.000Z</t>
         </is>
       </c>
     </row>
@@ -26305,7 +28393,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N38"/>
+  <dimension ref="A3:N41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -28902,6 +30990,222 @@
       <c r="N38" s="3" t="inlineStr">
         <is>
           <t>20250724T142626.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="B39" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="C39" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D39" s="2" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="F39" s="2" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="G39" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H39" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I39" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J39" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K39" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L39" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="M39" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="N39" s="3" t="inlineStr">
+        <is>
+          <t>20250724T151321.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="B40" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="C40" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D40" s="2" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="F40" s="2" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="G40" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H40" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I40" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J40" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K40" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L40" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="M40" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="N40" s="3" t="inlineStr">
+        <is>
+          <t>20250724T151102.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="B41" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="C41" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D41" s="2" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="E41" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="F41" s="2" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="G41" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H41" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I41" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J41" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K41" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L41" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="M41" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="N41" s="3" t="inlineStr">
+        <is>
+          <t>20250724T150842.000Z</t>
         </is>
       </c>
     </row>
@@ -28916,7 +31220,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N28"/>
+  <dimension ref="A3:N39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -30793,6 +33097,798 @@
       <c r="N28" s="3" t="inlineStr">
         <is>
           <t>20250724T141524.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="B29" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="C29" s="1" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E29" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="F29" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G29" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H29" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I29" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J29" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K29" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L29" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="M29" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="N29" s="3" t="inlineStr">
+        <is>
+          <t>20250724T150208.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="B30" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="C30" s="1" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="F30" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G30" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H30" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I30" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J30" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K30" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L30" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="M30" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="N30" s="3" t="inlineStr">
+        <is>
+          <t>20250724T150033.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B31" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="C31" s="1" t="inlineStr">
+        <is>
+          <t>PENNY</t>
+        </is>
+      </c>
+      <c r="D31" s="2" t="inlineStr">
+        <is>
+          <t>POCO</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F31" s="2" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="G31" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H31" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I31" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J31" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K31" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L31" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M31" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N31" s="3" t="inlineStr">
+        <is>
+          <t>20250724T145350.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="inlineStr">
+        <is>
+          <t>PENNY</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="inlineStr">
+        <is>
+          <t>POCO</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F32" s="2" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="G32" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H32" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I32" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J32" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K32" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L32" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M32" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N32" s="3" t="inlineStr">
+        <is>
+          <t>20250724T145143.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B33" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="C33" s="1" t="inlineStr">
+        <is>
+          <t>PENNY</t>
+        </is>
+      </c>
+      <c r="D33" s="2" t="inlineStr">
+        <is>
+          <t>POCO</t>
+        </is>
+      </c>
+      <c r="E33" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F33" s="2" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="G33" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H33" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I33" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J33" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K33" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L33" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M33" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N33" s="3" t="inlineStr">
+        <is>
+          <t>20250724T144915.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B34" s="1" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="C34" s="1" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E34" s="2" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="F34" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G34" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H34" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Bogdan</t>
+        </is>
+      </c>
+      <c r="I34" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Adrii</t>
+        </is>
+      </c>
+      <c r="J34" s="3" t="inlineStr">
+        <is>
+          <t>psychok1d</t>
+        </is>
+      </c>
+      <c r="K34" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="L34" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M34" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="N34" s="3" t="inlineStr">
+        <is>
+          <t>20250724T151522.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B35" s="1" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="C35" s="1" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="D35" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E35" s="2" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="F35" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G35" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H35" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Bogdan</t>
+        </is>
+      </c>
+      <c r="I35" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Adrii</t>
+        </is>
+      </c>
+      <c r="J35" s="3" t="inlineStr">
+        <is>
+          <t>psychok1d</t>
+        </is>
+      </c>
+      <c r="K35" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="L35" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M35" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="N35" s="3" t="inlineStr">
+        <is>
+          <t>20250724T151321.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="B36" s="1" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="C36" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D36" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="F36" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="G36" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H36" s="3" t="inlineStr">
+        <is>
+          <t>psychok1d</t>
+        </is>
+      </c>
+      <c r="I36" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Adrii</t>
+        </is>
+      </c>
+      <c r="J36" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Bogdan</t>
+        </is>
+      </c>
+      <c r="K36" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L36" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M36" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N36" s="3" t="inlineStr">
+        <is>
+          <t>20250724T150800.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B37" s="1" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="C37" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D37" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="F37" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="G37" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H37" s="3" t="inlineStr">
+        <is>
+          <t>psychok1d</t>
+        </is>
+      </c>
+      <c r="I37" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Adrii</t>
+        </is>
+      </c>
+      <c r="J37" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Bogdan</t>
+        </is>
+      </c>
+      <c r="K37" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L37" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M37" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N37" s="3" t="inlineStr">
+        <is>
+          <t>20250724T150426.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B38" s="1" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="C38" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D38" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="F38" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="G38" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H38" s="3" t="inlineStr">
+        <is>
+          <t>psychok1d</t>
+        </is>
+      </c>
+      <c r="I38" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Adrii</t>
+        </is>
+      </c>
+      <c r="J38" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Bogdan</t>
+        </is>
+      </c>
+      <c r="K38" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L38" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M38" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N38" s="3" t="inlineStr">
+        <is>
+          <t>20250724T150223.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B39" s="1" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="C39" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D39" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="F39" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="G39" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H39" s="3" t="inlineStr">
+        <is>
+          <t>psychok1d</t>
+        </is>
+      </c>
+      <c r="I39" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Adrii</t>
+        </is>
+      </c>
+      <c r="J39" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Bogdan</t>
+        </is>
+      </c>
+      <c r="K39" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L39" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M39" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N39" s="3" t="inlineStr">
+        <is>
+          <t>20250724T150032.000Z</t>
         </is>
       </c>
     </row>
@@ -30807,7 +33903,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N37"/>
+  <dimension ref="A3:N40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -33335,6 +36431,222 @@
         </is>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="B38" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C38" s="1" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="D38" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="inlineStr">
+        <is>
+          <t>BIBI</t>
+        </is>
+      </c>
+      <c r="F38" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="G38" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H38" s="3" t="inlineStr">
+        <is>
+          <t>psychok1d</t>
+        </is>
+      </c>
+      <c r="I38" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Bogdan</t>
+        </is>
+      </c>
+      <c r="J38" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Adrii</t>
+        </is>
+      </c>
+      <c r="K38" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="L38" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="M38" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="N38" s="3" t="inlineStr">
+        <is>
+          <t>20250724T145308.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="B39" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C39" s="1" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="D39" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="inlineStr">
+        <is>
+          <t>BIBI</t>
+        </is>
+      </c>
+      <c r="F39" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="G39" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H39" s="3" t="inlineStr">
+        <is>
+          <t>psychok1d</t>
+        </is>
+      </c>
+      <c r="I39" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Bogdan</t>
+        </is>
+      </c>
+      <c r="J39" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Adrii</t>
+        </is>
+      </c>
+      <c r="K39" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="L39" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="M39" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="N39" s="3" t="inlineStr">
+        <is>
+          <t>20250724T145136.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="B40" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C40" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="D40" s="2" t="inlineStr">
+        <is>
+          <t>BIBI</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F40" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="G40" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H40" s="3" t="inlineStr">
+        <is>
+          <t>psychok1d</t>
+        </is>
+      </c>
+      <c r="I40" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Adrii</t>
+        </is>
+      </c>
+      <c r="J40" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Bogdan</t>
+        </is>
+      </c>
+      <c r="K40" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L40" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="M40" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="N40" s="3" t="inlineStr">
+        <is>
+          <t>20250724T144705.000Z</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-24 17:49:31)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -10514,7 +10514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N43"/>
+  <dimension ref="A3:N52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13471,6 +13471,654 @@
       <c r="N43" s="3" t="inlineStr">
         <is>
           <t>20250724T134746.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="B44" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="C44" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D44" s="2" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="E44" s="2" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="F44" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G44" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H44" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="I44" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="J44" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="K44" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L44" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="M44" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="N44" s="3" t="inlineStr">
+        <is>
+          <t>20250724T154727.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="B45" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="C45" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D45" s="2" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="E45" s="2" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="F45" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G45" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H45" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="I45" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="J45" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="K45" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L45" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="M45" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="N45" s="3" t="inlineStr">
+        <is>
+          <t>20250724T154533.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="B46" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C46" s="1" t="inlineStr">
+        <is>
+          <t>SURGE</t>
+        </is>
+      </c>
+      <c r="D46" s="2" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="E46" s="2" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="F46" s="2" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="G46" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H46" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="I46" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="J46" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="K46" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="L46" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="M46" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="N46" s="3" t="inlineStr">
+        <is>
+          <t>20250724T153845.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="B47" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C47" s="1" t="inlineStr">
+        <is>
+          <t>SURGE</t>
+        </is>
+      </c>
+      <c r="D47" s="2" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="E47" s="2" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="F47" s="2" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="G47" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H47" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="I47" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="J47" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="K47" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="L47" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="M47" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="N47" s="3" t="inlineStr">
+        <is>
+          <t>20250724T153608.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B48" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="C48" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="D48" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="E48" s="2" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="F48" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="G48" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H48" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I48" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J48" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K48" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L48" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M48" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N48" s="3" t="inlineStr">
+        <is>
+          <t>20250724T154418.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B49" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="C49" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="D49" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="E49" s="2" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="F49" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="G49" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H49" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I49" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J49" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K49" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L49" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M49" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N49" s="3" t="inlineStr">
+        <is>
+          <t>20250724T154235.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="B50" s="1" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="C50" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D50" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="E50" s="2" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="F50" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="G50" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H50" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I50" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J50" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K50" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="L50" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="M50" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="N50" s="3" t="inlineStr">
+        <is>
+          <t>20250724T153558.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B51" s="1" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="C51" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="D51" s="2" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="E51" s="2" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="F51" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G51" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H51" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I51" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J51" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K51" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L51" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M51" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N51" s="3" t="inlineStr">
+        <is>
+          <t>20250724T153336.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B52" s="1" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="C52" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="D52" s="2" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="E52" s="2" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="F52" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G52" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H52" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I52" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J52" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K52" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="L52" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="M52" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="N52" s="3" t="inlineStr">
+        <is>
+          <t>20250724T153054.000Z</t>
         </is>
       </c>
     </row>
@@ -13485,7 +14133,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N43"/>
+  <dimension ref="A3:N54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16442,6 +17090,798 @@
       <c r="N43" s="3" t="inlineStr">
         <is>
           <t>20250724T151247.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="B44" s="1" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="C44" s="1" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="D44" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E44" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F44" s="2" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="G44" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H44" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="I44" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="J44" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="K44" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L44" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="M44" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N44" s="3" t="inlineStr">
+        <is>
+          <t>20250724T152732.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="B45" s="1" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="C45" s="1" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="D45" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E45" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F45" s="2" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="G45" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H45" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="I45" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="J45" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="K45" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L45" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="M45" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N45" s="3" t="inlineStr">
+        <is>
+          <t>20250724T152609.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>MAX</t>
+        </is>
+      </c>
+      <c r="B46" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C46" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="D46" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="E46" s="2" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="F46" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="G46" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H46" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="I46" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="J46" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="K46" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L46" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="M46" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="N46" s="3" t="inlineStr">
+        <is>
+          <t>20250724T151908.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>MAX</t>
+        </is>
+      </c>
+      <c r="B47" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C47" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="D47" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="E47" s="2" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="F47" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="G47" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H47" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="I47" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="J47" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="K47" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L47" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="M47" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob</t>
+        </is>
+      </c>
+      <c r="N47" s="3" t="inlineStr">
+        <is>
+          <t>20250724T151713.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B48" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C48" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D48" s="2" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="E48" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F48" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="G48" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H48" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I48" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J48" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K48" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="L48" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="M48" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="N48" s="3" t="inlineStr">
+        <is>
+          <t>20250724T152543.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B49" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C49" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D49" s="2" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="E49" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F49" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="G49" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H49" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I49" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J49" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K49" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="L49" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="M49" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="N49" s="3" t="inlineStr">
+        <is>
+          <t>20250724T152302.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B50" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C50" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D50" s="2" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="E50" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F50" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="G50" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H50" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I50" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J50" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K50" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="L50" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="M50" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="N50" s="3" t="inlineStr">
+        <is>
+          <t>20250724T152058.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="B51" s="1" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="C51" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D51" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="E51" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="F51" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="G51" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H51" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="I51" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="J51" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="K51" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L51" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="M51" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="N51" s="3" t="inlineStr">
+        <is>
+          <t>20250724T154550.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="B52" s="1" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="C52" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="D52" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="E52" s="2" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="F52" s="2" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="G52" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H52" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="I52" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="J52" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="K52" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L52" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M52" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N52" s="3" t="inlineStr">
+        <is>
+          <t>20250724T153944.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="B53" s="1" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="C53" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="D53" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="E53" s="2" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="F53" s="2" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="G53" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H53" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="I53" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="J53" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="K53" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L53" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M53" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N53" s="3" t="inlineStr">
+        <is>
+          <t>20250724T153639.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="B54" s="1" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="C54" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D54" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="E54" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="F54" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="G54" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H54" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="I54" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="J54" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="K54" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L54" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="M54" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="N54" s="3" t="inlineStr">
+        <is>
+          <t>20250724T154814.000Z</t>
         </is>
       </c>
     </row>
@@ -16456,7 +17896,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N60"/>
+  <dimension ref="A3:N65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20637,6 +22077,366 @@
       <c r="N60" s="3" t="inlineStr">
         <is>
           <t>20250724T145308.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="B61" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="C61" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D61" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="E61" s="2" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="F61" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="G61" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H61" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="I61" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="J61" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="K61" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L61" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M61" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N61" s="3" t="inlineStr">
+        <is>
+          <t>20250724T153042.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="B62" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="C62" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D62" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="E62" s="2" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="F62" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="G62" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H62" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="I62" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="J62" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="K62" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L62" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M62" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N62" s="3" t="inlineStr">
+        <is>
+          <t>20250724T152754.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="B63" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="C63" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D63" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="E63" s="2" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="F63" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="G63" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H63" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="I63" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="J63" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="K63" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L63" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M63" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N63" s="3" t="inlineStr">
+        <is>
+          <t>20250724T152556.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="B64" s="1" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="C64" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D64" s="2" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="E64" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F64" s="2" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="G64" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H64" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="I64" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="J64" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="K64" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L64" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M64" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N64" s="3" t="inlineStr">
+        <is>
+          <t>20250724T152025.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="B65" s="1" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="C65" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D65" s="2" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="E65" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F65" s="2" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="G65" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H65" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="I65" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="J65" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="K65" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L65" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M65" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N65" s="3" t="inlineStr">
+        <is>
+          <t>20250724T151916.000Z</t>
         </is>
       </c>
     </row>
@@ -28393,7 +30193,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N41"/>
+  <dimension ref="A3:N43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -31206,6 +33006,150 @@
       <c r="N41" s="3" t="inlineStr">
         <is>
           <t>20250724T150842.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B42" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="C42" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D42" s="2" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="E42" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F42" s="2" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="G42" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H42" s="3" t="inlineStr">
+        <is>
+          <t>psychok1d</t>
+        </is>
+      </c>
+      <c r="I42" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Adrii</t>
+        </is>
+      </c>
+      <c r="J42" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Bogdan</t>
+        </is>
+      </c>
+      <c r="K42" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L42" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M42" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N42" s="3" t="inlineStr">
+        <is>
+          <t>20250724T153309.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B43" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="C43" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D43" s="2" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="E43" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F43" s="2" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="G43" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H43" s="3" t="inlineStr">
+        <is>
+          <t>psychok1d</t>
+        </is>
+      </c>
+      <c r="I43" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Adrii</t>
+        </is>
+      </c>
+      <c r="J43" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Bogdan</t>
+        </is>
+      </c>
+      <c r="K43" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L43" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M43" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N43" s="3" t="inlineStr">
+        <is>
+          <t>20250724T153102.000Z</t>
         </is>
       </c>
     </row>
@@ -31220,7 +33164,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N39"/>
+  <dimension ref="A3:N41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -33889,6 +35833,150 @@
       <c r="N39" s="3" t="inlineStr">
         <is>
           <t>20250724T150032.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B40" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="C40" s="1" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="D40" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F40" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="G40" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H40" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Adrii</t>
+        </is>
+      </c>
+      <c r="I40" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Bogdan</t>
+        </is>
+      </c>
+      <c r="J40" s="3" t="inlineStr">
+        <is>
+          <t>psychok1d</t>
+        </is>
+      </c>
+      <c r="K40" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L40" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="M40" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="N40" s="3" t="inlineStr">
+        <is>
+          <t>20250724T152337.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B41" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="C41" s="1" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="D41" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="E41" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F41" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="G41" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H41" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Adrii</t>
+        </is>
+      </c>
+      <c r="I41" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Bogdan</t>
+        </is>
+      </c>
+      <c r="J41" s="3" t="inlineStr">
+        <is>
+          <t>psychok1d</t>
+        </is>
+      </c>
+      <c r="K41" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L41" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="M41" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="N41" s="3" t="inlineStr">
+        <is>
+          <t>20250724T152112.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-24 18:20:54)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -26574,7 +26574,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N52"/>
+  <dimension ref="A3:N57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -30179,6 +30179,366 @@
       <c r="N52" s="3" t="inlineStr">
         <is>
           <t>20250724T144604.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="B53" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="C53" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D53" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="E53" s="2" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="F53" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G53" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H53" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="I53" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J53" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K53" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="L53" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="M53" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="N53" s="3" t="inlineStr">
+        <is>
+          <t>20250724T161622.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="B54" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C54" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D54" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="E54" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="F54" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G54" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H54" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="I54" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="J54" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="K54" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="L54" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="M54" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="N54" s="3" t="inlineStr">
+        <is>
+          <t>20250724T161308.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="B55" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C55" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D55" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="E55" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="F55" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G55" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H55" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="I55" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="J55" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="K55" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="L55" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="M55" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="N55" s="3" t="inlineStr">
+        <is>
+          <t>20250724T161047.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="B56" s="1" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="C56" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="D56" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E56" s="2" t="inlineStr">
+        <is>
+          <t>JESSIE</t>
+        </is>
+      </c>
+      <c r="F56" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G56" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H56" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I56" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J56" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K56" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="L56" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="M56" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="N56" s="3" t="inlineStr">
+        <is>
+          <t>20250724T161648.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="B57" s="1" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="C57" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="D57" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E57" s="2" t="inlineStr">
+        <is>
+          <t>JESSIE</t>
+        </is>
+      </c>
+      <c r="F57" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G57" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H57" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I57" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J57" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K57" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="L57" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="M57" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="N57" s="3" t="inlineStr">
+        <is>
+          <t>20250724T161427.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-24 18:52:14)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -460,7 +460,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N42"/>
+  <dimension ref="A3:N47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3345,6 +3345,366 @@
       <c r="N42" s="3" t="inlineStr">
         <is>
           <t>20250724T142316.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B43" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C43" s="1" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="D43" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="E43" s="2" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="F43" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G43" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H43" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="I43" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="J43" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="K43" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L43" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M43" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N43" s="3" t="inlineStr">
+        <is>
+          <t>20250724T165035.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B44" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C44" s="1" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="D44" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="E44" s="2" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="F44" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G44" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H44" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="I44" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="J44" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="K44" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L44" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M44" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N44" s="3" t="inlineStr">
+        <is>
+          <t>20250724T164730.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B45" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="C45" s="1" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="D45" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E45" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F45" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="G45" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H45" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I45" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J45" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K45" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L45" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M45" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N45" s="3" t="inlineStr">
+        <is>
+          <t>20250724T164056.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B46" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="C46" s="1" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="D46" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E46" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F46" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="G46" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H46" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I46" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J46" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K46" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L46" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M46" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N46" s="3" t="inlineStr">
+        <is>
+          <t>20250724T163801.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B47" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="C47" s="1" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="D47" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E47" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F47" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="G47" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H47" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I47" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J47" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K47" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L47" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M47" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N47" s="3" t="inlineStr">
+        <is>
+          <t>20250724T163442.000Z</t>
         </is>
       </c>
     </row>
@@ -22451,7 +22811,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N59"/>
+  <dimension ref="A3:N64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26560,6 +26920,366 @@
       <c r="N59" s="3" t="inlineStr">
         <is>
           <t>20250724T145703.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="B60" s="1" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="C60" s="1" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="D60" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="E60" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="F60" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="G60" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H60" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="I60" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="J60" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="K60" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="L60" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="M60" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="N60" s="3" t="inlineStr">
+        <is>
+          <t>20250724T164723.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="B61" s="1" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="C61" s="1" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="D61" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="E61" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="F61" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="G61" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H61" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="I61" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="J61" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="K61" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="L61" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="M61" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="N61" s="3" t="inlineStr">
+        <is>
+          <t>20250724T164518.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="B62" s="1" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="C62" s="1" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="D62" s="2" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="E62" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="F62" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="G62" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H62" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="I62" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="J62" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="K62" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="L62" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="M62" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="N62" s="3" t="inlineStr">
+        <is>
+          <t>20250724T163927.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="B63" s="1" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="C63" s="1" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="D63" s="2" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="E63" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="F63" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="G63" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H63" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="I63" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="J63" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="K63" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="L63" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="M63" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="N63" s="3" t="inlineStr">
+        <is>
+          <t>20250724T163707.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="B64" s="1" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="C64" s="1" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="D64" s="2" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="E64" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="F64" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="G64" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H64" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="I64" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="J64" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="K64" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="L64" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="M64" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="N64" s="3" t="inlineStr">
+        <is>
+          <t>20250724T163447.000Z</t>
         </is>
       </c>
     </row>
@@ -26574,7 +27294,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N57"/>
+  <dimension ref="A3:N63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -30539,6 +31259,438 @@
       <c r="N57" s="3" t="inlineStr">
         <is>
           <t>20250724T161427.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="B58" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C58" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="D58" s="2" t="inlineStr">
+        <is>
+          <t>SURGE</t>
+        </is>
+      </c>
+      <c r="E58" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F58" s="2" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="G58" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H58" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="I58" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="J58" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="K58" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="L58" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="M58" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="N58" s="3" t="inlineStr">
+        <is>
+          <t>20250724T162646.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="B59" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C59" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="D59" s="2" t="inlineStr">
+        <is>
+          <t>SURGE</t>
+        </is>
+      </c>
+      <c r="E59" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F59" s="2" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="G59" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H59" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="I59" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="J59" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="K59" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="L59" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="M59" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="N59" s="3" t="inlineStr">
+        <is>
+          <t>20250724T162502.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="B60" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C60" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="D60" s="2" t="inlineStr">
+        <is>
+          <t>SURGE</t>
+        </is>
+      </c>
+      <c r="E60" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F60" s="2" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="G60" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H60" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="I60" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="J60" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="K60" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="L60" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="M60" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="N60" s="3" t="inlineStr">
+        <is>
+          <t>20250724T162244.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="B61" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C61" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="D61" s="2" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="E61" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F61" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="G61" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H61" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I61" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="J61" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="K61" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L61" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M61" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N61" s="3" t="inlineStr">
+        <is>
+          <t>20250724T162726.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="B62" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C62" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="D62" s="2" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="E62" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F62" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="G62" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H62" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I62" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="J62" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="K62" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L62" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M62" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N62" s="3" t="inlineStr">
+        <is>
+          <t>20250724T162536.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="B63" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C63" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="D63" s="2" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="E63" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F63" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="G63" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H63" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I63" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="J63" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="K63" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L63" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M63" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N63" s="3" t="inlineStr">
+        <is>
+          <t>20250724T162252.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-24 19:23:34)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -14493,7 +14493,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N54"/>
+  <dimension ref="A3:N58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18242,6 +18242,294 @@
       <c r="N54" s="3" t="inlineStr">
         <is>
           <t>20250724T154814.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="B55" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="C55" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="D55" s="2" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="E55" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="F55" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G55" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H55" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="I55" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="J55" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="K55" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="L55" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="M55" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="N55" s="3" t="inlineStr">
+        <is>
+          <t>20250724T171923.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="B56" s="1" t="inlineStr">
+        <is>
+          <t>PIPER</t>
+        </is>
+      </c>
+      <c r="C56" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="D56" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="E56" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="F56" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G56" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H56" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="I56" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="J56" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="K56" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="L56" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="M56" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="N56" s="3" t="inlineStr">
+        <is>
+          <t>20250724T171418.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="B57" s="1" t="inlineStr">
+        <is>
+          <t>PIPER</t>
+        </is>
+      </c>
+      <c r="C57" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="D57" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="E57" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="F57" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G57" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H57" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="I57" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="J57" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="K57" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="L57" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="M57" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="N57" s="3" t="inlineStr">
+        <is>
+          <t>20250724T171203.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="B58" s="1" t="inlineStr">
+        <is>
+          <t>PIPER</t>
+        </is>
+      </c>
+      <c r="C58" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="D58" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="E58" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="F58" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G58" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H58" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="I58" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="J58" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="K58" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="L58" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="M58" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="N58" s="3" t="inlineStr">
+        <is>
+          <t>20250724T171023.000Z</t>
         </is>
       </c>
     </row>
@@ -18256,7 +18544,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N65"/>
+  <dimension ref="A3:N72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22797,6 +23085,510 @@
       <c r="N65" s="3" t="inlineStr">
         <is>
           <t>20250724T151916.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="B66" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C66" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D66" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E66" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="F66" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="G66" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H66" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="I66" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="J66" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="K66" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="L66" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="M66" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="N66" s="3" t="inlineStr">
+        <is>
+          <t>20250724T170441.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="B67" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C67" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D67" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E67" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="F67" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="G67" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H67" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="I67" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="J67" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="K67" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="L67" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="M67" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="N67" s="3" t="inlineStr">
+        <is>
+          <t>20250724T170217.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="B68" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C68" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D68" s="2" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="E68" s="2" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="F68" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G68" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H68" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="I68" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="J68" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="K68" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="L68" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="M68" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="N68" s="3" t="inlineStr">
+        <is>
+          <t>20250724T165610.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="B69" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C69" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D69" s="2" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="E69" s="2" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="F69" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G69" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H69" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="I69" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="J69" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="K69" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="L69" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="M69" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="N69" s="3" t="inlineStr">
+        <is>
+          <t>20250724T165350.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="B70" s="1" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="C70" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="D70" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="E70" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F70" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G70" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H70" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I70" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J70" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K70" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L70" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M70" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N70" s="3" t="inlineStr">
+        <is>
+          <t>20250724T171633.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="B71" s="1" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="C71" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="D71" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="E71" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F71" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G71" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H71" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I71" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J71" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K71" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L71" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M71" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N71" s="3" t="inlineStr">
+        <is>
+          <t>20250724T171435.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B72" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="C72" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="D72" s="2" t="inlineStr">
+        <is>
+          <t>JESSIE</t>
+        </is>
+      </c>
+      <c r="E72" s="2" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="F72" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G72" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H72" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I72" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J72" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K72" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="L72" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="M72" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N72" s="3" t="inlineStr">
+        <is>
+          <t>20250724T172202.000Z</t>
         </is>
       </c>
     </row>
@@ -22811,7 +23603,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N64"/>
+  <dimension ref="A3:N69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -27280,6 +28072,366 @@
       <c r="N64" s="3" t="inlineStr">
         <is>
           <t>20250724T163447.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="B65" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="C65" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D65" s="2" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="E65" s="2" t="inlineStr">
+        <is>
+          <t>POCO</t>
+        </is>
+      </c>
+      <c r="F65" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="G65" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H65" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I65" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="J65" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="K65" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L65" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M65" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N65" s="3" t="inlineStr">
+        <is>
+          <t>20250724T170831.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="B66" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="C66" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D66" s="2" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="E66" s="2" t="inlineStr">
+        <is>
+          <t>POCO</t>
+        </is>
+      </c>
+      <c r="F66" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="G66" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H66" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I66" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="J66" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="K66" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L66" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M66" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N66" s="3" t="inlineStr">
+        <is>
+          <t>20250724T170617.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="B67" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="C67" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D67" s="2" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="E67" s="2" t="inlineStr">
+        <is>
+          <t>POCO</t>
+        </is>
+      </c>
+      <c r="F67" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="G67" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H67" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I67" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="J67" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="K67" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L67" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M67" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N67" s="3" t="inlineStr">
+        <is>
+          <t>20250724T170356.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B68" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C68" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="D68" s="2" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="E68" s="2" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="F68" s="2" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="G68" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H68" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="I68" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="J68" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="K68" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L68" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M68" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N68" s="3" t="inlineStr">
+        <is>
+          <t>20250724T165826.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B69" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C69" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="D69" s="2" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="E69" s="2" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="F69" s="2" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="G69" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H69" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="I69" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="J69" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="K69" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L69" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M69" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N69" s="3" t="inlineStr">
+        <is>
+          <t>20250724T165702.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-24 19:54:55)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -14493,7 +14493,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N58"/>
+  <dimension ref="A3:N64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18530,6 +18530,438 @@
       <c r="N58" s="3" t="inlineStr">
         <is>
           <t>20250724T171023.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="B59" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="C59" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="D59" s="2" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="E59" s="2" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="F59" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G59" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H59" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="I59" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="J59" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="K59" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="L59" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="M59" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="N59" s="3" t="inlineStr">
+        <is>
+          <t>20250724T172257.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="B60" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C60" s="1" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="D60" s="2" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="E60" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="F60" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G60" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H60" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="I60" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="J60" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="K60" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="L60" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="M60" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="N60" s="3" t="inlineStr">
+        <is>
+          <t>20250724T174707.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="B61" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C61" s="1" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="D61" s="2" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="E61" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="F61" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G61" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H61" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="I61" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="J61" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="K61" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="L61" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="M61" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="N61" s="3" t="inlineStr">
+        <is>
+          <t>20250724T174359.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="B62" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C62" s="1" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="D62" s="2" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="E62" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="F62" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G62" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H62" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="I62" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="J62" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="K62" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="L62" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="M62" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="N62" s="3" t="inlineStr">
+        <is>
+          <t>20250724T174137.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="B63" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="C63" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D63" s="2" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="E63" s="2" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="F63" s="2" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="G63" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H63" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I63" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J63" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K63" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="L63" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M63" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="N63" s="3" t="inlineStr">
+        <is>
+          <t>20250724T173429.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="B64" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="C64" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D64" s="2" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="E64" s="2" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="F64" s="2" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="G64" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H64" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I64" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J64" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K64" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="L64" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M64" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="N64" s="3" t="inlineStr">
+        <is>
+          <t>20250724T173209.000Z</t>
         </is>
       </c>
     </row>
@@ -18544,7 +18976,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N72"/>
+  <dimension ref="A3:N73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23589,6 +24021,78 @@
       <c r="N72" s="3" t="inlineStr">
         <is>
           <t>20250724T172202.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B73" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="C73" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="D73" s="2" t="inlineStr">
+        <is>
+          <t>JESSIE</t>
+        </is>
+      </c>
+      <c r="E73" s="2" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="F73" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G73" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H73" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I73" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J73" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K73" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="L73" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="M73" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N73" s="3" t="inlineStr">
+        <is>
+          <t>20250724T172343.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-24 20:26:16)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -5053,7 +5053,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N15"/>
+  <dimension ref="A3:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5994,6 +5994,150 @@
       <c r="N15" s="3" t="inlineStr">
         <is>
           <t>20250724T124909.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G16" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H16" s="3" t="inlineStr">
+        <is>
+          <t>Buzko</t>
+        </is>
+      </c>
+      <c r="I16" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="J16" s="3" t="inlineStr">
+        <is>
+          <t>psychok1d</t>
+        </is>
+      </c>
+      <c r="K16" s="3" t="inlineStr">
+        <is>
+          <t>LLC|kellow</t>
+        </is>
+      </c>
+      <c r="L16" s="3" t="inlineStr">
+        <is>
+          <t>KDS|Remica</t>
+        </is>
+      </c>
+      <c r="M16" s="3" t="inlineStr">
+        <is>
+          <t>KDS|치로🩵</t>
+        </is>
+      </c>
+      <c r="N16" s="3" t="inlineStr">
+        <is>
+          <t>20250724T181051.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G17" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H17" s="3" t="inlineStr">
+        <is>
+          <t>Buzko</t>
+        </is>
+      </c>
+      <c r="I17" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="J17" s="3" t="inlineStr">
+        <is>
+          <t>psychok1d</t>
+        </is>
+      </c>
+      <c r="K17" s="3" t="inlineStr">
+        <is>
+          <t>LLC|kellow</t>
+        </is>
+      </c>
+      <c r="L17" s="3" t="inlineStr">
+        <is>
+          <t>KDS|Remica</t>
+        </is>
+      </c>
+      <c r="M17" s="3" t="inlineStr">
+        <is>
+          <t>KDS|치로🩵</t>
+        </is>
+      </c>
+      <c r="N17" s="3" t="inlineStr">
+        <is>
+          <t>20250724T180804.000Z</t>
         </is>
       </c>
     </row>
@@ -7179,7 +7323,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N9"/>
+  <dimension ref="A3:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7688,6 +7832,222 @@
       <c r="N9" s="3" t="inlineStr">
         <is>
           <t>20250724T001957.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H10" s="3" t="inlineStr">
+        <is>
+          <t>Buzko</t>
+        </is>
+      </c>
+      <c r="I10" s="3" t="inlineStr">
+        <is>
+          <t>psychok1d</t>
+        </is>
+      </c>
+      <c r="J10" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="K10" s="3" t="inlineStr">
+        <is>
+          <t>LLC|kellow</t>
+        </is>
+      </c>
+      <c r="L10" s="3" t="inlineStr">
+        <is>
+          <t>KDS|치로🩵</t>
+        </is>
+      </c>
+      <c r="M10" s="3" t="inlineStr">
+        <is>
+          <t>KDS|Remica</t>
+        </is>
+      </c>
+      <c r="N10" s="3" t="inlineStr">
+        <is>
+          <t>20250724T182129.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G11" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H11" s="3" t="inlineStr">
+        <is>
+          <t>Buzko</t>
+        </is>
+      </c>
+      <c r="I11" s="3" t="inlineStr">
+        <is>
+          <t>psychok1d</t>
+        </is>
+      </c>
+      <c r="J11" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="K11" s="3" t="inlineStr">
+        <is>
+          <t>LLC|kellow</t>
+        </is>
+      </c>
+      <c r="L11" s="3" t="inlineStr">
+        <is>
+          <t>KDS|치로🩵</t>
+        </is>
+      </c>
+      <c r="M11" s="3" t="inlineStr">
+        <is>
+          <t>KDS|Remica</t>
+        </is>
+      </c>
+      <c r="N11" s="3" t="inlineStr">
+        <is>
+          <t>20250724T181822.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G12" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H12" s="3" t="inlineStr">
+        <is>
+          <t>Buzko</t>
+        </is>
+      </c>
+      <c r="I12" s="3" t="inlineStr">
+        <is>
+          <t>psychok1d</t>
+        </is>
+      </c>
+      <c r="J12" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="K12" s="3" t="inlineStr">
+        <is>
+          <t>LLC|kellow</t>
+        </is>
+      </c>
+      <c r="L12" s="3" t="inlineStr">
+        <is>
+          <t>KDS|치로🩵</t>
+        </is>
+      </c>
+      <c r="M12" s="3" t="inlineStr">
+        <is>
+          <t>KDS|Remica</t>
+        </is>
+      </c>
+      <c r="N12" s="3" t="inlineStr">
+        <is>
+          <t>20250724T181709.000Z</t>
         </is>
       </c>
     </row>
@@ -10874,7 +11234,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N52"/>
+  <dimension ref="A3:N55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14479,6 +14839,222 @@
       <c r="N52" s="3" t="inlineStr">
         <is>
           <t>20250724T153054.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="B53" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C53" s="1" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="D53" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E53" s="2" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="F53" s="2" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="G53" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H53" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I53" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J53" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K53" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L53" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M53" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N53" s="3" t="inlineStr">
+        <is>
+          <t>20250724T182158.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="B54" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C54" s="1" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="D54" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E54" s="2" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="F54" s="2" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="G54" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H54" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I54" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J54" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K54" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L54" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M54" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N54" s="3" t="inlineStr">
+        <is>
+          <t>20250724T181843.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="B55" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C55" s="1" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="D55" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E55" s="2" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="F55" s="2" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="G55" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H55" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I55" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J55" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K55" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L55" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M55" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N55" s="3" t="inlineStr">
+        <is>
+          <t>20250724T181621.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-24 20:57:36)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -4098,7 +4098,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N15"/>
+  <dimension ref="A3:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5039,6 +5039,150 @@
       <c r="N15" s="3" t="inlineStr">
         <is>
           <t>20250724T132544.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="G16" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H16" s="3" t="inlineStr">
+        <is>
+          <t>Buzko</t>
+        </is>
+      </c>
+      <c r="I16" s="3" t="inlineStr">
+        <is>
+          <t>psychok1d</t>
+        </is>
+      </c>
+      <c r="J16" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="K16" s="3" t="inlineStr">
+        <is>
+          <t>CNE|ReMa🦊</t>
+        </is>
+      </c>
+      <c r="L16" s="3" t="inlineStr">
+        <is>
+          <t>KDS|치로🩵</t>
+        </is>
+      </c>
+      <c r="M16" s="3" t="inlineStr">
+        <is>
+          <t>KDS|Remica</t>
+        </is>
+      </c>
+      <c r="N16" s="3" t="inlineStr">
+        <is>
+          <t>20250724T184221.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="G17" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H17" s="3" t="inlineStr">
+        <is>
+          <t>Buzko</t>
+        </is>
+      </c>
+      <c r="I17" s="3" t="inlineStr">
+        <is>
+          <t>psychok1d</t>
+        </is>
+      </c>
+      <c r="J17" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="K17" s="3" t="inlineStr">
+        <is>
+          <t>CNE|ReMa🦊</t>
+        </is>
+      </c>
+      <c r="L17" s="3" t="inlineStr">
+        <is>
+          <t>KDS|치로🩵</t>
+        </is>
+      </c>
+      <c r="M17" s="3" t="inlineStr">
+        <is>
+          <t>KDS|Remica</t>
+        </is>
+      </c>
+      <c r="N17" s="3" t="inlineStr">
+        <is>
+          <t>20250724T183822.000Z</t>
         </is>
       </c>
     </row>
@@ -8062,7 +8206,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N9"/>
+  <dimension ref="A3:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8571,6 +8715,150 @@
       <c r="N9" s="3" t="inlineStr">
         <is>
           <t>20250718T234259.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>PEARL</t>
+        </is>
+      </c>
+      <c r="G10" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H10" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="I10" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="J10" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K10" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L10" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M10" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N10" s="3" t="inlineStr">
+        <is>
+          <t>20250724T185402.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>PEARL</t>
+        </is>
+      </c>
+      <c r="G11" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H11" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="I11" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="J11" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K11" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L11" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M11" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N11" s="3" t="inlineStr">
+        <is>
+          <t>20250724T185236.000Z</t>
         </is>
       </c>
     </row>
@@ -11234,7 +11522,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N55"/>
+  <dimension ref="A3:N57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15055,6 +15343,150 @@
       <c r="N55" s="3" t="inlineStr">
         <is>
           <t>20250724T181621.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="B56" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="C56" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="D56" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E56" s="2" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="F56" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G56" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H56" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I56" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J56" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K56" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L56" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="M56" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="N56" s="3" t="inlineStr">
+        <is>
+          <t>20250724T182918.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="B57" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="C57" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="D57" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E57" s="2" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="F57" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G57" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H57" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I57" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J57" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K57" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L57" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="M57" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="N57" s="3" t="inlineStr">
+        <is>
+          <t>20250724T182657.000Z</t>
         </is>
       </c>
     </row>
@@ -33937,7 +34369,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N43"/>
+  <dimension ref="A3:N46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -36894,6 +37326,222 @@
       <c r="N43" s="3" t="inlineStr">
         <is>
           <t>20250724T153102.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="B44" s="1" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="C44" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D44" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E44" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F44" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="G44" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H44" s="3" t="inlineStr">
+        <is>
+          <t>Buzko</t>
+        </is>
+      </c>
+      <c r="I44" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="J44" s="3" t="inlineStr">
+        <is>
+          <t>psychok1d</t>
+        </is>
+      </c>
+      <c r="K44" s="3" t="inlineStr">
+        <is>
+          <t>CNE|ReMa🦊</t>
+        </is>
+      </c>
+      <c r="L44" s="3" t="inlineStr">
+        <is>
+          <t>KDS|Remica</t>
+        </is>
+      </c>
+      <c r="M44" s="3" t="inlineStr">
+        <is>
+          <t>KDS|치로🩵</t>
+        </is>
+      </c>
+      <c r="N44" s="3" t="inlineStr">
+        <is>
+          <t>20250724T183034.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="B45" s="1" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="C45" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D45" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E45" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F45" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="G45" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H45" s="3" t="inlineStr">
+        <is>
+          <t>Buzko</t>
+        </is>
+      </c>
+      <c r="I45" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="J45" s="3" t="inlineStr">
+        <is>
+          <t>psychok1d</t>
+        </is>
+      </c>
+      <c r="K45" s="3" t="inlineStr">
+        <is>
+          <t>CNE|ReMa🦊</t>
+        </is>
+      </c>
+      <c r="L45" s="3" t="inlineStr">
+        <is>
+          <t>KDS|Remica</t>
+        </is>
+      </c>
+      <c r="M45" s="3" t="inlineStr">
+        <is>
+          <t>KDS|치로🩵</t>
+        </is>
+      </c>
+      <c r="N45" s="3" t="inlineStr">
+        <is>
+          <t>20250724T182814.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="B46" s="1" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="C46" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D46" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E46" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F46" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="G46" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H46" s="3" t="inlineStr">
+        <is>
+          <t>Buzko</t>
+        </is>
+      </c>
+      <c r="I46" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="J46" s="3" t="inlineStr">
+        <is>
+          <t>psychok1d</t>
+        </is>
+      </c>
+      <c r="K46" s="3" t="inlineStr">
+        <is>
+          <t>CNE|ReMa🦊</t>
+        </is>
+      </c>
+      <c r="L46" s="3" t="inlineStr">
+        <is>
+          <t>KDS|Remica</t>
+        </is>
+      </c>
+      <c r="M46" s="3" t="inlineStr">
+        <is>
+          <t>KDS|치로🩵</t>
+        </is>
+      </c>
+      <c r="N46" s="3" t="inlineStr">
+        <is>
+          <t>20250724T182608.000Z</t>
         </is>
       </c>
     </row>
@@ -36908,7 +37556,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N41"/>
+  <dimension ref="A3:N44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -39721,6 +40369,222 @@
       <c r="N41" s="3" t="inlineStr">
         <is>
           <t>20250724T152112.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B42" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="C42" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D42" s="2" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="E42" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F42" s="2" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="G42" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H42" s="3" t="inlineStr">
+        <is>
+          <t>Buzko</t>
+        </is>
+      </c>
+      <c r="I42" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="J42" s="3" t="inlineStr">
+        <is>
+          <t>psychok1d</t>
+        </is>
+      </c>
+      <c r="K42" s="3" t="inlineStr">
+        <is>
+          <t>LLC|kellow</t>
+        </is>
+      </c>
+      <c r="L42" s="3" t="inlineStr">
+        <is>
+          <t>KDS|Remica</t>
+        </is>
+      </c>
+      <c r="M42" s="3" t="inlineStr">
+        <is>
+          <t>KDS|치로🩵</t>
+        </is>
+      </c>
+      <c r="N42" s="3" t="inlineStr">
+        <is>
+          <t>20250724T185413.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B43" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="C43" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D43" s="2" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="E43" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F43" s="2" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="G43" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H43" s="3" t="inlineStr">
+        <is>
+          <t>Buzko</t>
+        </is>
+      </c>
+      <c r="I43" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="J43" s="3" t="inlineStr">
+        <is>
+          <t>psychok1d</t>
+        </is>
+      </c>
+      <c r="K43" s="3" t="inlineStr">
+        <is>
+          <t>LLC|kellow</t>
+        </is>
+      </c>
+      <c r="L43" s="3" t="inlineStr">
+        <is>
+          <t>KDS|Remica</t>
+        </is>
+      </c>
+      <c r="M43" s="3" t="inlineStr">
+        <is>
+          <t>KDS|치로🩵</t>
+        </is>
+      </c>
+      <c r="N43" s="3" t="inlineStr">
+        <is>
+          <t>20250724T185207.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B44" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="C44" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D44" s="2" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="E44" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F44" s="2" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="G44" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H44" s="3" t="inlineStr">
+        <is>
+          <t>Buzko</t>
+        </is>
+      </c>
+      <c r="I44" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="J44" s="3" t="inlineStr">
+        <is>
+          <t>psychok1d</t>
+        </is>
+      </c>
+      <c r="K44" s="3" t="inlineStr">
+        <is>
+          <t>LLC|kellow</t>
+        </is>
+      </c>
+      <c r="L44" s="3" t="inlineStr">
+        <is>
+          <t>KDS|Remica</t>
+        </is>
+      </c>
+      <c r="M44" s="3" t="inlineStr">
+        <is>
+          <t>KDS|치로🩵</t>
+        </is>
+      </c>
+      <c r="N44" s="3" t="inlineStr">
+        <is>
+          <t>20250724T184938.000Z</t>
         </is>
       </c>
     </row>
@@ -39735,7 +40599,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N40"/>
+  <dimension ref="A3:N45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -42479,6 +43343,366 @@
         </is>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B41" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="C41" s="1" t="inlineStr">
+        <is>
+          <t>SHELLY</t>
+        </is>
+      </c>
+      <c r="D41" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="E41" s="2" t="inlineStr">
+        <is>
+          <t>EDGAR</t>
+        </is>
+      </c>
+      <c r="F41" s="2" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="G41" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H41" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I41" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J41" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K41" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="L41" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="M41" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="N41" s="3" t="inlineStr">
+        <is>
+          <t>20250724T184642.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B42" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="C42" s="1" t="inlineStr">
+        <is>
+          <t>SHELLY</t>
+        </is>
+      </c>
+      <c r="D42" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="E42" s="2" t="inlineStr">
+        <is>
+          <t>EDGAR</t>
+        </is>
+      </c>
+      <c r="F42" s="2" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="G42" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H42" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I42" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J42" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K42" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="L42" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="M42" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="N42" s="3" t="inlineStr">
+        <is>
+          <t>20250724T184500.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B43" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="C43" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="D43" s="2" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="E43" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F43" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="G43" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H43" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="I43" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="J43" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="K43" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L43" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M43" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N43" s="3" t="inlineStr">
+        <is>
+          <t>20250724T184014.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B44" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="C44" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="D44" s="2" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="E44" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F44" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="G44" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H44" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="I44" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="J44" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="K44" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L44" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M44" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N44" s="3" t="inlineStr">
+        <is>
+          <t>20250724T183751.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B45" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="C45" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="D45" s="2" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="E45" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F45" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="G45" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H45" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="I45" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="J45" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="K45" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L45" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M45" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N45" s="3" t="inlineStr">
+        <is>
+          <t>20250724T183607.000Z</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-24 21:28:59)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -460,7 +460,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N47"/>
+  <dimension ref="A3:N49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3705,6 +3705,150 @@
       <c r="N47" s="3" t="inlineStr">
         <is>
           <t>20250724T163442.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="B48" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="C48" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D48" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="E48" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="F48" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="G48" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H48" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="I48" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="J48" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="K48" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Ferissa</t>
+        </is>
+      </c>
+      <c r="L48" s="3" t="inlineStr">
+        <is>
+          <t>FUT|DeMaster</t>
+        </is>
+      </c>
+      <c r="M48" s="3" t="inlineStr">
+        <is>
+          <t>FUT|ZеyroX🕊️</t>
+        </is>
+      </c>
+      <c r="N48" s="3" t="inlineStr">
+        <is>
+          <t>20250724T192428.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="B49" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="C49" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D49" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="E49" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="F49" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="G49" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H49" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="I49" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="J49" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="K49" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Ferissa</t>
+        </is>
+      </c>
+      <c r="L49" s="3" t="inlineStr">
+        <is>
+          <t>FUT|DeMaster</t>
+        </is>
+      </c>
+      <c r="M49" s="3" t="inlineStr">
+        <is>
+          <t>FUT|ZеyroX🕊️</t>
+        </is>
+      </c>
+      <c r="N49" s="3" t="inlineStr">
+        <is>
+          <t>20250724T192118.000Z</t>
         </is>
       </c>
     </row>
@@ -3719,7 +3863,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N7"/>
+  <dimension ref="A3:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4084,6 +4228,222 @@
       <c r="N7" s="3" t="inlineStr">
         <is>
           <t>20250723T174615.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="G8" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H8" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I8" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J8" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K8" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L8" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M8" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N8" s="3" t="inlineStr">
+        <is>
+          <t>20250724T191738.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="G9" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H9" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I9" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J9" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K9" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L9" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M9" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N9" s="3" t="inlineStr">
+        <is>
+          <t>20250724T191448.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H10" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I10" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J10" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K10" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L10" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M10" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N10" s="3" t="inlineStr">
+        <is>
+          <t>20250724T191208.000Z</t>
         </is>
       </c>
     </row>
@@ -6296,7 +6656,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N18"/>
+  <dimension ref="A3:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7453,6 +7813,222 @@
       <c r="N18" s="3" t="inlineStr">
         <is>
           <t>20250724T124044.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F19" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G19" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H19" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="I19" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="J19" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="K19" s="3" t="inlineStr">
+        <is>
+          <t>FUT|ZеyroX🕊️</t>
+        </is>
+      </c>
+      <c r="L19" s="3" t="inlineStr">
+        <is>
+          <t>FUT|DeMaster</t>
+        </is>
+      </c>
+      <c r="M19" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Ferissa</t>
+        </is>
+      </c>
+      <c r="N19" s="3" t="inlineStr">
+        <is>
+          <t>20250724T191615.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F20" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G20" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H20" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="I20" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="J20" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="K20" s="3" t="inlineStr">
+        <is>
+          <t>FUT|ZеyroX🕊️</t>
+        </is>
+      </c>
+      <c r="L20" s="3" t="inlineStr">
+        <is>
+          <t>FUT|DeMaster</t>
+        </is>
+      </c>
+      <c r="M20" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Ferissa</t>
+        </is>
+      </c>
+      <c r="N20" s="3" t="inlineStr">
+        <is>
+          <t>20250724T191426.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="C21" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F21" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G21" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H21" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="I21" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="J21" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="K21" s="3" t="inlineStr">
+        <is>
+          <t>FUT|ZеyroX🕊️</t>
+        </is>
+      </c>
+      <c r="L21" s="3" t="inlineStr">
+        <is>
+          <t>FUT|DeMaster</t>
+        </is>
+      </c>
+      <c r="M21" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Ferissa</t>
+        </is>
+      </c>
+      <c r="N21" s="3" t="inlineStr">
+        <is>
+          <t>20250724T191247.000Z</t>
         </is>
       </c>
     </row>
@@ -8206,7 +8782,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N11"/>
+  <dimension ref="A3:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8859,6 +9435,222 @@
       <c r="N11" s="3" t="inlineStr">
         <is>
           <t>20250724T185236.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="G12" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H12" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I12" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J12" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K12" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L12" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M12" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N12" s="3" t="inlineStr">
+        <is>
+          <t>20250724T190533.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="G13" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H13" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I13" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J13" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K13" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L13" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M13" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N13" s="3" t="inlineStr">
+        <is>
+          <t>20250724T190331.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="G14" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H14" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J14" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K14" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L14" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M14" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N14" s="3" t="inlineStr">
+        <is>
+          <t>20250724T190100.000Z</t>
         </is>
       </c>
     </row>
@@ -11143,7 +11935,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N7"/>
+  <dimension ref="A3:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11508,6 +12300,150 @@
       <c r="N7" s="3" t="inlineStr">
         <is>
           <t>20250724T144617.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="G8" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H8" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="I8" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J8" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K8" s="3" t="inlineStr">
+        <is>
+          <t>FUT|ZеyroX🕊️</t>
+        </is>
+      </c>
+      <c r="L8" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Ferissa</t>
+        </is>
+      </c>
+      <c r="M8" s="3" t="inlineStr">
+        <is>
+          <t>FUT|DeMaster</t>
+        </is>
+      </c>
+      <c r="N8" s="3" t="inlineStr">
+        <is>
+          <t>20250724T190618.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="G9" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H9" s="3" t="inlineStr">
+        <is>
+          <t>SK|Joker</t>
+        </is>
+      </c>
+      <c r="I9" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Lukii</t>
+        </is>
+      </c>
+      <c r="J9" s="3" t="inlineStr">
+        <is>
+          <t>HMB|Symantec</t>
+        </is>
+      </c>
+      <c r="K9" s="3" t="inlineStr">
+        <is>
+          <t>FUT|ZеyroX🕊️</t>
+        </is>
+      </c>
+      <c r="L9" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Ferissa</t>
+        </is>
+      </c>
+      <c r="M9" s="3" t="inlineStr">
+        <is>
+          <t>FUT|DeMaster</t>
+        </is>
+      </c>
+      <c r="N9" s="3" t="inlineStr">
+        <is>
+          <t>20250724T190323.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-24 22:00:19)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -12458,7 +12458,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N57"/>
+  <dimension ref="A3:N59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16423,6 +16423,150 @@
       <c r="N57" s="3" t="inlineStr">
         <is>
           <t>20250724T182657.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="B58" s="1" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="C58" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D58" s="2" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="E58" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="F58" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G58" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H58" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="I58" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="J58" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="K58" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L58" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="M58" s="3" t="inlineStr">
+        <is>
+          <t>Drage🍥</t>
+        </is>
+      </c>
+      <c r="N58" s="3" t="inlineStr">
+        <is>
+          <t>20250724T195446.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="B59" s="1" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="C59" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D59" s="2" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="E59" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="F59" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G59" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H59" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="I59" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="J59" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="K59" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L59" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="M59" s="3" t="inlineStr">
+        <is>
+          <t>Drage🍥</t>
+        </is>
+      </c>
+      <c r="N59" s="3" t="inlineStr">
+        <is>
+          <t>20250724T195203.000Z</t>
         </is>
       </c>
     </row>
@@ -26051,7 +26195,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N69"/>
+  <dimension ref="A3:N71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -30880,6 +31024,150 @@
       <c r="N69" s="3" t="inlineStr">
         <is>
           <t>20250724T165702.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B70" s="1" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="C70" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D70" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E70" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="F70" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="G70" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H70" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="I70" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="J70" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="K70" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L70" s="3" t="inlineStr">
+        <is>
+          <t>Drage🍥</t>
+        </is>
+      </c>
+      <c r="M70" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N70" s="3" t="inlineStr">
+        <is>
+          <t>20250724T194507.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B71" s="1" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="C71" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D71" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E71" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="F71" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="G71" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H71" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="I71" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="J71" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="K71" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L71" s="3" t="inlineStr">
+        <is>
+          <t>Drage🍥</t>
+        </is>
+      </c>
+      <c r="M71" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N71" s="3" t="inlineStr">
+        <is>
+          <t>20250724T194246.000Z</t>
         </is>
       </c>
     </row>
@@ -41535,7 +41823,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N45"/>
+  <dimension ref="A3:N47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -44639,6 +44927,150 @@
         </is>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>EDGAR</t>
+        </is>
+      </c>
+      <c r="B46" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C46" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="D46" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E46" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F46" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="G46" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H46" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="I46" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="J46" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K46" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L46" s="3" t="inlineStr">
+        <is>
+          <t>Drage🍥</t>
+        </is>
+      </c>
+      <c r="M46" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N46" s="3" t="inlineStr">
+        <is>
+          <t>20250724T193517.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>EDGAR</t>
+        </is>
+      </c>
+      <c r="B47" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C47" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="D47" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E47" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F47" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="G47" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H47" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="I47" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="J47" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K47" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L47" s="3" t="inlineStr">
+        <is>
+          <t>Drage🍥</t>
+        </is>
+      </c>
+      <c r="M47" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N47" s="3" t="inlineStr">
+        <is>
+          <t>20250724T193312.000Z</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-24 22:31:38)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -460,7 +460,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N49"/>
+  <dimension ref="A3:N52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3849,6 +3849,222 @@
       <c r="N49" s="3" t="inlineStr">
         <is>
           <t>20250724T192118.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B50" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="C50" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D50" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E50" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="F50" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G50" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H50" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="I50" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="J50" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="K50" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L50" s="3" t="inlineStr">
+        <is>
+          <t>Drage🍥</t>
+        </is>
+      </c>
+      <c r="M50" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N50" s="3" t="inlineStr">
+        <is>
+          <t>20250724T201248.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B51" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="C51" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D51" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E51" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="F51" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G51" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H51" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="I51" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="J51" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="K51" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L51" s="3" t="inlineStr">
+        <is>
+          <t>Drage🍥</t>
+        </is>
+      </c>
+      <c r="M51" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N51" s="3" t="inlineStr">
+        <is>
+          <t>20250724T201056.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B52" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="C52" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D52" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E52" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="F52" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G52" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H52" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="I52" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="J52" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="K52" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L52" s="3" t="inlineStr">
+        <is>
+          <t>Drage🍥</t>
+        </is>
+      </c>
+      <c r="M52" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N52" s="3" t="inlineStr">
+        <is>
+          <t>20250724T200846.000Z</t>
         </is>
       </c>
     </row>
@@ -6656,7 +6872,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N21"/>
+  <dimension ref="A3:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8029,6 +8245,222 @@
       <c r="N21" s="3" t="inlineStr">
         <is>
           <t>20250724T191247.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="F22" s="2" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="G22" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H22" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="I22" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="J22" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="K22" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L22" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="M22" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="N22" s="3" t="inlineStr">
+        <is>
+          <t>20250724T201924.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="F23" s="2" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="G23" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H23" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="I23" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="J23" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="K23" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L23" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="M23" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="N23" s="3" t="inlineStr">
+        <is>
+          <t>20250724T201650.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="D24" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="F24" s="2" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="G24" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H24" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="I24" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="J24" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="K24" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L24" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="M24" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="N24" s="3" t="inlineStr">
+        <is>
+          <t>20250724T201500.000Z</t>
         </is>
       </c>
     </row>
@@ -9665,7 +10097,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N24"/>
+  <dimension ref="A3:N27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11254,6 +11686,222 @@
       <c r="N24" s="3" t="inlineStr">
         <is>
           <t>20250724T141643.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="C25" s="1" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="D25" s="2" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="F25" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G25" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H25" s="3" t="inlineStr">
+        <is>
+          <t>KRO|Nanoxx</t>
+        </is>
+      </c>
+      <c r="I25" s="3" t="inlineStr">
+        <is>
+          <t>YT : GuGu</t>
+        </is>
+      </c>
+      <c r="J25" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="K25" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L25" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="M25" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="N25" s="3" t="inlineStr">
+        <is>
+          <t>20250724T202642.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B26" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="C26" s="1" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="F26" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G26" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H26" s="3" t="inlineStr">
+        <is>
+          <t>KRO|Nanoxx</t>
+        </is>
+      </c>
+      <c r="I26" s="3" t="inlineStr">
+        <is>
+          <t>YT : GuGu</t>
+        </is>
+      </c>
+      <c r="J26" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="K26" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L26" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="M26" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="N26" s="3" t="inlineStr">
+        <is>
+          <t>20250724T202428.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B27" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="C27" s="1" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="D27" s="2" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G27" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H27" s="3" t="inlineStr">
+        <is>
+          <t>KRO|Nanoxx</t>
+        </is>
+      </c>
+      <c r="I27" s="3" t="inlineStr">
+        <is>
+          <t>YT : GuGu</t>
+        </is>
+      </c>
+      <c r="J27" s="3" t="inlineStr">
+        <is>
+          <t>SK|Ope</t>
+        </is>
+      </c>
+      <c r="K27" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L27" s="3" t="inlineStr">
+        <is>
+          <t>HMB|BosS</t>
+        </is>
+      </c>
+      <c r="M27" s="3" t="inlineStr">
+        <is>
+          <t>SK|Yoshi825</t>
+        </is>
+      </c>
+      <c r="N27" s="3" t="inlineStr">
+        <is>
+          <t>20250724T202128.000Z</t>
         </is>
       </c>
     </row>
@@ -16581,7 +17229,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N64"/>
+  <dimension ref="A3:N66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21050,6 +21698,150 @@
       <c r="N64" s="3" t="inlineStr">
         <is>
           <t>20250724T173209.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="inlineStr">
+        <is>
+          <t>SPROUT</t>
+        </is>
+      </c>
+      <c r="B65" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="C65" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="D65" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="E65" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="F65" s="2" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="G65" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H65" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="I65" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="J65" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="K65" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L65" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="M65" s="3" t="inlineStr">
+        <is>
+          <t>Drage🍥</t>
+        </is>
+      </c>
+      <c r="N65" s="3" t="inlineStr">
+        <is>
+          <t>20250724T200251.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="inlineStr">
+        <is>
+          <t>SPROUT</t>
+        </is>
+      </c>
+      <c r="B66" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="C66" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="D66" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="E66" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="F66" s="2" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="G66" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H66" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="I66" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="J66" s="3" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="K66" s="3" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L66" s="3" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="M66" s="3" t="inlineStr">
+        <is>
+          <t>Drage🍥</t>
+        </is>
+      </c>
+      <c r="N66" s="3" t="inlineStr">
+        <is>
+          <t>20250724T200112.000Z</t>
         </is>
       </c>
     </row>
@@ -31182,7 +31974,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N63"/>
+  <dimension ref="A3:N66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -35579,6 +36371,222 @@
       <c r="N63" s="3" t="inlineStr">
         <is>
           <t>20250724T162252.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B64" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C64" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D64" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E64" s="2" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="F64" s="2" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="G64" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H64" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="I64" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="J64" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="K64" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="L64" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="M64" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="N64" s="3" t="inlineStr">
+        <is>
+          <t>20250724T203010.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B65" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C65" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D65" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E65" s="2" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="F65" s="2" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="G65" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H65" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="I65" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="J65" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="K65" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="L65" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="M65" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="N65" s="3" t="inlineStr">
+        <is>
+          <t>20250724T202813.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B66" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C66" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D66" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E66" s="2" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="F66" s="2" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="G66" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H66" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="I66" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="J66" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="K66" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="L66" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="M66" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="N66" s="3" t="inlineStr">
+        <is>
+          <t>20250724T202553.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-24 23:34:19)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -17445,7 +17445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N66"/>
+  <dimension ref="A3:N69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22058,6 +22058,222 @@
       <c r="N66" s="3" t="inlineStr">
         <is>
           <t>20250724T200112.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="B67" s="1" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="C67" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="D67" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="E67" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F67" s="2" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="G67" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H67" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="I67" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="J67" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="K67" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L67" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="M67" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="N67" s="3" t="inlineStr">
+        <is>
+          <t>20250724T212546.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="B68" s="1" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="C68" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="D68" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="E68" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F68" s="2" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="G68" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H68" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="I68" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="J68" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="K68" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L68" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="M68" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="N68" s="3" t="inlineStr">
+        <is>
+          <t>20250724T212413.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="B69" s="1" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="C69" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="D69" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="E69" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F69" s="2" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="G69" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H69" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="I69" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="J69" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="K69" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L69" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="M69" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="N69" s="3" t="inlineStr">
+        <is>
+          <t>20250724T212118.000Z</t>
         </is>
       </c>
     </row>
@@ -27707,7 +27923,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N72"/>
+  <dimension ref="A3:N76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -32752,6 +32968,294 @@
       <c r="N72" s="3" t="inlineStr">
         <is>
           <t>20250724T210034.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="B73" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="C73" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D73" s="2" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="E73" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F73" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="G73" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H73" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="I73" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="J73" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="K73" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L73" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="M73" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="N73" s="3" t="inlineStr">
+        <is>
+          <t>20250724T211333.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="B74" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="C74" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D74" s="2" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="E74" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F74" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="G74" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H74" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="I74" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="J74" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="K74" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L74" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="M74" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="N74" s="3" t="inlineStr">
+        <is>
+          <t>20250724T211114.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="B75" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="C75" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D75" s="2" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="E75" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F75" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="G75" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H75" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="I75" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="J75" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="K75" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L75" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="M75" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="N75" s="3" t="inlineStr">
+        <is>
+          <t>20250724T210857.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="B76" s="1" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="C76" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D76" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="E76" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="F76" s="2" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="G76" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H76" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="I76" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="J76" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="K76" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L76" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="M76" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="N76" s="3" t="inlineStr">
+        <is>
+          <t>20250724T210254.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-25 00:05:38)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -13322,7 +13322,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N59"/>
+  <dimension ref="A3:N64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17431,6 +17431,366 @@
       <c r="N59" s="3" t="inlineStr">
         <is>
           <t>20250724T195203.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="B60" s="1" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="C60" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D60" s="2" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="E60" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F60" s="2" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="G60" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H60" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="I60" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="J60" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="K60" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L60" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="M60" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="N60" s="3" t="inlineStr">
+        <is>
+          <t>20250724T220116.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="B61" s="1" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="C61" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D61" s="2" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="E61" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F61" s="2" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="G61" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H61" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="I61" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="J61" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="K61" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L61" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="M61" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="N61" s="3" t="inlineStr">
+        <is>
+          <t>20250724T215851.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B62" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C62" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="D62" s="2" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="E62" s="2" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="F62" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G62" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H62" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="I62" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="J62" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="K62" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L62" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="M62" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="N62" s="3" t="inlineStr">
+        <is>
+          <t>20250724T215243.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B63" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C63" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="D63" s="2" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="E63" s="2" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="F63" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G63" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H63" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="I63" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="J63" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="K63" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L63" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="M63" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="N63" s="3" t="inlineStr">
+        <is>
+          <t>20250724T215024.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B64" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C64" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="D64" s="2" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="E64" s="2" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="F64" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G64" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H64" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="I64" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="J64" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="K64" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L64" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="M64" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="N64" s="3" t="inlineStr">
+        <is>
+          <t>20250724T214817.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-25 00:36:58)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -22648,7 +22648,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N80"/>
+  <dimension ref="A3:N82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -28269,6 +28269,150 @@
       <c r="N80" s="3" t="inlineStr">
         <is>
           <t>20250724T204358.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B81" s="1" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="C81" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="D81" s="2" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="E81" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F81" s="2" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="G81" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H81" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="I81" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="J81" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="K81" s="3" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="L81" s="3" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="M81" s="3" t="inlineStr">
+        <is>
+          <t>CODE|OG</t>
+        </is>
+      </c>
+      <c r="N81" s="3" t="inlineStr">
+        <is>
+          <t>20250724T223516.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B82" s="1" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="C82" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="D82" s="2" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="E82" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F82" s="2" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="G82" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H82" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="I82" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="J82" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="K82" s="3" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="L82" s="3" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="M82" s="3" t="inlineStr">
+        <is>
+          <t>CODE|OG</t>
+        </is>
+      </c>
+      <c r="N82" s="3" t="inlineStr">
+        <is>
+          <t>20250724T223402.000Z</t>
         </is>
       </c>
     </row>
@@ -33630,7 +33774,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N71"/>
+  <dimension ref="A3:N78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -38603,6 +38747,510 @@
       <c r="N71" s="3" t="inlineStr">
         <is>
           <t>20250724T203646.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B72" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="C72" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D72" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E72" s="2" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="F72" s="2" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="G72" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H72" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I72" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="J72" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K72" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L72" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="M72" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="N72" s="3" t="inlineStr">
+        <is>
+          <t>20250724T223419.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B73" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="C73" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D73" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E73" s="2" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="F73" s="2" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="G73" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H73" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I73" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="J73" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K73" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L73" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="M73" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="N73" s="3" t="inlineStr">
+        <is>
+          <t>20250724T223216.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B74" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C74" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="D74" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="E74" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F74" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="G74" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H74" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="I74" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="J74" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="K74" s="3" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="L74" s="3" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="M74" s="3" t="inlineStr">
+        <is>
+          <t>CODE|OG</t>
+        </is>
+      </c>
+      <c r="N74" s="3" t="inlineStr">
+        <is>
+          <t>20250724T222525.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B75" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C75" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="D75" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="E75" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F75" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="G75" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H75" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="I75" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="J75" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="K75" s="3" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="L75" s="3" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="M75" s="3" t="inlineStr">
+        <is>
+          <t>CODE|OG</t>
+        </is>
+      </c>
+      <c r="N75" s="3" t="inlineStr">
+        <is>
+          <t>20250724T222340.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B76" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C76" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="D76" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="E76" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F76" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="G76" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H76" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="I76" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="J76" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="K76" s="3" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="L76" s="3" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="M76" s="3" t="inlineStr">
+        <is>
+          <t>CODE|OG</t>
+        </is>
+      </c>
+      <c r="N76" s="3" t="inlineStr">
+        <is>
+          <t>20250724T222120.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B77" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C77" s="1" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="D77" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="E77" s="2" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="F77" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="G77" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H77" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="I77" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="J77" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="K77" s="3" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="L77" s="3" t="inlineStr">
+        <is>
+          <t>CODE|OG</t>
+        </is>
+      </c>
+      <c r="M77" s="3" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="N77" s="3" t="inlineStr">
+        <is>
+          <t>20250724T221548.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B78" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C78" s="1" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="D78" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="E78" s="2" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="F78" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="G78" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H78" s="3" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="I78" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="J78" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="K78" s="3" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="L78" s="3" t="inlineStr">
+        <is>
+          <t>CODE|OG</t>
+        </is>
+      </c>
+      <c r="M78" s="3" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="N78" s="3" t="inlineStr">
+        <is>
+          <t>20250724T221304.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-25 01:08:19)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -22648,7 +22648,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N82"/>
+  <dimension ref="A3:N84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -28413,6 +28413,150 @@
       <c r="N82" s="3" t="inlineStr">
         <is>
           <t>20250724T223402.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="B83" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="C83" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="D83" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="E83" s="2" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="F83" s="2" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="G83" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H83" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="I83" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="J83" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Zoulan</t>
+        </is>
+      </c>
+      <c r="K83" s="3" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="L83" s="3" t="inlineStr">
+        <is>
+          <t>CODE|OG</t>
+        </is>
+      </c>
+      <c r="M83" s="3" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="N83" s="3" t="inlineStr">
+        <is>
+          <t>20250724T224249.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="B84" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="C84" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="D84" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="E84" s="2" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="F84" s="2" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="G84" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H84" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="I84" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="J84" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Zoulan</t>
+        </is>
+      </c>
+      <c r="K84" s="3" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="L84" s="3" t="inlineStr">
+        <is>
+          <t>CODE|OG</t>
+        </is>
+      </c>
+      <c r="M84" s="3" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="N84" s="3" t="inlineStr">
+        <is>
+          <t>20250724T224058.000Z</t>
         </is>
       </c>
     </row>
@@ -28427,7 +28571,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N76"/>
+  <dimension ref="A3:N84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -33760,6 +33904,582 @@
       <c r="N76" s="3" t="inlineStr">
         <is>
           <t>20250724T210254.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="B77" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="C77" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D77" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="E77" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="F77" s="2" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="G77" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H77" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="I77" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="J77" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K77" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Killer_17</t>
+        </is>
+      </c>
+      <c r="L77" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="M77" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="N77" s="3" t="inlineStr">
+        <is>
+          <t>20250724T230443.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="B78" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="C78" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D78" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="E78" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="F78" s="2" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="G78" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H78" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="I78" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="J78" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K78" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Killer_17</t>
+        </is>
+      </c>
+      <c r="L78" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="M78" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="N78" s="3" t="inlineStr">
+        <is>
+          <t>20250724T230223.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B79" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="C79" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="D79" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E79" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="F79" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="G79" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H79" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I79" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="J79" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="K79" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L79" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="M79" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="N79" s="3" t="inlineStr">
+        <is>
+          <t>20250724T225504.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B80" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="C80" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="D80" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E80" s="2" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="F80" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="G80" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H80" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I80" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="J80" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="K80" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L80" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="M80" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="N80" s="3" t="inlineStr">
+        <is>
+          <t>20250724T225248.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="B81" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="C81" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D81" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="E81" s="2" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="F81" s="2" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="G81" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H81" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="I81" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="J81" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K81" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Killer_17</t>
+        </is>
+      </c>
+      <c r="L81" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="M81" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="N81" s="3" t="inlineStr">
+        <is>
+          <t>20250724T230703.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B82" s="1" t="inlineStr">
+        <is>
+          <t>CHESTER</t>
+        </is>
+      </c>
+      <c r="C82" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D82" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E82" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="F82" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="G82" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H82" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="I82" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="J82" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Zoulan</t>
+        </is>
+      </c>
+      <c r="K82" s="3" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="L82" s="3" t="inlineStr">
+        <is>
+          <t>CODE|OG</t>
+        </is>
+      </c>
+      <c r="M82" s="3" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="N82" s="3" t="inlineStr">
+        <is>
+          <t>20250724T225419.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B83" s="1" t="inlineStr">
+        <is>
+          <t>CHESTER</t>
+        </is>
+      </c>
+      <c r="C83" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D83" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E83" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="F83" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="G83" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H83" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="I83" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="J83" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Zoulan</t>
+        </is>
+      </c>
+      <c r="K83" s="3" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="L83" s="3" t="inlineStr">
+        <is>
+          <t>CODE|OG</t>
+        </is>
+      </c>
+      <c r="M83" s="3" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="N83" s="3" t="inlineStr">
+        <is>
+          <t>20250724T225200.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B84" s="1" t="inlineStr">
+        <is>
+          <t>CHESTER</t>
+        </is>
+      </c>
+      <c r="C84" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D84" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E84" s="2" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="F84" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="G84" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H84" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="I84" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="J84" s="3" t="inlineStr">
+        <is>
+          <t>KCP|Zoulan</t>
+        </is>
+      </c>
+      <c r="K84" s="3" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="L84" s="3" t="inlineStr">
+        <is>
+          <t>CODE|OG</t>
+        </is>
+      </c>
+      <c r="M84" s="3" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="N84" s="3" t="inlineStr">
+        <is>
+          <t>20250724T224944.000Z</t>
         </is>
       </c>
     </row>
@@ -33774,7 +34494,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N78"/>
+  <dimension ref="A3:N81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -39251,6 +39971,222 @@
       <c r="N78" s="3" t="inlineStr">
         <is>
           <t>20250724T221304.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="inlineStr">
+        <is>
+          <t>JESSIE</t>
+        </is>
+      </c>
+      <c r="B79" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="C79" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="D79" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E79" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="F79" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G79" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H79" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I79" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="J79" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K79" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L79" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="M79" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="N79" s="3" t="inlineStr">
+        <is>
+          <t>20250724T224522.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="inlineStr">
+        <is>
+          <t>JESSIE</t>
+        </is>
+      </c>
+      <c r="B80" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="C80" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="D80" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E80" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="F80" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G80" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H80" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I80" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="J80" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K80" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L80" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="M80" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="N80" s="3" t="inlineStr">
+        <is>
+          <t>20250724T224317.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="inlineStr">
+        <is>
+          <t>JESSIE</t>
+        </is>
+      </c>
+      <c r="B81" s="1" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="C81" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="D81" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E81" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="F81" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G81" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H81" s="3" t="inlineStr">
+        <is>
+          <t>TE|Rafikii</t>
+        </is>
+      </c>
+      <c r="I81" s="3" t="inlineStr">
+        <is>
+          <t>TE|Ezlivi</t>
+        </is>
+      </c>
+      <c r="J81" s="3" t="inlineStr">
+        <is>
+          <t>TE|Belal</t>
+        </is>
+      </c>
+      <c r="K81" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L81" s="3" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="M81" s="3" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="N81" s="3" t="inlineStr">
+        <is>
+          <t>20250724T224058.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-25 14:23:01)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -4079,7 +4079,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N10"/>
+  <dimension ref="A3:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4660,6 +4660,150 @@
       <c r="N10" s="3" t="inlineStr">
         <is>
           <t>20250724T191208.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>OTIS</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="G11" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H11" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="I11" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="J11" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="K11" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L11" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M11" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N11" s="3" t="inlineStr">
+        <is>
+          <t>20250725T121622.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>OTIS</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="G12" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H12" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="I12" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="J12" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="K12" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L12" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M12" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N12" s="3" t="inlineStr">
+        <is>
+          <t>20250725T121332.000Z</t>
         </is>
       </c>
     </row>
@@ -34494,7 +34638,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N81"/>
+  <dimension ref="A3:N84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -40187,6 +40331,222 @@
       <c r="N81" s="3" t="inlineStr">
         <is>
           <t>20250724T224058.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B82" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C82" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="D82" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E82" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="F82" s="2" t="inlineStr">
+        <is>
+          <t>CHESTER</t>
+        </is>
+      </c>
+      <c r="G82" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H82" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="I82" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="J82" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="K82" s="3" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="L82" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="M82" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="N82" s="3" t="inlineStr">
+        <is>
+          <t>20250725T121935.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B83" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C83" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="D83" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E83" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="F83" s="2" t="inlineStr">
+        <is>
+          <t>CHESTER</t>
+        </is>
+      </c>
+      <c r="G83" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H83" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="I83" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="J83" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="K83" s="3" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="L83" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="M83" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="N83" s="3" t="inlineStr">
+        <is>
+          <t>20250725T121749.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B84" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C84" s="1" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="D84" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E84" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="F84" s="2" t="inlineStr">
+        <is>
+          <t>CHESTER</t>
+        </is>
+      </c>
+      <c r="G84" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H84" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="I84" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="J84" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="K84" s="3" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="L84" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="M84" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="N84" s="3" t="inlineStr">
+        <is>
+          <t>20250725T121550.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-25 14:54:22)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -4079,7 +4079,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N12"/>
+  <dimension ref="A3:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4804,6 +4804,222 @@
       <c r="N12" s="3" t="inlineStr">
         <is>
           <t>20250725T121332.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="G13" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H13" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="I13" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="J13" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="K13" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L13" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M13" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N13" s="3" t="inlineStr">
+        <is>
+          <t>20250725T122729.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="G14" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H14" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="J14" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="K14" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L14" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M14" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N14" s="3" t="inlineStr">
+        <is>
+          <t>20250725T122425.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="G15" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H15" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="J15" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="K15" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L15" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M15" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N15" s="3" t="inlineStr">
+        <is>
+          <t>20250725T122303.000Z</t>
         </is>
       </c>
     </row>
@@ -22792,7 +23008,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N84"/>
+  <dimension ref="A3:N85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -28701,6 +28917,78 @@
       <c r="N84" s="3" t="inlineStr">
         <is>
           <t>20250724T224058.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="B85" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C85" s="1" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="D85" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E85" s="2" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="F85" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G85" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H85" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I85" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J85" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K85" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="L85" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="M85" s="3" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="N85" s="3" t="inlineStr">
+        <is>
+          <t>20250725T125209.000Z</t>
         </is>
       </c>
     </row>
@@ -28715,7 +29003,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N84"/>
+  <dimension ref="A3:N91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -34624,6 +34912,510 @@
       <c r="N84" s="3" t="inlineStr">
         <is>
           <t>20250724T224944.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="B85" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="C85" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D85" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E85" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="F85" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="G85" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H85" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="I85" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="J85" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="K85" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="L85" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="M85" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="N85" s="3" t="inlineStr">
+        <is>
+          <t>20250725T124704.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="B86" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="C86" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D86" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E86" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="F86" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="G86" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H86" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="I86" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="J86" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="K86" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="L86" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="M86" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="N86" s="3" t="inlineStr">
+        <is>
+          <t>20250725T124444.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B87" s="1" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="C87" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="D87" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="E87" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="F87" s="2" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="G87" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H87" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I87" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J87" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K87" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="L87" s="3" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="M87" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="N87" s="3" t="inlineStr">
+        <is>
+          <t>20250725T124656.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B88" s="1" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="C88" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="D88" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="E88" s="2" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="F88" s="2" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="G88" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H88" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I88" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J88" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K88" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="L88" s="3" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="M88" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="N88" s="3" t="inlineStr">
+        <is>
+          <t>20250725T124436.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B89" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="C89" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="D89" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E89" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F89" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="G89" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H89" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I89" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J89" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K89" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="L89" s="3" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="M89" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="N89" s="3" t="inlineStr">
+        <is>
+          <t>20250725T123824.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B90" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="C90" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="D90" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E90" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F90" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="G90" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H90" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I90" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J90" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K90" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="L90" s="3" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="M90" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="N90" s="3" t="inlineStr">
+        <is>
+          <t>20250725T123604.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B91" s="1" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="C91" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="D91" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E91" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F91" s="2" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="G91" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H91" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I91" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J91" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K91" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="L91" s="3" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="M91" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="N91" s="3" t="inlineStr">
+        <is>
+          <t>20250725T123348.000Z</t>
         </is>
       </c>
     </row>
@@ -34638,7 +35430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N84"/>
+  <dimension ref="A3:N92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -40547,6 +41339,582 @@
       <c r="N84" s="3" t="inlineStr">
         <is>
           <t>20250725T121550.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="B85" s="1" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="C85" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D85" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E85" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="F85" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G85" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H85" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="I85" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="J85" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="K85" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="L85" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="M85" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="N85" s="3" t="inlineStr">
+        <is>
+          <t>20250725T123812.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="B86" s="1" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="C86" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D86" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E86" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="F86" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G86" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H86" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="I86" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="J86" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="K86" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="L86" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="M86" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="N86" s="3" t="inlineStr">
+        <is>
+          <t>20250725T123620.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="B87" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C87" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D87" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E87" s="2" t="inlineStr">
+        <is>
+          <t>COLETTE</t>
+        </is>
+      </c>
+      <c r="F87" s="2" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="G87" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H87" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="I87" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="J87" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="K87" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="L87" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="M87" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="N87" s="3" t="inlineStr">
+        <is>
+          <t>20250725T123042.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="B88" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C88" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D88" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E88" s="2" t="inlineStr">
+        <is>
+          <t>COLETTE</t>
+        </is>
+      </c>
+      <c r="F88" s="2" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="G88" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H88" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="I88" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="J88" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="K88" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="L88" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="M88" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="N88" s="3" t="inlineStr">
+        <is>
+          <t>20250725T122841.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="B89" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C89" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D89" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E89" s="2" t="inlineStr">
+        <is>
+          <t>COLETTE</t>
+        </is>
+      </c>
+      <c r="F89" s="2" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="G89" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H89" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="I89" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="J89" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="K89" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="L89" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="M89" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="N89" s="3" t="inlineStr">
+        <is>
+          <t>20250725T122607.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B90" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="C90" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D90" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E90" s="2" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="F90" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G90" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H90" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I90" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J90" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K90" s="3" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="L90" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="M90" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="N90" s="3" t="inlineStr">
+        <is>
+          <t>20250725T122835.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B91" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="C91" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D91" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E91" s="2" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="F91" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G91" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H91" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I91" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J91" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K91" s="3" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="L91" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="M91" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="N91" s="3" t="inlineStr">
+        <is>
+          <t>20250725T122636.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B92" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="C92" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D92" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E92" s="2" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="F92" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G92" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H92" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I92" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J92" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K92" s="3" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="L92" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="M92" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="N92" s="3" t="inlineStr">
+        <is>
+          <t>20250725T122447.000Z</t>
         </is>
       </c>
     </row>
@@ -40561,7 +41929,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N46"/>
+  <dimension ref="A3:N47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -43734,6 +45102,78 @@
       <c r="N46" s="3" t="inlineStr">
         <is>
           <t>20250724T182608.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="B47" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="C47" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D47" s="2" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="E47" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F47" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G47" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H47" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="I47" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="J47" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="K47" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L47" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M47" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N47" s="3" t="inlineStr">
+        <is>
+          <t>20250725T125327.000Z</t>
         </is>
       </c>
     </row>
@@ -46791,7 +48231,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N47"/>
+  <dimension ref="A3:N51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -50039,6 +51479,294 @@
         </is>
       </c>
     </row>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B48" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="C48" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D48" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E48" s="2" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="F48" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="G48" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H48" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="I48" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="J48" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="K48" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L48" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M48" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N48" s="3" t="inlineStr">
+        <is>
+          <t>20250725T124552.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B49" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="C49" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D49" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E49" s="2" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="F49" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="G49" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H49" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="I49" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="J49" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="K49" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L49" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M49" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N49" s="3" t="inlineStr">
+        <is>
+          <t>20250725T124333.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="B50" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C50" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D50" s="2" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="E50" s="2" t="inlineStr">
+        <is>
+          <t>DYNAMIKE</t>
+        </is>
+      </c>
+      <c r="F50" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="G50" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H50" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="I50" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="J50" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="K50" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L50" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M50" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N50" s="3" t="inlineStr">
+        <is>
+          <t>20250725T123721.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="B51" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C51" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D51" s="2" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="E51" s="2" t="inlineStr">
+        <is>
+          <t>DYNAMIKE</t>
+        </is>
+      </c>
+      <c r="F51" s="2" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="G51" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H51" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="I51" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="J51" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="K51" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L51" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M51" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N51" s="3" t="inlineStr">
+        <is>
+          <t>20250725T123431.000Z</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-25 15:25:41)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -13159,7 +13159,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N9"/>
+  <dimension ref="A3:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13668,6 +13668,294 @@
       <c r="N9" s="3" t="inlineStr">
         <is>
           <t>20250724T190323.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>JACKY</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H10" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="I10" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="J10" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="K10" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L10" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M10" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N10" s="3" t="inlineStr">
+        <is>
+          <t>20250725T132220.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>JACKY</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>ROSA</t>
+        </is>
+      </c>
+      <c r="G11" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H11" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="I11" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="J11" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="K11" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="L11" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="M11" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N11" s="3" t="inlineStr">
+        <is>
+          <t>20250725T131650.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>JACKY</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>ROSA</t>
+        </is>
+      </c>
+      <c r="G12" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H12" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="I12" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="J12" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="K12" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="L12" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="M12" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N12" s="3" t="inlineStr">
+        <is>
+          <t>20250725T131450.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>JACKY</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="G13" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H13" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="I13" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="J13" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="K13" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L13" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M13" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N13" s="3" t="inlineStr">
+        <is>
+          <t>20250725T132435.000Z</t>
         </is>
       </c>
     </row>
@@ -18165,7 +18453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N69"/>
+  <dimension ref="A3:N77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22994,6 +23282,582 @@
       <c r="N69" s="3" t="inlineStr">
         <is>
           <t>20250724T212118.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B70" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C70" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D70" s="2" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="E70" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="F70" s="2" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="G70" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H70" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="I70" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="J70" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="K70" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="L70" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="M70" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="N70" s="3" t="inlineStr">
+        <is>
+          <t>20250725T132324.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B71" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C71" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D71" s="2" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="E71" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="F71" s="2" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="G71" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H71" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="I71" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="J71" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="K71" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="L71" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="M71" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="N71" s="3" t="inlineStr">
+        <is>
+          <t>20250725T132108.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B72" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C72" s="1" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D72" s="2" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="E72" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="F72" s="2" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="G72" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H72" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="I72" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="J72" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="K72" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="L72" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="M72" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="N72" s="3" t="inlineStr">
+        <is>
+          <t>20250725T131838.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="B73" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C73" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D73" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E73" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F73" s="2" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="G73" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H73" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="I73" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="J73" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K73" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="L73" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="M73" s="3" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="N73" s="3" t="inlineStr">
+        <is>
+          <t>20250725T132300.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="B74" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C74" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D74" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E74" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F74" s="2" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="G74" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H74" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="I74" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="J74" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K74" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="L74" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="M74" s="3" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="N74" s="3" t="inlineStr">
+        <is>
+          <t>20250725T131911.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="B75" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C75" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D75" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E75" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F75" s="2" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="G75" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H75" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="I75" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="J75" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K75" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="L75" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="M75" s="3" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="N75" s="3" t="inlineStr">
+        <is>
+          <t>20250725T131701.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B76" s="1" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="C76" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="D76" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E76" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F76" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G76" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H76" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I76" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J76" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K76" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="L76" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="M76" s="3" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="N76" s="3" t="inlineStr">
+        <is>
+          <t>20250725T131000.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B77" s="1" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="C77" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="D77" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E77" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F77" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G77" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H77" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I77" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J77" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K77" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="L77" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="M77" s="3" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="N77" s="3" t="inlineStr">
+        <is>
+          <t>20250725T130752.000Z</t>
         </is>
       </c>
     </row>
@@ -23008,7 +23872,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N85"/>
+  <dimension ref="A3:N93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -28989,6 +29853,582 @@
       <c r="N85" s="3" t="inlineStr">
         <is>
           <t>20250725T125209.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="B86" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="C86" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="D86" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E86" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F86" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="G86" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H86" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="I86" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="J86" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="K86" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="L86" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M86" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N86" s="3" t="inlineStr">
+        <is>
+          <t>20250725T131035.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="B87" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="C87" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="D87" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E87" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F87" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="G87" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H87" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="I87" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="J87" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="K87" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="L87" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M87" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N87" s="3" t="inlineStr">
+        <is>
+          <t>20250725T130933.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B88" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C88" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="D88" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="E88" s="2" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="F88" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G88" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H88" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="I88" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="J88" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="K88" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="L88" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M88" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N88" s="3" t="inlineStr">
+        <is>
+          <t>20250725T130418.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B89" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C89" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="D89" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="E89" s="2" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="F89" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G89" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H89" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="I89" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="J89" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="K89" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="L89" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M89" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N89" s="3" t="inlineStr">
+        <is>
+          <t>20250725T130225.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B90" s="1" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="C90" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D90" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E90" s="2" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="F90" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G90" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H90" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I90" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="J90" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="K90" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L90" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="M90" s="3" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="N90" s="3" t="inlineStr">
+        <is>
+          <t>20250725T130042.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B91" s="1" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="C91" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D91" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E91" s="2" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="F91" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G91" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H91" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I91" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="J91" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="K91" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L91" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="M91" s="3" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="N91" s="3" t="inlineStr">
+        <is>
+          <t>20250725T125911.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="B92" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C92" s="1" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="D92" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E92" s="2" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="F92" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G92" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H92" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I92" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J92" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K92" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="L92" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="M92" s="3" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="N92" s="3" t="inlineStr">
+        <is>
+          <t>20250725T125452.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="B93" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C93" s="1" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="D93" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E93" s="2" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="F93" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G93" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H93" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I93" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J93" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K93" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="L93" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="M93" s="3" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="N93" s="3" t="inlineStr">
+        <is>
+          <t>20250725T125319.000Z</t>
         </is>
       </c>
     </row>
@@ -29003,7 +30443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N91"/>
+  <dimension ref="A3:N93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -35416,6 +36856,150 @@
       <c r="N91" s="3" t="inlineStr">
         <is>
           <t>20250725T123348.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="B92" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C92" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D92" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="E92" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="F92" s="2" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="G92" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H92" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="I92" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="J92" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="K92" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="L92" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="M92" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="N92" s="3" t="inlineStr">
+        <is>
+          <t>20250725T125631.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="B93" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C93" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D93" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="E93" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="F93" s="2" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="G93" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H93" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="I93" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="J93" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="K93" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="L93" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="M93" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="N93" s="3" t="inlineStr">
+        <is>
+          <t>20250725T125411.000Z</t>
         </is>
       </c>
     </row>
@@ -41929,7 +43513,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N47"/>
+  <dimension ref="A3:N52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -45174,6 +46758,366 @@
       <c r="N47" s="3" t="inlineStr">
         <is>
           <t>20250725T125327.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="B48" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C48" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D48" s="2" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="E48" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="F48" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="G48" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H48" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="I48" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="J48" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="K48" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="L48" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="M48" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N48" s="3" t="inlineStr">
+        <is>
+          <t>20250725T130846.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="B49" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C49" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D49" s="2" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="E49" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="F49" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="G49" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H49" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="I49" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="J49" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="K49" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="L49" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="M49" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N49" s="3" t="inlineStr">
+        <is>
+          <t>20250725T130627.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="B50" s="1" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C50" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D50" s="2" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="E50" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="F50" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="G50" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H50" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="I50" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="J50" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="K50" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="L50" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="M50" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N50" s="3" t="inlineStr">
+        <is>
+          <t>20250725T130423.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="B51" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="C51" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D51" s="2" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="E51" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F51" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G51" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H51" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="I51" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="J51" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="K51" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L51" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M51" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N51" s="3" t="inlineStr">
+        <is>
+          <t>20250725T125806.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="B52" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="C52" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D52" s="2" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="E52" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F52" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G52" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H52" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="I52" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="J52" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="K52" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L52" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M52" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N52" s="3" t="inlineStr">
+        <is>
+          <t>20250725T125547.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-25 15:57:01)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -460,7 +460,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N52"/>
+  <dimension ref="A3:N55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4065,6 +4065,222 @@
       <c r="N52" s="3" t="inlineStr">
         <is>
           <t>20250724T200846.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="B53" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="C53" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="D53" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="E53" s="2" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="F53" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G53" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H53" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I53" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J53" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K53" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="L53" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="M53" s="3" t="inlineStr">
+        <is>
+          <t>CR|Tensai</t>
+        </is>
+      </c>
+      <c r="N53" s="3" t="inlineStr">
+        <is>
+          <t>20250725T135359.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="B54" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="C54" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="D54" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="E54" s="2" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="F54" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G54" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H54" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I54" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J54" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K54" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="L54" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="M54" s="3" t="inlineStr">
+        <is>
+          <t>CR|Tensai</t>
+        </is>
+      </c>
+      <c r="N54" s="3" t="inlineStr">
+        <is>
+          <t>20250725T135055.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="B55" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="C55" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="D55" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="E55" s="2" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="F55" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G55" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H55" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I55" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J55" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K55" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="L55" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="M55" s="3" t="inlineStr">
+        <is>
+          <t>CR|Tensai</t>
+        </is>
+      </c>
+      <c r="N55" s="3" t="inlineStr">
+        <is>
+          <t>20250725T134922.000Z</t>
         </is>
       </c>
     </row>
@@ -13159,7 +13375,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N13"/>
+  <dimension ref="A3:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13956,6 +14172,222 @@
       <c r="N13" s="3" t="inlineStr">
         <is>
           <t>20250725T132435.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="G14" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H14" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="J14" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="K14" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="L14" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M14" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="N14" s="3" t="inlineStr">
+        <is>
+          <t>20250725T133435.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="G15" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H15" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="J15" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="K15" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="L15" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M15" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="N15" s="3" t="inlineStr">
+        <is>
+          <t>20250725T133236.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="G16" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H16" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="I16" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="J16" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="K16" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="L16" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M16" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="N16" s="3" t="inlineStr">
+        <is>
+          <t>20250725T133038.000Z</t>
         </is>
       </c>
     </row>
@@ -13970,7 +14402,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N64"/>
+  <dimension ref="A3:N72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18439,6 +18871,582 @@
       <c r="N64" s="3" t="inlineStr">
         <is>
           <t>20250724T214817.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B65" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="C65" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D65" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E65" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F65" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="G65" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H65" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="I65" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="J65" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="K65" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="L65" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M65" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N65" s="3" t="inlineStr">
+        <is>
+          <t>20250725T135312.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B66" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="C66" s="1" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D66" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E66" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F66" s="2" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="G66" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H66" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="I66" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="J66" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="K66" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="L66" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M66" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N66" s="3" t="inlineStr">
+        <is>
+          <t>20250725T134954.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B67" s="1" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="C67" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="D67" s="2" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="E67" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F67" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G67" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H67" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="I67" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="J67" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="K67" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="L67" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M67" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N67" s="3" t="inlineStr">
+        <is>
+          <t>20250725T134347.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B68" s="1" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="C68" s="1" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="D68" s="2" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="E68" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F68" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G68" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H68" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="I68" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="J68" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="K68" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="L68" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M68" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N68" s="3" t="inlineStr">
+        <is>
+          <t>20250725T134103.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="inlineStr">
+        <is>
+          <t>SURGE</t>
+        </is>
+      </c>
+      <c r="B69" s="1" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="C69" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="D69" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E69" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="F69" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G69" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H69" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I69" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J69" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K69" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L69" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="M69" s="3" t="inlineStr">
+        <is>
+          <t>CR|Tensai</t>
+        </is>
+      </c>
+      <c r="N69" s="3" t="inlineStr">
+        <is>
+          <t>20250725T134230.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="inlineStr">
+        <is>
+          <t>SURGE</t>
+        </is>
+      </c>
+      <c r="B70" s="1" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="C70" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="D70" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E70" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="F70" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G70" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H70" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I70" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J70" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K70" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L70" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="M70" s="3" t="inlineStr">
+        <is>
+          <t>CR|Tensai</t>
+        </is>
+      </c>
+      <c r="N70" s="3" t="inlineStr">
+        <is>
+          <t>20250725T134014.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B71" s="1" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="C71" s="1" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="D71" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="E71" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="F71" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="G71" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H71" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I71" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="J71" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="K71" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="L71" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="M71" s="3" t="inlineStr">
+        <is>
+          <t>CR|Tensai</t>
+        </is>
+      </c>
+      <c r="N71" s="3" t="inlineStr">
+        <is>
+          <t>20250725T133349.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B72" s="1" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="C72" s="1" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="D72" s="2" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="E72" s="2" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="F72" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="G72" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H72" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I72" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="J72" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="K72" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="L72" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="M72" s="3" t="inlineStr">
+        <is>
+          <t>CR|Tensai</t>
+        </is>
+      </c>
+      <c r="N72" s="3" t="inlineStr">
+        <is>
+          <t>20250725T133034.000Z</t>
         </is>
       </c>
     </row>
@@ -18453,7 +19461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N77"/>
+  <dimension ref="A3:N80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23858,6 +24866,222 @@
       <c r="N77" s="3" t="inlineStr">
         <is>
           <t>20250725T130752.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="B78" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C78" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D78" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="E78" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="F78" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="G78" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H78" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="I78" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="J78" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="K78" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="L78" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="M78" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="N78" s="3" t="inlineStr">
+        <is>
+          <t>20250725T133446.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="B79" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C79" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D79" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="E79" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="F79" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="G79" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H79" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="I79" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="J79" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="K79" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="L79" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="M79" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="N79" s="3" t="inlineStr">
+        <is>
+          <t>20250725T133209.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="B80" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C80" s="1" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D80" s="2" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="E80" s="2" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="F80" s="2" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="G80" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H80" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="I80" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="J80" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="K80" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="L80" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="M80" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="N80" s="3" t="inlineStr">
+        <is>
+          <t>20250725T133026.000Z</t>
         </is>
       </c>
     </row>
@@ -47132,7 +48356,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N44"/>
+  <dimension ref="A3:N48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -50161,6 +51385,294 @@
       <c r="N44" s="3" t="inlineStr">
         <is>
           <t>20250724T184938.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>LOLA</t>
+        </is>
+      </c>
+      <c r="B45" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="C45" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="D45" s="2" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="E45" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F45" s="2" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="G45" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H45" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="I45" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="J45" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="K45" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="L45" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M45" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="N45" s="3" t="inlineStr">
+        <is>
+          <t>20250725T135440.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="B46" s="1" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="C46" s="1" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="D46" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E46" s="2" t="inlineStr">
+        <is>
+          <t>PENNY</t>
+        </is>
+      </c>
+      <c r="F46" s="2" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="G46" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H46" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="I46" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="J46" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="K46" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="L46" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M46" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="N46" s="3" t="inlineStr">
+        <is>
+          <t>20250725T134642.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="B47" s="1" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="C47" s="1" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="D47" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E47" s="2" t="inlineStr">
+        <is>
+          <t>PENNY</t>
+        </is>
+      </c>
+      <c r="F47" s="2" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="G47" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H47" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="I47" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="J47" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="K47" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="L47" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M47" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="N47" s="3" t="inlineStr">
+        <is>
+          <t>20250725T134342.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="B48" s="1" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="C48" s="1" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="D48" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E48" s="2" t="inlineStr">
+        <is>
+          <t>PENNY</t>
+        </is>
+      </c>
+      <c r="F48" s="2" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="G48" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H48" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="I48" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="J48" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="K48" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="L48" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M48" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="N48" s="3" t="inlineStr">
+        <is>
+          <t>20250725T134134.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-25 16:28:21)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -460,7 +460,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N55"/>
+  <dimension ref="A3:N70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4281,6 +4281,1086 @@
       <c r="N55" s="3" t="inlineStr">
         <is>
           <t>20250725T134922.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="B56" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="C56" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D56" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="E56" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="F56" s="2" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="G56" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H56" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="I56" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="J56" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="K56" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="L56" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M56" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N56" s="3" t="inlineStr">
+        <is>
+          <t>20250725T141332.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="B57" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="C57" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D57" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="E57" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="F57" s="2" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="G57" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H57" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="I57" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="J57" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="K57" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="L57" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M57" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N57" s="3" t="inlineStr">
+        <is>
+          <t>20250725T141040.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B58" s="1" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="C58" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D58" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="E58" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F58" s="2" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="G58" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H58" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="I58" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="J58" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="K58" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="L58" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M58" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N58" s="3" t="inlineStr">
+        <is>
+          <t>20250725T140459.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B59" s="1" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="C59" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D59" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="E59" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F59" s="2" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="G59" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H59" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="I59" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="J59" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="K59" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="L59" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M59" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N59" s="3" t="inlineStr">
+        <is>
+          <t>20250725T140208.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B60" s="1" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="C60" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D60" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="E60" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F60" s="2" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="G60" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H60" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="I60" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="J60" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="K60" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="L60" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M60" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N60" s="3" t="inlineStr">
+        <is>
+          <t>20250725T140044.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="B61" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="C61" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D61" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E61" s="2" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="F61" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G61" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H61" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="I61" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="J61" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="K61" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="L61" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="M61" s="3" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="N61" s="3" t="inlineStr">
+        <is>
+          <t>20250725T140308.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="B62" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="C62" s="1" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D62" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E62" s="2" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="F62" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G62" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H62" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="I62" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="J62" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="K62" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="L62" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="M62" s="3" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="N62" s="3" t="inlineStr">
+        <is>
+          <t>20250725T140154.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="B63" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="C63" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="D63" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E63" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F63" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G63" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H63" s="3" t="inlineStr">
+        <is>
+          <t>Yannic🐀</t>
+        </is>
+      </c>
+      <c r="I63" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Adrii</t>
+        </is>
+      </c>
+      <c r="J63" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Bogdan</t>
+        </is>
+      </c>
+      <c r="K63" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L63" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="M63" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="N63" s="3" t="inlineStr">
+        <is>
+          <t>20250725T142427.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="B64" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="C64" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="D64" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E64" s="2" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F64" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G64" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H64" s="3" t="inlineStr">
+        <is>
+          <t>Yannic🐀</t>
+        </is>
+      </c>
+      <c r="I64" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Adrii</t>
+        </is>
+      </c>
+      <c r="J64" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Bogdan</t>
+        </is>
+      </c>
+      <c r="K64" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L64" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="M64" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="N64" s="3" t="inlineStr">
+        <is>
+          <t>20250725T142203.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="B65" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C65" s="1" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="D65" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E65" s="2" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="F65" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="G65" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H65" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Bogdan</t>
+        </is>
+      </c>
+      <c r="I65" s="3" t="inlineStr">
+        <is>
+          <t>Yannic🐀</t>
+        </is>
+      </c>
+      <c r="J65" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Adrii</t>
+        </is>
+      </c>
+      <c r="K65" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="L65" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="M65" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="N65" s="3" t="inlineStr">
+        <is>
+          <t>20250725T141449.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="B66" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C66" s="1" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="D66" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E66" s="2" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="F66" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="G66" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H66" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Bogdan</t>
+        </is>
+      </c>
+      <c r="I66" s="3" t="inlineStr">
+        <is>
+          <t>Yannic🐀</t>
+        </is>
+      </c>
+      <c r="J66" s="3" t="inlineStr">
+        <is>
+          <t>BBO|Adrii</t>
+        </is>
+      </c>
+      <c r="K66" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="L66" s="3" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="M66" s="3" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="N66" s="3" t="inlineStr">
+        <is>
+          <t>20250725T141340.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="B67" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="C67" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="D67" s="2" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="E67" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="F67" s="2" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="G67" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H67" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="I67" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="J67" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="K67" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="L67" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M67" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="N67" s="3" t="inlineStr">
+        <is>
+          <t>20250725T142555.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B68" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="C68" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="D68" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E68" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F68" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G68" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H68" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="I68" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="J68" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="K68" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="L68" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="M68" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N68" s="3" t="inlineStr">
+        <is>
+          <t>20250725T142031.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B69" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="C69" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="D69" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E69" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F69" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G69" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H69" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="I69" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="J69" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="K69" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="L69" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="M69" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N69" s="3" t="inlineStr">
+        <is>
+          <t>20250725T141649.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B70" s="1" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="C70" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="D70" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E70" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F70" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G70" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H70" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="I70" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="J70" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="K70" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="L70" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="M70" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N70" s="3" t="inlineStr">
+        <is>
+          <t>20250725T141422.000Z</t>
         </is>
       </c>
     </row>
@@ -38238,7 +39318,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N92"/>
+  <dimension ref="A3:N100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -44723,6 +45803,582 @@
       <c r="N92" s="3" t="inlineStr">
         <is>
           <t>20250725T122447.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B93" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="C93" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D93" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E93" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="F93" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G93" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H93" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I93" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="J93" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="K93" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="L93" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="M93" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="N93" s="3" t="inlineStr">
+        <is>
+          <t>20250725T142146.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B94" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="C94" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D94" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E94" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="F94" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G94" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H94" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I94" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="J94" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="K94" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="L94" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="M94" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="N94" s="3" t="inlineStr">
+        <is>
+          <t>20250725T141922.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B95" s="1" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="C95" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D95" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E95" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="F95" s="2" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G95" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H95" s="3" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I95" s="3" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="J95" s="3" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="K95" s="3" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="L95" s="3" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="M95" s="3" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="N95" s="3" t="inlineStr">
+        <is>
+          <t>20250725T141708.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B96" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C96" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="D96" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E96" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="F96" s="2" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="G96" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H96" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I96" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J96" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K96" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L96" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="M96" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N96" s="3" t="inlineStr">
+        <is>
+          <t>20250725T142528.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B97" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C97" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="D97" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E97" s="2" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="F97" s="2" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="G97" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H97" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I97" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J97" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K97" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L97" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="M97" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N97" s="3" t="inlineStr">
+        <is>
+          <t>20250725T142326.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B98" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="C98" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D98" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="E98" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F98" s="2" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="G98" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H98" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I98" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J98" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K98" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L98" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="M98" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N98" s="3" t="inlineStr">
+        <is>
+          <t>20250725T141726.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B99" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="C99" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D99" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="E99" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F99" s="2" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="G99" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H99" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I99" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J99" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K99" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L99" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="M99" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N99" s="3" t="inlineStr">
+        <is>
+          <t>20250725T141514.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B100" s="1" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="C100" s="1" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D100" s="2" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="E100" s="2" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F100" s="2" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="G100" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H100" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I100" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J100" s="3" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K100" s="3" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L100" s="3" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="M100" s="3" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N100" s="3" t="inlineStr">
+        <is>
+          <t>20250725T141225.000Z</t>
         </is>
       </c>
     </row>
@@ -48356,7 +50012,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N48"/>
+  <dimension ref="A3:N54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -51673,6 +53329,438 @@
       <c r="N48" s="3" t="inlineStr">
         <is>
           <t>20250725T134134.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="B49" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="C49" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="D49" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="E49" s="2" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="F49" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G49" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H49" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="I49" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="J49" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="K49" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L49" s="3" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="M49" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="N49" s="3" t="inlineStr">
+        <is>
+          <t>20250725T142507.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="B50" s="1" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="C50" s="1" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="D50" s="2" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="E50" s="2" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="F50" s="2" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G50" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H50" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="I50" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="J50" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="K50" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L50" s="3" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="M50" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="N50" s="3" t="inlineStr">
+        <is>
+          <t>20250725T142311.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="B51" s="1" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="C51" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="D51" s="2" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="E51" s="2" t="inlineStr">
+        <is>
+          <t>PENNY</t>
+        </is>
+      </c>
+      <c r="F51" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="G51" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H51" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="I51" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="J51" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="K51" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L51" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M51" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N51" s="3" t="inlineStr">
+        <is>
+          <t>20250725T140736.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="B52" s="1" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="C52" s="1" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="D52" s="2" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="E52" s="2" t="inlineStr">
+        <is>
+          <t>PENNY</t>
+        </is>
+      </c>
+      <c r="F52" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="G52" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H52" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="I52" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="J52" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="K52" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L52" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M52" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N52" s="3" t="inlineStr">
+        <is>
+          <t>20250725T140453.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>LOLA</t>
+        </is>
+      </c>
+      <c r="B53" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="C53" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="D53" s="2" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="E53" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F53" s="2" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="G53" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H53" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="I53" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="J53" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="K53" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="L53" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M53" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="N53" s="3" t="inlineStr">
+        <is>
+          <t>20250725T135834.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>LOLA</t>
+        </is>
+      </c>
+      <c r="B54" s="1" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="C54" s="1" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="D54" s="2" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="E54" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F54" s="2" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="G54" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H54" s="3" t="inlineStr">
+        <is>
+          <t>GEN|cookie</t>
+        </is>
+      </c>
+      <c r="I54" s="3" t="inlineStr">
+        <is>
+          <t>GEN|BONOX2</t>
+        </is>
+      </c>
+      <c r="J54" s="3" t="inlineStr">
+        <is>
+          <t>GEN|Moding</t>
+        </is>
+      </c>
+      <c r="K54" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="L54" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M54" s="3" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="N54" s="3" t="inlineStr">
+        <is>
+          <t>20250725T135659.000Z</t>
         </is>
       </c>
     </row>
@@ -51687,7 +53775,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N51"/>
+  <dimension ref="A3:N58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -55223,6 +57311,510 @@
         </is>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="B52" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="C52" s="1" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="D52" s="2" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E52" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F52" s="2" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="G52" s="5" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H52" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="I52" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="J52" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="K52" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="L52" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M52" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N52" s="3" t="inlineStr">
+        <is>
+          <t>20250725T142527.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>BIBI</t>
+        </is>
+      </c>
+      <c r="B53" s="1" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="C53" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D53" s="2" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="E53" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F53" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="G53" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H53" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="I53" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="J53" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="K53" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="L53" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M53" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N53" s="3" t="inlineStr">
+        <is>
+          <t>20250725T142100.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>BIBI</t>
+        </is>
+      </c>
+      <c r="B54" s="1" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="C54" s="1" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D54" s="2" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="E54" s="2" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F54" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="G54" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H54" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="I54" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="J54" s="3" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="K54" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="L54" s="3" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M54" s="3" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N54" s="3" t="inlineStr">
+        <is>
+          <t>20250725T141916.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="B55" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="C55" s="1" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="D55" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E55" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="F55" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G55" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H55" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I55" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="J55" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="K55" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L55" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="M55" s="3" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="N55" s="3" t="inlineStr">
+        <is>
+          <t>20250725T141705.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="B56" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="C56" s="1" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="D56" s="2" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E56" s="2" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="F56" s="2" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G56" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H56" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I56" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="J56" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="K56" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="L56" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="M56" s="3" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="N56" s="3" t="inlineStr">
+        <is>
+          <t>20250725T141539.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="B57" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C57" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="D57" s="2" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="E57" s="2" t="inlineStr">
+        <is>
+          <t>SAM</t>
+        </is>
+      </c>
+      <c r="F57" s="2" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="G57" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H57" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I57" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J57" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K57" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="L57" s="3" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="M57" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="N57" s="3" t="inlineStr">
+        <is>
+          <t>20250725T141051.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="B58" s="1" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C58" s="1" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="D58" s="2" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="E58" s="2" t="inlineStr">
+        <is>
+          <t>SAM</t>
+        </is>
+      </c>
+      <c r="F58" s="2" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="G58" s="4" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H58" s="3" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I58" s="3" t="inlineStr">
+        <is>
+          <t>RC|Battoman</t>
+        </is>
+      </c>
+      <c r="J58" s="3" t="inlineStr">
+        <is>
+          <t>RC|Shu</t>
+        </is>
+      </c>
+      <c r="K58" s="3" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="L58" s="3" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="M58" s="3" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="N58" s="3" t="inlineStr">
+        <is>
+          <t>20250725T140913.000Z</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-25 17:31:25)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -494,7 +494,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N61"/>
+  <dimension ref="A3:N66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P16" sqref="A4:P16"/>
@@ -4747,6 +4747,366 @@
       <c r="N61" s="10" t="inlineStr">
         <is>
           <t>20250723T233746.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="7" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="B62" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C62" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D62" s="8" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="E62" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F62" s="8" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="G62" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H62" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I62" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J62" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K62" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L62" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="M62" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N62" s="10" t="inlineStr">
+        <is>
+          <t>20250725T151521.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="7" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="B63" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C63" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D63" s="8" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="E63" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F63" s="8" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="G63" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H63" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I63" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J63" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K63" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L63" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="M63" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N63" s="10" t="inlineStr">
+        <is>
+          <t>20250725T151333.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="7" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="B64" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C64" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D64" s="8" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="E64" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F64" s="8" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="G64" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H64" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I64" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J64" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K64" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L64" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="M64" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N64" s="10" t="inlineStr">
+        <is>
+          <t>20250725T151101.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="7" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="B65" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C65" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D65" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E65" s="8" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="F65" s="8" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="G65" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H65" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I65" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J65" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K65" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L65" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="M65" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="N65" s="10" t="inlineStr">
+        <is>
+          <t>20250725T150453.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="7" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="B66" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C66" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D66" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E66" s="8" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="F66" s="8" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="G66" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H66" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I66" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J66" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K66" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L66" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="M66" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="N66" s="10" t="inlineStr">
+        <is>
+          <t>20250725T150208.000Z</t>
         </is>
       </c>
     </row>
@@ -16327,7 +16687,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N55"/>
+  <dimension ref="A3:N59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R30" sqref="R30"/>
@@ -20148,6 +20508,294 @@
       <c r="N55" s="3" t="inlineStr">
         <is>
           <t>20250725T133026.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="7" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="B56" s="7" t="inlineStr">
+        <is>
+          <t>SPROUT</t>
+        </is>
+      </c>
+      <c r="C56" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D56" s="8" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E56" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="F56" s="8" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="G56" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H56" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="I56" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="J56" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="K56" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="L56" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="M56" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="N56" s="10" t="inlineStr">
+        <is>
+          <t>20250725T152526.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="7" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="B57" s="7" t="inlineStr">
+        <is>
+          <t>SPROUT</t>
+        </is>
+      </c>
+      <c r="C57" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D57" s="8" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E57" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="F57" s="8" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="G57" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H57" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="I57" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="J57" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="K57" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="L57" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="M57" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="N57" s="10" t="inlineStr">
+        <is>
+          <t>20250725T152409.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="B58" s="7" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="C58" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="D58" s="8" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="E58" s="8" t="inlineStr">
+        <is>
+          <t>SPROUT</t>
+        </is>
+      </c>
+      <c r="F58" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G58" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H58" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I58" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J58" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K58" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L58" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M58" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N58" s="10" t="inlineStr">
+        <is>
+          <t>20250725T151814.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="B59" s="7" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="C59" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="D59" s="8" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="E59" s="8" t="inlineStr">
+        <is>
+          <t>SPROUT</t>
+        </is>
+      </c>
+      <c r="F59" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G59" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H59" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I59" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J59" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K59" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L59" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M59" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N59" s="10" t="inlineStr">
+        <is>
+          <t>20250725T151644.000Z</t>
         </is>
       </c>
     </row>
@@ -20162,7 +20810,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N65"/>
+  <dimension ref="A3:N69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="T38" sqref="T38"/>
@@ -24703,6 +25351,294 @@
       <c r="N65" s="10" t="inlineStr">
         <is>
           <t>20250725T144633.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="7" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="B66" s="7" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C66" s="7" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="D66" s="8" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="E66" s="8" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="F66" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G66" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H66" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="I66" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="J66" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="K66" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L66" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M66" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N66" s="10" t="inlineStr">
+        <is>
+          <t>20250725T150918.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="7" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="B67" s="7" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C67" s="7" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="D67" s="8" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="E67" s="8" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="F67" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G67" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H67" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="I67" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="J67" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="K67" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L67" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M67" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N67" s="10" t="inlineStr">
+        <is>
+          <t>20250725T150641.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="7" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="B68" s="7" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="C68" s="7" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="D68" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E68" s="8" t="inlineStr">
+        <is>
+          <t>COLETTE</t>
+        </is>
+      </c>
+      <c r="F68" s="8" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="G68" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H68" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I68" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J68" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K68" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L68" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M68" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N68" s="10" t="inlineStr">
+        <is>
+          <t>20250725T150043.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="7" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="B69" s="7" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="C69" s="7" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="D69" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E69" s="8" t="inlineStr">
+        <is>
+          <t>COLETTE</t>
+        </is>
+      </c>
+      <c r="F69" s="8" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="G69" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H69" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I69" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J69" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K69" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L69" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M69" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N69" s="10" t="inlineStr">
+        <is>
+          <t>20250725T145901.000Z</t>
         </is>
       </c>
     </row>
@@ -29992,7 +30928,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N82"/>
+  <dimension ref="A3:N86"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="P25" sqref="A4:P25"/>
@@ -35757,6 +36693,294 @@
       <c r="N82" s="10" t="inlineStr">
         <is>
           <t>20250724T002947.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="7" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="B83" s="7" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C83" s="7" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D83" s="8" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="E83" s="8" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="F83" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G83" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H83" s="10" t="inlineStr">
+        <is>
+          <t>BBO|Adrii</t>
+        </is>
+      </c>
+      <c r="I83" s="10" t="inlineStr">
+        <is>
+          <t>BBO|Bogdan</t>
+        </is>
+      </c>
+      <c r="J83" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Salty</t>
+        </is>
+      </c>
+      <c r="K83" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L83" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M83" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N83" s="10" t="inlineStr">
+        <is>
+          <t>20250725T151340.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="7" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="B84" s="7" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C84" s="7" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D84" s="8" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="E84" s="8" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="F84" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G84" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H84" s="10" t="inlineStr">
+        <is>
+          <t>BBO|Adrii</t>
+        </is>
+      </c>
+      <c r="I84" s="10" t="inlineStr">
+        <is>
+          <t>BBO|Bogdan</t>
+        </is>
+      </c>
+      <c r="J84" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Salty</t>
+        </is>
+      </c>
+      <c r="K84" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L84" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M84" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N84" s="10" t="inlineStr">
+        <is>
+          <t>20250725T151126.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B85" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C85" s="7" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="D85" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E85" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="F85" s="8" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="G85" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H85" s="10" t="inlineStr">
+        <is>
+          <t>Yannic🐀</t>
+        </is>
+      </c>
+      <c r="I85" s="10" t="inlineStr">
+        <is>
+          <t>BBO|Adrii</t>
+        </is>
+      </c>
+      <c r="J85" s="10" t="inlineStr">
+        <is>
+          <t>BBO|Bogdan</t>
+        </is>
+      </c>
+      <c r="K85" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L85" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="M85" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N85" s="10" t="inlineStr">
+        <is>
+          <t>20250725T150543.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B86" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C86" s="7" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="D86" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E86" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="F86" s="8" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="G86" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H86" s="10" t="inlineStr">
+        <is>
+          <t>Yannic🐀</t>
+        </is>
+      </c>
+      <c r="I86" s="10" t="inlineStr">
+        <is>
+          <t>BBO|Adrii</t>
+        </is>
+      </c>
+      <c r="J86" s="10" t="inlineStr">
+        <is>
+          <t>BBO|Bogdan</t>
+        </is>
+      </c>
+      <c r="K86" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L86" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="M86" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N86" s="10" t="inlineStr">
+        <is>
+          <t>20250725T150315.000Z</t>
         </is>
       </c>
     </row>
@@ -35771,7 +36995,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N36"/>
+  <dimension ref="A3:N42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J36" sqref="J36"/>
@@ -38224,6 +39448,438 @@
       <c r="N36" s="10" t="inlineStr">
         <is>
           <t>20250718T233314.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="B37" s="7" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="C37" s="7" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="D37" s="8" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="E37" s="8" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="F37" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G37" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H37" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="I37" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="J37" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="K37" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="L37" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M37" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N37" s="10" t="inlineStr">
+        <is>
+          <t>20250725T150348.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="B38" s="7" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="C38" s="7" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="D38" s="8" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="E38" s="8" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="F38" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G38" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H38" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="I38" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="J38" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="K38" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="L38" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M38" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N38" s="10" t="inlineStr">
+        <is>
+          <t>20250725T150128.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="B39" s="7" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="C39" s="7" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="D39" s="8" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="E39" s="8" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="F39" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G39" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H39" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="I39" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="J39" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="K39" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしてたんぽ👍</t>
+        </is>
+      </c>
+      <c r="L39" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="M39" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="N39" s="10" t="inlineStr">
+        <is>
+          <t>20250725T145944.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="7" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="B40" s="7" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="C40" s="7" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="D40" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E40" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F40" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G40" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H40" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Salty</t>
+        </is>
+      </c>
+      <c r="I40" s="10" t="inlineStr">
+        <is>
+          <t>BBO|Adrii</t>
+        </is>
+      </c>
+      <c r="J40" s="10" t="inlineStr">
+        <is>
+          <t>BBO|Bogdan</t>
+        </is>
+      </c>
+      <c r="K40" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L40" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="M40" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="N40" s="10" t="inlineStr">
+        <is>
+          <t>20250725T152453.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="7" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="B41" s="7" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="C41" s="7" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="D41" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E41" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F41" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G41" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H41" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Salty</t>
+        </is>
+      </c>
+      <c r="I41" s="10" t="inlineStr">
+        <is>
+          <t>BBO|Adrii</t>
+        </is>
+      </c>
+      <c r="J41" s="10" t="inlineStr">
+        <is>
+          <t>BBO|Bogdan</t>
+        </is>
+      </c>
+      <c r="K41" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L41" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="M41" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="N41" s="10" t="inlineStr">
+        <is>
+          <t>20250725T152236.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="7" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="B42" s="7" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="C42" s="7" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="D42" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E42" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F42" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G42" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H42" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Salty</t>
+        </is>
+      </c>
+      <c r="I42" s="10" t="inlineStr">
+        <is>
+          <t>BBO|Adrii</t>
+        </is>
+      </c>
+      <c r="J42" s="10" t="inlineStr">
+        <is>
+          <t>BBO|Bogdan</t>
+        </is>
+      </c>
+      <c r="K42" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L42" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="M42" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="N42" s="10" t="inlineStr">
+        <is>
+          <t>20250725T152016.000Z</t>
         </is>
       </c>
     </row>
@@ -42145,7 +43801,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N51"/>
+  <dimension ref="A3:N54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R15" sqref="R15"/>
@@ -45681,6 +47337,222 @@
         </is>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B52" s="7" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="C52" s="7" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D52" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E52" s="8" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="F52" s="8" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="G52" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H52" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="I52" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="J52" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K52" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L52" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="M52" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="N52" s="10" t="inlineStr">
+        <is>
+          <t>20250725T152510.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B53" s="7" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="C53" s="7" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D53" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E53" s="8" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="F53" s="8" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="G53" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H53" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="I53" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="J53" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K53" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L53" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="M53" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="N53" s="10" t="inlineStr">
+        <is>
+          <t>20250725T152347.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B54" s="7" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="C54" s="7" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D54" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E54" s="8" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="F54" s="8" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="G54" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H54" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="I54" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="J54" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K54" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L54" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="M54" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="N54" s="10" t="inlineStr">
+        <is>
+          <t>20250725T152218.000Z</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-25 18:02:44)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -13140,7 +13140,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N51"/>
+  <dimension ref="A3:N54"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="Q30" sqref="Q30"/>
@@ -16673,6 +16673,222 @@
       <c r="N51" s="10" t="inlineStr">
         <is>
           <t>20250723T235543.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="7" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="B52" s="7" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="C52" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D52" s="8" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="E52" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F52" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G52" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H52" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I52" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J52" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K52" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L52" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M52" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N52" s="10" t="inlineStr">
+        <is>
+          <t>20250725T153816.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="7" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="B53" s="7" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="C53" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D53" s="8" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="E53" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F53" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G53" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H53" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I53" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J53" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K53" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L53" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M53" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N53" s="10" t="inlineStr">
+        <is>
+          <t>20250725T153601.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="7" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="B54" s="7" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="C54" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D54" s="8" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="E54" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F54" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G54" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H54" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="I54" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="J54" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="K54" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L54" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M54" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N54" s="10" t="inlineStr">
+        <is>
+          <t>20250725T153305.000Z</t>
         </is>
       </c>
     </row>
@@ -36995,7 +37211,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N42"/>
+  <dimension ref="A3:N44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J36" sqref="J36"/>
@@ -39880,6 +40096,150 @@
       <c r="N42" s="10" t="inlineStr">
         <is>
           <t>20250725T152016.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="7" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="B43" s="7" t="inlineStr">
+        <is>
+          <t>FANG</t>
+        </is>
+      </c>
+      <c r="C43" s="7" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="D43" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E43" s="8" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="F43" s="8" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="G43" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H43" s="10" t="inlineStr">
+        <is>
+          <t>BBO|Adrii</t>
+        </is>
+      </c>
+      <c r="I43" s="10" t="inlineStr">
+        <is>
+          <t>BBO|Bogdan</t>
+        </is>
+      </c>
+      <c r="J43" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Salty</t>
+        </is>
+      </c>
+      <c r="K43" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L43" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="M43" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="N43" s="10" t="inlineStr">
+        <is>
+          <t>20250725T153419.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="7" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="B44" s="7" t="inlineStr">
+        <is>
+          <t>FANG</t>
+        </is>
+      </c>
+      <c r="C44" s="7" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="D44" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E44" s="8" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="F44" s="8" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="G44" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H44" s="10" t="inlineStr">
+        <is>
+          <t>BBO|Adrii</t>
+        </is>
+      </c>
+      <c r="I44" s="10" t="inlineStr">
+        <is>
+          <t>BBO|Bogdan</t>
+        </is>
+      </c>
+      <c r="J44" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Salty</t>
+        </is>
+      </c>
+      <c r="K44" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L44" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="M44" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="N44" s="10" t="inlineStr">
+        <is>
+          <t>20250725T153158.000Z</t>
         </is>
       </c>
     </row>
@@ -43801,7 +44161,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N54"/>
+  <dimension ref="A3:N56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R15" sqref="R15"/>
@@ -47553,6 +47913,150 @@
         </is>
       </c>
     </row>
+    <row r="55">
+      <c r="A55" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B55" s="7" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="C55" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D55" s="8" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="E55" s="8" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="F55" s="8" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="G55" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H55" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I55" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J55" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K55" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L55" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="M55" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N55" s="10" t="inlineStr">
+        <is>
+          <t>20250725T153226.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B56" s="7" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="C56" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D56" s="8" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="E56" s="8" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="F56" s="8" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="G56" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H56" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I56" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J56" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K56" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="L56" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="M56" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="N56" s="10" t="inlineStr">
+        <is>
+          <t>20250725T153043.000Z</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-25 18:34:04)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -31144,7 +31144,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N86"/>
+  <dimension ref="A3:N92"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="P25" sqref="A4:P25"/>
@@ -37197,6 +37197,438 @@
       <c r="N86" s="10" t="inlineStr">
         <is>
           <t>20250725T150315.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B87" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="C87" s="7" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="D87" s="8" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E87" s="8" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="F87" s="8" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G87" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H87" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I87" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J87" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="K87" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L87" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M87" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N87" s="10" t="inlineStr">
+        <is>
+          <t>20250725T162956.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B88" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="C88" s="7" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="D88" s="8" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E88" s="8" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="F88" s="8" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G88" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H88" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I88" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J88" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="K88" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L88" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M88" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N88" s="10" t="inlineStr">
+        <is>
+          <t>20250725T162725.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="7" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="B89" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C89" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="D89" s="8" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="E89" s="8" t="inlineStr">
+        <is>
+          <t>JACKY</t>
+        </is>
+      </c>
+      <c r="F89" s="8" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="G89" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H89" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="I89" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J89" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="K89" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="L89" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M89" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="N89" s="10" t="inlineStr">
+        <is>
+          <t>20250725T162033.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="7" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="B90" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C90" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="D90" s="8" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="E90" s="8" t="inlineStr">
+        <is>
+          <t>JACKY</t>
+        </is>
+      </c>
+      <c r="F90" s="8" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="G90" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H90" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="I90" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J90" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="K90" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="L90" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M90" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="N90" s="10" t="inlineStr">
+        <is>
+          <t>20250725T161759.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="7" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="B91" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C91" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="D91" s="8" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="E91" s="8" t="inlineStr">
+        <is>
+          <t>JACKY</t>
+        </is>
+      </c>
+      <c r="F91" s="8" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="G91" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H91" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="I91" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J91" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="K91" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="L91" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M91" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="N91" s="10" t="inlineStr">
+        <is>
+          <t>20250725T161548.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B92" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="C92" s="7" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="D92" s="8" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E92" s="8" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="F92" s="8" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G92" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H92" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I92" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J92" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="K92" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L92" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M92" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N92" s="10" t="inlineStr">
+        <is>
+          <t>20250725T163225.000Z</t>
         </is>
       </c>
     </row>
@@ -40254,7 +40686,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N56"/>
+  <dimension ref="A3:N65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P15" sqref="A4:P15"/>
@@ -44147,6 +44579,654 @@
       <c r="N56" s="10" t="inlineStr">
         <is>
           <t>20250724T013157.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B57" s="7" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C57" s="7" t="inlineStr">
+        <is>
+          <t>8-BIT</t>
+        </is>
+      </c>
+      <c r="D57" s="8" t="inlineStr">
+        <is>
+          <t>POCO</t>
+        </is>
+      </c>
+      <c r="E57" s="8" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="F57" s="8" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G57" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H57" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I57" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="J57" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K57" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L57" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="M57" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="N57" s="10" t="inlineStr">
+        <is>
+          <t>20250725T163036.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B58" s="7" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C58" s="7" t="inlineStr">
+        <is>
+          <t>8-BIT</t>
+        </is>
+      </c>
+      <c r="D58" s="8" t="inlineStr">
+        <is>
+          <t>POCO</t>
+        </is>
+      </c>
+      <c r="E58" s="8" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="F58" s="8" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G58" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H58" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I58" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="J58" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K58" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L58" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="M58" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="N58" s="10" t="inlineStr">
+        <is>
+          <t>20250725T162852.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B59" s="7" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="C59" s="7" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D59" s="8" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E59" s="8" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="F59" s="8" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="G59" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H59" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="I59" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="J59" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="K59" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="L59" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="M59" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="N59" s="10" t="inlineStr">
+        <is>
+          <t>20250725T162258.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B60" s="7" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="C60" s="7" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="D60" s="8" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E60" s="8" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="F60" s="8" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="G60" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H60" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I60" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="J60" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K60" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L60" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M60" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N60" s="10" t="inlineStr">
+        <is>
+          <t>20250725T162013.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B61" s="7" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="C61" s="7" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="D61" s="8" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E61" s="8" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="F61" s="8" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="G61" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H61" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I61" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="J61" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K61" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L61" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M61" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N61" s="10" t="inlineStr">
+        <is>
+          <t>20250725T161805.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="B62" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C62" s="7" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="D62" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="E62" s="8" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="F62" s="8" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="G62" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H62" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="I62" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="J62" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="K62" s="10" t="inlineStr">
+        <is>
+          <t>Bielz</t>
+        </is>
+      </c>
+      <c r="L62" s="10" t="inlineStr">
+        <is>
+          <t>Tilo🍥</t>
+        </is>
+      </c>
+      <c r="M62" s="10" t="inlineStr">
+        <is>
+          <t>GO|Yichy❦</t>
+        </is>
+      </c>
+      <c r="N62" s="10" t="inlineStr">
+        <is>
+          <t>20250725T162724.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="B63" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C63" s="7" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="D63" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="E63" s="8" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="F63" s="8" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="G63" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H63" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="I63" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="J63" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="K63" s="10" t="inlineStr">
+        <is>
+          <t>Bielz</t>
+        </is>
+      </c>
+      <c r="L63" s="10" t="inlineStr">
+        <is>
+          <t>Tilo🍥</t>
+        </is>
+      </c>
+      <c r="M63" s="10" t="inlineStr">
+        <is>
+          <t>GO|Yichy❦</t>
+        </is>
+      </c>
+      <c r="N63" s="10" t="inlineStr">
+        <is>
+          <t>20250725T162518.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B64" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C64" s="7" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D64" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="E64" s="8" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="F64" s="8" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="G64" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H64" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="I64" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="J64" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="K64" s="10" t="inlineStr">
+        <is>
+          <t>GO|Yichy❦</t>
+        </is>
+      </c>
+      <c r="L64" s="10" t="inlineStr">
+        <is>
+          <t>Tilo🍥</t>
+        </is>
+      </c>
+      <c r="M64" s="10" t="inlineStr">
+        <is>
+          <t>Bielz</t>
+        </is>
+      </c>
+      <c r="N64" s="10" t="inlineStr">
+        <is>
+          <t>20250725T161912.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B65" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C65" s="7" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D65" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="E65" s="8" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="F65" s="8" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="G65" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H65" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="I65" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="J65" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="K65" s="10" t="inlineStr">
+        <is>
+          <t>GO|Yichy❦</t>
+        </is>
+      </c>
+      <c r="L65" s="10" t="inlineStr">
+        <is>
+          <t>Tilo🍥</t>
+        </is>
+      </c>
+      <c r="M65" s="10" t="inlineStr">
+        <is>
+          <t>Bielz</t>
+        </is>
+      </c>
+      <c r="N65" s="10" t="inlineStr">
+        <is>
+          <t>20250725T161652.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-25 19:05:24)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -50,7 +50,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill/>
     </fill>
@@ -80,6 +80,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00F4CCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D9D9D9"/>
       </patternFill>
     </fill>
   </fills>
@@ -116,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -129,6 +134,7 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,7 +500,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N66"/>
+  <dimension ref="A3:N69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P16" sqref="A4:P16"/>
@@ -5107,6 +5113,222 @@
       <c r="N66" s="10" t="inlineStr">
         <is>
           <t>20250725T150208.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="7" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="B67" s="7" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="C67" s="7" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="D67" s="8" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E67" s="8" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="F67" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G67" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H67" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I67" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="J67" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K67" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L67" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M67" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N67" s="10" t="inlineStr">
+        <is>
+          <t>20250725T170154.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B68" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="C68" s="7" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="D68" s="8" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="E68" s="8" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="F68" s="8" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G68" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H68" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I68" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="J68" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="K68" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="L68" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="M68" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="N68" s="10" t="inlineStr">
+        <is>
+          <t>20250725T165519.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B69" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="C69" s="7" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="D69" s="8" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="E69" s="8" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="F69" s="8" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G69" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H69" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I69" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="J69" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="K69" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="L69" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="M69" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="N69" s="10" t="inlineStr">
+        <is>
+          <t>20250725T165324.000Z</t>
         </is>
       </c>
     </row>
@@ -5121,7 +5343,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N11"/>
+  <dimension ref="A3:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P7" sqref="A4:P7"/>
@@ -5774,6 +5996,438 @@
       <c r="N11" s="3" t="inlineStr">
         <is>
           <t>20250725T122303.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D12" s="8" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="E12" s="8" t="inlineStr">
+        <is>
+          <t>CHESTER</t>
+        </is>
+      </c>
+      <c r="F12" s="8" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="G12" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H12" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="I12" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="J12" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="K12" s="10" t="inlineStr">
+        <is>
+          <t>Bielz</t>
+        </is>
+      </c>
+      <c r="L12" s="10" t="inlineStr">
+        <is>
+          <t>GO|Yichy❦</t>
+        </is>
+      </c>
+      <c r="M12" s="10" t="inlineStr">
+        <is>
+          <t>Tilo🍥</t>
+        </is>
+      </c>
+      <c r="N12" s="10" t="inlineStr">
+        <is>
+          <t>20250725T165057.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D13" s="8" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="E13" s="8" t="inlineStr">
+        <is>
+          <t>CHESTER</t>
+        </is>
+      </c>
+      <c r="F13" s="8" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="G13" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H13" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="I13" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="J13" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="K13" s="10" t="inlineStr">
+        <is>
+          <t>Bielz</t>
+        </is>
+      </c>
+      <c r="L13" s="10" t="inlineStr">
+        <is>
+          <t>GO|Yichy❦</t>
+        </is>
+      </c>
+      <c r="M13" s="10" t="inlineStr">
+        <is>
+          <t>Tilo🍥</t>
+        </is>
+      </c>
+      <c r="N13" s="10" t="inlineStr">
+        <is>
+          <t>20250725T164844.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B14" s="7" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="C14" s="7" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D14" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="E14" s="8" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="F14" s="8" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="G14" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H14" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="I14" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="J14" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="K14" s="10" t="inlineStr">
+        <is>
+          <t>Bielz</t>
+        </is>
+      </c>
+      <c r="L14" s="10" t="inlineStr">
+        <is>
+          <t>Tilo🍥</t>
+        </is>
+      </c>
+      <c r="M14" s="10" t="inlineStr">
+        <is>
+          <t>GO|Yichy❦</t>
+        </is>
+      </c>
+      <c r="N14" s="10" t="inlineStr">
+        <is>
+          <t>20250725T164220.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B15" s="7" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="C15" s="7" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D15" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="E15" s="8" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="F15" s="8" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="G15" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H15" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="I15" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="J15" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="K15" s="10" t="inlineStr">
+        <is>
+          <t>Bielz</t>
+        </is>
+      </c>
+      <c r="L15" s="10" t="inlineStr">
+        <is>
+          <t>Tilo🍥</t>
+        </is>
+      </c>
+      <c r="M15" s="10" t="inlineStr">
+        <is>
+          <t>GO|Yichy❦</t>
+        </is>
+      </c>
+      <c r="N15" s="10" t="inlineStr">
+        <is>
+          <t>20250725T164014.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B16" s="7" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="C16" s="7" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D16" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="E16" s="8" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="F16" s="8" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="G16" s="12" t="inlineStr">
+        <is>
+          <t>Empate</t>
+        </is>
+      </c>
+      <c r="H16" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="I16" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="J16" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="K16" s="10" t="inlineStr">
+        <is>
+          <t>Bielz</t>
+        </is>
+      </c>
+      <c r="L16" s="10" t="inlineStr">
+        <is>
+          <t>Tilo🍥</t>
+        </is>
+      </c>
+      <c r="M16" s="10" t="inlineStr">
+        <is>
+          <t>GO|Yichy❦</t>
+        </is>
+      </c>
+      <c r="N16" s="10" t="inlineStr">
+        <is>
+          <t>20250725T163753.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B17" s="7" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="C17" s="7" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="D17" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="E17" s="8" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="F17" s="8" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="G17" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H17" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="I17" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="J17" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="K17" s="10" t="inlineStr">
+        <is>
+          <t>Bielz</t>
+        </is>
+      </c>
+      <c r="L17" s="10" t="inlineStr">
+        <is>
+          <t>Tilo🍥</t>
+        </is>
+      </c>
+      <c r="M17" s="10" t="inlineStr">
+        <is>
+          <t>GO|Yichy❦</t>
+        </is>
+      </c>
+      <c r="N17" s="10" t="inlineStr">
+        <is>
+          <t>20250725T163402.000Z</t>
         </is>
       </c>
     </row>
@@ -21026,7 +21680,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N69"/>
+  <dimension ref="A3:N74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="T38" sqref="T38"/>
@@ -25855,6 +26509,366 @@
       <c r="N69" s="10" t="inlineStr">
         <is>
           <t>20250725T145901.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B70" s="7" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="C70" s="7" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="D70" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E70" s="8" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="F70" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G70" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H70" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I70" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J70" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="K70" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="L70" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M70" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="N70" s="10" t="inlineStr">
+        <is>
+          <t>20250725T170221.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="7" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="B71" s="7" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="C71" s="7" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D71" s="8" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E71" s="8" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="F71" s="8" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="G71" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H71" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I71" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J71" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="K71" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L71" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M71" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N71" s="10" t="inlineStr">
+        <is>
+          <t>20250725T165545.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="7" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="B72" s="7" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="C72" s="7" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D72" s="8" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E72" s="8" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="F72" s="8" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="G72" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H72" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I72" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J72" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="K72" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L72" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M72" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N72" s="10" t="inlineStr">
+        <is>
+          <t>20250725T165430.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="7" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="B73" s="7" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="C73" s="7" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D73" s="8" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E73" s="8" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="F73" s="8" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="G73" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H73" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I73" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J73" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="K73" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L73" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M73" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N73" s="10" t="inlineStr">
+        <is>
+          <t>20250725T165301.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B74" s="7" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="C74" s="7" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="D74" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E74" s="8" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="F74" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G74" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H74" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I74" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J74" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="K74" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="L74" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M74" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="N74" s="10" t="inlineStr">
+        <is>
+          <t>20250725T170407.000Z</t>
         </is>
       </c>
     </row>
@@ -25869,7 +26883,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N75"/>
+  <dimension ref="A3:N79"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="P38" sqref="P38"/>
@@ -31130,6 +32144,294 @@
       <c r="N75" s="10" t="inlineStr">
         <is>
           <t>20250725T143229.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="7" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="B76" s="7" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="C76" s="7" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="D76" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E76" s="8" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="F76" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G76" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H76" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="I76" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="J76" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="K76" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L76" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M76" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N76" s="10" t="inlineStr">
+        <is>
+          <t>20250725T164827.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="7" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="B77" s="7" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="C77" s="7" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="D77" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E77" s="8" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="F77" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G77" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H77" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="I77" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="J77" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="K77" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L77" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M77" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N77" s="10" t="inlineStr">
+        <is>
+          <t>20250725T164620.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B78" s="7" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="C78" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="D78" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E78" s="8" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="F78" s="8" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="G78" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H78" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I78" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J78" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="K78" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L78" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M78" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N78" s="10" t="inlineStr">
+        <is>
+          <t>20250725T163953.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B79" s="7" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="C79" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="D79" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E79" s="8" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="F79" s="8" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="G79" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H79" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I79" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J79" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="K79" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L79" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M79" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N79" s="10" t="inlineStr">
+        <is>
+          <t>20250725T163806.000Z</t>
         </is>
       </c>
     </row>
@@ -37643,7 +38945,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N44"/>
+  <dimension ref="A3:N46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J36" sqref="J36"/>
@@ -40672,6 +41974,150 @@
       <c r="N44" s="10" t="inlineStr">
         <is>
           <t>20250725T153158.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="7" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B45" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="C45" s="7" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="D45" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="E45" s="8" t="inlineStr">
+        <is>
+          <t>MAX</t>
+        </is>
+      </c>
+      <c r="F45" s="8" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="G45" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H45" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="I45" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="J45" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="K45" s="10" t="inlineStr">
+        <is>
+          <t>Bielz</t>
+        </is>
+      </c>
+      <c r="L45" s="10" t="inlineStr">
+        <is>
+          <t>Tilo🍥</t>
+        </is>
+      </c>
+      <c r="M45" s="10" t="inlineStr">
+        <is>
+          <t>GO|Yichy❦</t>
+        </is>
+      </c>
+      <c r="N45" s="10" t="inlineStr">
+        <is>
+          <t>20250725T170152.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="7" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B46" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="C46" s="7" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="D46" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="E46" s="8" t="inlineStr">
+        <is>
+          <t>MAX</t>
+        </is>
+      </c>
+      <c r="F46" s="8" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="G46" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H46" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="I46" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="J46" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="K46" s="10" t="inlineStr">
+        <is>
+          <t>Bielz</t>
+        </is>
+      </c>
+      <c r="L46" s="10" t="inlineStr">
+        <is>
+          <t>Tilo🍥</t>
+        </is>
+      </c>
+      <c r="M46" s="10" t="inlineStr">
+        <is>
+          <t>GO|Yichy❦</t>
+        </is>
+      </c>
+      <c r="N46" s="10" t="inlineStr">
+        <is>
+          <t>20250725T165931.000Z</t>
         </is>
       </c>
     </row>
@@ -45241,7 +46687,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N56"/>
+  <dimension ref="A3:N62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R15" sqref="R15"/>
@@ -49137,6 +50583,438 @@
         </is>
       </c>
     </row>
+    <row r="57">
+      <c r="A57" s="7" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="B57" s="7" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="C57" s="7" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D57" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E57" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F57" s="8" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="G57" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H57" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="I57" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="J57" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="K57" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L57" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="M57" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="N57" s="10" t="inlineStr">
+        <is>
+          <t>20250725T164737.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="7" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="B58" s="7" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="C58" s="7" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D58" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E58" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F58" s="8" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="G58" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H58" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="I58" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="J58" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="K58" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L58" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="M58" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="N58" s="10" t="inlineStr">
+        <is>
+          <t>20250725T164601.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="7" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="B59" s="7" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="C59" s="7" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D59" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E59" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F59" s="8" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="G59" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H59" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="I59" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="J59" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="K59" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L59" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="M59" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="N59" s="10" t="inlineStr">
+        <is>
+          <t>20250725T164442.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="7" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="B60" s="7" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="C60" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D60" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E60" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F60" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G60" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H60" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I60" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="J60" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K60" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L60" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="M60" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N60" s="10" t="inlineStr">
+        <is>
+          <t>20250725T164035.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="7" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="B61" s="7" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="C61" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D61" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E61" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F61" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G61" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H61" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I61" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="J61" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K61" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L61" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="M61" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N61" s="10" t="inlineStr">
+        <is>
+          <t>20250725T163830.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="7" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="B62" s="7" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="C62" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D62" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E62" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F62" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G62" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H62" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I62" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="J62" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K62" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L62" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="M62" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N62" s="10" t="inlineStr">
+        <is>
+          <t>20250725T163617.000Z</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-25 19:36:43)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -500,7 +500,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N69"/>
+  <dimension ref="A3:N76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P16" sqref="A4:P16"/>
@@ -5329,6 +5329,510 @@
       <c r="N69" s="10" t="inlineStr">
         <is>
           <t>20250725T165324.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="B70" s="7" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="C70" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D70" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E70" s="8" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F70" s="8" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="G70" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H70" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I70" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="J70" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K70" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L70" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M70" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="N70" s="10" t="inlineStr">
+        <is>
+          <t>20250725T173454.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="B71" s="7" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="C71" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D71" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E71" s="8" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F71" s="8" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="G71" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H71" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I71" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="J71" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K71" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L71" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M71" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="N71" s="10" t="inlineStr">
+        <is>
+          <t>20250725T173227.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="7" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="B72" s="7" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="C72" s="7" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="D72" s="8" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E72" s="8" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="F72" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G72" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H72" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I72" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="J72" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K72" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L72" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M72" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N72" s="10" t="inlineStr">
+        <is>
+          <t>20250725T170828.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="7" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="B73" s="7" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="C73" s="7" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="D73" s="8" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E73" s="8" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="F73" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G73" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H73" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I73" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="J73" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K73" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L73" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M73" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="N73" s="10" t="inlineStr">
+        <is>
+          <t>20250725T170444.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B74" s="7" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="C74" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D74" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E74" s="8" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="F74" s="8" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="G74" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H74" s="10" t="inlineStr">
+        <is>
+          <t>Jus</t>
+        </is>
+      </c>
+      <c r="I74" s="10" t="inlineStr">
+        <is>
+          <t>KDS|Remica</t>
+        </is>
+      </c>
+      <c r="J74" s="10" t="inlineStr">
+        <is>
+          <t>A 🤍</t>
+        </is>
+      </c>
+      <c r="K74" s="10" t="inlineStr">
+        <is>
+          <t>Yannic🐀</t>
+        </is>
+      </c>
+      <c r="L74" s="10" t="inlineStr">
+        <is>
+          <t>KDS|치로🩵</t>
+        </is>
+      </c>
+      <c r="M74" s="10" t="inlineStr">
+        <is>
+          <t>CoVeRzZz 🐀</t>
+        </is>
+      </c>
+      <c r="N74" s="10" t="inlineStr">
+        <is>
+          <t>20250725T170956.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B75" s="7" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="C75" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D75" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E75" s="8" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="F75" s="8" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="G75" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H75" s="10" t="inlineStr">
+        <is>
+          <t>Jus</t>
+        </is>
+      </c>
+      <c r="I75" s="10" t="inlineStr">
+        <is>
+          <t>KDS|Remica</t>
+        </is>
+      </c>
+      <c r="J75" s="10" t="inlineStr">
+        <is>
+          <t>A 🤍</t>
+        </is>
+      </c>
+      <c r="K75" s="10" t="inlineStr">
+        <is>
+          <t>Yannic🐀</t>
+        </is>
+      </c>
+      <c r="L75" s="10" t="inlineStr">
+        <is>
+          <t>KDS|치로🩵</t>
+        </is>
+      </c>
+      <c r="M75" s="10" t="inlineStr">
+        <is>
+          <t>CoVeRzZz 🐀</t>
+        </is>
+      </c>
+      <c r="N75" s="10" t="inlineStr">
+        <is>
+          <t>20250725T170729.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="7" t="inlineStr">
+        <is>
+          <t>JACKY</t>
+        </is>
+      </c>
+      <c r="B76" s="7" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="C76" s="7" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="D76" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="E76" s="8" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="F76" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G76" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H76" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="I76" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="J76" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="K76" s="10" t="inlineStr">
+        <is>
+          <t>Bielz</t>
+        </is>
+      </c>
+      <c r="L76" s="10" t="inlineStr">
+        <is>
+          <t>Tilo🍥</t>
+        </is>
+      </c>
+      <c r="M76" s="10" t="inlineStr">
+        <is>
+          <t>GO|Yichy❦</t>
+        </is>
+      </c>
+      <c r="N76" s="10" t="inlineStr">
+        <is>
+          <t>20250725T173509.000Z</t>
         </is>
       </c>
     </row>
@@ -9758,7 +10262,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N14"/>
+  <dimension ref="A3:N18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
@@ -10627,6 +11131,294 @@
       <c r="N14" s="10" t="inlineStr">
         <is>
           <t>20250718T234259.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="7" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="B15" s="7" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="C15" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="D15" s="8" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="E15" s="8" t="inlineStr">
+        <is>
+          <t>PIPER</t>
+        </is>
+      </c>
+      <c r="F15" s="8" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="G15" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H15" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="I15" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="J15" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="K15" s="10" t="inlineStr">
+        <is>
+          <t>Bielz</t>
+        </is>
+      </c>
+      <c r="L15" s="10" t="inlineStr">
+        <is>
+          <t>Tilo🍥</t>
+        </is>
+      </c>
+      <c r="M15" s="10" t="inlineStr">
+        <is>
+          <t>GO|Yichy❦</t>
+        </is>
+      </c>
+      <c r="N15" s="10" t="inlineStr">
+        <is>
+          <t>20250725T172937.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="7" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="B16" s="7" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="C16" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="D16" s="8" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="E16" s="8" t="inlineStr">
+        <is>
+          <t>PIPER</t>
+        </is>
+      </c>
+      <c r="F16" s="8" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="G16" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H16" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="I16" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="J16" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="K16" s="10" t="inlineStr">
+        <is>
+          <t>Bielz</t>
+        </is>
+      </c>
+      <c r="L16" s="10" t="inlineStr">
+        <is>
+          <t>Tilo🍥</t>
+        </is>
+      </c>
+      <c r="M16" s="10" t="inlineStr">
+        <is>
+          <t>GO|Yichy❦</t>
+        </is>
+      </c>
+      <c r="N16" s="10" t="inlineStr">
+        <is>
+          <t>20250725T172751.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="7" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="B17" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C17" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="D17" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E17" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F17" s="8" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="G17" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H17" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="I17" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="J17" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="K17" s="10" t="inlineStr">
+        <is>
+          <t>Tilo🍥</t>
+        </is>
+      </c>
+      <c r="L17" s="10" t="inlineStr">
+        <is>
+          <t>GO|Yichy❦</t>
+        </is>
+      </c>
+      <c r="M17" s="10" t="inlineStr">
+        <is>
+          <t>Bielz</t>
+        </is>
+      </c>
+      <c r="N17" s="10" t="inlineStr">
+        <is>
+          <t>20250725T172054.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="7" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="B18" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C18" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="D18" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E18" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F18" s="8" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="G18" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H18" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="I18" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="J18" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="K18" s="10" t="inlineStr">
+        <is>
+          <t>Tilo🍥</t>
+        </is>
+      </c>
+      <c r="L18" s="10" t="inlineStr">
+        <is>
+          <t>GO|Yichy❦</t>
+        </is>
+      </c>
+      <c r="M18" s="10" t="inlineStr">
+        <is>
+          <t>Bielz</t>
+        </is>
+      </c>
+      <c r="N18" s="10" t="inlineStr">
+        <is>
+          <t>20250725T171843.000Z</t>
         </is>
       </c>
     </row>
@@ -12767,7 +13559,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N16"/>
+  <dimension ref="A3:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="S12" sqref="S12"/>
@@ -13780,6 +14572,150 @@
       <c r="N16" s="3" t="inlineStr">
         <is>
           <t>20250725T133038.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="7" t="inlineStr">
+        <is>
+          <t>PEARL</t>
+        </is>
+      </c>
+      <c r="B17" s="7" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="C17" s="7" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="D17" s="8" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="E17" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="F17" s="8" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="G17" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H17" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I17" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="J17" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K17" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L17" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="M17" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="N17" s="10" t="inlineStr">
+        <is>
+          <t>20250725T173140.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="7" t="inlineStr">
+        <is>
+          <t>PEARL</t>
+        </is>
+      </c>
+      <c r="B18" s="7" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="C18" s="7" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="D18" s="8" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="E18" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="F18" s="8" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="G18" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H18" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I18" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="J18" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K18" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L18" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="M18" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="N18" s="10" t="inlineStr">
+        <is>
+          <t>20250725T173000.000Z</t>
         </is>
       </c>
     </row>
@@ -17557,7 +18493,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N59"/>
+  <dimension ref="A3:N64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R30" sqref="R30"/>
@@ -21666,6 +22602,366 @@
       <c r="N59" s="10" t="inlineStr">
         <is>
           <t>20250725T151644.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B60" s="7" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C60" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D60" s="8" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="E60" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="F60" s="8" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="G60" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H60" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I60" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J60" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="K60" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L60" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M60" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="N60" s="10" t="inlineStr">
+        <is>
+          <t>20250725T172714.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B61" s="7" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C61" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D61" s="8" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="E61" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="F61" s="8" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="G61" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H61" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I61" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J61" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="K61" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L61" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M61" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="N61" s="10" t="inlineStr">
+        <is>
+          <t>20250725T172537.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B62" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C62" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="D62" s="8" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="E62" s="8" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="F62" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G62" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H62" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="I62" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="J62" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="K62" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L62" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M62" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N62" s="10" t="inlineStr">
+        <is>
+          <t>20250725T171821.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B63" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C63" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="D63" s="8" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="E63" s="8" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="F63" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G63" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H63" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="I63" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="J63" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="K63" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L63" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M63" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N63" s="10" t="inlineStr">
+        <is>
+          <t>20250725T171448.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B64" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C64" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="D64" s="8" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="E64" s="8" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="F64" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G64" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H64" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="I64" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="J64" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="K64" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L64" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M64" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N64" s="10" t="inlineStr">
+        <is>
+          <t>20250725T171208.000Z</t>
         </is>
       </c>
     </row>
@@ -38945,7 +40241,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N46"/>
+  <dimension ref="A3:N53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J36" sqref="J36"/>
@@ -42118,6 +43414,510 @@
       <c r="N46" s="10" t="inlineStr">
         <is>
           <t>20250725T165931.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="7" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="B47" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C47" s="7" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="D47" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E47" s="8" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="F47" s="8" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="G47" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H47" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I47" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="J47" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K47" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L47" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="M47" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="N47" s="10" t="inlineStr">
+        <is>
+          <t>20250725T172404.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="7" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="B48" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C48" s="7" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="D48" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E48" s="8" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="F48" s="8" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="G48" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H48" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I48" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="J48" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K48" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="L48" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="M48" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="N48" s="10" t="inlineStr">
+        <is>
+          <t>20250725T172144.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B49" s="7" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="C49" s="7" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="D49" s="8" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="E49" s="8" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="F49" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G49" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H49" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I49" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="J49" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K49" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="L49" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="M49" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="N49" s="10" t="inlineStr">
+        <is>
+          <t>20250725T171631.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B50" s="7" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="C50" s="7" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="D50" s="8" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="E50" s="8" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="F50" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G50" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H50" s="10" t="inlineStr">
+        <is>
+          <t>TH|LeNain</t>
+        </is>
+      </c>
+      <c r="I50" s="10" t="inlineStr">
+        <is>
+          <t>TH|iKaoss</t>
+        </is>
+      </c>
+      <c r="J50" s="10" t="inlineStr">
+        <is>
+          <t>TH|Zhar</t>
+        </is>
+      </c>
+      <c r="K50" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="L50" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="M50" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="N50" s="10" t="inlineStr">
+        <is>
+          <t>20250725T171411.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="B51" s="7" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="C51" s="7" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="D51" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E51" s="8" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="F51" s="8" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="G51" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H51" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="I51" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="J51" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="K51" s="10" t="inlineStr">
+        <is>
+          <t>Tilo🍥</t>
+        </is>
+      </c>
+      <c r="L51" s="10" t="inlineStr">
+        <is>
+          <t>Bielz</t>
+        </is>
+      </c>
+      <c r="M51" s="10" t="inlineStr">
+        <is>
+          <t>GO|Yichy❦</t>
+        </is>
+      </c>
+      <c r="N51" s="10" t="inlineStr">
+        <is>
+          <t>20250725T171250.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="B52" s="7" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="C52" s="7" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="D52" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E52" s="8" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="F52" s="8" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="G52" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H52" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="I52" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="J52" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="K52" s="10" t="inlineStr">
+        <is>
+          <t>Tilo🍥</t>
+        </is>
+      </c>
+      <c r="L52" s="10" t="inlineStr">
+        <is>
+          <t>Bielz</t>
+        </is>
+      </c>
+      <c r="M52" s="10" t="inlineStr">
+        <is>
+          <t>GO|Yichy❦</t>
+        </is>
+      </c>
+      <c r="N52" s="10" t="inlineStr">
+        <is>
+          <t>20250725T171037.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="B53" s="7" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="C53" s="7" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="D53" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E53" s="8" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="F53" s="8" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="G53" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H53" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="I53" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="J53" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="K53" s="10" t="inlineStr">
+        <is>
+          <t>Tilo🍥</t>
+        </is>
+      </c>
+      <c r="L53" s="10" t="inlineStr">
+        <is>
+          <t>Bielz</t>
+        </is>
+      </c>
+      <c r="M53" s="10" t="inlineStr">
+        <is>
+          <t>GO|Yichy❦</t>
+        </is>
+      </c>
+      <c r="N53" s="10" t="inlineStr">
+        <is>
+          <t>20250725T170819.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-25 20:08:03)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -500,7 +500,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N76"/>
+  <dimension ref="A3:N84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P16" sqref="A4:P16"/>
@@ -5833,6 +5833,582 @@
       <c r="N76" s="10" t="inlineStr">
         <is>
           <t>20250725T173509.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="7" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="B77" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C77" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D77" s="8" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E77" s="8" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="F77" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G77" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H77" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I77" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="J77" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K77" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L77" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M77" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N77" s="10" t="inlineStr">
+        <is>
+          <t>20250725T174703.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="7" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="B78" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C78" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D78" s="8" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E78" s="8" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="F78" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G78" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H78" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I78" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="J78" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K78" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L78" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M78" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N78" s="10" t="inlineStr">
+        <is>
+          <t>20250725T174520.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="7" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="B79" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C79" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D79" s="8" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E79" s="8" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="F79" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G79" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H79" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I79" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="J79" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K79" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L79" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M79" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N79" s="10" t="inlineStr">
+        <is>
+          <t>20250725T174143.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B80" s="7" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="C80" s="7" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="D80" s="8" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="E80" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F80" s="8" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="G80" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H80" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="I80" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="J80" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="K80" s="10" t="inlineStr">
+        <is>
+          <t>Bielz</t>
+        </is>
+      </c>
+      <c r="L80" s="10" t="inlineStr">
+        <is>
+          <t>GO|Yichy❦</t>
+        </is>
+      </c>
+      <c r="M80" s="10" t="inlineStr">
+        <is>
+          <t>Tilo🍥</t>
+        </is>
+      </c>
+      <c r="N80" s="10" t="inlineStr">
+        <is>
+          <t>20250725T175130.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B81" s="7" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="C81" s="7" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="D81" s="8" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="E81" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F81" s="8" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="G81" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H81" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="I81" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="J81" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="K81" s="10" t="inlineStr">
+        <is>
+          <t>Bielz</t>
+        </is>
+      </c>
+      <c r="L81" s="10" t="inlineStr">
+        <is>
+          <t>GO|Yichy❦</t>
+        </is>
+      </c>
+      <c r="M81" s="10" t="inlineStr">
+        <is>
+          <t>Tilo🍥</t>
+        </is>
+      </c>
+      <c r="N81" s="10" t="inlineStr">
+        <is>
+          <t>20250725T174908.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B82" s="7" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="C82" s="7" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="D82" s="8" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="E82" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F82" s="8" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="G82" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H82" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="I82" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="J82" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="K82" s="10" t="inlineStr">
+        <is>
+          <t>Bielz</t>
+        </is>
+      </c>
+      <c r="L82" s="10" t="inlineStr">
+        <is>
+          <t>GO|Yichy❦</t>
+        </is>
+      </c>
+      <c r="M82" s="10" t="inlineStr">
+        <is>
+          <t>Tilo🍥</t>
+        </is>
+      </c>
+      <c r="N82" s="10" t="inlineStr">
+        <is>
+          <t>20250725T174655.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="7" t="inlineStr">
+        <is>
+          <t>JACKY</t>
+        </is>
+      </c>
+      <c r="B83" s="7" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="C83" s="7" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="D83" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="E83" s="8" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="F83" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G83" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H83" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="I83" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="J83" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="K83" s="10" t="inlineStr">
+        <is>
+          <t>Bielz</t>
+        </is>
+      </c>
+      <c r="L83" s="10" t="inlineStr">
+        <is>
+          <t>Tilo🍥</t>
+        </is>
+      </c>
+      <c r="M83" s="10" t="inlineStr">
+        <is>
+          <t>GO|Yichy❦</t>
+        </is>
+      </c>
+      <c r="N83" s="10" t="inlineStr">
+        <is>
+          <t>20250725T174051.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="7" t="inlineStr">
+        <is>
+          <t>JACKY</t>
+        </is>
+      </c>
+      <c r="B84" s="7" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="C84" s="7" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="D84" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="E84" s="8" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="F84" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G84" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H84" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="I84" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="J84" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="K84" s="10" t="inlineStr">
+        <is>
+          <t>Bielz</t>
+        </is>
+      </c>
+      <c r="L84" s="10" t="inlineStr">
+        <is>
+          <t>Tilo🍥</t>
+        </is>
+      </c>
+      <c r="M84" s="10" t="inlineStr">
+        <is>
+          <t>GO|Yichy❦</t>
+        </is>
+      </c>
+      <c r="N84" s="10" t="inlineStr">
+        <is>
+          <t>20250725T173759.000Z</t>
         </is>
       </c>
     </row>
@@ -43932,7 +44508,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N65"/>
+  <dimension ref="A3:N67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P15" sqref="A4:P15"/>
@@ -48473,6 +49049,150 @@
       <c r="N65" s="10" t="inlineStr">
         <is>
           <t>20250725T161652.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="7" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="B66" s="7" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="C66" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="D66" s="8" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="E66" s="8" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="F66" s="8" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="G66" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H66" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I66" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="J66" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K66" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L66" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M66" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N66" s="10" t="inlineStr">
+        <is>
+          <t>20250725T175704.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="7" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="B67" s="7" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="C67" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="D67" s="8" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="E67" s="8" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="F67" s="8" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="G67" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H67" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I67" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="J67" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K67" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L67" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="M67" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="N67" s="10" t="inlineStr">
+        <is>
+          <t>20250725T175410.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-25 20:39:26)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -44508,7 +44508,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N67"/>
+  <dimension ref="A3:N73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P15" sqref="A4:P15"/>
@@ -49193,6 +49193,438 @@
       <c r="N67" s="10" t="inlineStr">
         <is>
           <t>20250725T175410.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B68" s="7" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C68" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D68" s="8" t="inlineStr">
+        <is>
+          <t>JESSIE</t>
+        </is>
+      </c>
+      <c r="E68" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="F68" s="8" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="G68" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H68" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I68" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J68" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="K68" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L68" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M68" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="N68" s="10" t="inlineStr">
+        <is>
+          <t>20250725T181128.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B69" s="7" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C69" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D69" s="8" t="inlineStr">
+        <is>
+          <t>JESSIE</t>
+        </is>
+      </c>
+      <c r="E69" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="F69" s="8" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="G69" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H69" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I69" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J69" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="K69" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L69" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M69" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="N69" s="10" t="inlineStr">
+        <is>
+          <t>20250725T180936.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B70" s="7" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C70" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D70" s="8" t="inlineStr">
+        <is>
+          <t>JESSIE</t>
+        </is>
+      </c>
+      <c r="E70" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="F70" s="8" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="G70" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H70" s="10" t="inlineStr">
+        <is>
+          <t>IC|Mebius</t>
+        </is>
+      </c>
+      <c r="I70" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="J70" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="K70" s="10" t="inlineStr">
+        <is>
+          <t>FUT|GeRo</t>
+        </is>
+      </c>
+      <c r="L70" s="10" t="inlineStr">
+        <is>
+          <t>FUT|MeOw</t>
+        </is>
+      </c>
+      <c r="M70" s="10" t="inlineStr">
+        <is>
+          <t>FUT|Nowy297</t>
+        </is>
+      </c>
+      <c r="N70" s="10" t="inlineStr">
+        <is>
+          <t>20250725T180748.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="7" t="inlineStr">
+        <is>
+          <t>PENNY</t>
+        </is>
+      </c>
+      <c r="B71" s="7" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="C71" s="7" t="inlineStr">
+        <is>
+          <t>8-BIT</t>
+        </is>
+      </c>
+      <c r="D71" s="8" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E71" s="8" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="F71" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G71" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H71" s="10" t="inlineStr">
+        <is>
+          <t>MBC|Kapi</t>
+        </is>
+      </c>
+      <c r="I71" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="J71" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K71" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="L71" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M71" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="N71" s="10" t="inlineStr">
+        <is>
+          <t>20250725T183542.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="7" t="inlineStr">
+        <is>
+          <t>PENNY</t>
+        </is>
+      </c>
+      <c r="B72" s="7" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="C72" s="7" t="inlineStr">
+        <is>
+          <t>8-BIT</t>
+        </is>
+      </c>
+      <c r="D72" s="8" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E72" s="8" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="F72" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G72" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H72" s="10" t="inlineStr">
+        <is>
+          <t>MBC|Kapi</t>
+        </is>
+      </c>
+      <c r="I72" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="J72" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K72" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="L72" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M72" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="N72" s="10" t="inlineStr">
+        <is>
+          <t>20250725T183300.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="7" t="inlineStr">
+        <is>
+          <t>PENNY</t>
+        </is>
+      </c>
+      <c r="B73" s="7" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="C73" s="7" t="inlineStr">
+        <is>
+          <t>8-BIT</t>
+        </is>
+      </c>
+      <c r="D73" s="8" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E73" s="8" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="F73" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G73" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H73" s="10" t="inlineStr">
+        <is>
+          <t>MBC|Kapi</t>
+        </is>
+      </c>
+      <c r="I73" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="J73" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K73" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="L73" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="M73" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="N73" s="10" t="inlineStr">
+        <is>
+          <t>20250725T183037.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-25 21:10:47)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -44508,7 +44508,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N73"/>
+  <dimension ref="A3:N76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P15" sqref="A4:P15"/>
@@ -49625,6 +49625,222 @@
       <c r="N73" s="10" t="inlineStr">
         <is>
           <t>20250725T183037.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="7" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="B74" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C74" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D74" s="8" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="E74" s="8" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="F74" s="8" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="G74" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H74" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="I74" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="J74" s="10" t="inlineStr">
+        <is>
+          <t>MBC|Kapi</t>
+        </is>
+      </c>
+      <c r="K74" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L74" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="M74" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="N74" s="10" t="inlineStr">
+        <is>
+          <t>20250725T184857.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B75" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C75" s="7" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D75" s="8" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E75" s="8" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="F75" s="8" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="G75" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H75" s="10" t="inlineStr">
+        <is>
+          <t>MBC|Kapi</t>
+        </is>
+      </c>
+      <c r="I75" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="J75" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K75" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L75" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="M75" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="N75" s="10" t="inlineStr">
+        <is>
+          <t>20250725T184539.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B76" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C76" s="7" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D76" s="8" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E76" s="8" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="F76" s="8" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="G76" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H76" s="10" t="inlineStr">
+        <is>
+          <t>MBC|Kapi</t>
+        </is>
+      </c>
+      <c r="I76" s="10" t="inlineStr">
+        <is>
+          <t>IC|Nob?</t>
+        </is>
+      </c>
+      <c r="J76" s="10" t="inlineStr">
+        <is>
+          <t>IC|RamaZR</t>
+        </is>
+      </c>
+      <c r="K76" s="10" t="inlineStr">
+        <is>
+          <t>NXT|amos</t>
+        </is>
+      </c>
+      <c r="L76" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Arthur</t>
+        </is>
+      </c>
+      <c r="M76" s="10" t="inlineStr">
+        <is>
+          <t>NXT|Rup</t>
+        </is>
+      </c>
+      <c r="N76" s="10" t="inlineStr">
+        <is>
+          <t>20250725T184343.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-26 10:22:15)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -500,7 +500,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N84"/>
+  <dimension ref="A3:N87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P16" sqref="A4:P16"/>
@@ -6409,6 +6409,222 @@
       <c r="N84" s="10" t="inlineStr">
         <is>
           <t>20250725T173759.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B85" s="7" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="C85" s="7" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="D85" s="8" t="inlineStr">
+        <is>
+          <t>CHESTER</t>
+        </is>
+      </c>
+      <c r="E85" s="8" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="F85" s="8" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="G85" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H85" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="I85" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="J85" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="K85" s="10" t="inlineStr">
+        <is>
+          <t>FX|Wesley</t>
+        </is>
+      </c>
+      <c r="L85" s="10" t="inlineStr">
+        <is>
+          <t>FX|REI DO FUT</t>
+        </is>
+      </c>
+      <c r="M85" s="10" t="inlineStr">
+        <is>
+          <t>FX|CaueBr</t>
+        </is>
+      </c>
+      <c r="N85" s="10" t="inlineStr">
+        <is>
+          <t>20250726T013408.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B86" s="7" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="C86" s="7" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="D86" s="8" t="inlineStr">
+        <is>
+          <t>CHESTER</t>
+        </is>
+      </c>
+      <c r="E86" s="8" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="F86" s="8" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="G86" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H86" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="I86" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="J86" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="K86" s="10" t="inlineStr">
+        <is>
+          <t>FX|Wesley</t>
+        </is>
+      </c>
+      <c r="L86" s="10" t="inlineStr">
+        <is>
+          <t>FX|REI DO FUT</t>
+        </is>
+      </c>
+      <c r="M86" s="10" t="inlineStr">
+        <is>
+          <t>FX|CaueBr</t>
+        </is>
+      </c>
+      <c r="N86" s="10" t="inlineStr">
+        <is>
+          <t>20250726T013118.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B87" s="7" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="C87" s="7" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="D87" s="8" t="inlineStr">
+        <is>
+          <t>CHESTER</t>
+        </is>
+      </c>
+      <c r="E87" s="8" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="F87" s="8" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="G87" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H87" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="I87" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="J87" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="K87" s="10" t="inlineStr">
+        <is>
+          <t>FX|Wesley</t>
+        </is>
+      </c>
+      <c r="L87" s="10" t="inlineStr">
+        <is>
+          <t>FX|REI DO FUT</t>
+        </is>
+      </c>
+      <c r="M87" s="10" t="inlineStr">
+        <is>
+          <t>FX|CaueBr</t>
+        </is>
+      </c>
+      <c r="N87" s="10" t="inlineStr">
+        <is>
+          <t>20250726T012802.000Z</t>
         </is>
       </c>
     </row>
@@ -8784,7 +9000,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N19"/>
+  <dimension ref="A3:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
@@ -10013,6 +10229,150 @@
       <c r="N19" s="10" t="inlineStr">
         <is>
           <t>20250725T143004.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="7" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="B20" s="7" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="C20" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="D20" s="8" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E20" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F20" s="8" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="G20" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H20" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="I20" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="J20" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="K20" s="10" t="inlineStr">
+        <is>
+          <t>BKB|❄️IC€CRØW❄️</t>
+        </is>
+      </c>
+      <c r="L20" s="10" t="inlineStr">
+        <is>
+          <t>YT:BrabaoBS🎩</t>
+        </is>
+      </c>
+      <c r="M20" s="10" t="inlineStr">
+        <is>
+          <t>Golden💘Mai</t>
+        </is>
+      </c>
+      <c r="N20" s="10" t="inlineStr">
+        <is>
+          <t>20250726T005331.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="7" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="B21" s="7" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="C21" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="D21" s="8" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E21" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F21" s="8" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="G21" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H21" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="I21" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="J21" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="K21" s="10" t="inlineStr">
+        <is>
+          <t>BKB|❄️IC€CRØW❄️</t>
+        </is>
+      </c>
+      <c r="L21" s="10" t="inlineStr">
+        <is>
+          <t>YT:BrabaoBS🎩</t>
+        </is>
+      </c>
+      <c r="M21" s="10" t="inlineStr">
+        <is>
+          <t>Golden💘Mai</t>
+        </is>
+      </c>
+      <c r="N21" s="10" t="inlineStr">
+        <is>
+          <t>20250726T005121.000Z</t>
         </is>
       </c>
     </row>
@@ -10027,7 +10387,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N13"/>
+  <dimension ref="A3:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
@@ -10824,6 +11184,150 @@
       <c r="N13" s="10" t="inlineStr">
         <is>
           <t>20250720T193837.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="7" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B14" s="7" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="C14" s="7" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="D14" s="8" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="E14" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="F14" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G14" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H14" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Derrp</t>
+        </is>
+      </c>
+      <c r="I14" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Jubileubr</t>
+        </is>
+      </c>
+      <c r="J14" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Loko</t>
+        </is>
+      </c>
+      <c r="K14" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L14" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="M14" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="N14" s="10" t="inlineStr">
+        <is>
+          <t>20250725T231511.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="7" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B15" s="7" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="C15" s="7" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="D15" s="8" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="E15" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="F15" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G15" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H15" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Derrp</t>
+        </is>
+      </c>
+      <c r="I15" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Jubileubr</t>
+        </is>
+      </c>
+      <c r="J15" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Loko</t>
+        </is>
+      </c>
+      <c r="K15" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L15" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="M15" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="N15" s="10" t="inlineStr">
+        <is>
+          <t>20250725T231223.000Z</t>
         </is>
       </c>
     </row>
@@ -10838,7 +11342,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N18"/>
+  <dimension ref="A3:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
@@ -11995,6 +12499,150 @@
       <c r="N18" s="10" t="inlineStr">
         <is>
           <t>20250725T171843.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="7" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="B19" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C19" s="7" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="D19" s="8" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="E19" s="8" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="F19" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="G19" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H19" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="I19" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="J19" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="K19" s="10" t="inlineStr">
+        <is>
+          <t>FX|CaueBr</t>
+        </is>
+      </c>
+      <c r="L19" s="10" t="inlineStr">
+        <is>
+          <t>FX|Wesley</t>
+        </is>
+      </c>
+      <c r="M19" s="10" t="inlineStr">
+        <is>
+          <t>FX|REI DO FUT</t>
+        </is>
+      </c>
+      <c r="N19" s="10" t="inlineStr">
+        <is>
+          <t>20250726T012103.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="7" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="B20" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C20" s="7" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="D20" s="8" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="E20" s="8" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="F20" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="G20" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H20" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="I20" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="J20" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="K20" s="10" t="inlineStr">
+        <is>
+          <t>FX|CaueBr</t>
+        </is>
+      </c>
+      <c r="L20" s="10" t="inlineStr">
+        <is>
+          <t>FX|Wesley</t>
+        </is>
+      </c>
+      <c r="M20" s="10" t="inlineStr">
+        <is>
+          <t>FX|REI DO FUT</t>
+        </is>
+      </c>
+      <c r="N20" s="10" t="inlineStr">
+        <is>
+          <t>20250726T011903.000Z</t>
         </is>
       </c>
     </row>
@@ -12009,7 +12657,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N22"/>
+  <dimension ref="A3:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P8" sqref="A4:P8"/>
@@ -13454,6 +14102,150 @@
       <c r="N22" s="3" t="inlineStr">
         <is>
           <t>20250724T202128.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="7" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="B23" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="C23" s="7" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="D23" s="8" t="inlineStr">
+        <is>
+          <t>CHESTER</t>
+        </is>
+      </c>
+      <c r="E23" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="F23" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G23" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H23" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Derrp</t>
+        </is>
+      </c>
+      <c r="I23" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Jubileubr</t>
+        </is>
+      </c>
+      <c r="J23" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Loko</t>
+        </is>
+      </c>
+      <c r="K23" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L23" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="M23" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="N23" s="10" t="inlineStr">
+        <is>
+          <t>20250725T232336.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="7" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="B24" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="C24" s="7" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="D24" s="8" t="inlineStr">
+        <is>
+          <t>CHESTER</t>
+        </is>
+      </c>
+      <c r="E24" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="F24" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G24" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H24" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Derrp</t>
+        </is>
+      </c>
+      <c r="I24" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Jubileubr</t>
+        </is>
+      </c>
+      <c r="J24" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Loko</t>
+        </is>
+      </c>
+      <c r="K24" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L24" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="M24" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="N24" s="10" t="inlineStr">
+        <is>
+          <t>20250725T232115.000Z</t>
         </is>
       </c>
     </row>
@@ -14135,7 +14927,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N18"/>
+  <dimension ref="A3:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="S12" sqref="S12"/>
@@ -15292,6 +16084,222 @@
       <c r="N18" s="10" t="inlineStr">
         <is>
           <t>20250725T173000.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="7" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="B19" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C19" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D19" s="8" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="E19" s="8" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F19" s="8" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="G19" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H19" s="10" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="I19" s="10" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="J19" s="10" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="K19" s="10" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="L19" s="10" t="inlineStr">
+        <is>
+          <t>@MathGamerBS</t>
+        </is>
+      </c>
+      <c r="M19" s="10" t="inlineStr">
+        <is>
+          <t>LLC|Kirito💘</t>
+        </is>
+      </c>
+      <c r="N19" s="10" t="inlineStr">
+        <is>
+          <t>20250726T020951.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="7" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="B20" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C20" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D20" s="8" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="E20" s="8" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F20" s="8" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="G20" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H20" s="10" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="I20" s="10" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="J20" s="10" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="K20" s="10" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="L20" s="10" t="inlineStr">
+        <is>
+          <t>@MathGamerBS</t>
+        </is>
+      </c>
+      <c r="M20" s="10" t="inlineStr">
+        <is>
+          <t>LLC|Kirito💘</t>
+        </is>
+      </c>
+      <c r="N20" s="10" t="inlineStr">
+        <is>
+          <t>20250726T020740.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="7" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="B21" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C21" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D21" s="8" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="E21" s="8" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F21" s="8" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="G21" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H21" s="10" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="I21" s="10" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="J21" s="10" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="K21" s="10" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="L21" s="10" t="inlineStr">
+        <is>
+          <t>@MathGamerBS</t>
+        </is>
+      </c>
+      <c r="M21" s="10" t="inlineStr">
+        <is>
+          <t>LLC|Kirito💘</t>
+        </is>
+      </c>
+      <c r="N21" s="10" t="inlineStr">
+        <is>
+          <t>20250726T020551.000Z</t>
         </is>
       </c>
     </row>
@@ -15306,7 +16314,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N54"/>
+  <dimension ref="A3:N64"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="Q30" sqref="Q30"/>
@@ -19055,6 +20063,726 @@
       <c r="N54" s="10" t="inlineStr">
         <is>
           <t>20250725T153305.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="7" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="B55" s="7" t="inlineStr">
+        <is>
+          <t>FANG</t>
+        </is>
+      </c>
+      <c r="C55" s="7" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="D55" s="8" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="E55" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="F55" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G55" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H55" s="10" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="I55" s="10" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="J55" s="10" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="K55" s="10" t="inlineStr">
+        <is>
+          <t>Patchy🍽️</t>
+        </is>
+      </c>
+      <c r="L55" s="10" t="inlineStr">
+        <is>
+          <t>sans🍽️</t>
+        </is>
+      </c>
+      <c r="M55" s="10" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="N55" s="10" t="inlineStr">
+        <is>
+          <t>20250726T000231.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="7" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="B56" s="7" t="inlineStr">
+        <is>
+          <t>FANG</t>
+        </is>
+      </c>
+      <c r="C56" s="7" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="D56" s="8" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="E56" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="F56" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G56" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H56" s="10" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="I56" s="10" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="J56" s="10" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="K56" s="10" t="inlineStr">
+        <is>
+          <t>Patchy🍽️</t>
+        </is>
+      </c>
+      <c r="L56" s="10" t="inlineStr">
+        <is>
+          <t>sans🍽️</t>
+        </is>
+      </c>
+      <c r="M56" s="10" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="N56" s="10" t="inlineStr">
+        <is>
+          <t>20250725T235945.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="7" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="B57" s="7" t="inlineStr">
+        <is>
+          <t>FANG</t>
+        </is>
+      </c>
+      <c r="C57" s="7" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="D57" s="8" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="E57" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="F57" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G57" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H57" s="10" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="I57" s="10" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="J57" s="10" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="K57" s="10" t="inlineStr">
+        <is>
+          <t>Patchy🍽️</t>
+        </is>
+      </c>
+      <c r="L57" s="10" t="inlineStr">
+        <is>
+          <t>sans🍽️</t>
+        </is>
+      </c>
+      <c r="M57" s="10" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="N57" s="10" t="inlineStr">
+        <is>
+          <t>20250725T235731.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="7" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="B58" s="7" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="C58" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D58" s="8" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E58" s="8" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F58" s="8" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="G58" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H58" s="10" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="I58" s="10" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="J58" s="10" t="inlineStr">
+        <is>
+          <t>sans🍽️</t>
+        </is>
+      </c>
+      <c r="K58" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Memxn</t>
+        </is>
+      </c>
+      <c r="L58" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Alyanys</t>
+        </is>
+      </c>
+      <c r="M58" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Frixi</t>
+        </is>
+      </c>
+      <c r="N58" s="10" t="inlineStr">
+        <is>
+          <t>20250726T014656.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="7" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="B59" s="7" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="C59" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D59" s="8" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E59" s="8" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F59" s="8" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="G59" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H59" s="10" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="I59" s="10" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="J59" s="10" t="inlineStr">
+        <is>
+          <t>sans🍽️</t>
+        </is>
+      </c>
+      <c r="K59" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Memxn</t>
+        </is>
+      </c>
+      <c r="L59" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Alyanys</t>
+        </is>
+      </c>
+      <c r="M59" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Frixi</t>
+        </is>
+      </c>
+      <c r="N59" s="10" t="inlineStr">
+        <is>
+          <t>20250726T014400.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B60" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C60" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D60" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E60" s="8" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="F60" s="8" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="G60" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H60" s="10" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="I60" s="10" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="J60" s="10" t="inlineStr">
+        <is>
+          <t>sans🍽️</t>
+        </is>
+      </c>
+      <c r="K60" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Frixi</t>
+        </is>
+      </c>
+      <c r="L60" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Memxn</t>
+        </is>
+      </c>
+      <c r="M60" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Alyanys</t>
+        </is>
+      </c>
+      <c r="N60" s="10" t="inlineStr">
+        <is>
+          <t>20250726T013723.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B61" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C61" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D61" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E61" s="8" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="F61" s="8" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="G61" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H61" s="10" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="I61" s="10" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="J61" s="10" t="inlineStr">
+        <is>
+          <t>sans🍽️</t>
+        </is>
+      </c>
+      <c r="K61" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Frixi</t>
+        </is>
+      </c>
+      <c r="L61" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Memxn</t>
+        </is>
+      </c>
+      <c r="M61" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Alyanys</t>
+        </is>
+      </c>
+      <c r="N61" s="10" t="inlineStr">
+        <is>
+          <t>20250726T013537.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B62" s="7" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="C62" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="D62" s="8" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="E62" s="8" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="F62" s="8" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="G62" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H62" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I62" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="J62" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="K62" s="10" t="inlineStr">
+        <is>
+          <t>BKB|❄️IC€CRØW❄️</t>
+        </is>
+      </c>
+      <c r="L62" s="10" t="inlineStr">
+        <is>
+          <t>YT:BrabaoBS🎩</t>
+        </is>
+      </c>
+      <c r="M62" s="10" t="inlineStr">
+        <is>
+          <t>Golden💘Mai</t>
+        </is>
+      </c>
+      <c r="N62" s="10" t="inlineStr">
+        <is>
+          <t>20250726T003211.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B63" s="7" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="C63" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="D63" s="8" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="E63" s="8" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="F63" s="8" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="G63" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H63" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I63" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="J63" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="K63" s="10" t="inlineStr">
+        <is>
+          <t>BKB|❄️IC€CRØW❄️</t>
+        </is>
+      </c>
+      <c r="L63" s="10" t="inlineStr">
+        <is>
+          <t>YT:BrabaoBS🎩</t>
+        </is>
+      </c>
+      <c r="M63" s="10" t="inlineStr">
+        <is>
+          <t>Golden💘Mai</t>
+        </is>
+      </c>
+      <c r="N63" s="10" t="inlineStr">
+        <is>
+          <t>20250726T002957.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B64" s="7" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="C64" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="D64" s="8" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="E64" s="8" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="F64" s="8" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="G64" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H64" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I64" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="J64" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="K64" s="10" t="inlineStr">
+        <is>
+          <t>BKB|❄️IC€CRØW❄️</t>
+        </is>
+      </c>
+      <c r="L64" s="10" t="inlineStr">
+        <is>
+          <t>YT:BrabaoBS🎩</t>
+        </is>
+      </c>
+      <c r="M64" s="10" t="inlineStr">
+        <is>
+          <t>Golden💘Mai</t>
+        </is>
+      </c>
+      <c r="N64" s="10" t="inlineStr">
+        <is>
+          <t>20250726T002806.000Z</t>
         </is>
       </c>
     </row>
@@ -19069,7 +20797,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N64"/>
+  <dimension ref="A3:N77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R30" sqref="R30"/>
@@ -23538,6 +25266,942 @@
       <c r="N64" s="10" t="inlineStr">
         <is>
           <t>20250725T171208.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="7" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B65" s="7" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="C65" s="7" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="D65" s="8" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="E65" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F65" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="G65" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H65" s="10" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="I65" s="10" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="J65" s="10" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="K65" s="10" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="L65" s="10" t="inlineStr">
+        <is>
+          <t>Patchy🍽️</t>
+        </is>
+      </c>
+      <c r="M65" s="10" t="inlineStr">
+        <is>
+          <t>sans🍽️</t>
+        </is>
+      </c>
+      <c r="N65" s="10" t="inlineStr">
+        <is>
+          <t>20250725T235033.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="7" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="B66" s="7" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="C66" s="7" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="D66" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E66" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="F66" s="8" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="G66" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H66" s="10" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="I66" s="10" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="J66" s="10" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="K66" s="10" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="L66" s="10" t="inlineStr">
+        <is>
+          <t>sans🍽️</t>
+        </is>
+      </c>
+      <c r="M66" s="10" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="N66" s="10" t="inlineStr">
+        <is>
+          <t>20250725T234630.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="7" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="B67" s="7" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="C67" s="7" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="D67" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E67" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="F67" s="8" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="G67" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H67" s="10" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="I67" s="10" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="J67" s="10" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="K67" s="10" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="L67" s="10" t="inlineStr">
+        <is>
+          <t>sans🍽️</t>
+        </is>
+      </c>
+      <c r="M67" s="10" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="N67" s="10" t="inlineStr">
+        <is>
+          <t>20250725T234458.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="B68" s="7" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="C68" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D68" s="8" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="E68" s="8" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="F68" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G68" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H68" s="10" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="I68" s="10" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="J68" s="10" t="inlineStr">
+        <is>
+          <t>sans🍽️</t>
+        </is>
+      </c>
+      <c r="K68" s="10" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="L68" s="10" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="M68" s="10" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="N68" s="10" t="inlineStr">
+        <is>
+          <t>20250725T233801.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="7" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="B69" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="C69" s="7" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="D69" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E69" s="8" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="F69" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G69" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H69" s="10" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="I69" s="10" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="J69" s="10" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="K69" s="10" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="L69" s="10" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="M69" s="10" t="inlineStr">
+        <is>
+          <t>sans🍽️</t>
+        </is>
+      </c>
+      <c r="N69" s="10" t="inlineStr">
+        <is>
+          <t>20250725T233504.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="7" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="B70" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="C70" s="7" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="D70" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E70" s="8" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="F70" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G70" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H70" s="10" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="I70" s="10" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="J70" s="10" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="K70" s="10" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="L70" s="10" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="M70" s="10" t="inlineStr">
+        <is>
+          <t>sans🍽️</t>
+        </is>
+      </c>
+      <c r="N70" s="10" t="inlineStr">
+        <is>
+          <t>20250725T233223.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="B71" s="7" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="C71" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D71" s="8" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="E71" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F71" s="8" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="G71" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H71" s="10" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="I71" s="10" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="J71" s="10" t="inlineStr">
+        <is>
+          <t>sans🍽️</t>
+        </is>
+      </c>
+      <c r="K71" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Frixi</t>
+        </is>
+      </c>
+      <c r="L71" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Memxn</t>
+        </is>
+      </c>
+      <c r="M71" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Alyanys</t>
+        </is>
+      </c>
+      <c r="N71" s="10" t="inlineStr">
+        <is>
+          <t>20250726T012926.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="B72" s="7" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="C72" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D72" s="8" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="E72" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F72" s="8" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="G72" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H72" s="10" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="I72" s="10" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="J72" s="10" t="inlineStr">
+        <is>
+          <t>sans🍽️</t>
+        </is>
+      </c>
+      <c r="K72" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Frixi</t>
+        </is>
+      </c>
+      <c r="L72" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Memxn</t>
+        </is>
+      </c>
+      <c r="M72" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Alyanys</t>
+        </is>
+      </c>
+      <c r="N72" s="10" t="inlineStr">
+        <is>
+          <t>20250726T012728.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="7" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="B73" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C73" s="7" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="D73" s="8" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="E73" s="8" t="inlineStr">
+        <is>
+          <t>PIPER</t>
+        </is>
+      </c>
+      <c r="F73" s="8" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="G73" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H73" s="10" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="I73" s="10" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="J73" s="10" t="inlineStr">
+        <is>
+          <t>sans🍽️</t>
+        </is>
+      </c>
+      <c r="K73" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Frixi</t>
+        </is>
+      </c>
+      <c r="L73" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Alyanys</t>
+        </is>
+      </c>
+      <c r="M73" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Betuchiz🍑</t>
+        </is>
+      </c>
+      <c r="N73" s="10" t="inlineStr">
+        <is>
+          <t>20250726T012045.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="7" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="B74" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C74" s="7" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="D74" s="8" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="E74" s="8" t="inlineStr">
+        <is>
+          <t>PIPER</t>
+        </is>
+      </c>
+      <c r="F74" s="8" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="G74" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H74" s="10" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="I74" s="10" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="J74" s="10" t="inlineStr">
+        <is>
+          <t>sans🍽️</t>
+        </is>
+      </c>
+      <c r="K74" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Frixi</t>
+        </is>
+      </c>
+      <c r="L74" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Alyanys</t>
+        </is>
+      </c>
+      <c r="M74" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Betuchiz🍑</t>
+        </is>
+      </c>
+      <c r="N74" s="10" t="inlineStr">
+        <is>
+          <t>20250726T011726.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="B75" s="7" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="C75" s="7" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="D75" s="8" t="inlineStr">
+        <is>
+          <t>PIPER</t>
+        </is>
+      </c>
+      <c r="E75" s="8" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="F75" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="G75" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H75" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Derrp</t>
+        </is>
+      </c>
+      <c r="I75" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Jubileubr</t>
+        </is>
+      </c>
+      <c r="J75" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Loko</t>
+        </is>
+      </c>
+      <c r="K75" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L75" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="M75" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="N75" s="10" t="inlineStr">
+        <is>
+          <t>20250725T233751.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="B76" s="7" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="C76" s="7" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="D76" s="8" t="inlineStr">
+        <is>
+          <t>PIPER</t>
+        </is>
+      </c>
+      <c r="E76" s="8" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="F76" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="G76" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H76" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Derrp</t>
+        </is>
+      </c>
+      <c r="I76" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Jubileubr</t>
+        </is>
+      </c>
+      <c r="J76" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Loko</t>
+        </is>
+      </c>
+      <c r="K76" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L76" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="M76" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="N76" s="10" t="inlineStr">
+        <is>
+          <t>20250725T233437.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="B77" s="7" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="C77" s="7" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="D77" s="8" t="inlineStr">
+        <is>
+          <t>PIPER</t>
+        </is>
+      </c>
+      <c r="E77" s="8" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="F77" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="G77" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H77" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Derrp</t>
+        </is>
+      </c>
+      <c r="I77" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Jubileubr</t>
+        </is>
+      </c>
+      <c r="J77" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Loko</t>
+        </is>
+      </c>
+      <c r="K77" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L77" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="M77" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="N77" s="10" t="inlineStr">
+        <is>
+          <t>20250725T233151.000Z</t>
         </is>
       </c>
     </row>
@@ -23552,7 +26216,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N74"/>
+  <dimension ref="A3:N80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="T38" sqref="T38"/>
@@ -28741,6 +31405,438 @@
       <c r="N74" s="10" t="inlineStr">
         <is>
           <t>20250725T170407.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B75" s="7" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="C75" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="D75" s="8" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="E75" s="8" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="F75" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G75" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H75" s="10" t="inlineStr">
+        <is>
+          <t>TRB|Zeus 解開</t>
+        </is>
+      </c>
+      <c r="I75" s="10" t="inlineStr">
+        <is>
+          <t>TRB|R B M</t>
+        </is>
+      </c>
+      <c r="J75" s="10" t="inlineStr">
+        <is>
+          <t>TRB|Lxffy</t>
+        </is>
+      </c>
+      <c r="K75" s="10" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="L75" s="10" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="M75" s="10" t="inlineStr">
+        <is>
+          <t>sans🍽️</t>
+        </is>
+      </c>
+      <c r="N75" s="10" t="inlineStr">
+        <is>
+          <t>20250725T232719.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="7" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="B76" s="7" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="C76" s="7" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="D76" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="E76" s="8" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="F76" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="G76" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H76" s="10" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="I76" s="10" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="J76" s="10" t="inlineStr">
+        <is>
+          <t>sans🍽️</t>
+        </is>
+      </c>
+      <c r="K76" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Frixi</t>
+        </is>
+      </c>
+      <c r="L76" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Alyanys</t>
+        </is>
+      </c>
+      <c r="M76" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Betuchiz🍑</t>
+        </is>
+      </c>
+      <c r="N76" s="10" t="inlineStr">
+        <is>
+          <t>20250726T011115.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="7" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="B77" s="7" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="C77" s="7" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="D77" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="E77" s="8" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="F77" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="G77" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H77" s="10" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="I77" s="10" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="J77" s="10" t="inlineStr">
+        <is>
+          <t>sans🍽️</t>
+        </is>
+      </c>
+      <c r="K77" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Frixi</t>
+        </is>
+      </c>
+      <c r="L77" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Alyanys</t>
+        </is>
+      </c>
+      <c r="M77" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Betuchiz🍑</t>
+        </is>
+      </c>
+      <c r="N77" s="10" t="inlineStr">
+        <is>
+          <t>20250726T010925.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="7" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="B78" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C78" s="7" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="D78" s="8" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E78" s="8" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="F78" s="8" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="G78" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H78" s="10" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="I78" s="10" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="J78" s="10" t="inlineStr">
+        <is>
+          <t>sans🍽️</t>
+        </is>
+      </c>
+      <c r="K78" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Frixi</t>
+        </is>
+      </c>
+      <c r="L78" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Alyanys</t>
+        </is>
+      </c>
+      <c r="M78" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Betuchiz🍑</t>
+        </is>
+      </c>
+      <c r="N78" s="10" t="inlineStr">
+        <is>
+          <t>20250726T010310.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="7" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="B79" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C79" s="7" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="D79" s="8" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E79" s="8" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="F79" s="8" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="G79" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H79" s="10" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="I79" s="10" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="J79" s="10" t="inlineStr">
+        <is>
+          <t>sans🍽️</t>
+        </is>
+      </c>
+      <c r="K79" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Frixi</t>
+        </is>
+      </c>
+      <c r="L79" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Alyanys</t>
+        </is>
+      </c>
+      <c r="M79" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Betuchiz🍑</t>
+        </is>
+      </c>
+      <c r="N79" s="10" t="inlineStr">
+        <is>
+          <t>20250726T010147.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="7" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="B80" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C80" s="7" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="D80" s="8" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E80" s="8" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="F80" s="8" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="G80" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H80" s="10" t="inlineStr">
+        <is>
+          <t>SSG|bobby</t>
+        </is>
+      </c>
+      <c r="I80" s="10" t="inlineStr">
+        <is>
+          <t>SSG|chino</t>
+        </is>
+      </c>
+      <c r="J80" s="10" t="inlineStr">
+        <is>
+          <t>sans🍽️</t>
+        </is>
+      </c>
+      <c r="K80" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Frixi</t>
+        </is>
+      </c>
+      <c r="L80" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Alyanys</t>
+        </is>
+      </c>
+      <c r="M80" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Betuchiz🍑</t>
+        </is>
+      </c>
+      <c r="N80" s="10" t="inlineStr">
+        <is>
+          <t>20250726T010020.000Z</t>
         </is>
       </c>
     </row>
@@ -40817,7 +43913,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N53"/>
+  <dimension ref="A3:N60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J36" sqref="J36"/>
@@ -44494,6 +47590,510 @@
       <c r="N53" s="10" t="inlineStr">
         <is>
           <t>20250725T170819.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="7" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="B54" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="C54" s="7" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="D54" s="8" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="E54" s="8" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="F54" s="8" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="G54" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H54" s="10" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="I54" s="10" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="J54" s="10" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="K54" s="10" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="L54" s="10" t="inlineStr">
+        <is>
+          <t>@MathGamerBS</t>
+        </is>
+      </c>
+      <c r="M54" s="10" t="inlineStr">
+        <is>
+          <t>LLC|Kirito💘</t>
+        </is>
+      </c>
+      <c r="N54" s="10" t="inlineStr">
+        <is>
+          <t>20250726T020104.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="7" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="B55" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="C55" s="7" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="D55" s="8" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="E55" s="8" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="F55" s="8" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="G55" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H55" s="10" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="I55" s="10" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="J55" s="10" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="K55" s="10" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="L55" s="10" t="inlineStr">
+        <is>
+          <t>@MathGamerBS</t>
+        </is>
+      </c>
+      <c r="M55" s="10" t="inlineStr">
+        <is>
+          <t>LLC|Kirito💘</t>
+        </is>
+      </c>
+      <c r="N55" s="10" t="inlineStr">
+        <is>
+          <t>20250726T015844.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B56" s="7" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="C56" s="7" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="D56" s="8" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="E56" s="8" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="F56" s="8" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="G56" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H56" s="10" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="I56" s="10" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="J56" s="10" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="K56" s="10" t="inlineStr">
+        <is>
+          <t>@MathGamerBS</t>
+        </is>
+      </c>
+      <c r="L56" s="10" t="inlineStr">
+        <is>
+          <t>LLC|Kirito💘</t>
+        </is>
+      </c>
+      <c r="M56" s="10" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="N56" s="10" t="inlineStr">
+        <is>
+          <t>20250726T015246.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B57" s="7" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="C57" s="7" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="D57" s="8" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="E57" s="8" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="F57" s="8" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="G57" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H57" s="10" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="I57" s="10" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="J57" s="10" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="K57" s="10" t="inlineStr">
+        <is>
+          <t>@MathGamerBS</t>
+        </is>
+      </c>
+      <c r="L57" s="10" t="inlineStr">
+        <is>
+          <t>LLC|Kirito💘</t>
+        </is>
+      </c>
+      <c r="M57" s="10" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="N57" s="10" t="inlineStr">
+        <is>
+          <t>20250726T015036.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B58" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C58" s="7" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="D58" s="8" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="E58" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F58" s="8" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G58" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H58" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="I58" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="J58" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="K58" s="10" t="inlineStr">
+        <is>
+          <t>FX|CaueBr</t>
+        </is>
+      </c>
+      <c r="L58" s="10" t="inlineStr">
+        <is>
+          <t>FX|Wesley</t>
+        </is>
+      </c>
+      <c r="M58" s="10" t="inlineStr">
+        <is>
+          <t>FX|REI DO FUT</t>
+        </is>
+      </c>
+      <c r="N58" s="10" t="inlineStr">
+        <is>
+          <t>20250726T011051.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B59" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C59" s="7" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="D59" s="8" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="E59" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F59" s="8" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G59" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H59" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="I59" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="J59" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="K59" s="10" t="inlineStr">
+        <is>
+          <t>FX|CaueBr</t>
+        </is>
+      </c>
+      <c r="L59" s="10" t="inlineStr">
+        <is>
+          <t>FX|Wesley</t>
+        </is>
+      </c>
+      <c r="M59" s="10" t="inlineStr">
+        <is>
+          <t>FX|REI DO FUT</t>
+        </is>
+      </c>
+      <c r="N59" s="10" t="inlineStr">
+        <is>
+          <t>20250726T010831.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B60" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C60" s="7" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="D60" s="8" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="E60" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F60" s="8" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G60" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H60" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="I60" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="J60" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="K60" s="10" t="inlineStr">
+        <is>
+          <t>FX|CaueBr</t>
+        </is>
+      </c>
+      <c r="L60" s="10" t="inlineStr">
+        <is>
+          <t>FX|Wesley</t>
+        </is>
+      </c>
+      <c r="M60" s="10" t="inlineStr">
+        <is>
+          <t>FX|REI DO FUT</t>
+        </is>
+      </c>
+      <c r="N60" s="10" t="inlineStr">
+        <is>
+          <t>20250726T010611.000Z</t>
         </is>
       </c>
     </row>
@@ -44508,7 +48108,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N76"/>
+  <dimension ref="A3:N81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P15" sqref="A4:P15"/>
@@ -49841,6 +53441,366 @@
       <c r="N76" s="10" t="inlineStr">
         <is>
           <t>20250725T184343.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="7" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="B77" s="7" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="C77" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D77" s="8" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="E77" s="8" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="F77" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="G77" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H77" s="10" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="I77" s="10" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="J77" s="10" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="K77" s="10" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="L77" s="10" t="inlineStr">
+        <is>
+          <t>@MathGamerBS</t>
+        </is>
+      </c>
+      <c r="M77" s="10" t="inlineStr">
+        <is>
+          <t>LLC|Kirito💘</t>
+        </is>
+      </c>
+      <c r="N77" s="10" t="inlineStr">
+        <is>
+          <t>20250726T014355.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="7" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="B78" s="7" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="C78" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D78" s="8" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="E78" s="8" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="F78" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="G78" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H78" s="10" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="I78" s="10" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="J78" s="10" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="K78" s="10" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="L78" s="10" t="inlineStr">
+        <is>
+          <t>@MathGamerBS</t>
+        </is>
+      </c>
+      <c r="M78" s="10" t="inlineStr">
+        <is>
+          <t>LLC|Kirito💘</t>
+        </is>
+      </c>
+      <c r="N78" s="10" t="inlineStr">
+        <is>
+          <t>20250726T014121.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="7" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="B79" s="7" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="C79" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D79" s="8" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="E79" s="8" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="F79" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="G79" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H79" s="10" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="I79" s="10" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="J79" s="10" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="K79" s="10" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="L79" s="10" t="inlineStr">
+        <is>
+          <t>@MathGamerBS</t>
+        </is>
+      </c>
+      <c r="M79" s="10" t="inlineStr">
+        <is>
+          <t>LLC|Kirito💘</t>
+        </is>
+      </c>
+      <c r="N79" s="10" t="inlineStr">
+        <is>
+          <t>20250726T013848.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B80" s="7" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="C80" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="D80" s="8" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="E80" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F80" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G80" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H80" s="10" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="I80" s="10" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="J80" s="10" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="K80" s="10" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="L80" s="10" t="inlineStr">
+        <is>
+          <t>LLC|roledu</t>
+        </is>
+      </c>
+      <c r="M80" s="10" t="inlineStr">
+        <is>
+          <t>LLC|Kirito💘</t>
+        </is>
+      </c>
+      <c r="N80" s="10" t="inlineStr">
+        <is>
+          <t>20250726T012026.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B81" s="7" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="C81" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="D81" s="8" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="E81" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F81" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G81" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H81" s="10" t="inlineStr">
+        <is>
+          <t>NHG|Bayarea</t>
+        </is>
+      </c>
+      <c r="I81" s="10" t="inlineStr">
+        <is>
+          <t>NHG|GN</t>
+        </is>
+      </c>
+      <c r="J81" s="10" t="inlineStr">
+        <is>
+          <t>NHG|Xemp</t>
+        </is>
+      </c>
+      <c r="K81" s="10" t="inlineStr">
+        <is>
+          <t>PLP|BrriN</t>
+        </is>
+      </c>
+      <c r="L81" s="10" t="inlineStr">
+        <is>
+          <t>LLC|roledu</t>
+        </is>
+      </c>
+      <c r="M81" s="10" t="inlineStr">
+        <is>
+          <t>LLC|Kirito💘</t>
+        </is>
+      </c>
+      <c r="N81" s="10" t="inlineStr">
+        <is>
+          <t>20250726T011823.000Z</t>
         </is>
       </c>
     </row>
@@ -49855,7 +53815,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N62"/>
+  <dimension ref="A3:N65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R15" sqref="R15"/>
@@ -54183,6 +58143,222 @@
         </is>
       </c>
     </row>
+    <row r="63">
+      <c r="A63" s="7" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="B63" s="7" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="C63" s="7" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="D63" s="8" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="E63" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F63" s="8" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="G63" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H63" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I63" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="J63" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="K63" s="10" t="inlineStr">
+        <is>
+          <t>BKB|❄️IC€CRØW❄️</t>
+        </is>
+      </c>
+      <c r="L63" s="10" t="inlineStr">
+        <is>
+          <t>YT:BrabaoBS🎩</t>
+        </is>
+      </c>
+      <c r="M63" s="10" t="inlineStr">
+        <is>
+          <t>Golden💘Mai</t>
+        </is>
+      </c>
+      <c r="N63" s="10" t="inlineStr">
+        <is>
+          <t>20250726T004346.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="7" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="B64" s="7" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="C64" s="7" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="D64" s="8" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="E64" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F64" s="8" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="G64" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H64" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I64" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="J64" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="K64" s="10" t="inlineStr">
+        <is>
+          <t>BKB|❄️IC€CRØW❄️</t>
+        </is>
+      </c>
+      <c r="L64" s="10" t="inlineStr">
+        <is>
+          <t>YT:BrabaoBS🎩</t>
+        </is>
+      </c>
+      <c r="M64" s="10" t="inlineStr">
+        <is>
+          <t>Golden💘Mai</t>
+        </is>
+      </c>
+      <c r="N64" s="10" t="inlineStr">
+        <is>
+          <t>20250726T004135.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="7" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="B65" s="7" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="C65" s="7" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="D65" s="8" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="E65" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F65" s="8" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="G65" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H65" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I65" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="J65" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="K65" s="10" t="inlineStr">
+        <is>
+          <t>BKB|❄️IC€CRØW❄️</t>
+        </is>
+      </c>
+      <c r="L65" s="10" t="inlineStr">
+        <is>
+          <t>YT:BrabaoBS🎩</t>
+        </is>
+      </c>
+      <c r="M65" s="10" t="inlineStr">
+        <is>
+          <t>Golden💘Mai</t>
+        </is>
+      </c>
+      <c r="N65" s="10" t="inlineStr">
+        <is>
+          <t>20250726T003944.000Z</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-26 14:35:07)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -12657,7 +12657,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N24"/>
+  <dimension ref="A3:N29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P8" sqref="A4:P8"/>
@@ -14246,6 +14246,366 @@
       <c r="N24" s="10" t="inlineStr">
         <is>
           <t>20250725T232115.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="7" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="B25" s="7" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="C25" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="D25" s="8" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="E25" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F25" s="8" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="G25" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H25" s="10" t="inlineStr">
+        <is>
+          <t>Shall🦋.*</t>
+        </is>
+      </c>
+      <c r="I25" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="J25" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="K25" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L25" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M25" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N25" s="10" t="inlineStr">
+        <is>
+          <t>20250726T123158.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="7" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="B26" s="7" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="C26" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="D26" s="8" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="E26" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F26" s="8" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="G26" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H26" s="10" t="inlineStr">
+        <is>
+          <t>Shall🦋.*</t>
+        </is>
+      </c>
+      <c r="I26" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="J26" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="K26" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L26" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M26" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N26" s="10" t="inlineStr">
+        <is>
+          <t>20250726T122916.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="B27" s="7" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="C27" s="7" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="D27" s="8" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="E27" s="8" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="F27" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G27" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H27" s="10" t="inlineStr">
+        <is>
+          <t>Shall🦋.*</t>
+        </is>
+      </c>
+      <c r="I27" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="J27" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="K27" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L27" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M27" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N27" s="10" t="inlineStr">
+        <is>
+          <t>20250726T122143.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="B28" s="7" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="C28" s="7" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="D28" s="8" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="E28" s="8" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="F28" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G28" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H28" s="10" t="inlineStr">
+        <is>
+          <t>Shall🦋.*</t>
+        </is>
+      </c>
+      <c r="I28" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="J28" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="K28" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L28" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M28" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N28" s="10" t="inlineStr">
+        <is>
+          <t>20250726T121949.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="B29" s="7" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="C29" s="7" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="D29" s="8" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="E29" s="8" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="F29" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G29" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H29" s="10" t="inlineStr">
+        <is>
+          <t>Shall🦋.*</t>
+        </is>
+      </c>
+      <c r="I29" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="J29" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="K29" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L29" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M29" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N29" s="10" t="inlineStr">
+        <is>
+          <t>20250726T121725.000Z</t>
         </is>
       </c>
     </row>
@@ -37414,7 +37774,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N92"/>
+  <dimension ref="A3:N94"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="P25" sqref="A4:P25"/>
@@ -43899,6 +44259,150 @@
       <c r="N92" s="10" t="inlineStr">
         <is>
           <t>20250725T163225.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="7" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="B93" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C93" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D93" s="8" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="E93" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F93" s="8" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="G93" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H93" s="10" t="inlineStr">
+        <is>
+          <t>ER|Naipishu😎</t>
+        </is>
+      </c>
+      <c r="I93" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J93" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="K93" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L93" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="M93" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="N93" s="10" t="inlineStr">
+        <is>
+          <t>20250726T123013.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="7" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="B94" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C94" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D94" s="8" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="E94" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F94" s="8" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="G94" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H94" s="10" t="inlineStr">
+        <is>
+          <t>ER|Naipishu😎</t>
+        </is>
+      </c>
+      <c r="I94" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J94" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="K94" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L94" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="M94" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="N94" s="10" t="inlineStr">
+        <is>
+          <t>20250726T122823.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-26 15:06:49)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -500,7 +500,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N87"/>
+  <dimension ref="A3:N91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P16" sqref="A4:P16"/>
@@ -6625,6 +6625,294 @@
       <c r="N87" s="10" t="inlineStr">
         <is>
           <t>20250726T012802.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="7" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="B88" s="7" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="C88" s="7" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="D88" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="E88" s="8" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="F88" s="8" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="G88" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H88" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="I88" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="J88" s="10" t="inlineStr">
+        <is>
+          <t>ER|Wahochi</t>
+        </is>
+      </c>
+      <c r="K88" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L88" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M88" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N88" s="10" t="inlineStr">
+        <is>
+          <t>20250726T125912.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="7" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="B89" s="7" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="C89" s="7" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="D89" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="E89" s="8" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="F89" s="8" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="G89" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H89" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="I89" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="J89" s="10" t="inlineStr">
+        <is>
+          <t>ER|Wahochi</t>
+        </is>
+      </c>
+      <c r="K89" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L89" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M89" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N89" s="10" t="inlineStr">
+        <is>
+          <t>20250726T125753.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="7" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="B90" s="7" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="C90" s="7" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="D90" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E90" s="8" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="F90" s="8" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="G90" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H90" s="10" t="inlineStr">
+        <is>
+          <t>ER|Wahochi</t>
+        </is>
+      </c>
+      <c r="I90" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="J90" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="K90" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L90" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M90" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N90" s="10" t="inlineStr">
+        <is>
+          <t>20250726T125019.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="7" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="B91" s="7" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="C91" s="7" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="D91" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E91" s="8" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="F91" s="8" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="G91" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H91" s="10" t="inlineStr">
+        <is>
+          <t>ER|Wahochi</t>
+        </is>
+      </c>
+      <c r="I91" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="J91" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="K91" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L91" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M91" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N91" s="10" t="inlineStr">
+        <is>
+          <t>20250726T124720.000Z</t>
         </is>
       </c>
     </row>
@@ -32211,7 +32499,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N79"/>
+  <dimension ref="A3:N85"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="P38" sqref="P38"/>
@@ -37760,6 +38048,438 @@
       <c r="N79" s="10" t="inlineStr">
         <is>
           <t>20250725T163806.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="7" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B80" s="7" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="C80" s="7" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="D80" s="8" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E80" s="8" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="F80" s="8" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="G80" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H80" s="10" t="inlineStr">
+        <is>
+          <t>ER|Naipishu😎</t>
+        </is>
+      </c>
+      <c r="I80" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J80" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="K80" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L80" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="M80" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="N80" s="10" t="inlineStr">
+        <is>
+          <t>20250726T130158.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="7" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B81" s="7" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="C81" s="7" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="D81" s="8" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E81" s="8" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="F81" s="8" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="G81" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H81" s="10" t="inlineStr">
+        <is>
+          <t>ER|Naipishu😎</t>
+        </is>
+      </c>
+      <c r="I81" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J81" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="K81" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L81" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="M81" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="N81" s="10" t="inlineStr">
+        <is>
+          <t>20250726T125938.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="7" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B82" s="7" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="C82" s="7" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="D82" s="8" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E82" s="8" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="F82" s="8" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="G82" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H82" s="10" t="inlineStr">
+        <is>
+          <t>ER|Naipishu😎</t>
+        </is>
+      </c>
+      <c r="I82" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J82" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="K82" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L82" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="M82" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="N82" s="10" t="inlineStr">
+        <is>
+          <t>20250726T125718.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="7" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="B83" s="7" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C83" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D83" s="8" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="E83" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F83" s="8" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="G83" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H83" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="I83" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J83" s="10" t="inlineStr">
+        <is>
+          <t>ER|Naipishu😎</t>
+        </is>
+      </c>
+      <c r="K83" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L83" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="M83" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="N83" s="10" t="inlineStr">
+        <is>
+          <t>20250726T125112.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="7" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="B84" s="7" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C84" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D84" s="8" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="E84" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F84" s="8" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="G84" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H84" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="I84" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J84" s="10" t="inlineStr">
+        <is>
+          <t>ER|Naipishu😎</t>
+        </is>
+      </c>
+      <c r="K84" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L84" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="M84" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="N84" s="10" t="inlineStr">
+        <is>
+          <t>20250726T124852.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="7" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="B85" s="7" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C85" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D85" s="8" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="E85" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F85" s="8" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="G85" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H85" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="I85" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J85" s="10" t="inlineStr">
+        <is>
+          <t>ER|Naipishu😎</t>
+        </is>
+      </c>
+      <c r="K85" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L85" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="M85" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="N85" s="10" t="inlineStr">
+        <is>
+          <t>20250726T124633.000Z</t>
         </is>
       </c>
     </row>
@@ -37774,7 +38494,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N94"/>
+  <dimension ref="A3:N97"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="P25" sqref="A4:P25"/>
@@ -44403,6 +45123,222 @@
       <c r="N94" s="10" t="inlineStr">
         <is>
           <t>20250726T122823.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B95" s="7" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="C95" s="7" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="D95" s="8" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="E95" s="8" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="F95" s="8" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G95" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H95" s="10" t="inlineStr">
+        <is>
+          <t>ER|Naipishu😎</t>
+        </is>
+      </c>
+      <c r="I95" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="J95" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="K95" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L95" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="M95" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="N95" s="10" t="inlineStr">
+        <is>
+          <t>20250726T124101.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B96" s="7" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="C96" s="7" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="D96" s="8" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="E96" s="8" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="F96" s="8" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G96" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H96" s="10" t="inlineStr">
+        <is>
+          <t>ER|Naipishu😎</t>
+        </is>
+      </c>
+      <c r="I96" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="J96" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="K96" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L96" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="M96" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="N96" s="10" t="inlineStr">
+        <is>
+          <t>20250726T123857.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B97" s="7" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="C97" s="7" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="D97" s="8" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="E97" s="8" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="F97" s="8" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G97" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H97" s="10" t="inlineStr">
+        <is>
+          <t>ER|Naipishu😎</t>
+        </is>
+      </c>
+      <c r="I97" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="J97" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="K97" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L97" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="M97" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="N97" s="10" t="inlineStr">
+        <is>
+          <t>20250726T123628.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-26 15:38:34)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -16962,7 +16962,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N64"/>
+  <dimension ref="A3:N67"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="Q30" sqref="Q30"/>
@@ -21431,6 +21431,222 @@
       <c r="N64" s="10" t="inlineStr">
         <is>
           <t>20250726T002806.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B65" s="7" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="C65" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D65" s="8" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="E65" s="8" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F65" s="8" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="G65" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H65" s="10" t="inlineStr">
+        <is>
+          <t>ER|Naipishu😎</t>
+        </is>
+      </c>
+      <c r="I65" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J65" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="K65" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L65" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="M65" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="N65" s="10" t="inlineStr">
+        <is>
+          <t>20250726T133554.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="7" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="B66" s="7" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="C66" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="D66" s="8" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="E66" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F66" s="8" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="G66" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H66" s="10" t="inlineStr">
+        <is>
+          <t>ER|Naipishu😎</t>
+        </is>
+      </c>
+      <c r="I66" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J66" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="K66" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L66" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="M66" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="N66" s="10" t="inlineStr">
+        <is>
+          <t>20250726T132900.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="7" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="B67" s="7" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="C67" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="D67" s="8" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="E67" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F67" s="8" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="G67" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H67" s="10" t="inlineStr">
+        <is>
+          <t>ER|Naipishu😎</t>
+        </is>
+      </c>
+      <c r="I67" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J67" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="K67" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L67" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="M67" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="N67" s="10" t="inlineStr">
+        <is>
+          <t>20250726T132657.000Z</t>
         </is>
       </c>
     </row>
@@ -26864,7 +27080,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N80"/>
+  <dimension ref="A3:N84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="T38" sqref="T38"/>
@@ -32485,6 +32701,294 @@
       <c r="N80" s="10" t="inlineStr">
         <is>
           <t>20250726T010020.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="7" t="inlineStr">
+        <is>
+          <t>EDGAR</t>
+        </is>
+      </c>
+      <c r="B81" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C81" s="7" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="D81" s="8" t="inlineStr">
+        <is>
+          <t>FANG</t>
+        </is>
+      </c>
+      <c r="E81" s="8" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F81" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G81" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H81" s="10" t="inlineStr">
+        <is>
+          <t>ER|Naipishu😎</t>
+        </is>
+      </c>
+      <c r="I81" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J81" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="K81" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L81" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="M81" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="N81" s="10" t="inlineStr">
+        <is>
+          <t>20250726T132043.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="7" t="inlineStr">
+        <is>
+          <t>EDGAR</t>
+        </is>
+      </c>
+      <c r="B82" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C82" s="7" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="D82" s="8" t="inlineStr">
+        <is>
+          <t>FANG</t>
+        </is>
+      </c>
+      <c r="E82" s="8" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F82" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G82" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H82" s="10" t="inlineStr">
+        <is>
+          <t>ER|Naipishu😎</t>
+        </is>
+      </c>
+      <c r="I82" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J82" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="K82" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L82" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="M82" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="N82" s="10" t="inlineStr">
+        <is>
+          <t>20250726T131852.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="7" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="B83" s="7" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="C83" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D83" s="8" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="E83" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F83" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G83" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H83" s="10" t="inlineStr">
+        <is>
+          <t>ER|Naipishu😎</t>
+        </is>
+      </c>
+      <c r="I83" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J83" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="K83" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L83" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="M83" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="N83" s="10" t="inlineStr">
+        <is>
+          <t>20250726T131220.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="7" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="B84" s="7" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="C84" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D84" s="8" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="E84" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F84" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G84" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H84" s="10" t="inlineStr">
+        <is>
+          <t>ER|Naipishu😎</t>
+        </is>
+      </c>
+      <c r="I84" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J84" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="K84" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L84" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="M84" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="N84" s="10" t="inlineStr">
+        <is>
+          <t>20250726T131015.000Z</t>
         </is>
       </c>
     </row>
@@ -32499,7 +33003,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N85"/>
+  <dimension ref="A3:N88"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="P38" sqref="P38"/>
@@ -38480,6 +38984,222 @@
       <c r="N85" s="10" t="inlineStr">
         <is>
           <t>20250726T124633.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B86" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C86" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="D86" s="8" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="E86" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F86" s="8" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="G86" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H86" s="10" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="I86" s="10" t="inlineStr">
+        <is>
+          <t>CR|Tensai</t>
+        </is>
+      </c>
+      <c r="J86" s="10" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="K86" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="L86" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="M86" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="N86" s="10" t="inlineStr">
+        <is>
+          <t>20250726T133545.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B87" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C87" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="D87" s="8" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="E87" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F87" s="8" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="G87" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H87" s="10" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="I87" s="10" t="inlineStr">
+        <is>
+          <t>CR|Tensai</t>
+        </is>
+      </c>
+      <c r="J87" s="10" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="K87" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="L87" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="M87" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="N87" s="10" t="inlineStr">
+        <is>
+          <t>20250726T133325.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B88" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C88" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="D88" s="8" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="E88" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F88" s="8" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="G88" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H88" s="10" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="I88" s="10" t="inlineStr">
+        <is>
+          <t>CR|Tensai</t>
+        </is>
+      </c>
+      <c r="J88" s="10" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="K88" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="L88" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="M88" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="N88" s="10" t="inlineStr">
+        <is>
+          <t>20250726T133106.000Z</t>
         </is>
       </c>
     </row>
@@ -38494,7 +39214,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N97"/>
+  <dimension ref="A3:N101"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="P25" sqref="A4:P25"/>
@@ -45339,6 +46059,294 @@
       <c r="N97" s="10" t="inlineStr">
         <is>
           <t>20250726T123628.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="7" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="B98" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C98" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D98" s="8" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="E98" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F98" s="8" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="G98" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H98" s="10" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="I98" s="10" t="inlineStr">
+        <is>
+          <t>CR|Tensai</t>
+        </is>
+      </c>
+      <c r="J98" s="10" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="K98" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="L98" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="M98" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="N98" s="10" t="inlineStr">
+        <is>
+          <t>20250726T132427.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="7" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="B99" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C99" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D99" s="8" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="E99" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F99" s="8" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="G99" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H99" s="10" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="I99" s="10" t="inlineStr">
+        <is>
+          <t>CR|Tensai</t>
+        </is>
+      </c>
+      <c r="J99" s="10" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="K99" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="L99" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="M99" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="N99" s="10" t="inlineStr">
+        <is>
+          <t>20250726T132157.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="7" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="B100" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C100" s="7" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="D100" s="8" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="E100" s="8" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="F100" s="8" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G100" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H100" s="10" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="I100" s="10" t="inlineStr">
+        <is>
+          <t>CR|Tensai</t>
+        </is>
+      </c>
+      <c r="J100" s="10" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="K100" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="L100" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="M100" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="N100" s="10" t="inlineStr">
+        <is>
+          <t>20250726T131616.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="7" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="B101" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C101" s="7" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="D101" s="8" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="E101" s="8" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="F101" s="8" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G101" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H101" s="10" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="I101" s="10" t="inlineStr">
+        <is>
+          <t>CR|Tensai</t>
+        </is>
+      </c>
+      <c r="J101" s="10" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="K101" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="L101" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="M101" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="N101" s="10" t="inlineStr">
+        <is>
+          <t>20250726T131428.000Z</t>
         </is>
       </c>
     </row>
@@ -45353,7 +46361,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N60"/>
+  <dimension ref="A3:N63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J36" sqref="J36"/>
@@ -49534,6 +50542,222 @@
       <c r="N60" s="10" t="inlineStr">
         <is>
           <t>20250726T010611.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="B61" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="C61" s="7" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="D61" s="8" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="E61" s="8" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="F61" s="8" t="inlineStr">
+        <is>
+          <t>8-BIT</t>
+        </is>
+      </c>
+      <c r="G61" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H61" s="10" t="inlineStr">
+        <is>
+          <t>ER|Wahochi</t>
+        </is>
+      </c>
+      <c r="I61" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="J61" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="K61" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="L61" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M61" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="N61" s="10" t="inlineStr">
+        <is>
+          <t>20250726T133300.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="B62" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="C62" s="7" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="D62" s="8" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="E62" s="8" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="F62" s="8" t="inlineStr">
+        <is>
+          <t>8-BIT</t>
+        </is>
+      </c>
+      <c r="G62" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H62" s="10" t="inlineStr">
+        <is>
+          <t>ER|Wahochi</t>
+        </is>
+      </c>
+      <c r="I62" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="J62" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="K62" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="L62" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M62" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="N62" s="10" t="inlineStr">
+        <is>
+          <t>20250726T133040.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="B63" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="C63" s="7" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="D63" s="8" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="E63" s="8" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="F63" s="8" t="inlineStr">
+        <is>
+          <t>8-BIT</t>
+        </is>
+      </c>
+      <c r="G63" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H63" s="10" t="inlineStr">
+        <is>
+          <t>ER|Wahochi</t>
+        </is>
+      </c>
+      <c r="I63" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="J63" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="K63" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="L63" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M63" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="N63" s="10" t="inlineStr">
+        <is>
+          <t>20250726T132821.000Z</t>
         </is>
       </c>
     </row>
@@ -49548,7 +50772,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N81"/>
+  <dimension ref="A3:N87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P15" sqref="A4:P15"/>
@@ -55241,6 +56465,438 @@
       <c r="N81" s="10" t="inlineStr">
         <is>
           <t>20250726T011823.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="7" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="B82" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C82" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D82" s="8" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="E82" s="8" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="F82" s="8" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="G82" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H82" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="I82" s="10" t="inlineStr">
+        <is>
+          <t>ER|Wahochi</t>
+        </is>
+      </c>
+      <c r="J82" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="K82" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L82" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M82" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N82" s="10" t="inlineStr">
+        <is>
+          <t>20250726T132134.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="7" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="B83" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C83" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D83" s="8" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="E83" s="8" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="F83" s="8" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="G83" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H83" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="I83" s="10" t="inlineStr">
+        <is>
+          <t>ER|Wahochi</t>
+        </is>
+      </c>
+      <c r="J83" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="K83" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L83" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M83" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N83" s="10" t="inlineStr">
+        <is>
+          <t>20250726T131935.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="7" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="B84" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C84" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D84" s="8" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="E84" s="8" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="F84" s="8" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="G84" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H84" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="I84" s="10" t="inlineStr">
+        <is>
+          <t>ER|Wahochi</t>
+        </is>
+      </c>
+      <c r="J84" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="K84" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L84" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M84" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N84" s="10" t="inlineStr">
+        <is>
+          <t>20250726T131722.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="7" t="inlineStr">
+        <is>
+          <t>PENNY</t>
+        </is>
+      </c>
+      <c r="B85" s="7" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="C85" s="7" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="D85" s="8" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="E85" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F85" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G85" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H85" s="10" t="inlineStr">
+        <is>
+          <t>ER|Wahochi</t>
+        </is>
+      </c>
+      <c r="I85" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="J85" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="K85" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L85" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M85" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N85" s="10" t="inlineStr">
+        <is>
+          <t>20250726T131048.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="7" t="inlineStr">
+        <is>
+          <t>PENNY</t>
+        </is>
+      </c>
+      <c r="B86" s="7" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="C86" s="7" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="D86" s="8" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="E86" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F86" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G86" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H86" s="10" t="inlineStr">
+        <is>
+          <t>ER|Wahochi</t>
+        </is>
+      </c>
+      <c r="I86" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="J86" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="K86" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L86" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M86" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N86" s="10" t="inlineStr">
+        <is>
+          <t>20250726T130820.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="7" t="inlineStr">
+        <is>
+          <t>PENNY</t>
+        </is>
+      </c>
+      <c r="B87" s="7" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="C87" s="7" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="D87" s="8" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="E87" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F87" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G87" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H87" s="10" t="inlineStr">
+        <is>
+          <t>ER|Wahochi</t>
+        </is>
+      </c>
+      <c r="I87" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="J87" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="K87" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L87" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M87" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N87" s="10" t="inlineStr">
+        <is>
+          <t>20250726T130615.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-26 16:10:15)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -8621,7 +8621,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N11"/>
+  <dimension ref="A3:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N19" sqref="N19"/>
@@ -9274,6 +9274,366 @@
       <c r="N11" s="10" t="inlineStr">
         <is>
           <t>20250723T232641.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="D12" s="8" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="E12" s="8" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="F12" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="G12" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H12" s="10" t="inlineStr">
+        <is>
+          <t>ER|Wahochi</t>
+        </is>
+      </c>
+      <c r="I12" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="J12" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="K12" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L12" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M12" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N12" s="10" t="inlineStr">
+        <is>
+          <t>20250726T140201.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="D13" s="8" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="E13" s="8" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="F13" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="G13" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H13" s="10" t="inlineStr">
+        <is>
+          <t>ER|Wahochi</t>
+        </is>
+      </c>
+      <c r="I13" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="J13" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="K13" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L13" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M13" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N13" s="10" t="inlineStr">
+        <is>
+          <t>20250726T140003.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="B14" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C14" s="7" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="D14" s="8" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="E14" s="8" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="F14" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="G14" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H14" s="10" t="inlineStr">
+        <is>
+          <t>ER|Wahochi</t>
+        </is>
+      </c>
+      <c r="I14" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="J14" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="K14" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L14" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M14" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N14" s="10" t="inlineStr">
+        <is>
+          <t>20250726T135821.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="7" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="B15" s="7" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="C15" s="7" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="D15" s="8" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="E15" s="8" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="F15" s="8" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="G15" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H15" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="I15" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="J15" s="10" t="inlineStr">
+        <is>
+          <t>ER|Wahochi</t>
+        </is>
+      </c>
+      <c r="K15" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L15" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M15" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N15" s="10" t="inlineStr">
+        <is>
+          <t>20250726T135125.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="7" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="B16" s="7" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="C16" s="7" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="D16" s="8" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="E16" s="8" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="F16" s="8" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="G16" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H16" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="I16" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="J16" s="10" t="inlineStr">
+        <is>
+          <t>ER|Wahochi</t>
+        </is>
+      </c>
+      <c r="K16" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L16" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M16" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N16" s="10" t="inlineStr">
+        <is>
+          <t>20250726T134941.000Z</t>
         </is>
       </c>
     </row>
@@ -16962,7 +17322,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N67"/>
+  <dimension ref="A3:N68"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="Q30" sqref="Q30"/>
@@ -21647,6 +22007,78 @@
       <c r="N67" s="10" t="inlineStr">
         <is>
           <t>20250726T132657.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B68" s="7" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="C68" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D68" s="8" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="E68" s="8" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F68" s="8" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="G68" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H68" s="10" t="inlineStr">
+        <is>
+          <t>ER|Naipishu😎</t>
+        </is>
+      </c>
+      <c r="I68" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J68" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="K68" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L68" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="M68" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="N68" s="10" t="inlineStr">
+        <is>
+          <t>20250726T133843.000Z</t>
         </is>
       </c>
     </row>
@@ -21661,7 +22093,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N77"/>
+  <dimension ref="A3:N84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R30" sqref="R30"/>
@@ -27066,6 +27498,510 @@
       <c r="N77" s="10" t="inlineStr">
         <is>
           <t>20250725T233151.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="7" t="inlineStr">
+        <is>
+          <t>NANI</t>
+        </is>
+      </c>
+      <c r="B78" s="7" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="C78" s="7" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="D78" s="8" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="E78" s="8" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="F78" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G78" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H78" s="10" t="inlineStr">
+        <is>
+          <t>ER|Naipishu😎</t>
+        </is>
+      </c>
+      <c r="I78" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J78" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="K78" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L78" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="M78" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="N78" s="10" t="inlineStr">
+        <is>
+          <t>20250726T135942.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="7" t="inlineStr">
+        <is>
+          <t>NANI</t>
+        </is>
+      </c>
+      <c r="B79" s="7" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="C79" s="7" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="D79" s="8" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="E79" s="8" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="F79" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G79" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H79" s="10" t="inlineStr">
+        <is>
+          <t>ER|Naipishu😎</t>
+        </is>
+      </c>
+      <c r="I79" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J79" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="K79" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L79" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="M79" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="N79" s="10" t="inlineStr">
+        <is>
+          <t>20250726T135640.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="7" t="inlineStr">
+        <is>
+          <t>NANI</t>
+        </is>
+      </c>
+      <c r="B80" s="7" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="C80" s="7" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="D80" s="8" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="E80" s="8" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="F80" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G80" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H80" s="10" t="inlineStr">
+        <is>
+          <t>ER|Naipishu😎</t>
+        </is>
+      </c>
+      <c r="I80" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J80" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="K80" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L80" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="M80" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="N80" s="10" t="inlineStr">
+        <is>
+          <t>20250726T135351.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="7" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="B81" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="C81" s="7" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="D81" s="8" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="E81" s="8" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="F81" s="8" t="inlineStr">
+        <is>
+          <t>PIPER</t>
+        </is>
+      </c>
+      <c r="G81" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H81" s="10" t="inlineStr">
+        <is>
+          <t>ER|Naipishu😎</t>
+        </is>
+      </c>
+      <c r="I81" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="J81" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="K81" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="L81" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="M81" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="N81" s="10" t="inlineStr">
+        <is>
+          <t>20250726T134827.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="7" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="B82" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="C82" s="7" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="D82" s="8" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="E82" s="8" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="F82" s="8" t="inlineStr">
+        <is>
+          <t>PIPER</t>
+        </is>
+      </c>
+      <c r="G82" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H82" s="10" t="inlineStr">
+        <is>
+          <t>ER|Naipishu😎</t>
+        </is>
+      </c>
+      <c r="I82" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="J82" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="K82" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="L82" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="M82" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="N82" s="10" t="inlineStr">
+        <is>
+          <t>20250726T134604.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="7" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="B83" s="7" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="C83" s="7" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="D83" s="8" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="E83" s="8" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="F83" s="8" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G83" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H83" s="10" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="I83" s="10" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="J83" s="10" t="inlineStr">
+        <is>
+          <t>CR|Tensai</t>
+        </is>
+      </c>
+      <c r="K83" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="L83" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="M83" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="N83" s="10" t="inlineStr">
+        <is>
+          <t>20250726T140633.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="7" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="B84" s="7" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="C84" s="7" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="D84" s="8" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="E84" s="8" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="F84" s="8" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G84" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H84" s="10" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="I84" s="10" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="J84" s="10" t="inlineStr">
+        <is>
+          <t>CR|Tensai</t>
+        </is>
+      </c>
+      <c r="K84" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="L84" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="M84" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="N84" s="10" t="inlineStr">
+        <is>
+          <t>20250726T140353.000Z</t>
         </is>
       </c>
     </row>
@@ -27080,7 +28016,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N84"/>
+  <dimension ref="A3:N88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="T38" sqref="T38"/>
@@ -32989,6 +33925,294 @@
       <c r="N84" s="10" t="inlineStr">
         <is>
           <t>20250726T131015.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B85" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C85" s="7" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="D85" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E85" s="8" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="F85" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G85" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H85" s="10" t="inlineStr">
+        <is>
+          <t>CR|Tensai</t>
+        </is>
+      </c>
+      <c r="I85" s="10" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="J85" s="10" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="K85" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="L85" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="M85" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="N85" s="10" t="inlineStr">
+        <is>
+          <t>20250726T135701.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="B86" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C86" s="7" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="D86" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E86" s="8" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="F86" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G86" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H86" s="10" t="inlineStr">
+        <is>
+          <t>CR|Tensai</t>
+        </is>
+      </c>
+      <c r="I86" s="10" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="J86" s="10" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="K86" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="L86" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="M86" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="N86" s="10" t="inlineStr">
+        <is>
+          <t>20250726T135506.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="7" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="B87" s="7" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="C87" s="7" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="D87" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E87" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F87" s="8" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="G87" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H87" s="10" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="I87" s="10" t="inlineStr">
+        <is>
+          <t>CR|Tensai</t>
+        </is>
+      </c>
+      <c r="J87" s="10" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="K87" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="L87" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="M87" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="N87" s="10" t="inlineStr">
+        <is>
+          <t>20250726T134958.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="7" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="B88" s="7" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="C88" s="7" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="D88" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E88" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F88" s="8" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="G88" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H88" s="10" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="I88" s="10" t="inlineStr">
+        <is>
+          <t>CR|Tensai</t>
+        </is>
+      </c>
+      <c r="J88" s="10" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="K88" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="L88" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="M88" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="N88" s="10" t="inlineStr">
+        <is>
+          <t>20250726T134824.000Z</t>
         </is>
       </c>
     </row>
@@ -33003,7 +34227,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N88"/>
+  <dimension ref="A3:N90"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="P38" sqref="P38"/>
@@ -39200,6 +40424,150 @@
       <c r="N88" s="10" t="inlineStr">
         <is>
           <t>20250726T133106.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="7" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B89" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C89" s="7" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="D89" s="8" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E89" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F89" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="G89" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H89" s="10" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="I89" s="10" t="inlineStr">
+        <is>
+          <t>CR|Tensai</t>
+        </is>
+      </c>
+      <c r="J89" s="10" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="K89" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="L89" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="M89" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="N89" s="10" t="inlineStr">
+        <is>
+          <t>20250726T134342.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="7" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="B90" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C90" s="7" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="D90" s="8" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="E90" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F90" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="G90" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H90" s="10" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="I90" s="10" t="inlineStr">
+        <is>
+          <t>CR|Tensai</t>
+        </is>
+      </c>
+      <c r="J90" s="10" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="K90" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="L90" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="M90" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="N90" s="10" t="inlineStr">
+        <is>
+          <t>20250726T134126.000Z</t>
         </is>
       </c>
     </row>
@@ -46361,7 +47729,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N63"/>
+  <dimension ref="A3:N65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J36" sqref="J36"/>
@@ -50758,6 +52126,150 @@
       <c r="N63" s="10" t="inlineStr">
         <is>
           <t>20250726T132821.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="B64" s="7" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="C64" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D64" s="8" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="E64" s="8" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="F64" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G64" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H64" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="I64" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="J64" s="10" t="inlineStr">
+        <is>
+          <t>ER|Wahochi</t>
+        </is>
+      </c>
+      <c r="K64" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L64" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M64" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N64" s="10" t="inlineStr">
+        <is>
+          <t>20250726T134150.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="B65" s="7" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="C65" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D65" s="8" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="E65" s="8" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="F65" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G65" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H65" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="I65" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="J65" s="10" t="inlineStr">
+        <is>
+          <t>ER|Wahochi</t>
+        </is>
+      </c>
+      <c r="K65" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L65" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M65" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N65" s="10" t="inlineStr">
+        <is>
+          <t>20250726T133933.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-26 16:41:44)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -8026,7 +8026,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N10"/>
+  <dimension ref="A3:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M21" sqref="M21"/>
@@ -8607,6 +8607,294 @@
       <c r="N10" s="3" t="inlineStr">
         <is>
           <t>20250724T183822.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="D11" s="8" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="E11" s="8" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="F11" s="8" t="inlineStr">
+        <is>
+          <t>SPROUT</t>
+        </is>
+      </c>
+      <c r="G11" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H11" s="10" t="inlineStr">
+        <is>
+          <t>ER|Wahochi</t>
+        </is>
+      </c>
+      <c r="I11" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="J11" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="K11" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L11" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M11" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N11" s="10" t="inlineStr">
+        <is>
+          <t>20250726T143610.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="D12" s="8" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="E12" s="8" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="F12" s="8" t="inlineStr">
+        <is>
+          <t>SPROUT</t>
+        </is>
+      </c>
+      <c r="G12" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H12" s="10" t="inlineStr">
+        <is>
+          <t>ER|Wahochi</t>
+        </is>
+      </c>
+      <c r="I12" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="J12" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="K12" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L12" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M12" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N12" s="10" t="inlineStr">
+        <is>
+          <t>20250726T143336.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="D13" s="8" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="E13" s="8" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="F13" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="G13" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H13" s="10" t="inlineStr">
+        <is>
+          <t>ER|Wahochi</t>
+        </is>
+      </c>
+      <c r="I13" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="J13" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="K13" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L13" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M13" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N13" s="10" t="inlineStr">
+        <is>
+          <t>20250726T142559.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="7" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="B14" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C14" s="7" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="D14" s="8" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="E14" s="8" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="F14" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="G14" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H14" s="10" t="inlineStr">
+        <is>
+          <t>ER|Wahochi</t>
+        </is>
+      </c>
+      <c r="I14" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="J14" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="K14" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L14" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="M14" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="N14" s="10" t="inlineStr">
+        <is>
+          <t>20250726T142452.000Z</t>
         </is>
       </c>
     </row>
@@ -17322,7 +17610,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N68"/>
+  <dimension ref="A3:N73"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="Q30" sqref="Q30"/>
@@ -22079,6 +22367,366 @@
       <c r="N68" s="10" t="inlineStr">
         <is>
           <t>20250726T133843.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B69" s="7" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="C69" s="7" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="D69" s="8" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="E69" s="8" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="F69" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G69" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H69" s="10" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="I69" s="10" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="J69" s="10" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="K69" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="L69" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="M69" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="N69" s="10" t="inlineStr">
+        <is>
+          <t>20250726T143835.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B70" s="7" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="C70" s="7" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="D70" s="8" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="E70" s="8" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="F70" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G70" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H70" s="10" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="I70" s="10" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="J70" s="10" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="K70" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="L70" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="M70" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="N70" s="10" t="inlineStr">
+        <is>
+          <t>20250726T143637.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B71" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C71" s="7" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="D71" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E71" s="8" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="F71" s="8" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="G71" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H71" s="10" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="I71" s="10" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="J71" s="10" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="K71" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="L71" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="M71" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="N71" s="10" t="inlineStr">
+        <is>
+          <t>20250726T143101.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B72" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C72" s="7" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="D72" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E72" s="8" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="F72" s="8" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="G72" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H72" s="10" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="I72" s="10" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="J72" s="10" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="K72" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="L72" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="M72" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="N72" s="10" t="inlineStr">
+        <is>
+          <t>20250726T142849.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B73" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C73" s="7" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="D73" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="E73" s="8" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="F73" s="8" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="G73" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H73" s="10" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="I73" s="10" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="J73" s="10" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="K73" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="L73" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="M73" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="N73" s="10" t="inlineStr">
+        <is>
+          <t>20250726T142648.000Z</t>
         </is>
       </c>
     </row>
@@ -22093,7 +22741,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N84"/>
+  <dimension ref="A3:N87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R30" sqref="R30"/>
@@ -28002,6 +28650,222 @@
       <c r="N84" s="10" t="inlineStr">
         <is>
           <t>20250726T140353.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="7" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="B85" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C85" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D85" s="8" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="E85" s="8" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="F85" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G85" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H85" s="10" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="I85" s="10" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="J85" s="10" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="K85" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="L85" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="M85" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="N85" s="10" t="inlineStr">
+        <is>
+          <t>20250726T142014.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="7" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="B86" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C86" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D86" s="8" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="E86" s="8" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="F86" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G86" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H86" s="10" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="I86" s="10" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="J86" s="10" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="K86" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="L86" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="M86" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="N86" s="10" t="inlineStr">
+        <is>
+          <t>20250726T141617.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="7" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="B87" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C87" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D87" s="8" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="E87" s="8" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="F87" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G87" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H87" s="10" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="I87" s="10" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="J87" s="10" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="K87" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="L87" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="M87" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="N87" s="10" t="inlineStr">
+        <is>
+          <t>20250726T141330.000Z</t>
         </is>
       </c>
     </row>
@@ -34227,7 +35091,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N90"/>
+  <dimension ref="A3:N97"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="P38" sqref="P38"/>
@@ -40568,6 +41432,510 @@
       <c r="N90" s="10" t="inlineStr">
         <is>
           <t>20250726T134126.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="7" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="B91" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C91" s="7" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="D91" s="8" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="E91" s="8" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="F91" s="8" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="G91" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H91" s="10" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I91" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J91" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="K91" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L91" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="M91" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="N91" s="10" t="inlineStr">
+        <is>
+          <t>20250726T143928.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="7" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="B92" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C92" s="7" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="D92" s="8" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="E92" s="8" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="F92" s="8" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="G92" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H92" s="10" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I92" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J92" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="K92" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L92" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="M92" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="N92" s="10" t="inlineStr">
+        <is>
+          <t>20250726T143708.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="7" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="B93" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C93" s="7" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="D93" s="8" t="inlineStr">
+        <is>
+          <t>OLLIE</t>
+        </is>
+      </c>
+      <c r="E93" s="8" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="F93" s="8" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="G93" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H93" s="10" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I93" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J93" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="K93" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L93" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="M93" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="N93" s="10" t="inlineStr">
+        <is>
+          <t>20250726T143448.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="7" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="B94" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C94" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D94" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E94" s="8" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="F94" s="8" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="G94" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H94" s="10" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I94" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="J94" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="K94" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="L94" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="M94" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="N94" s="10" t="inlineStr">
+        <is>
+          <t>20250726T142853.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="7" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="B95" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C95" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D95" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E95" s="8" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="F95" s="8" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="G95" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H95" s="10" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I95" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="J95" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="K95" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="L95" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="M95" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="N95" s="10" t="inlineStr">
+        <is>
+          <t>20250726T142653.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="7" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="B96" s="7" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="C96" s="7" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="D96" s="8" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="E96" s="8" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="F96" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G96" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H96" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="I96" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="J96" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="K96" s="10" t="inlineStr">
+        <is>
+          <t>Refresh 🍉</t>
+        </is>
+      </c>
+      <c r="L96" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M96" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N96" s="10" t="inlineStr">
+        <is>
+          <t>20250726T143954.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="7" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="B97" s="7" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="C97" s="7" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="D97" s="8" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="E97" s="8" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="F97" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G97" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H97" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="I97" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="J97" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="K97" s="10" t="inlineStr">
+        <is>
+          <t>Refresh 🍉</t>
+        </is>
+      </c>
+      <c r="L97" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M97" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N97" s="10" t="inlineStr">
+        <is>
+          <t>20250726T143734.000Z</t>
         </is>
       </c>
     </row>
@@ -40582,7 +41950,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N101"/>
+  <dimension ref="A3:N111"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="P25" sqref="A4:P25"/>
@@ -47715,6 +49083,726 @@
       <c r="N101" s="10" t="inlineStr">
         <is>
           <t>20250726T131428.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="7" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="B102" s="7" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="C102" s="7" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D102" s="8" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="E102" s="8" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="F102" s="8" t="inlineStr">
+        <is>
+          <t>DYNAMIKE</t>
+        </is>
+      </c>
+      <c r="G102" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H102" s="10" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I102" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J102" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="K102" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L102" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="M102" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="N102" s="10" t="inlineStr">
+        <is>
+          <t>20250726T142048.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="7" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="B103" s="7" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="C103" s="7" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="D103" s="8" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="E103" s="8" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="F103" s="8" t="inlineStr">
+        <is>
+          <t>DYNAMIKE</t>
+        </is>
+      </c>
+      <c r="G103" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H103" s="10" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I103" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J103" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="K103" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L103" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="M103" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="N103" s="10" t="inlineStr">
+        <is>
+          <t>20250726T141901.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="7" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="B104" s="7" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="C104" s="7" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="D104" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="E104" s="8" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="F104" s="8" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G104" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H104" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="I104" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="J104" s="10" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="K104" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L104" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="M104" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="N104" s="10" t="inlineStr">
+        <is>
+          <t>20250726T141313.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="7" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="B105" s="7" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="C105" s="7" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="D105" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="E105" s="8" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="F105" s="8" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G105" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H105" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="I105" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="J105" s="10" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="K105" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L105" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="M105" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="N105" s="10" t="inlineStr">
+        <is>
+          <t>20250726T141102.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="7" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="B106" s="7" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="C106" s="7" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="D106" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="E106" s="8" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="F106" s="8" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="G106" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H106" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="I106" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="J106" s="10" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="K106" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="L106" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="M106" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="N106" s="10" t="inlineStr">
+        <is>
+          <t>20250726T140846.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="B107" s="7" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="C107" s="7" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="D107" s="8" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="E107" s="8" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="F107" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G107" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H107" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="I107" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="J107" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="K107" s="10" t="inlineStr">
+        <is>
+          <t>Refresh 🍉</t>
+        </is>
+      </c>
+      <c r="L107" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M107" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N107" s="10" t="inlineStr">
+        <is>
+          <t>20250726T143139.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="B108" s="7" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="C108" s="7" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="D108" s="8" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="E108" s="8" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="F108" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G108" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H108" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="I108" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="J108" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="K108" s="10" t="inlineStr">
+        <is>
+          <t>Refresh 🍉</t>
+        </is>
+      </c>
+      <c r="L108" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M108" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N108" s="10" t="inlineStr">
+        <is>
+          <t>20250726T142937.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="B109" s="7" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="C109" s="7" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="D109" s="8" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="E109" s="8" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="F109" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G109" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H109" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="I109" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="J109" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="K109" s="10" t="inlineStr">
+        <is>
+          <t>Refresh 🍉</t>
+        </is>
+      </c>
+      <c r="L109" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M109" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N109" s="10" t="inlineStr">
+        <is>
+          <t>20250726T142735.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="7" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="B110" s="7" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="C110" s="7" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="D110" s="8" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="E110" s="8" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="F110" s="8" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="G110" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H110" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="I110" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="J110" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="K110" s="10" t="inlineStr">
+        <is>
+          <t>Refresh 🍉</t>
+        </is>
+      </c>
+      <c r="L110" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M110" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N110" s="10" t="inlineStr">
+        <is>
+          <t>20250726T142150.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="7" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="B111" s="7" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="C111" s="7" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="D111" s="8" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="E111" s="8" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="F111" s="8" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="G111" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H111" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="I111" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="J111" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="K111" s="10" t="inlineStr">
+        <is>
+          <t>Refresh 🍉</t>
+        </is>
+      </c>
+      <c r="L111" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M111" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N111" s="10" t="inlineStr">
+        <is>
+          <t>20250726T141938.000Z</t>
         </is>
       </c>
     </row>
@@ -58423,7 +60511,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N65"/>
+  <dimension ref="A3:N69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R15" sqref="R15"/>
@@ -62967,6 +65055,294 @@
         </is>
       </c>
     </row>
+    <row r="66">
+      <c r="A66" s="7" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="B66" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C66" s="7" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="D66" s="8" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E66" s="8" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="F66" s="8" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="G66" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H66" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="I66" s="10" t="inlineStr">
+        <is>
+          <t>ER|Wahochi</t>
+        </is>
+      </c>
+      <c r="J66" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="K66" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L66" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M66" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N66" s="10" t="inlineStr">
+        <is>
+          <t>20250726T141718.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="7" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="B67" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C67" s="7" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="D67" s="8" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="E67" s="8" t="inlineStr">
+        <is>
+          <t>DARRYL</t>
+        </is>
+      </c>
+      <c r="F67" s="8" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="G67" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H67" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="I67" s="10" t="inlineStr">
+        <is>
+          <t>ER|Wahochi</t>
+        </is>
+      </c>
+      <c r="J67" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="K67" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="L67" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M67" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="N67" s="10" t="inlineStr">
+        <is>
+          <t>20250726T141554.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="7" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="B68" s="7" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="C68" s="7" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="D68" s="8" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="E68" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F68" s="8" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="G68" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H68" s="10" t="inlineStr">
+        <is>
+          <t>ER|Wahochi</t>
+        </is>
+      </c>
+      <c r="I68" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="J68" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="K68" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="L68" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M68" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="N68" s="10" t="inlineStr">
+        <is>
+          <t>20250726T141119.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="7" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="B69" s="7" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="C69" s="7" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="D69" s="8" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="E69" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F69" s="8" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="G69" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H69" s="10" t="inlineStr">
+        <is>
+          <t>ER|Wahochi</t>
+        </is>
+      </c>
+      <c r="I69" s="10" t="inlineStr">
+        <is>
+          <t>FG|Rujao</t>
+        </is>
+      </c>
+      <c r="J69" s="10" t="inlineStr">
+        <is>
+          <t>FG|Nem🌙·̩͙⋆͛</t>
+        </is>
+      </c>
+      <c r="K69" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Toridesu</t>
+        </is>
+      </c>
+      <c r="L69" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Danshari</t>
+        </is>
+      </c>
+      <c r="M69" s="10" t="inlineStr">
+        <is>
+          <t>FZ|Mira</t>
+        </is>
+      </c>
+      <c r="N69" s="10" t="inlineStr">
+        <is>
+          <t>20250726T140953.000Z</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-26 17:13:10)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -22741,7 +22741,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N87"/>
+  <dimension ref="A3:N93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R30" sqref="R30"/>
@@ -28866,6 +28866,438 @@
       <c r="N87" s="10" t="inlineStr">
         <is>
           <t>20250726T141330.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="B88" s="7" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C88" s="7" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="D88" s="8" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="E88" s="8" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="F88" s="8" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="G88" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H88" s="10" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I88" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J88" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="K88" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="L88" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="M88" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="N88" s="10" t="inlineStr">
+        <is>
+          <t>20250726T150435.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="B89" s="7" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C89" s="7" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="D89" s="8" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="E89" s="8" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="F89" s="8" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="G89" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H89" s="10" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I89" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J89" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="K89" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="L89" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="M89" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="N89" s="10" t="inlineStr">
+        <is>
+          <t>20250726T150217.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="7" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="B90" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C90" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D90" s="8" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="E90" s="8" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="F90" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G90" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H90" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="I90" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="J90" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="K90" s="10" t="inlineStr">
+        <is>
+          <t>Refresh 🍉</t>
+        </is>
+      </c>
+      <c r="L90" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M90" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N90" s="10" t="inlineStr">
+        <is>
+          <t>20250726T150415.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="7" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="B91" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C91" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D91" s="8" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="E91" s="8" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="F91" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="G91" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H91" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="I91" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="J91" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="K91" s="10" t="inlineStr">
+        <is>
+          <t>Refresh 🍉</t>
+        </is>
+      </c>
+      <c r="L91" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M91" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N91" s="10" t="inlineStr">
+        <is>
+          <t>20250726T150026.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="7" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="B92" s="7" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="C92" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="D92" s="8" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="E92" s="8" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="F92" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G92" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H92" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="I92" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="J92" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="K92" s="10" t="inlineStr">
+        <is>
+          <t>Refresh 🍉</t>
+        </is>
+      </c>
+      <c r="L92" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="M92" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="N92" s="10" t="inlineStr">
+        <is>
+          <t>20250726T145437.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="7" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="B93" s="7" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="C93" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="D93" s="8" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="E93" s="8" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="F93" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G93" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H93" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="I93" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="J93" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="K93" s="10" t="inlineStr">
+        <is>
+          <t>Refresh 🍉</t>
+        </is>
+      </c>
+      <c r="L93" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="M93" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="N93" s="10" t="inlineStr">
+        <is>
+          <t>20250726T145309.000Z</t>
         </is>
       </c>
     </row>
@@ -28880,7 +29312,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N88"/>
+  <dimension ref="A3:N95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="T38" sqref="T38"/>
@@ -35077,6 +35509,510 @@
       <c r="N88" s="10" t="inlineStr">
         <is>
           <t>20250726T134824.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="7" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="B89" s="7" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="C89" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D89" s="8" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="E89" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F89" s="8" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="G89" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H89" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="I89" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J89" s="10" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="K89" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="L89" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="M89" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="N89" s="10" t="inlineStr">
+        <is>
+          <t>20250726T145415.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="7" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="B90" s="7" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="C90" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D90" s="8" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="E90" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F90" s="8" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="G90" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H90" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="I90" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J90" s="10" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="K90" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="L90" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="M90" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="N90" s="10" t="inlineStr">
+        <is>
+          <t>20250726T145243.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="7" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="B91" s="7" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="C91" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D91" s="8" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="E91" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F91" s="8" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="G91" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H91" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="I91" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J91" s="10" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="K91" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="L91" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="M91" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="N91" s="10" t="inlineStr">
+        <is>
+          <t>20250726T145056.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="7" t="inlineStr">
+        <is>
+          <t>JESSIE</t>
+        </is>
+      </c>
+      <c r="B92" s="7" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="C92" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D92" s="8" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E92" s="8" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="F92" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G92" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H92" s="10" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I92" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J92" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="K92" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="L92" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="M92" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="N92" s="10" t="inlineStr">
+        <is>
+          <t>20250726T144615.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="7" t="inlineStr">
+        <is>
+          <t>JESSIE</t>
+        </is>
+      </c>
+      <c r="B93" s="7" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="C93" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D93" s="8" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="E93" s="8" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="F93" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G93" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H93" s="10" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="I93" s="10" t="inlineStr">
+        <is>
+          <t>あの頃のしずく👍</t>
+        </is>
+      </c>
+      <c r="J93" s="10" t="inlineStr">
+        <is>
+          <t>ZETA|Levi</t>
+        </is>
+      </c>
+      <c r="K93" s="10" t="inlineStr">
+        <is>
+          <t>RVL|I see</t>
+        </is>
+      </c>
+      <c r="L93" s="10" t="inlineStr">
+        <is>
+          <t>RVL|Terry</t>
+        </is>
+      </c>
+      <c r="M93" s="10" t="inlineStr">
+        <is>
+          <t>Mameshi</t>
+        </is>
+      </c>
+      <c r="N93" s="10" t="inlineStr">
+        <is>
+          <t>20250726T144424.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="7" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="B94" s="7" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="C94" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D94" s="8" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="E94" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F94" s="8" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="G94" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H94" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="I94" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="J94" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="K94" s="10" t="inlineStr">
+        <is>
+          <t>Refresh 🍉</t>
+        </is>
+      </c>
+      <c r="L94" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M94" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N94" s="10" t="inlineStr">
+        <is>
+          <t>20250726T151040.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="7" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="B95" s="7" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="C95" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D95" s="8" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="E95" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F95" s="8" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="G95" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H95" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="I95" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="J95" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="K95" s="10" t="inlineStr">
+        <is>
+          <t>Refresh 🍉</t>
+        </is>
+      </c>
+      <c r="L95" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M95" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N95" s="10" t="inlineStr">
+        <is>
+          <t>20250726T150929.000Z</t>
         </is>
       </c>
     </row>
@@ -35091,7 +36027,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N97"/>
+  <dimension ref="A3:N99"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="P38" sqref="P38"/>
@@ -41936,6 +42872,150 @@
       <c r="N97" s="10" t="inlineStr">
         <is>
           <t>20250726T143734.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="7" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="B98" s="7" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="C98" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D98" s="8" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="E98" s="8" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="F98" s="8" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="G98" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H98" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="I98" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="J98" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="K98" s="10" t="inlineStr">
+        <is>
+          <t>Refresh 🍉</t>
+        </is>
+      </c>
+      <c r="L98" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M98" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N98" s="10" t="inlineStr">
+        <is>
+          <t>20250726T144839.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="7" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="B99" s="7" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="C99" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="D99" s="8" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="E99" s="8" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="F99" s="8" t="inlineStr">
+        <is>
+          <t>BUSTER</t>
+        </is>
+      </c>
+      <c r="G99" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H99" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="I99" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="J99" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="K99" s="10" t="inlineStr">
+        <is>
+          <t>Refresh 🍉</t>
+        </is>
+      </c>
+      <c r="L99" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M99" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N99" s="10" t="inlineStr">
+        <is>
+          <t>20250726T144619.000Z</t>
         </is>
       </c>
     </row>
@@ -41950,7 +43030,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N111"/>
+  <dimension ref="A3:N116"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="P25" sqref="A4:P25"/>
@@ -49803,6 +50883,366 @@
       <c r="N111" s="10" t="inlineStr">
         <is>
           <t>20250726T141938.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="7" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="B112" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C112" s="7" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="D112" s="8" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="E112" s="8" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F112" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G112" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H112" s="10" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="I112" s="10" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="J112" s="10" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="K112" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="L112" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="M112" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="N112" s="10" t="inlineStr">
+        <is>
+          <t>20250726T145821.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="7" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="B113" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C113" s="7" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="D113" s="8" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="E113" s="8" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F113" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G113" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H113" s="10" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="I113" s="10" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="J113" s="10" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="K113" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="L113" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="M113" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="N113" s="10" t="inlineStr">
+        <is>
+          <t>20250726T145603.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="7" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="B114" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C114" s="7" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="D114" s="8" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="E114" s="8" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="F114" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G114" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H114" s="10" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="I114" s="10" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="J114" s="10" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="K114" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="L114" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="M114" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="N114" s="10" t="inlineStr">
+        <is>
+          <t>20250726T145412.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="7" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="B115" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C115" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D115" s="8" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="E115" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F115" s="8" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="G115" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H115" s="10" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="I115" s="10" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="J115" s="10" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="K115" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="L115" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="M115" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="N115" s="10" t="inlineStr">
+        <is>
+          <t>20250726T144813.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="7" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="B116" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C116" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D116" s="8" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="E116" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F116" s="8" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="G116" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H116" s="10" t="inlineStr">
+        <is>
+          <t>CR|Milkreo</t>
+        </is>
+      </c>
+      <c r="I116" s="10" t="inlineStr">
+        <is>
+          <t>CR|Moya</t>
+        </is>
+      </c>
+      <c r="J116" s="10" t="inlineStr">
+        <is>
+          <t>Tensai 천재</t>
+        </is>
+      </c>
+      <c r="K116" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Achapi</t>
+        </is>
+      </c>
+      <c r="L116" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Ryohei</t>
+        </is>
+      </c>
+      <c r="M116" s="10" t="inlineStr">
+        <is>
+          <t>NAVI|Kuru</t>
+        </is>
+      </c>
+      <c r="N116" s="10" t="inlineStr">
+        <is>
+          <t>20250726T144542.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-26 17:44:31)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -17610,7 +17610,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N73"/>
+  <dimension ref="A3:N77"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="Q30" sqref="Q30"/>
@@ -22727,6 +22727,294 @@
       <c r="N73" s="10" t="inlineStr">
         <is>
           <t>20250726T142648.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="7" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="B74" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="C74" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="D74" s="8" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="E74" s="8" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="F74" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G74" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H74" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="I74" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="J74" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="K74" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="L74" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M74" s="10" t="inlineStr">
+        <is>
+          <t>Refresh 🍉</t>
+        </is>
+      </c>
+      <c r="N74" s="10" t="inlineStr">
+        <is>
+          <t>20250726T153301.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="7" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="B75" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="C75" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="D75" s="8" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="E75" s="8" t="inlineStr">
+        <is>
+          <t>ALLI</t>
+        </is>
+      </c>
+      <c r="F75" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G75" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H75" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="I75" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="J75" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="K75" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="L75" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M75" s="10" t="inlineStr">
+        <is>
+          <t>Refresh 🍉</t>
+        </is>
+      </c>
+      <c r="N75" s="10" t="inlineStr">
+        <is>
+          <t>20250726T153107.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="7" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="B76" s="7" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="C76" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D76" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="E76" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F76" s="8" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="G76" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H76" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="I76" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="J76" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="K76" s="10" t="inlineStr">
+        <is>
+          <t>Refresh 🍉</t>
+        </is>
+      </c>
+      <c r="L76" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M76" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N76" s="10" t="inlineStr">
+        <is>
+          <t>20250726T152540.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="7" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="B77" s="7" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="C77" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D77" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="E77" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="F77" s="8" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="G77" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H77" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="I77" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="J77" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="K77" s="10" t="inlineStr">
+        <is>
+          <t>Refresh 🍉</t>
+        </is>
+      </c>
+      <c r="L77" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M77" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N77" s="10" t="inlineStr">
+        <is>
+          <t>20250726T152248.000Z</t>
         </is>
       </c>
     </row>
@@ -29312,7 +29600,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N95"/>
+  <dimension ref="A3:N97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="T38" sqref="T38"/>
@@ -36013,6 +36301,150 @@
       <c r="N95" s="10" t="inlineStr">
         <is>
           <t>20250726T150929.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="7" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="B96" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C96" s="7" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="D96" s="8" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="E96" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="F96" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G96" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H96" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="I96" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="J96" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="K96" s="10" t="inlineStr">
+        <is>
+          <t>Refresh 🍉</t>
+        </is>
+      </c>
+      <c r="L96" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M96" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N96" s="10" t="inlineStr">
+        <is>
+          <t>20250726T151653.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="7" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="B97" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C97" s="7" t="inlineStr">
+        <is>
+          <t>CHUCK</t>
+        </is>
+      </c>
+      <c r="D97" s="8" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="E97" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="F97" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G97" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H97" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Angelboy</t>
+        </is>
+      </c>
+      <c r="I97" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maury</t>
+        </is>
+      </c>
+      <c r="J97" s="10" t="inlineStr">
+        <is>
+          <t>TTM|Maru</t>
+        </is>
+      </c>
+      <c r="K97" s="10" t="inlineStr">
+        <is>
+          <t>Refresh 🍉</t>
+        </is>
+      </c>
+      <c r="L97" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M97" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N97" s="10" t="inlineStr">
+        <is>
+          <t>20250726T151520.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-26 18:15:55)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -43462,7 +43462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N116"/>
+  <dimension ref="A3:N118"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="P25" sqref="A4:P25"/>
@@ -51675,6 +51675,150 @@
       <c r="N116" s="10" t="inlineStr">
         <is>
           <t>20250726T144542.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B117" s="7" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="C117" s="7" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="D117" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="E117" s="8" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="F117" s="8" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="G117" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H117" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="I117" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J117" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="K117" s="10" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L117" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M117" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N117" s="10" t="inlineStr">
+        <is>
+          <t>20250726T161231.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B118" s="7" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="C118" s="7" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="D118" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="E118" s="8" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="F118" s="8" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="G118" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H118" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="I118" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J118" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="K118" s="10" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L118" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M118" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N118" s="10" t="inlineStr">
+        <is>
+          <t>20250726T161034.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-26 18:47:17)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -29600,7 +29600,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N97"/>
+  <dimension ref="A3:N98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="T38" sqref="T38"/>
@@ -36445,6 +36445,78 @@
       <c r="N97" s="10" t="inlineStr">
         <is>
           <t>20250726T151520.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B98" s="7" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="C98" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D98" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E98" s="8" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="F98" s="8" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="G98" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H98" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I98" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J98" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K98" s="10" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L98" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M98" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N98" s="10" t="inlineStr">
+        <is>
+          <t>20250726T164603.000Z</t>
         </is>
       </c>
     </row>
@@ -36459,7 +36531,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N99"/>
+  <dimension ref="A3:N104"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="P38" sqref="P38"/>
@@ -43448,6 +43520,366 @@
       <c r="N99" s="10" t="inlineStr">
         <is>
           <t>20250726T144619.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="7" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="B100" s="7" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="C100" s="7" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="D100" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E100" s="8" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="F100" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G100" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H100" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I100" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J100" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K100" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="L100" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="M100" s="10" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="N100" s="10" t="inlineStr">
+        <is>
+          <t>20250726T164108.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="7" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="B101" s="7" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="C101" s="7" t="inlineStr">
+        <is>
+          <t>BELLE</t>
+        </is>
+      </c>
+      <c r="D101" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E101" s="8" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="F101" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G101" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H101" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I101" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J101" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K101" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="L101" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="M101" s="10" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="N101" s="10" t="inlineStr">
+        <is>
+          <t>20250726T163859.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B102" s="7" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="C102" s="7" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="D102" s="8" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="E102" s="8" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="F102" s="8" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="G102" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H102" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I102" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J102" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K102" s="10" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L102" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M102" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N102" s="10" t="inlineStr">
+        <is>
+          <t>20250726T163254.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B103" s="7" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="C103" s="7" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="D103" s="8" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="E103" s="8" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="F103" s="8" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="G103" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H103" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I103" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J103" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K103" s="10" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L103" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M103" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N103" s="10" t="inlineStr">
+        <is>
+          <t>20250726T163034.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B104" s="7" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="C104" s="7" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="D104" s="8" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="E104" s="8" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="F104" s="8" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="G104" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H104" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I104" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="J104" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="K104" s="10" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L104" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M104" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N104" s="10" t="inlineStr">
+        <is>
+          <t>20250726T162856.000Z</t>
         </is>
       </c>
     </row>
@@ -43462,7 +43894,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N118"/>
+  <dimension ref="A3:N121"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="P25" sqref="A4:P25"/>
@@ -51819,6 +52251,222 @@
       <c r="N118" s="10" t="inlineStr">
         <is>
           <t>20250726T161034.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B119" s="7" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C119" s="7" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D119" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E119" s="8" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="F119" s="8" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="G119" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H119" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I119" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J119" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K119" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="L119" s="10" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="M119" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N119" s="10" t="inlineStr">
+        <is>
+          <t>20250726T162249.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B120" s="7" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C120" s="7" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D120" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E120" s="8" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="F120" s="8" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="G120" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H120" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I120" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J120" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K120" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="L120" s="10" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="M120" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N120" s="10" t="inlineStr">
+        <is>
+          <t>20250726T162027.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B121" s="7" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C121" s="7" t="inlineStr">
+        <is>
+          <t>LOU</t>
+        </is>
+      </c>
+      <c r="D121" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E121" s="8" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="F121" s="8" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="G121" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H121" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I121" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J121" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K121" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="L121" s="10" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="M121" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N121" s="10" t="inlineStr">
+        <is>
+          <t>20250726T161803.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-26 19:18:56)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -500,7 +500,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N91"/>
+  <dimension ref="A3:N94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P16" sqref="A4:P16"/>
@@ -6913,6 +6913,222 @@
       <c r="N91" s="10" t="inlineStr">
         <is>
           <t>20250726T124720.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="7" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="B92" s="7" t="inlineStr">
+        <is>
+          <t>SPROUT</t>
+        </is>
+      </c>
+      <c r="C92" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D92" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E92" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F92" s="8" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="G92" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H92" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I92" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J92" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K92" s="10" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L92" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M92" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N92" s="10" t="inlineStr">
+        <is>
+          <t>20250726T171216.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="7" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="B93" s="7" t="inlineStr">
+        <is>
+          <t>SPROUT</t>
+        </is>
+      </c>
+      <c r="C93" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D93" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E93" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F93" s="8" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="G93" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H93" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I93" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J93" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K93" s="10" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L93" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M93" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N93" s="10" t="inlineStr">
+        <is>
+          <t>20250726T170926.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="7" t="inlineStr">
+        <is>
+          <t>MEG</t>
+        </is>
+      </c>
+      <c r="B94" s="7" t="inlineStr">
+        <is>
+          <t>SPROUT</t>
+        </is>
+      </c>
+      <c r="C94" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D94" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E94" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="F94" s="8" t="inlineStr">
+        <is>
+          <t>JUJU</t>
+        </is>
+      </c>
+      <c r="G94" s="12" t="inlineStr">
+        <is>
+          <t>Empate</t>
+        </is>
+      </c>
+      <c r="H94" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I94" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J94" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K94" s="10" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L94" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M94" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N94" s="10" t="inlineStr">
+        <is>
+          <t>20250726T170637.000Z</t>
         </is>
       </c>
     </row>
@@ -29600,7 +29816,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N98"/>
+  <dimension ref="A3:N102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="T38" sqref="T38"/>
@@ -36517,6 +36733,294 @@
       <c r="N98" s="10" t="inlineStr">
         <is>
           <t>20250726T164603.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="7" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="B99" s="7" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="C99" s="7" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="D99" s="8" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="E99" s="8" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="F99" s="8" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="G99" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H99" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I99" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J99" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K99" s="10" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L99" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="M99" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="N99" s="10" t="inlineStr">
+        <is>
+          <t>20250726T165906.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="7" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="B100" s="7" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="C100" s="7" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="D100" s="8" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="E100" s="8" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="F100" s="8" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="G100" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H100" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I100" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J100" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K100" s="10" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L100" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="M100" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="N100" s="10" t="inlineStr">
+        <is>
+          <t>20250726T165744.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="7" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="B101" s="7" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="C101" s="7" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="D101" s="8" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="E101" s="8" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="F101" s="8" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="G101" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H101" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I101" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J101" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K101" s="10" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L101" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="M101" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="N101" s="10" t="inlineStr">
+        <is>
+          <t>20250726T165454.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="B102" s="7" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="C102" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D102" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E102" s="8" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="F102" s="8" t="inlineStr">
+        <is>
+          <t>EMZ</t>
+        </is>
+      </c>
+      <c r="G102" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H102" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I102" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J102" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K102" s="10" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L102" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="M102" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="N102" s="10" t="inlineStr">
+        <is>
+          <t>20250726T164737.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-26 19:50:40)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -500,7 +500,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N94"/>
+  <dimension ref="A3:N96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P16" sqref="A4:P16"/>
@@ -7129,6 +7129,150 @@
       <c r="N94" s="10" t="inlineStr">
         <is>
           <t>20250726T170637.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B95" s="7" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="C95" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D95" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E95" s="8" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="F95" s="8" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="G95" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H95" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I95" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J95" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K95" s="10" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L95" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="M95" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="N95" s="10" t="inlineStr">
+        <is>
+          <t>20250726T172123.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B96" s="7" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="C96" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D96" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="E96" s="8" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="F96" s="8" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="G96" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H96" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Subeme</t>
+        </is>
+      </c>
+      <c r="I96" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Marco</t>
+        </is>
+      </c>
+      <c r="J96" s="10" t="inlineStr">
+        <is>
+          <t>NOVO|Biso</t>
+        </is>
+      </c>
+      <c r="K96" s="10" t="inlineStr">
+        <is>
+          <t>Enraged 💔</t>
+        </is>
+      </c>
+      <c r="L96" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Tomzy</t>
+        </is>
+      </c>
+      <c r="M96" s="10" t="inlineStr">
+        <is>
+          <t>SUP|Filippo神</t>
+        </is>
+      </c>
+      <c r="N96" s="10" t="inlineStr">
+        <is>
+          <t>20250726T171827.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-26 22:50:15)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -17970,7 +17970,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N77"/>
+  <dimension ref="A3:N82"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="Q30" sqref="Q30"/>
@@ -23375,6 +23375,366 @@
       <c r="N77" s="10" t="inlineStr">
         <is>
           <t>20250726T152248.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B78" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="C78" s="7" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="D78" s="8" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="E78" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F78" s="8" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G78" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H78" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I78" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="J78" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="K78" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L78" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="M78" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="N78" s="10" t="inlineStr">
+        <is>
+          <t>20250726T204323.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B79" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="C79" s="7" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="D79" s="8" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="E79" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F79" s="8" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G79" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H79" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I79" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="J79" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="K79" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L79" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="M79" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="N79" s="10" t="inlineStr">
+        <is>
+          <t>20250726T204115.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="B80" s="7" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="C80" s="7" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="D80" s="8" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="E80" s="8" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F80" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="G80" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H80" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="I80" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="J80" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="K80" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="L80" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="M80" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="N80" s="10" t="inlineStr">
+        <is>
+          <t>20250726T203608.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="7" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="B81" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C81" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D81" s="8" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E81" s="8" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="F81" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G81" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H81" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I81" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="J81" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="K81" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L81" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="M81" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="N81" s="10" t="inlineStr">
+        <is>
+          <t>20250726T203346.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="7" t="inlineStr">
+        <is>
+          <t>KENJI</t>
+        </is>
+      </c>
+      <c r="B82" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="C82" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D82" s="8" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E82" s="8" t="inlineStr">
+        <is>
+          <t>STU</t>
+        </is>
+      </c>
+      <c r="F82" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G82" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H82" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I82" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="J82" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="K82" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L82" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="M82" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="N82" s="10" t="inlineStr">
+        <is>
+          <t>20250726T203125.000Z</t>
         </is>
       </c>
     </row>
@@ -57684,7 +58044,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N87"/>
+  <dimension ref="A3:N88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P15" sqref="A4:P15"/>
@@ -63809,6 +64169,78 @@
       <c r="N87" s="10" t="inlineStr">
         <is>
           <t>20250726T130615.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B88" s="7" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="C88" s="7" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="D88" s="8" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="E88" s="8" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F88" s="8" t="inlineStr">
+        <is>
+          <t>POCO</t>
+        </is>
+      </c>
+      <c r="G88" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H88" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I88" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="J88" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="K88" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L88" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="M88" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="N88" s="10" t="inlineStr">
+        <is>
+          <t>20250726T204953.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-26 23:21:39)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -10296,7 +10296,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N21"/>
+  <dimension ref="A3:N25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
@@ -11669,6 +11669,294 @@
       <c r="N21" s="10" t="inlineStr">
         <is>
           <t>20250726T005121.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B22" s="7" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="C22" s="7" t="inlineStr">
+        <is>
+          <t>EDGAR</t>
+        </is>
+      </c>
+      <c r="D22" s="8" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="E22" s="8" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F22" s="8" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="G22" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H22" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I22" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="J22" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="K22" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L22" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="M22" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="N22" s="10" t="inlineStr">
+        <is>
+          <t>20250726T211805.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B23" s="7" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="C23" s="7" t="inlineStr">
+        <is>
+          <t>EDGAR</t>
+        </is>
+      </c>
+      <c r="D23" s="8" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="E23" s="8" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F23" s="8" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="G23" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H23" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I23" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="J23" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="K23" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L23" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="M23" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="N23" s="10" t="inlineStr">
+        <is>
+          <t>20250726T211559.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="7" t="inlineStr">
+        <is>
+          <t>DYNAMIKE</t>
+        </is>
+      </c>
+      <c r="B24" s="7" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C24" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="D24" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="E24" s="8" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F24" s="8" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G24" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H24" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I24" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="J24" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="K24" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L24" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="M24" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="N24" s="10" t="inlineStr">
+        <is>
+          <t>20250726T211014.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="7" t="inlineStr">
+        <is>
+          <t>DYNAMIKE</t>
+        </is>
+      </c>
+      <c r="B25" s="7" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="C25" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="D25" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="E25" s="8" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F25" s="8" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G25" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H25" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I25" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="J25" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="K25" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L25" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="M25" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="N25" s="10" t="inlineStr">
+        <is>
+          <t>20250726T210758.000Z</t>
         </is>
       </c>
     </row>
@@ -58044,7 +58332,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N88"/>
+  <dimension ref="A3:N92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P15" sqref="A4:P15"/>
@@ -64241,6 +64529,294 @@
       <c r="N88" s="10" t="inlineStr">
         <is>
           <t>20250726T204953.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B89" s="7" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="C89" s="7" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="D89" s="8" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="E89" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F89" s="8" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G89" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H89" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I89" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="J89" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="K89" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L89" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="M89" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="N89" s="10" t="inlineStr">
+        <is>
+          <t>20250726T210251.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B90" s="7" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="C90" s="7" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="D90" s="8" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="E90" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F90" s="8" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G90" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H90" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I90" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="J90" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="K90" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L90" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="M90" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="N90" s="10" t="inlineStr">
+        <is>
+          <t>20250726T210041.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B91" s="7" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="C91" s="7" t="inlineStr">
+        <is>
+          <t>BONNIE</t>
+        </is>
+      </c>
+      <c r="D91" s="8" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="E91" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F91" s="8" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G91" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H91" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I91" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="J91" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="K91" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L91" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="M91" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="N91" s="10" t="inlineStr">
+        <is>
+          <t>20250726T205814.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B92" s="7" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="C92" s="7" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="D92" s="8" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="E92" s="8" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F92" s="8" t="inlineStr">
+        <is>
+          <t>POCO</t>
+        </is>
+      </c>
+      <c r="G92" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H92" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I92" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="J92" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="K92" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L92" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="M92" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="N92" s="10" t="inlineStr">
+        <is>
+          <t>20250726T205220.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-26 23:53:05)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -7287,7 +7287,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N17"/>
+  <dimension ref="A3:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P7" sqref="A4:P7"/>
@@ -8372,6 +8372,366 @@
       <c r="N17" s="10" t="inlineStr">
         <is>
           <t>20250725T163402.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B18" s="7" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="C18" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="D18" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E18" s="8" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="F18" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G18" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H18" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I18" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="J18" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="K18" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="L18" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="M18" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="N18" s="10" t="inlineStr">
+        <is>
+          <t>20250726T214104.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="B19" s="7" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="C19" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="D19" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="E19" s="8" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="F19" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="G19" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H19" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I19" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="J19" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="K19" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="L19" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="M19" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="N19" s="10" t="inlineStr">
+        <is>
+          <t>20250726T213840.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B20" s="7" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="C20" s="7" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="D20" s="8" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="E20" s="8" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="F20" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="G20" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H20" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I20" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="J20" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="K20" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L20" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="M20" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="N20" s="10" t="inlineStr">
+        <is>
+          <t>20250726T212647.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B21" s="7" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="C21" s="7" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="D21" s="8" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="E21" s="8" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="F21" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="G21" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H21" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I21" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="J21" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="K21" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L21" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="M21" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="N21" s="10" t="inlineStr">
+        <is>
+          <t>20250726T212532.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="B22" s="7" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="C22" s="7" t="inlineStr">
+        <is>
+          <t>SPIKE</t>
+        </is>
+      </c>
+      <c r="D22" s="8" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="E22" s="8" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="F22" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="G22" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H22" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I22" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="J22" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="K22" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L22" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="M22" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="N22" s="10" t="inlineStr">
+        <is>
+          <t>20250726T212422.000Z</t>
         </is>
       </c>
     </row>
@@ -9269,7 +9629,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N16"/>
+  <dimension ref="A3:N19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N19" sqref="N19"/>
@@ -10282,6 +10642,222 @@
       <c r="N16" s="10" t="inlineStr">
         <is>
           <t>20250726T134941.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="7" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="B17" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C17" s="7" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="D17" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E17" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F17" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G17" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H17" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I17" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="J17" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="K17" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L17" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="M17" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="N17" s="10" t="inlineStr">
+        <is>
+          <t>20250726T215010.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="7" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="B18" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C18" s="7" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="D18" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E18" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F18" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G18" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H18" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I18" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="J18" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="K18" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L18" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="M18" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="N18" s="10" t="inlineStr">
+        <is>
+          <t>20250726T214802.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="7" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="B19" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C19" s="7" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="D19" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E19" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="F19" s="8" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="G19" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H19" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I19" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="J19" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="K19" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L19" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="M19" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="N19" s="10" t="inlineStr">
+        <is>
+          <t>20250726T215300.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-27 00:24:25)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -500,7 +500,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N96"/>
+  <dimension ref="A3:N98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P16" sqref="A4:P16"/>
@@ -7273,6 +7273,150 @@
       <c r="N96" s="10" t="inlineStr">
         <is>
           <t>20250726T171827.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="7" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="B97" s="7" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="C97" s="7" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="D97" s="8" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="E97" s="8" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F97" s="8" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="G97" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H97" s="10" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="I97" s="10" t="inlineStr">
+        <is>
+          <t>KCP|Zoulan</t>
+        </is>
+      </c>
+      <c r="J97" s="10" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="K97" s="10" t="inlineStr">
+        <is>
+          <t>second❤️lena</t>
+        </is>
+      </c>
+      <c r="L97" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Memxn</t>
+        </is>
+      </c>
+      <c r="M97" s="10" t="inlineStr">
+        <is>
+          <t>CODE|OG</t>
+        </is>
+      </c>
+      <c r="N97" s="10" t="inlineStr">
+        <is>
+          <t>20250726T220300.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="7" t="inlineStr">
+        <is>
+          <t>LARRY &amp; LAWRIE</t>
+        </is>
+      </c>
+      <c r="B98" s="7" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="C98" s="7" t="inlineStr">
+        <is>
+          <t>SHADE</t>
+        </is>
+      </c>
+      <c r="D98" s="8" t="inlineStr">
+        <is>
+          <t>BUZZ</t>
+        </is>
+      </c>
+      <c r="E98" s="8" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="F98" s="8" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="G98" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H98" s="10" t="inlineStr">
+        <is>
+          <t>KCP|Fade</t>
+        </is>
+      </c>
+      <c r="I98" s="10" t="inlineStr">
+        <is>
+          <t>KCP|Zoulan</t>
+        </is>
+      </c>
+      <c r="J98" s="10" t="inlineStr">
+        <is>
+          <t>KCP|Tyrant</t>
+        </is>
+      </c>
+      <c r="K98" s="10" t="inlineStr">
+        <is>
+          <t>second❤️lena</t>
+        </is>
+      </c>
+      <c r="L98" s="10" t="inlineStr">
+        <is>
+          <t>ETN|Memxn</t>
+        </is>
+      </c>
+      <c r="M98" s="10" t="inlineStr">
+        <is>
+          <t>CODE|OG</t>
+        </is>
+      </c>
+      <c r="N98" s="10" t="inlineStr">
+        <is>
+          <t>20250726T220017.000Z</t>
         </is>
       </c>
     </row>
@@ -8746,7 +8890,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N14"/>
+  <dimension ref="A3:N19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M21" sqref="M21"/>
@@ -9615,6 +9759,366 @@
       <c r="N14" s="10" t="inlineStr">
         <is>
           <t>20250726T142452.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="7" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="B15" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C15" s="7" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="D15" s="8" t="inlineStr">
+        <is>
+          <t>SPROUT</t>
+        </is>
+      </c>
+      <c r="E15" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="F15" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="G15" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H15" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I15" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="J15" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="K15" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L15" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="M15" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="N15" s="10" t="inlineStr">
+        <is>
+          <t>20250726T222346.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="7" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="B16" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C16" s="7" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="D16" s="8" t="inlineStr">
+        <is>
+          <t>SPROUT</t>
+        </is>
+      </c>
+      <c r="E16" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="F16" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="G16" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H16" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I16" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="J16" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="K16" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L16" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="M16" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="N16" s="10" t="inlineStr">
+        <is>
+          <t>20250726T222145.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="7" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="B17" s="7" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="C17" s="7" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="D17" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="E17" s="8" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="F17" s="8" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="G17" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H17" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I17" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="J17" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="K17" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L17" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="M17" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="N17" s="10" t="inlineStr">
+        <is>
+          <t>20250726T221541.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="7" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="B18" s="7" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="C18" s="7" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="D18" s="8" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="E18" s="8" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="F18" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="G18" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H18" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I18" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="J18" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="K18" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L18" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="M18" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="N18" s="10" t="inlineStr">
+        <is>
+          <t>20250726T221209.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="7" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="B19" s="7" t="inlineStr">
+        <is>
+          <t>BROCK</t>
+        </is>
+      </c>
+      <c r="C19" s="7" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="D19" s="8" t="inlineStr">
+        <is>
+          <t>BYRON</t>
+        </is>
+      </c>
+      <c r="E19" s="8" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="F19" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="G19" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H19" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I19" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="J19" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="K19" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L19" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="M19" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="N19" s="10" t="inlineStr">
+        <is>
+          <t>20250726T220918.000Z</t>
         </is>
       </c>
     </row>
@@ -9629,7 +10133,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N19"/>
+  <dimension ref="A3:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N19" sqref="N19"/>
@@ -10858,6 +11362,150 @@
       <c r="N19" s="10" t="inlineStr">
         <is>
           <t>20250726T215300.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="7" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="B20" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C20" s="7" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="D20" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E20" s="8" t="inlineStr">
+        <is>
+          <t>8-BIT</t>
+        </is>
+      </c>
+      <c r="F20" s="8" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="G20" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H20" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I20" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="J20" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="K20" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L20" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="M20" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="N20" s="10" t="inlineStr">
+        <is>
+          <t>20250726T220148.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="7" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="B21" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C21" s="7" t="inlineStr">
+        <is>
+          <t>GRIFF</t>
+        </is>
+      </c>
+      <c r="D21" s="8" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="E21" s="8" t="inlineStr">
+        <is>
+          <t>8-BIT</t>
+        </is>
+      </c>
+      <c r="F21" s="8" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="G21" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H21" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I21" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="J21" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="K21" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L21" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="M21" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="N21" s="10" t="inlineStr">
+        <is>
+          <t>20250726T215857.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-27 00:55:52)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -8890,7 +8890,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N19"/>
+  <dimension ref="A3:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M21" sqref="M21"/>
@@ -10119,6 +10119,150 @@
       <c r="N19" s="10" t="inlineStr">
         <is>
           <t>20250726T220918.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="B20" s="7" t="inlineStr">
+        <is>
+          <t>SPROUT</t>
+        </is>
+      </c>
+      <c r="C20" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="D20" s="8" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="E20" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F20" s="8" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="G20" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H20" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I20" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="J20" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="K20" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L20" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="M20" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="N20" s="10" t="inlineStr">
+        <is>
+          <t>20250726T223146.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="7" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="B21" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="C21" s="7" t="inlineStr">
+        <is>
+          <t>SQUEAK</t>
+        </is>
+      </c>
+      <c r="D21" s="8" t="inlineStr">
+        <is>
+          <t>SPROUT</t>
+        </is>
+      </c>
+      <c r="E21" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="F21" s="8" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="G21" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H21" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="I21" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="J21" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="K21" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="L21" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="M21" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="N21" s="10" t="inlineStr">
+        <is>
+          <t>20250726T222734.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-27 01:27:13)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -500,7 +500,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N98"/>
+  <dimension ref="A3:N100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P16" sqref="A4:P16"/>
@@ -7417,6 +7417,150 @@
       <c r="N98" s="10" t="inlineStr">
         <is>
           <t>20250726T220017.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B99" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C99" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D99" s="8" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="E99" s="8" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="F99" s="8" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="G99" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H99" s="10" t="inlineStr">
+        <is>
+          <t>FX|CaueBr</t>
+        </is>
+      </c>
+      <c r="I99" s="10" t="inlineStr">
+        <is>
+          <t>FX|Wesley</t>
+        </is>
+      </c>
+      <c r="J99" s="10" t="inlineStr">
+        <is>
+          <t>FX|REI DO FUT</t>
+        </is>
+      </c>
+      <c r="K99" s="10" t="inlineStr">
+        <is>
+          <t>Satisfyer🌺</t>
+        </is>
+      </c>
+      <c r="L99" s="10" t="inlineStr">
+        <is>
+          <t>Bicho🐦‍🔥</t>
+        </is>
+      </c>
+      <c r="M99" s="10" t="inlineStr">
+        <is>
+          <t>Fv7🐦‍🔥</t>
+        </is>
+      </c>
+      <c r="N99" s="10" t="inlineStr">
+        <is>
+          <t>20250726T231156.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="B100" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C100" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D100" s="8" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="E100" s="8" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="F100" s="8" t="inlineStr">
+        <is>
+          <t>FRANK</t>
+        </is>
+      </c>
+      <c r="G100" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H100" s="10" t="inlineStr">
+        <is>
+          <t>FX|CaueBr</t>
+        </is>
+      </c>
+      <c r="I100" s="10" t="inlineStr">
+        <is>
+          <t>FX|Wesley</t>
+        </is>
+      </c>
+      <c r="J100" s="10" t="inlineStr">
+        <is>
+          <t>FX|REI DO FUT</t>
+        </is>
+      </c>
+      <c r="K100" s="10" t="inlineStr">
+        <is>
+          <t>Satisfyer🌺</t>
+        </is>
+      </c>
+      <c r="L100" s="10" t="inlineStr">
+        <is>
+          <t>Bicho🐦‍🔥</t>
+        </is>
+      </c>
+      <c r="M100" s="10" t="inlineStr">
+        <is>
+          <t>Fv7🐦‍🔥</t>
+        </is>
+      </c>
+      <c r="N100" s="10" t="inlineStr">
+        <is>
+          <t>20250726T230911.000Z</t>
         </is>
       </c>
     </row>
@@ -7431,7 +7575,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N22"/>
+  <dimension ref="A3:N25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P7" sqref="A4:P7"/>
@@ -8876,6 +9020,222 @@
       <c r="N22" s="10" t="inlineStr">
         <is>
           <t>20250726T212422.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="7" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="B23" s="7" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="C23" s="7" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="D23" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E23" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="F23" s="8" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="G23" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H23" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Derrp</t>
+        </is>
+      </c>
+      <c r="I23" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Jubileubr</t>
+        </is>
+      </c>
+      <c r="J23" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Loko</t>
+        </is>
+      </c>
+      <c r="K23" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="L23" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="M23" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="N23" s="10" t="inlineStr">
+        <is>
+          <t>20250726T232131.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="7" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="B24" s="7" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="C24" s="7" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="D24" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E24" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="F24" s="8" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="G24" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H24" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Derrp</t>
+        </is>
+      </c>
+      <c r="I24" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Jubileubr</t>
+        </is>
+      </c>
+      <c r="J24" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Loko</t>
+        </is>
+      </c>
+      <c r="K24" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="L24" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="M24" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="N24" s="10" t="inlineStr">
+        <is>
+          <t>20250726T231840.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="7" t="inlineStr">
+        <is>
+          <t>BEA</t>
+        </is>
+      </c>
+      <c r="B25" s="7" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="C25" s="7" t="inlineStr">
+        <is>
+          <t>RICO</t>
+        </is>
+      </c>
+      <c r="D25" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="E25" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="F25" s="8" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="G25" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H25" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Derrp</t>
+        </is>
+      </c>
+      <c r="I25" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Jubileubr</t>
+        </is>
+      </c>
+      <c r="J25" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Loko</t>
+        </is>
+      </c>
+      <c r="K25" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="L25" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="M25" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="N25" s="10" t="inlineStr">
+        <is>
+          <t>20250726T231633.000Z</t>
         </is>
       </c>
     </row>
@@ -11664,7 +12024,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N25"/>
+  <dimension ref="A3:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
@@ -13325,6 +13685,222 @@
       <c r="N25" s="10" t="inlineStr">
         <is>
           <t>20250726T210758.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="7" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="B26" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C26" s="7" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="D26" s="8" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E26" s="8" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="F26" s="8" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="G26" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H26" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="I26" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="J26" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="K26" s="10" t="inlineStr">
+        <is>
+          <t>Dreww :D</t>
+        </is>
+      </c>
+      <c r="L26" s="10" t="inlineStr">
+        <is>
+          <t>Fire Murilø:D🧸</t>
+        </is>
+      </c>
+      <c r="M26" s="10" t="inlineStr">
+        <is>
+          <t>Buk :D</t>
+        </is>
+      </c>
+      <c r="N26" s="10" t="inlineStr">
+        <is>
+          <t>20250726T231751.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="7" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="B27" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C27" s="7" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="D27" s="8" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E27" s="8" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="F27" s="8" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="G27" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H27" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="I27" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="J27" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="K27" s="10" t="inlineStr">
+        <is>
+          <t>Dreww :D</t>
+        </is>
+      </c>
+      <c r="L27" s="10" t="inlineStr">
+        <is>
+          <t>Fire Murilø:D🧸</t>
+        </is>
+      </c>
+      <c r="M27" s="10" t="inlineStr">
+        <is>
+          <t>Buk :D</t>
+        </is>
+      </c>
+      <c r="N27" s="10" t="inlineStr">
+        <is>
+          <t>20250726T231521.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="7" t="inlineStr">
+        <is>
+          <t>GRAY</t>
+        </is>
+      </c>
+      <c r="B28" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="C28" s="7" t="inlineStr">
+        <is>
+          <t>BARLEY</t>
+        </is>
+      </c>
+      <c r="D28" s="8" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E28" s="8" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="F28" s="8" t="inlineStr">
+        <is>
+          <t>ASH</t>
+        </is>
+      </c>
+      <c r="G28" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H28" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="I28" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="J28" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="K28" s="10" t="inlineStr">
+        <is>
+          <t>Dreww :D</t>
+        </is>
+      </c>
+      <c r="L28" s="10" t="inlineStr">
+        <is>
+          <t>Fire Murilø:D🧸</t>
+        </is>
+      </c>
+      <c r="M28" s="10" t="inlineStr">
+        <is>
+          <t>Buk :D</t>
+        </is>
+      </c>
+      <c r="N28" s="10" t="inlineStr">
+        <is>
+          <t>20250726T231234.000Z</t>
         </is>
       </c>
     </row>
@@ -31976,7 +32552,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N102"/>
+  <dimension ref="A3:N105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="T38" sqref="T38"/>
@@ -39181,6 +39757,222 @@
       <c r="N102" s="10" t="inlineStr">
         <is>
           <t>20250726T164737.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="7" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="B103" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C103" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D103" s="8" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="E103" s="8" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F103" s="8" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="G103" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H103" s="10" t="inlineStr">
+        <is>
+          <t>FX|CaueBr</t>
+        </is>
+      </c>
+      <c r="I103" s="10" t="inlineStr">
+        <is>
+          <t>FX|Wesley</t>
+        </is>
+      </c>
+      <c r="J103" s="10" t="inlineStr">
+        <is>
+          <t>FX|REI DO FUT</t>
+        </is>
+      </c>
+      <c r="K103" s="10" t="inlineStr">
+        <is>
+          <t>Satisfyer🌺</t>
+        </is>
+      </c>
+      <c r="L103" s="10" t="inlineStr">
+        <is>
+          <t>Bicho🐦‍🔥</t>
+        </is>
+      </c>
+      <c r="M103" s="10" t="inlineStr">
+        <is>
+          <t>Fv7🐦‍🔥</t>
+        </is>
+      </c>
+      <c r="N103" s="10" t="inlineStr">
+        <is>
+          <t>20250726T232138.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="7" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="B104" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C104" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D104" s="8" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="E104" s="8" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F104" s="8" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="G104" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H104" s="10" t="inlineStr">
+        <is>
+          <t>FX|CaueBr</t>
+        </is>
+      </c>
+      <c r="I104" s="10" t="inlineStr">
+        <is>
+          <t>FX|Wesley</t>
+        </is>
+      </c>
+      <c r="J104" s="10" t="inlineStr">
+        <is>
+          <t>FX|REI DO FUT</t>
+        </is>
+      </c>
+      <c r="K104" s="10" t="inlineStr">
+        <is>
+          <t>Satisfyer🌺</t>
+        </is>
+      </c>
+      <c r="L104" s="10" t="inlineStr">
+        <is>
+          <t>Bicho🐦‍🔥</t>
+        </is>
+      </c>
+      <c r="M104" s="10" t="inlineStr">
+        <is>
+          <t>Fv7🐦‍🔥</t>
+        </is>
+      </c>
+      <c r="N104" s="10" t="inlineStr">
+        <is>
+          <t>20250726T232026.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="7" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="B105" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="C105" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D105" s="8" t="inlineStr">
+        <is>
+          <t>NITA</t>
+        </is>
+      </c>
+      <c r="E105" s="8" t="inlineStr">
+        <is>
+          <t>BERRY</t>
+        </is>
+      </c>
+      <c r="F105" s="8" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="G105" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H105" s="10" t="inlineStr">
+        <is>
+          <t>FX|CaueBr</t>
+        </is>
+      </c>
+      <c r="I105" s="10" t="inlineStr">
+        <is>
+          <t>FX|Wesley</t>
+        </is>
+      </c>
+      <c r="J105" s="10" t="inlineStr">
+        <is>
+          <t>FX|REI DO FUT</t>
+        </is>
+      </c>
+      <c r="K105" s="10" t="inlineStr">
+        <is>
+          <t>Satisfyer🌺</t>
+        </is>
+      </c>
+      <c r="L105" s="10" t="inlineStr">
+        <is>
+          <t>Bicho🐦‍🔥</t>
+        </is>
+      </c>
+      <c r="M105" s="10" t="inlineStr">
+        <is>
+          <t>Fv7🐦‍🔥</t>
+        </is>
+      </c>
+      <c r="N105" s="10" t="inlineStr">
+        <is>
+          <t>20250726T231826.000Z</t>
         </is>
       </c>
     </row>
@@ -59700,7 +60492,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N92"/>
+  <dimension ref="A3:N94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P15" sqref="A4:P15"/>
@@ -66185,6 +66977,150 @@
       <c r="N92" s="10" t="inlineStr">
         <is>
           <t>20250726T205220.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="7" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="B93" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C93" s="7" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D93" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E93" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F93" s="8" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="G93" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H93" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Derrp</t>
+        </is>
+      </c>
+      <c r="I93" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Jubileubr</t>
+        </is>
+      </c>
+      <c r="J93" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Loko</t>
+        </is>
+      </c>
+      <c r="K93" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="L93" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="M93" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="N93" s="10" t="inlineStr">
+        <is>
+          <t>20250726T231102.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="7" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="B94" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="C94" s="7" t="inlineStr">
+        <is>
+          <t>MEEPLE</t>
+        </is>
+      </c>
+      <c r="D94" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="E94" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F94" s="8" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="G94" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H94" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Derrp</t>
+        </is>
+      </c>
+      <c r="I94" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Jubileubr</t>
+        </is>
+      </c>
+      <c r="J94" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Loko</t>
+        </is>
+      </c>
+      <c r="K94" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="L94" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="M94" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="N94" s="10" t="inlineStr">
+        <is>
+          <t>20250726T230912.000Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-27 01:58:40)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -10637,7 +10637,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N21"/>
+  <dimension ref="A3:N23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N19" sqref="N19"/>
@@ -12010,6 +12010,150 @@
       <c r="N21" s="10" t="inlineStr">
         <is>
           <t>20250726T215857.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="7" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="B22" s="7" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="C22" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D22" s="8" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="E22" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F22" s="8" t="inlineStr">
+        <is>
+          <t>LOLA</t>
+        </is>
+      </c>
+      <c r="G22" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H22" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Jubileubr</t>
+        </is>
+      </c>
+      <c r="I22" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Derrp</t>
+        </is>
+      </c>
+      <c r="J22" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Loko</t>
+        </is>
+      </c>
+      <c r="K22" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="L22" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="M22" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="N22" s="10" t="inlineStr">
+        <is>
+          <t>20250726T233222.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="7" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="B23" s="7" t="inlineStr">
+        <is>
+          <t>ANGELO</t>
+        </is>
+      </c>
+      <c r="C23" s="7" t="inlineStr">
+        <is>
+          <t>CROW</t>
+        </is>
+      </c>
+      <c r="D23" s="8" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="E23" s="8" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="F23" s="8" t="inlineStr">
+        <is>
+          <t>LOLA</t>
+        </is>
+      </c>
+      <c r="G23" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H23" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Jubileubr</t>
+        </is>
+      </c>
+      <c r="I23" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Derrp</t>
+        </is>
+      </c>
+      <c r="J23" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Loko</t>
+        </is>
+      </c>
+      <c r="K23" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Rhz</t>
+        </is>
+      </c>
+      <c r="L23" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Kr</t>
+        </is>
+      </c>
+      <c r="M23" s="10" t="inlineStr">
+        <is>
+          <t>SKC|Prozy</t>
+        </is>
+      </c>
+      <c r="N23" s="10" t="inlineStr">
+        <is>
+          <t>20250726T232932.000Z</t>
         </is>
       </c>
     </row>
@@ -13915,7 +14059,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N15"/>
+  <dimension ref="A3:N18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
@@ -14856,6 +15000,222 @@
       <c r="N15" s="10" t="inlineStr">
         <is>
           <t>20250725T231223.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="7" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="B16" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="C16" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="D16" s="8" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="E16" s="8" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="F16" s="8" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="G16" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H16" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="I16" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="J16" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="K16" s="10" t="inlineStr">
+        <is>
+          <t>Fire Murilø:D🧸</t>
+        </is>
+      </c>
+      <c r="L16" s="10" t="inlineStr">
+        <is>
+          <t>Dreww :D</t>
+        </is>
+      </c>
+      <c r="M16" s="10" t="inlineStr">
+        <is>
+          <t>Buk :D</t>
+        </is>
+      </c>
+      <c r="N16" s="10" t="inlineStr">
+        <is>
+          <t>20250726T233848.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="7" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="B17" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="C17" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="D17" s="8" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="E17" s="8" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="F17" s="8" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="G17" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H17" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="I17" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="J17" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="K17" s="10" t="inlineStr">
+        <is>
+          <t>Fire Murilø:D🧸</t>
+        </is>
+      </c>
+      <c r="L17" s="10" t="inlineStr">
+        <is>
+          <t>Dreww :D</t>
+        </is>
+      </c>
+      <c r="M17" s="10" t="inlineStr">
+        <is>
+          <t>Buk :D</t>
+        </is>
+      </c>
+      <c r="N17" s="10" t="inlineStr">
+        <is>
+          <t>20250726T233557.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="7" t="inlineStr">
+        <is>
+          <t>BULL</t>
+        </is>
+      </c>
+      <c r="B18" s="7" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="C18" s="7" t="inlineStr">
+        <is>
+          <t>KIT</t>
+        </is>
+      </c>
+      <c r="D18" s="8" t="inlineStr">
+        <is>
+          <t>TARA</t>
+        </is>
+      </c>
+      <c r="E18" s="8" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="F18" s="8" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="G18" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H18" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="I18" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="J18" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="K18" s="10" t="inlineStr">
+        <is>
+          <t>Fire Murilø:D🧸</t>
+        </is>
+      </c>
+      <c r="L18" s="10" t="inlineStr">
+        <is>
+          <t>Dreww :D</t>
+        </is>
+      </c>
+      <c r="M18" s="10" t="inlineStr">
+        <is>
+          <t>Buk :D</t>
+        </is>
+      </c>
+      <c r="N18" s="10" t="inlineStr">
+        <is>
+          <t>20250726T233435.000Z</t>
         </is>
       </c>
     </row>
@@ -16185,7 +16545,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N29"/>
+  <dimension ref="A3:N31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P8" sqref="A4:P8"/>
@@ -18134,6 +18494,150 @@
       <c r="N29" s="10" t="inlineStr">
         <is>
           <t>20250726T121725.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B30" s="7" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="C30" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D30" s="8" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E30" s="8" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="F30" s="8" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G30" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H30" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="I30" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="J30" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="K30" s="10" t="inlineStr">
+        <is>
+          <t>Fire Murilø:D🧸</t>
+        </is>
+      </c>
+      <c r="L30" s="10" t="inlineStr">
+        <is>
+          <t>Dreww :D</t>
+        </is>
+      </c>
+      <c r="M30" s="10" t="inlineStr">
+        <is>
+          <t>Buk :D</t>
+        </is>
+      </c>
+      <c r="N30" s="10" t="inlineStr">
+        <is>
+          <t>20250726T235824.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B31" s="7" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="C31" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D31" s="8" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E31" s="8" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="F31" s="8" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G31" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H31" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="I31" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="J31" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="K31" s="10" t="inlineStr">
+        <is>
+          <t>Fire Murilø:D🧸</t>
+        </is>
+      </c>
+      <c r="L31" s="10" t="inlineStr">
+        <is>
+          <t>Dreww :D</t>
+        </is>
+      </c>
+      <c r="M31" s="10" t="inlineStr">
+        <is>
+          <t>Buk :D</t>
+        </is>
+      </c>
+      <c r="N31" s="10" t="inlineStr">
+        <is>
+          <t>20250726T235614.000Z</t>
         </is>
       </c>
     </row>
@@ -67135,7 +67639,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N69"/>
+  <dimension ref="A3:N71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R15" sqref="R15"/>
@@ -71967,6 +72471,150 @@
         </is>
       </c>
     </row>
+    <row r="70">
+      <c r="A70" s="7" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B70" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C70" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D70" s="8" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E70" s="8" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="F70" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G70" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H70" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="I70" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="J70" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="K70" s="10" t="inlineStr">
+        <is>
+          <t>Dreww :D</t>
+        </is>
+      </c>
+      <c r="L70" s="10" t="inlineStr">
+        <is>
+          <t>Buk :D</t>
+        </is>
+      </c>
+      <c r="M70" s="10" t="inlineStr">
+        <is>
+          <t>Fire Murilø:D🧸</t>
+        </is>
+      </c>
+      <c r="N70" s="10" t="inlineStr">
+        <is>
+          <t>20250726T234816.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="7" t="inlineStr">
+        <is>
+          <t>CARL</t>
+        </is>
+      </c>
+      <c r="B71" s="7" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="C71" s="7" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="D71" s="8" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E71" s="8" t="inlineStr">
+        <is>
+          <t>MOE</t>
+        </is>
+      </c>
+      <c r="F71" s="8" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="G71" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H71" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="I71" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="J71" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="K71" s="10" t="inlineStr">
+        <is>
+          <t>Dreww :D</t>
+        </is>
+      </c>
+      <c r="L71" s="10" t="inlineStr">
+        <is>
+          <t>Buk :D</t>
+        </is>
+      </c>
+      <c r="M71" s="10" t="inlineStr">
+        <is>
+          <t>Fire Murilø:D🧸</t>
+        </is>
+      </c>
+      <c r="N71" s="10" t="inlineStr">
+        <is>
+          <t>20250726T234617.000Z</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización automática de scrims_actualizado.xlsx (2025-07-27 02:30:01)
</commit_message>
<xml_diff>
--- a/scrims_actualizado.xlsx
+++ b/scrims_actualizado.xlsx
@@ -9250,7 +9250,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N21"/>
+  <dimension ref="A3:N23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M21" sqref="M21"/>
@@ -10623,6 +10623,150 @@
       <c r="N21" s="10" t="inlineStr">
         <is>
           <t>20250726T222734.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="B22" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="C22" s="7" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="D22" s="8" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E22" s="8" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="F22" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G22" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H22" s="10" t="inlineStr">
+        <is>
+          <t>BKB|❄️IC€CRØW❄️</t>
+        </is>
+      </c>
+      <c r="I22" s="10" t="inlineStr">
+        <is>
+          <t>YT:BrabaoBS🎩</t>
+        </is>
+      </c>
+      <c r="J22" s="10" t="inlineStr">
+        <is>
+          <t>Golden💘Mai</t>
+        </is>
+      </c>
+      <c r="K22" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="L22" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="M22" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="N22" s="10" t="inlineStr">
+        <is>
+          <t>20250727T002931.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="7" t="inlineStr">
+        <is>
+          <t>R-T</t>
+        </is>
+      </c>
+      <c r="B23" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="C23" s="7" t="inlineStr">
+        <is>
+          <t>JAE-YONG</t>
+        </is>
+      </c>
+      <c r="D23" s="8" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="E23" s="8" t="inlineStr">
+        <is>
+          <t>TICK</t>
+        </is>
+      </c>
+      <c r="F23" s="8" t="inlineStr">
+        <is>
+          <t>GUS</t>
+        </is>
+      </c>
+      <c r="G23" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H23" s="10" t="inlineStr">
+        <is>
+          <t>BKB|❄️IC€CRØW❄️</t>
+        </is>
+      </c>
+      <c r="I23" s="10" t="inlineStr">
+        <is>
+          <t>YT:BrabaoBS🎩</t>
+        </is>
+      </c>
+      <c r="J23" s="10" t="inlineStr">
+        <is>
+          <t>Golden💘Mai</t>
+        </is>
+      </c>
+      <c r="K23" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="L23" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="M23" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="N23" s="10" t="inlineStr">
+        <is>
+          <t>20250727T002756.000Z</t>
         </is>
       </c>
     </row>
@@ -16545,7 +16689,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N31"/>
+  <dimension ref="A3:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P8" sqref="A4:P8"/>
@@ -18638,6 +18782,78 @@
       <c r="N31" s="10" t="inlineStr">
         <is>
           <t>20250726T235614.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="7" t="inlineStr">
+        <is>
+          <t>DRACO</t>
+        </is>
+      </c>
+      <c r="B32" s="7" t="inlineStr">
+        <is>
+          <t>RUFFS</t>
+        </is>
+      </c>
+      <c r="C32" s="7" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="D32" s="8" t="inlineStr">
+        <is>
+          <t>LILY</t>
+        </is>
+      </c>
+      <c r="E32" s="8" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="F32" s="8" t="inlineStr">
+        <is>
+          <t>HANK</t>
+        </is>
+      </c>
+      <c r="G32" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H32" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Pekka</t>
+        </is>
+      </c>
+      <c r="I32" s="10" t="inlineStr">
+        <is>
+          <t>CASA|Mohtep</t>
+        </is>
+      </c>
+      <c r="J32" s="10" t="inlineStr">
+        <is>
+          <t>Doritos🐉</t>
+        </is>
+      </c>
+      <c r="K32" s="10" t="inlineStr">
+        <is>
+          <t>Fire Murilø:D🧸</t>
+        </is>
+      </c>
+      <c r="L32" s="10" t="inlineStr">
+        <is>
+          <t>Dreww :D</t>
+        </is>
+      </c>
+      <c r="M32" s="10" t="inlineStr">
+        <is>
+          <t>Buk :D</t>
+        </is>
+      </c>
+      <c r="N32" s="10" t="inlineStr">
+        <is>
+          <t>20250727T000209.000Z</t>
         </is>
       </c>
     </row>
@@ -19319,7 +19535,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N21"/>
+  <dimension ref="A3:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="S12" sqref="S12"/>
@@ -20692,6 +20908,150 @@
       <c r="N21" s="10" t="inlineStr">
         <is>
           <t>20250726T020551.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="7" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="B22" s="7" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="C22" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D22" s="8" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="E22" s="8" t="inlineStr">
+        <is>
+          <t>PEARL</t>
+        </is>
+      </c>
+      <c r="F22" s="8" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="G22" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H22" s="10" t="inlineStr">
+        <is>
+          <t>Fire Murilø:D🧸</t>
+        </is>
+      </c>
+      <c r="I22" s="10" t="inlineStr">
+        <is>
+          <t>Dreww :D</t>
+        </is>
+      </c>
+      <c r="J22" s="10" t="inlineStr">
+        <is>
+          <t>Buk :D</t>
+        </is>
+      </c>
+      <c r="K22" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Derrp</t>
+        </is>
+      </c>
+      <c r="L22" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Jubileubr</t>
+        </is>
+      </c>
+      <c r="M22" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Loko</t>
+        </is>
+      </c>
+      <c r="N22" s="10" t="inlineStr">
+        <is>
+          <t>20250727T002855.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="7" t="inlineStr">
+        <is>
+          <t>BO</t>
+        </is>
+      </c>
+      <c r="B23" s="7" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="C23" s="7" t="inlineStr">
+        <is>
+          <t>LUMI</t>
+        </is>
+      </c>
+      <c r="D23" s="8" t="inlineStr">
+        <is>
+          <t>FINX</t>
+        </is>
+      </c>
+      <c r="E23" s="8" t="inlineStr">
+        <is>
+          <t>PEARL</t>
+        </is>
+      </c>
+      <c r="F23" s="8" t="inlineStr">
+        <is>
+          <t>SANDY</t>
+        </is>
+      </c>
+      <c r="G23" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H23" s="10" t="inlineStr">
+        <is>
+          <t>Fire Murilø:D🧸</t>
+        </is>
+      </c>
+      <c r="I23" s="10" t="inlineStr">
+        <is>
+          <t>Dreww :D</t>
+        </is>
+      </c>
+      <c r="J23" s="10" t="inlineStr">
+        <is>
+          <t>Buk :D</t>
+        </is>
+      </c>
+      <c r="K23" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Derrp</t>
+        </is>
+      </c>
+      <c r="L23" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Jubileubr</t>
+        </is>
+      </c>
+      <c r="M23" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Loko</t>
+        </is>
+      </c>
+      <c r="N23" s="10" t="inlineStr">
+        <is>
+          <t>20250727T002557.000Z</t>
         </is>
       </c>
     </row>
@@ -33056,7 +33416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N105"/>
+  <dimension ref="A3:N108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="T38" sqref="T38"/>
@@ -40477,6 +40837,222 @@
       <c r="N105" s="10" t="inlineStr">
         <is>
           <t>20250726T231826.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="7" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B106" s="7" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="C106" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D106" s="8" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="E106" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F106" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G106" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H106" s="10" t="inlineStr">
+        <is>
+          <t>Dreww :D</t>
+        </is>
+      </c>
+      <c r="I106" s="10" t="inlineStr">
+        <is>
+          <t>Buk :D</t>
+        </is>
+      </c>
+      <c r="J106" s="10" t="inlineStr">
+        <is>
+          <t>Fire Murilø:D🧸</t>
+        </is>
+      </c>
+      <c r="K106" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Derrp</t>
+        </is>
+      </c>
+      <c r="L106" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Loko</t>
+        </is>
+      </c>
+      <c r="M106" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Jubileubr</t>
+        </is>
+      </c>
+      <c r="N106" s="10" t="inlineStr">
+        <is>
+          <t>20250727T001934.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="7" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B107" s="7" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="C107" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D107" s="8" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="E107" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F107" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G107" s="11" t="inlineStr">
+        <is>
+          <t>Equipo 1</t>
+        </is>
+      </c>
+      <c r="H107" s="10" t="inlineStr">
+        <is>
+          <t>Dreww :D</t>
+        </is>
+      </c>
+      <c r="I107" s="10" t="inlineStr">
+        <is>
+          <t>Buk :D</t>
+        </is>
+      </c>
+      <c r="J107" s="10" t="inlineStr">
+        <is>
+          <t>Fire Murilø:D🧸</t>
+        </is>
+      </c>
+      <c r="K107" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Derrp</t>
+        </is>
+      </c>
+      <c r="L107" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Loko</t>
+        </is>
+      </c>
+      <c r="M107" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Jubileubr</t>
+        </is>
+      </c>
+      <c r="N107" s="10" t="inlineStr">
+        <is>
+          <t>20250727T001825.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="7" t="inlineStr">
+        <is>
+          <t>AMBER</t>
+        </is>
+      </c>
+      <c r="B108" s="7" t="inlineStr">
+        <is>
+          <t>MICO</t>
+        </is>
+      </c>
+      <c r="C108" s="7" t="inlineStr">
+        <is>
+          <t>CORDELIUS</t>
+        </is>
+      </c>
+      <c r="D108" s="8" t="inlineStr">
+        <is>
+          <t>MELODIE</t>
+        </is>
+      </c>
+      <c r="E108" s="8" t="inlineStr">
+        <is>
+          <t>CHARLIE</t>
+        </is>
+      </c>
+      <c r="F108" s="8" t="inlineStr">
+        <is>
+          <t>KAZE</t>
+        </is>
+      </c>
+      <c r="G108" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H108" s="10" t="inlineStr">
+        <is>
+          <t>Dreww :D</t>
+        </is>
+      </c>
+      <c r="I108" s="10" t="inlineStr">
+        <is>
+          <t>Buk :D</t>
+        </is>
+      </c>
+      <c r="J108" s="10" t="inlineStr">
+        <is>
+          <t>Fire Murilø:D🧸</t>
+        </is>
+      </c>
+      <c r="K108" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Derrp</t>
+        </is>
+      </c>
+      <c r="L108" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Loko</t>
+        </is>
+      </c>
+      <c r="M108" s="10" t="inlineStr">
+        <is>
+          <t>BC*|Jubileubr</t>
+        </is>
+      </c>
+      <c r="N108" s="10" t="inlineStr">
+        <is>
+          <t>20250727T001620.000Z</t>
         </is>
       </c>
     </row>
@@ -40491,7 +41067,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:N104"/>
+  <dimension ref="A3:N107"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="P38" sqref="P38"/>
@@ -47840,6 +48416,222 @@
       <c r="N104" s="10" t="inlineStr">
         <is>
           <t>20250726T162856.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="7" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="B105" s="7" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="C105" s="7" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="D105" s="8" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="E105" s="8" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="F105" s="8" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="G105" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H105" s="10" t="inlineStr">
+        <is>
+          <t>YT:BrabaoBS🎩</t>
+        </is>
+      </c>
+      <c r="I105" s="10" t="inlineStr">
+        <is>
+          <t>Golden💘Mai</t>
+        </is>
+      </c>
+      <c r="J105" s="10" t="inlineStr">
+        <is>
+          <t>BKB|❄️IC€CRØW❄️</t>
+        </is>
+      </c>
+      <c r="K105" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="L105" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="M105" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="N105" s="10" t="inlineStr">
+        <is>
+          <t>20250727T002052.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="7" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="B106" s="7" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+      <c r="C106" s="7" t="inlineStr">
+        <is>
+          <t>MORTIS</t>
+        </is>
+      </c>
+      <c r="D106" s="8" t="inlineStr">
+        <is>
+          <t>WILLOW</t>
+        </is>
+      </c>
+      <c r="E106" s="8" t="inlineStr">
+        <is>
+          <t>MR. P</t>
+        </is>
+      </c>
+      <c r="F106" s="8" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="G106" s="9" t="inlineStr">
+        <is>
+          <t>Equipo 2</t>
+        </is>
+      </c>
+      <c r="H106" s="10" t="inlineStr">
+        <is>
+          <t>YT:BrabaoBS🎩</t>
+        </is>
+      </c>
+      <c r="I106" s="10" t="inlineStr">
+        <is>
+          <t>Golden💘Mai</t>
+        </is>
+      </c>
+      <c r="J106" s="10" t="inlineStr">
+        <is>
+          <t>BKB|❄️IC€CRØW❄️</t>
+        </is>
+      </c>
+      <c r="K106" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|Edinho</t>
+        </is>
+      </c>
+      <c r="L106" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|KaioDog</t>
+        </is>
+      </c>
+      <c r="M106" s="10" t="inlineStr">
+        <is>
+          <t>LOUD|FireCrow</t>
+        </is>
+      </c>
+      <c r="N106" s="10" t="inlineStr">
+        <is>
+          <t>20250727T001831.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="7" t="inlineStr">
+        <is>
+          <t>GENE</t>
+        </is>
+      </c>
+      <c r="B107" s="7" t="inlineStr">
+        <is>
+          <t>JANET</t>
+        </is>
+      </c>
+  